<commit_message>
Saving and reading VOX delay.
</commit_message>
<xml_diff>
--- a/docs/UV K5 EEPROM.xlsx
+++ b/docs/UV K5 EEPROM.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1480" uniqueCount="1478">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1481" uniqueCount="1479">
   <si>
     <t xml:space="preserve">00</t>
   </si>
@@ -2092,6 +2092,9 @@
     <t xml:space="preserve">MIC Sensitivity</t>
   </si>
   <si>
+    <t xml:space="preserve">BACKLIGHT Max/Min</t>
+  </si>
+  <si>
     <t xml:space="preserve">MDF</t>
   </si>
   <si>
@@ -2185,7 +2188,7 @@
     <t xml:space="preserve">0x0EA0</t>
   </si>
   <si>
-    <t xml:space="preserve">VOICE PROMPT</t>
+    <t xml:space="preserve">VOX Delay</t>
   </si>
   <si>
     <t xml:space="preserve">AL-MOD</t>
@@ -4556,7 +4559,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -4582,6 +4585,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -4676,11 +4683,11 @@
   </sheetPr>
   <dimension ref="A1:Z1001"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A206" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="N235" activeCellId="0" sqref="N235"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A208" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F227" activeCellId="0" sqref="F227"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.66015625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.6796875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1"/>
@@ -12568,27 +12575,29 @@
       <c r="I233" s="4" t="s">
         <v>689</v>
       </c>
-      <c r="J233" s="5"/>
+      <c r="J233" s="6" t="s">
+        <v>690</v>
+      </c>
       <c r="K233" s="4" t="s">
-        <v>690</v>
+        <v>691</v>
       </c>
       <c r="L233" s="4" t="s">
-        <v>691</v>
+        <v>692</v>
       </c>
       <c r="M233" s="4" t="s">
-        <v>692</v>
+        <v>693</v>
       </c>
       <c r="N233" s="4" t="s">
-        <v>693</v>
+        <v>694</v>
       </c>
       <c r="O233" s="4" t="s">
-        <v>694</v>
+        <v>695</v>
       </c>
       <c r="P233" s="4" t="s">
-        <v>695</v>
+        <v>696</v>
       </c>
       <c r="Q233" s="4" t="s">
-        <v>696</v>
+        <v>697</v>
       </c>
       <c r="R233" s="1"/>
       <c r="S233" s="1"/>
@@ -12602,40 +12611,40 @@
     </row>
     <row r="234" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A234" s="2" t="s">
-        <v>697</v>
+        <v>698</v>
       </c>
       <c r="B234" s="4" t="s">
-        <v>698</v>
+        <v>699</v>
       </c>
       <c r="C234" s="4" t="s">
-        <v>699</v>
+        <v>700</v>
       </c>
       <c r="D234" s="4" t="s">
-        <v>700</v>
+        <v>701</v>
       </c>
       <c r="E234" s="4" t="s">
-        <v>701</v>
+        <v>702</v>
       </c>
       <c r="F234" s="4" t="s">
-        <v>702</v>
+        <v>703</v>
       </c>
       <c r="G234" s="4" t="s">
-        <v>703</v>
+        <v>704</v>
       </c>
       <c r="H234" s="4" t="s">
-        <v>704</v>
+        <v>705</v>
       </c>
       <c r="I234" s="4" t="s">
-        <v>705</v>
+        <v>706</v>
       </c>
       <c r="J234" s="4" t="s">
-        <v>706</v>
+        <v>707</v>
       </c>
       <c r="K234" s="4" t="s">
-        <v>707</v>
+        <v>708</v>
       </c>
       <c r="L234" s="4" t="s">
-        <v>708</v>
+        <v>709</v>
       </c>
       <c r="M234" s="5"/>
       <c r="N234" s="5"/>
@@ -12654,44 +12663,44 @@
     </row>
     <row r="235" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A235" s="2" t="s">
-        <v>709</v>
+        <v>710</v>
       </c>
       <c r="B235" s="4" t="s">
-        <v>710</v>
+        <v>711</v>
       </c>
       <c r="C235" s="4" t="s">
-        <v>711</v>
+        <v>712</v>
       </c>
       <c r="D235" s="4" t="s">
-        <v>712</v>
+        <v>713</v>
       </c>
       <c r="E235" s="4" t="s">
-        <v>713</v>
+        <v>714</v>
       </c>
       <c r="F235" s="4" t="s">
-        <v>714</v>
+        <v>715</v>
       </c>
       <c r="G235" s="4" t="s">
-        <v>715</v>
+        <v>716</v>
       </c>
       <c r="H235" s="4" t="s">
-        <v>716</v>
+        <v>717</v>
       </c>
       <c r="I235" s="4" t="s">
-        <v>717</v>
+        <v>718</v>
       </c>
       <c r="J235" s="3" t="s">
-        <v>718</v>
+        <v>719</v>
       </c>
       <c r="K235" s="3"/>
       <c r="L235" s="3"/>
       <c r="M235" s="3"/>
-      <c r="N235" s="6" t="s">
-        <v>719</v>
-      </c>
-      <c r="O235" s="6"/>
-      <c r="P235" s="6"/>
-      <c r="Q235" s="6"/>
+      <c r="N235" s="7" t="s">
+        <v>720</v>
+      </c>
+      <c r="O235" s="7"/>
+      <c r="P235" s="7"/>
+      <c r="Q235" s="7"/>
       <c r="R235" s="1"/>
       <c r="S235" s="1"/>
       <c r="T235" s="1"/>
@@ -12704,10 +12713,10 @@
     </row>
     <row r="236" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A236" s="2" t="s">
-        <v>720</v>
+        <v>721</v>
       </c>
       <c r="B236" s="4" t="s">
-        <v>721</v>
+        <v>722</v>
       </c>
       <c r="C236" s="5"/>
       <c r="D236" s="5"/>
@@ -12717,16 +12726,16 @@
       <c r="H236" s="5"/>
       <c r="I236" s="5"/>
       <c r="J236" s="4" t="s">
-        <v>722</v>
+        <v>723</v>
       </c>
       <c r="K236" s="4" t="s">
-        <v>723</v>
+        <v>724</v>
       </c>
       <c r="L236" s="4" t="s">
-        <v>724</v>
+        <v>725</v>
       </c>
       <c r="M236" s="4" t="s">
-        <v>725</v>
+        <v>726</v>
       </c>
       <c r="N236" s="5"/>
       <c r="O236" s="5"/>
@@ -12744,10 +12753,10 @@
     </row>
     <row r="237" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A237" s="2" t="s">
-        <v>726</v>
+        <v>727</v>
       </c>
       <c r="B237" s="3" t="s">
-        <v>727</v>
+        <v>728</v>
       </c>
       <c r="C237" s="3"/>
       <c r="D237" s="3"/>
@@ -12776,10 +12785,10 @@
     </row>
     <row r="238" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A238" s="2" t="s">
-        <v>728</v>
+        <v>729</v>
       </c>
       <c r="B238" s="3" t="s">
-        <v>729</v>
+        <v>730</v>
       </c>
       <c r="C238" s="3"/>
       <c r="D238" s="3"/>
@@ -12808,40 +12817,40 @@
     </row>
     <row r="239" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A239" s="2" t="s">
-        <v>730</v>
+        <v>731</v>
       </c>
       <c r="B239" s="4" t="s">
-        <v>731</v>
+        <v>732</v>
       </c>
       <c r="C239" s="4" t="s">
-        <v>732</v>
+        <v>733</v>
       </c>
       <c r="D239" s="4" t="s">
-        <v>733</v>
+        <v>734</v>
       </c>
       <c r="E239" s="4" t="s">
-        <v>734</v>
+        <v>735</v>
       </c>
       <c r="F239" s="4" t="s">
-        <v>735</v>
+        <v>736</v>
       </c>
       <c r="G239" s="4" t="s">
-        <v>736</v>
+        <v>737</v>
       </c>
       <c r="H239" s="4" t="s">
-        <v>737</v>
+        <v>738</v>
       </c>
       <c r="I239" s="4" t="s">
-        <v>738</v>
+        <v>739</v>
       </c>
       <c r="J239" s="4" t="s">
-        <v>739</v>
+        <v>740</v>
       </c>
       <c r="K239" s="4" t="s">
-        <v>740</v>
+        <v>741</v>
       </c>
       <c r="L239" s="4" t="s">
-        <v>741</v>
+        <v>742</v>
       </c>
       <c r="M239" s="5"/>
       <c r="N239" s="5"/>
@@ -12860,10 +12869,10 @@
     </row>
     <row r="240" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A240" s="2" t="s">
-        <v>742</v>
+        <v>743</v>
       </c>
       <c r="B240" s="3" t="s">
-        <v>743</v>
+        <v>744</v>
       </c>
       <c r="C240" s="3"/>
       <c r="D240" s="3"/>
@@ -12873,7 +12882,7 @@
       <c r="H240" s="3"/>
       <c r="I240" s="3"/>
       <c r="J240" s="3" t="s">
-        <v>744</v>
+        <v>745</v>
       </c>
       <c r="K240" s="3"/>
       <c r="L240" s="3"/>
@@ -12894,10 +12903,10 @@
     </row>
     <row r="241" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A241" s="2" t="s">
-        <v>745</v>
+        <v>746</v>
       </c>
       <c r="B241" s="3" t="s">
-        <v>746</v>
+        <v>747</v>
       </c>
       <c r="C241" s="3"/>
       <c r="D241" s="3"/>
@@ -12907,7 +12916,7 @@
       <c r="H241" s="3"/>
       <c r="I241" s="3"/>
       <c r="J241" s="3" t="s">
-        <v>747</v>
+        <v>748</v>
       </c>
       <c r="K241" s="3"/>
       <c r="L241" s="3"/>
@@ -12928,10 +12937,10 @@
     </row>
     <row r="242" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A242" s="2" t="s">
+        <v>749</v>
+      </c>
+      <c r="B242" s="3" t="s">
         <v>748</v>
-      </c>
-      <c r="B242" s="3" t="s">
-        <v>747</v>
       </c>
       <c r="C242" s="3"/>
       <c r="D242" s="3"/>
@@ -12941,7 +12950,7 @@
       <c r="H242" s="3"/>
       <c r="I242" s="3"/>
       <c r="J242" s="3" t="s">
-        <v>749</v>
+        <v>750</v>
       </c>
       <c r="K242" s="3"/>
       <c r="L242" s="3"/>
@@ -12962,10 +12971,10 @@
     </row>
     <row r="243" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A243" s="2" t="s">
+        <v>751</v>
+      </c>
+      <c r="B243" s="3" t="s">
         <v>750</v>
-      </c>
-      <c r="B243" s="3" t="s">
-        <v>749</v>
       </c>
       <c r="C243" s="3"/>
       <c r="D243" s="3"/>
@@ -12975,25 +12984,25 @@
       <c r="H243" s="3"/>
       <c r="I243" s="3"/>
       <c r="J243" s="4" t="s">
-        <v>751</v>
+        <v>752</v>
       </c>
       <c r="K243" s="4" t="s">
-        <v>752</v>
+        <v>753</v>
       </c>
       <c r="L243" s="4" t="s">
-        <v>753</v>
+        <v>754</v>
       </c>
       <c r="M243" s="4" t="s">
-        <v>754</v>
+        <v>755</v>
       </c>
       <c r="N243" s="4" t="s">
-        <v>755</v>
+        <v>756</v>
       </c>
       <c r="O243" s="4" t="s">
-        <v>756</v>
+        <v>757</v>
       </c>
       <c r="P243" s="4" t="s">
-        <v>757</v>
+        <v>758</v>
       </c>
       <c r="Q243" s="5"/>
       <c r="R243" s="1"/>
@@ -13008,7 +13017,7 @@
     </row>
     <row r="244" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A244" s="2" t="s">
-        <v>758</v>
+        <v>759</v>
       </c>
       <c r="B244" s="5"/>
       <c r="C244" s="5"/>
@@ -13038,10 +13047,10 @@
     </row>
     <row r="245" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A245" s="2" t="s">
-        <v>759</v>
+        <v>760</v>
       </c>
       <c r="B245" s="3" t="s">
-        <v>760</v>
+        <v>761</v>
       </c>
       <c r="C245" s="3"/>
       <c r="D245" s="3"/>
@@ -13070,28 +13079,28 @@
     </row>
     <row r="246" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A246" s="2" t="s">
-        <v>761</v>
+        <v>762</v>
       </c>
       <c r="B246" s="4" t="s">
-        <v>762</v>
+        <v>763</v>
       </c>
       <c r="C246" s="4" t="s">
-        <v>763</v>
+        <v>764</v>
       </c>
       <c r="D246" s="4" t="s">
-        <v>764</v>
+        <v>765</v>
       </c>
       <c r="E246" s="4" t="s">
-        <v>765</v>
+        <v>766</v>
       </c>
       <c r="F246" s="4" t="s">
-        <v>766</v>
+        <v>767</v>
       </c>
       <c r="G246" s="4" t="s">
-        <v>767</v>
+        <v>768</v>
       </c>
       <c r="H246" s="4" t="s">
-        <v>768</v>
+        <v>769</v>
       </c>
       <c r="I246" s="5"/>
       <c r="J246" s="5"/>
@@ -13114,10 +13123,10 @@
     </row>
     <row r="247" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A247" s="2" t="s">
-        <v>769</v>
+        <v>770</v>
       </c>
       <c r="B247" s="3" t="s">
-        <v>770</v>
+        <v>771</v>
       </c>
       <c r="C247" s="3"/>
       <c r="D247" s="3"/>
@@ -13146,10 +13155,10 @@
     </row>
     <row r="248" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A248" s="2" t="s">
-        <v>771</v>
+        <v>772</v>
       </c>
       <c r="B248" s="3" t="s">
-        <v>772</v>
+        <v>773</v>
       </c>
       <c r="C248" s="3"/>
       <c r="D248" s="3"/>
@@ -13178,10 +13187,10 @@
     </row>
     <row r="249" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A249" s="2" t="s">
-        <v>773</v>
+        <v>774</v>
       </c>
       <c r="B249" s="3" t="s">
-        <v>774</v>
+        <v>775</v>
       </c>
       <c r="C249" s="3"/>
       <c r="D249" s="3"/>
@@ -13210,10 +13219,10 @@
     </row>
     <row r="250" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A250" s="2" t="s">
-        <v>775</v>
+        <v>776</v>
       </c>
       <c r="B250" s="3" t="s">
-        <v>776</v>
+        <v>777</v>
       </c>
       <c r="C250" s="3"/>
       <c r="D250" s="3"/>
@@ -13242,10 +13251,10 @@
     </row>
     <row r="251" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A251" s="2" t="s">
-        <v>777</v>
+        <v>778</v>
       </c>
       <c r="B251" s="3" t="s">
-        <v>778</v>
+        <v>779</v>
       </c>
       <c r="C251" s="3"/>
       <c r="D251" s="3"/>
@@ -13274,10 +13283,10 @@
     </row>
     <row r="252" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A252" s="2" t="s">
-        <v>779</v>
+        <v>780</v>
       </c>
       <c r="B252" s="3" t="s">
-        <v>780</v>
+        <v>781</v>
       </c>
       <c r="C252" s="3"/>
       <c r="D252" s="3"/>
@@ -13306,10 +13315,10 @@
     </row>
     <row r="253" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A253" s="2" t="s">
-        <v>781</v>
+        <v>782</v>
       </c>
       <c r="B253" s="3" t="s">
-        <v>782</v>
+        <v>783</v>
       </c>
       <c r="C253" s="3"/>
       <c r="D253" s="3"/>
@@ -13338,10 +13347,10 @@
     </row>
     <row r="254" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A254" s="2" t="s">
-        <v>783</v>
+        <v>784</v>
       </c>
       <c r="B254" s="3" t="s">
-        <v>784</v>
+        <v>785</v>
       </c>
       <c r="C254" s="3"/>
       <c r="D254" s="3"/>
@@ -13370,10 +13379,10 @@
     </row>
     <row r="255" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A255" s="2" t="s">
-        <v>785</v>
+        <v>786</v>
       </c>
       <c r="B255" s="3" t="s">
-        <v>786</v>
+        <v>787</v>
       </c>
       <c r="C255" s="3"/>
       <c r="D255" s="3"/>
@@ -13402,10 +13411,10 @@
     </row>
     <row r="256" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A256" s="2" t="s">
-        <v>787</v>
+        <v>788</v>
       </c>
       <c r="B256" s="3" t="s">
-        <v>788</v>
+        <v>789</v>
       </c>
       <c r="C256" s="3"/>
       <c r="D256" s="3"/>
@@ -13434,10 +13443,10 @@
     </row>
     <row r="257" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A257" s="2" t="s">
-        <v>789</v>
+        <v>790</v>
       </c>
       <c r="B257" s="3" t="s">
-        <v>790</v>
+        <v>791</v>
       </c>
       <c r="C257" s="3"/>
       <c r="D257" s="3"/>
@@ -13466,10 +13475,10 @@
     </row>
     <row r="258" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A258" s="2" t="s">
-        <v>791</v>
+        <v>792</v>
       </c>
       <c r="B258" s="3" t="s">
-        <v>792</v>
+        <v>793</v>
       </c>
       <c r="C258" s="3"/>
       <c r="D258" s="3"/>
@@ -13498,10 +13507,10 @@
     </row>
     <row r="259" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A259" s="2" t="s">
-        <v>793</v>
+        <v>794</v>
       </c>
       <c r="B259" s="3" t="s">
-        <v>794</v>
+        <v>795</v>
       </c>
       <c r="C259" s="3"/>
       <c r="D259" s="3"/>
@@ -13530,10 +13539,10 @@
     </row>
     <row r="260" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A260" s="2" t="s">
-        <v>795</v>
+        <v>796</v>
       </c>
       <c r="B260" s="3" t="s">
-        <v>796</v>
+        <v>797</v>
       </c>
       <c r="C260" s="3"/>
       <c r="D260" s="3"/>
@@ -13562,10 +13571,10 @@
     </row>
     <row r="261" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A261" s="2" t="s">
-        <v>797</v>
+        <v>798</v>
       </c>
       <c r="B261" s="3" t="s">
-        <v>798</v>
+        <v>799</v>
       </c>
       <c r="C261" s="3"/>
       <c r="D261" s="3"/>
@@ -13594,10 +13603,10 @@
     </row>
     <row r="262" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A262" s="2" t="s">
-        <v>799</v>
+        <v>800</v>
       </c>
       <c r="B262" s="3" t="s">
-        <v>800</v>
+        <v>801</v>
       </c>
       <c r="C262" s="3"/>
       <c r="D262" s="3"/>
@@ -13626,10 +13635,10 @@
     </row>
     <row r="263" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A263" s="2" t="s">
-        <v>801</v>
+        <v>802</v>
       </c>
       <c r="B263" s="3" t="s">
-        <v>802</v>
+        <v>803</v>
       </c>
       <c r="C263" s="3"/>
       <c r="D263" s="3"/>
@@ -13658,10 +13667,10 @@
     </row>
     <row r="264" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A264" s="2" t="s">
-        <v>803</v>
+        <v>804</v>
       </c>
       <c r="B264" s="3" t="s">
-        <v>804</v>
+        <v>805</v>
       </c>
       <c r="C264" s="3"/>
       <c r="D264" s="3"/>
@@ -13690,10 +13699,10 @@
     </row>
     <row r="265" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A265" s="2" t="s">
-        <v>805</v>
+        <v>806</v>
       </c>
       <c r="B265" s="3" t="s">
-        <v>806</v>
+        <v>807</v>
       </c>
       <c r="C265" s="3"/>
       <c r="D265" s="3"/>
@@ -13722,10 +13731,10 @@
     </row>
     <row r="266" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A266" s="2" t="s">
-        <v>807</v>
+        <v>808</v>
       </c>
       <c r="B266" s="3" t="s">
-        <v>808</v>
+        <v>809</v>
       </c>
       <c r="C266" s="3"/>
       <c r="D266" s="3"/>
@@ -13754,10 +13763,10 @@
     </row>
     <row r="267" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A267" s="2" t="s">
-        <v>809</v>
+        <v>810</v>
       </c>
       <c r="B267" s="3" t="s">
-        <v>810</v>
+        <v>811</v>
       </c>
       <c r="C267" s="3"/>
       <c r="D267" s="3"/>
@@ -13786,10 +13795,10 @@
     </row>
     <row r="268" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A268" s="2" t="s">
-        <v>811</v>
+        <v>812</v>
       </c>
       <c r="B268" s="3" t="s">
-        <v>812</v>
+        <v>813</v>
       </c>
       <c r="C268" s="3"/>
       <c r="D268" s="3"/>
@@ -13818,10 +13827,10 @@
     </row>
     <row r="269" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A269" s="2" t="s">
-        <v>813</v>
+        <v>814</v>
       </c>
       <c r="B269" s="3" t="s">
-        <v>814</v>
+        <v>815</v>
       </c>
       <c r="C269" s="3"/>
       <c r="D269" s="3"/>
@@ -13850,10 +13859,10 @@
     </row>
     <row r="270" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A270" s="2" t="s">
-        <v>815</v>
+        <v>816</v>
       </c>
       <c r="B270" s="3" t="s">
-        <v>816</v>
+        <v>817</v>
       </c>
       <c r="C270" s="3"/>
       <c r="D270" s="3"/>
@@ -13882,10 +13891,10 @@
     </row>
     <row r="271" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A271" s="2" t="s">
-        <v>817</v>
+        <v>818</v>
       </c>
       <c r="B271" s="3" t="s">
-        <v>818</v>
+        <v>819</v>
       </c>
       <c r="C271" s="3"/>
       <c r="D271" s="3"/>
@@ -13914,10 +13923,10 @@
     </row>
     <row r="272" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A272" s="2" t="s">
-        <v>819</v>
+        <v>820</v>
       </c>
       <c r="B272" s="3" t="s">
-        <v>820</v>
+        <v>821</v>
       </c>
       <c r="C272" s="3"/>
       <c r="D272" s="3"/>
@@ -13946,10 +13955,10 @@
     </row>
     <row r="273" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A273" s="2" t="s">
-        <v>821</v>
+        <v>822</v>
       </c>
       <c r="B273" s="3" t="s">
-        <v>822</v>
+        <v>823</v>
       </c>
       <c r="C273" s="3"/>
       <c r="D273" s="3"/>
@@ -13978,10 +13987,10 @@
     </row>
     <row r="274" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A274" s="2" t="s">
-        <v>823</v>
+        <v>824</v>
       </c>
       <c r="B274" s="3" t="s">
-        <v>824</v>
+        <v>825</v>
       </c>
       <c r="C274" s="3"/>
       <c r="D274" s="3"/>
@@ -14010,10 +14019,10 @@
     </row>
     <row r="275" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A275" s="2" t="s">
-        <v>825</v>
+        <v>826</v>
       </c>
       <c r="B275" s="3" t="s">
-        <v>826</v>
+        <v>827</v>
       </c>
       <c r="C275" s="3"/>
       <c r="D275" s="3"/>
@@ -14042,10 +14051,10 @@
     </row>
     <row r="276" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A276" s="2" t="s">
-        <v>827</v>
+        <v>828</v>
       </c>
       <c r="B276" s="3" t="s">
-        <v>828</v>
+        <v>829</v>
       </c>
       <c r="C276" s="3"/>
       <c r="D276" s="3"/>
@@ -14074,10 +14083,10 @@
     </row>
     <row r="277" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A277" s="2" t="s">
-        <v>829</v>
+        <v>830</v>
       </c>
       <c r="B277" s="3" t="s">
-        <v>830</v>
+        <v>831</v>
       </c>
       <c r="C277" s="3"/>
       <c r="D277" s="3"/>
@@ -14106,10 +14115,10 @@
     </row>
     <row r="278" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A278" s="2" t="s">
-        <v>831</v>
+        <v>832</v>
       </c>
       <c r="B278" s="3" t="s">
-        <v>832</v>
+        <v>833</v>
       </c>
       <c r="C278" s="3"/>
       <c r="D278" s="3"/>
@@ -14138,10 +14147,10 @@
     </row>
     <row r="279" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A279" s="2" t="s">
-        <v>833</v>
+        <v>834</v>
       </c>
       <c r="B279" s="3" t="s">
-        <v>834</v>
+        <v>835</v>
       </c>
       <c r="C279" s="3"/>
       <c r="D279" s="3"/>
@@ -14170,10 +14179,10 @@
     </row>
     <row r="280" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A280" s="2" t="s">
-        <v>835</v>
+        <v>836</v>
       </c>
       <c r="B280" s="3" t="s">
-        <v>836</v>
+        <v>837</v>
       </c>
       <c r="C280" s="3"/>
       <c r="D280" s="3"/>
@@ -14202,10 +14211,10 @@
     </row>
     <row r="281" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A281" s="2" t="s">
-        <v>837</v>
+        <v>838</v>
       </c>
       <c r="B281" s="3" t="s">
-        <v>838</v>
+        <v>839</v>
       </c>
       <c r="C281" s="3"/>
       <c r="D281" s="3"/>
@@ -14234,10 +14243,10 @@
     </row>
     <row r="282" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A282" s="2" t="s">
-        <v>839</v>
+        <v>840</v>
       </c>
       <c r="B282" s="3" t="s">
-        <v>840</v>
+        <v>841</v>
       </c>
       <c r="C282" s="3"/>
       <c r="D282" s="3"/>
@@ -14266,10 +14275,10 @@
     </row>
     <row r="283" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A283" s="2" t="s">
-        <v>841</v>
+        <v>842</v>
       </c>
       <c r="B283" s="3" t="s">
-        <v>842</v>
+        <v>843</v>
       </c>
       <c r="C283" s="3"/>
       <c r="D283" s="3"/>
@@ -14298,10 +14307,10 @@
     </row>
     <row r="284" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A284" s="2" t="s">
-        <v>843</v>
+        <v>844</v>
       </c>
       <c r="B284" s="3" t="s">
-        <v>844</v>
+        <v>845</v>
       </c>
       <c r="C284" s="3"/>
       <c r="D284" s="3"/>
@@ -14330,10 +14339,10 @@
     </row>
     <row r="285" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A285" s="2" t="s">
-        <v>845</v>
+        <v>846</v>
       </c>
       <c r="B285" s="3" t="s">
-        <v>846</v>
+        <v>847</v>
       </c>
       <c r="C285" s="3"/>
       <c r="D285" s="3"/>
@@ -14362,10 +14371,10 @@
     </row>
     <row r="286" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A286" s="2" t="s">
-        <v>847</v>
+        <v>848</v>
       </c>
       <c r="B286" s="3" t="s">
-        <v>848</v>
+        <v>849</v>
       </c>
       <c r="C286" s="3"/>
       <c r="D286" s="3"/>
@@ -14394,10 +14403,10 @@
     </row>
     <row r="287" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A287" s="2" t="s">
-        <v>849</v>
+        <v>850</v>
       </c>
       <c r="B287" s="3" t="s">
-        <v>850</v>
+        <v>851</v>
       </c>
       <c r="C287" s="3"/>
       <c r="D287" s="3"/>
@@ -14426,10 +14435,10 @@
     </row>
     <row r="288" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A288" s="2" t="s">
-        <v>851</v>
+        <v>852</v>
       </c>
       <c r="B288" s="3" t="s">
-        <v>852</v>
+        <v>853</v>
       </c>
       <c r="C288" s="3"/>
       <c r="D288" s="3"/>
@@ -14458,10 +14467,10 @@
     </row>
     <row r="289" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A289" s="2" t="s">
-        <v>853</v>
+        <v>854</v>
       </c>
       <c r="B289" s="3" t="s">
-        <v>854</v>
+        <v>855</v>
       </c>
       <c r="C289" s="3"/>
       <c r="D289" s="3"/>
@@ -14490,10 +14499,10 @@
     </row>
     <row r="290" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A290" s="2" t="s">
-        <v>855</v>
+        <v>856</v>
       </c>
       <c r="B290" s="3" t="s">
-        <v>856</v>
+        <v>857</v>
       </c>
       <c r="C290" s="3"/>
       <c r="D290" s="3"/>
@@ -14522,10 +14531,10 @@
     </row>
     <row r="291" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A291" s="2" t="s">
-        <v>857</v>
+        <v>858</v>
       </c>
       <c r="B291" s="3" t="s">
-        <v>858</v>
+        <v>859</v>
       </c>
       <c r="C291" s="3"/>
       <c r="D291" s="3"/>
@@ -14554,10 +14563,10 @@
     </row>
     <row r="292" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A292" s="2" t="s">
-        <v>859</v>
+        <v>860</v>
       </c>
       <c r="B292" s="3" t="s">
-        <v>860</v>
+        <v>861</v>
       </c>
       <c r="C292" s="3"/>
       <c r="D292" s="3"/>
@@ -14586,10 +14595,10 @@
     </row>
     <row r="293" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A293" s="2" t="s">
-        <v>861</v>
+        <v>862</v>
       </c>
       <c r="B293" s="3" t="s">
-        <v>862</v>
+        <v>863</v>
       </c>
       <c r="C293" s="3"/>
       <c r="D293" s="3"/>
@@ -14618,10 +14627,10 @@
     </row>
     <row r="294" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A294" s="2" t="s">
-        <v>863</v>
+        <v>864</v>
       </c>
       <c r="B294" s="3" t="s">
-        <v>864</v>
+        <v>865</v>
       </c>
       <c r="C294" s="3"/>
       <c r="D294" s="3"/>
@@ -14650,10 +14659,10 @@
     </row>
     <row r="295" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A295" s="2" t="s">
-        <v>865</v>
+        <v>866</v>
       </c>
       <c r="B295" s="3" t="s">
-        <v>866</v>
+        <v>867</v>
       </c>
       <c r="C295" s="3"/>
       <c r="D295" s="3"/>
@@ -14682,10 +14691,10 @@
     </row>
     <row r="296" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A296" s="2" t="s">
-        <v>867</v>
+        <v>868</v>
       </c>
       <c r="B296" s="3" t="s">
-        <v>868</v>
+        <v>869</v>
       </c>
       <c r="C296" s="3"/>
       <c r="D296" s="3"/>
@@ -14714,10 +14723,10 @@
     </row>
     <row r="297" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A297" s="2" t="s">
-        <v>869</v>
+        <v>870</v>
       </c>
       <c r="B297" s="3" t="s">
-        <v>870</v>
+        <v>871</v>
       </c>
       <c r="C297" s="3"/>
       <c r="D297" s="3"/>
@@ -14746,10 +14755,10 @@
     </row>
     <row r="298" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A298" s="2" t="s">
-        <v>871</v>
+        <v>872</v>
       </c>
       <c r="B298" s="3" t="s">
-        <v>872</v>
+        <v>873</v>
       </c>
       <c r="C298" s="3"/>
       <c r="D298" s="3"/>
@@ -14778,10 +14787,10 @@
     </row>
     <row r="299" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A299" s="2" t="s">
-        <v>873</v>
+        <v>874</v>
       </c>
       <c r="B299" s="3" t="s">
-        <v>874</v>
+        <v>875</v>
       </c>
       <c r="C299" s="3"/>
       <c r="D299" s="3"/>
@@ -14810,10 +14819,10 @@
     </row>
     <row r="300" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A300" s="2" t="s">
-        <v>875</v>
+        <v>876</v>
       </c>
       <c r="B300" s="3" t="s">
-        <v>876</v>
+        <v>877</v>
       </c>
       <c r="C300" s="3"/>
       <c r="D300" s="3"/>
@@ -14842,10 +14851,10 @@
     </row>
     <row r="301" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A301" s="2" t="s">
-        <v>877</v>
+        <v>878</v>
       </c>
       <c r="B301" s="3" t="s">
-        <v>878</v>
+        <v>879</v>
       </c>
       <c r="C301" s="3"/>
       <c r="D301" s="3"/>
@@ -14874,10 +14883,10 @@
     </row>
     <row r="302" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A302" s="2" t="s">
-        <v>879</v>
+        <v>880</v>
       </c>
       <c r="B302" s="3" t="s">
-        <v>880</v>
+        <v>881</v>
       </c>
       <c r="C302" s="3"/>
       <c r="D302" s="3"/>
@@ -14906,10 +14915,10 @@
     </row>
     <row r="303" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A303" s="2" t="s">
-        <v>881</v>
+        <v>882</v>
       </c>
       <c r="B303" s="3" t="s">
-        <v>882</v>
+        <v>883</v>
       </c>
       <c r="C303" s="3"/>
       <c r="D303" s="3"/>
@@ -14938,10 +14947,10 @@
     </row>
     <row r="304" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A304" s="2" t="s">
-        <v>883</v>
+        <v>884</v>
       </c>
       <c r="B304" s="3" t="s">
-        <v>884</v>
+        <v>885</v>
       </c>
       <c r="C304" s="3"/>
       <c r="D304" s="3"/>
@@ -14970,10 +14979,10 @@
     </row>
     <row r="305" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A305" s="2" t="s">
-        <v>885</v>
+        <v>886</v>
       </c>
       <c r="B305" s="3" t="s">
-        <v>886</v>
+        <v>887</v>
       </c>
       <c r="C305" s="3"/>
       <c r="D305" s="3"/>
@@ -15002,10 +15011,10 @@
     </row>
     <row r="306" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A306" s="2" t="s">
-        <v>887</v>
+        <v>888</v>
       </c>
       <c r="B306" s="3" t="s">
-        <v>888</v>
+        <v>889</v>
       </c>
       <c r="C306" s="3"/>
       <c r="D306" s="3"/>
@@ -15034,10 +15043,10 @@
     </row>
     <row r="307" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A307" s="2" t="s">
-        <v>889</v>
+        <v>890</v>
       </c>
       <c r="B307" s="3" t="s">
-        <v>890</v>
+        <v>891</v>
       </c>
       <c r="C307" s="3"/>
       <c r="D307" s="3"/>
@@ -15066,10 +15075,10 @@
     </row>
     <row r="308" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A308" s="2" t="s">
-        <v>891</v>
+        <v>892</v>
       </c>
       <c r="B308" s="3" t="s">
-        <v>892</v>
+        <v>893</v>
       </c>
       <c r="C308" s="3"/>
       <c r="D308" s="3"/>
@@ -15098,10 +15107,10 @@
     </row>
     <row r="309" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A309" s="2" t="s">
-        <v>893</v>
+        <v>894</v>
       </c>
       <c r="B309" s="3" t="s">
-        <v>894</v>
+        <v>895</v>
       </c>
       <c r="C309" s="3"/>
       <c r="D309" s="3"/>
@@ -15130,10 +15139,10 @@
     </row>
     <row r="310" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A310" s="2" t="s">
-        <v>895</v>
+        <v>896</v>
       </c>
       <c r="B310" s="3" t="s">
-        <v>896</v>
+        <v>897</v>
       </c>
       <c r="C310" s="3"/>
       <c r="D310" s="3"/>
@@ -15162,10 +15171,10 @@
     </row>
     <row r="311" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A311" s="2" t="s">
-        <v>897</v>
+        <v>898</v>
       </c>
       <c r="B311" s="3" t="s">
-        <v>898</v>
+        <v>899</v>
       </c>
       <c r="C311" s="3"/>
       <c r="D311" s="3"/>
@@ -15194,10 +15203,10 @@
     </row>
     <row r="312" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A312" s="2" t="s">
-        <v>899</v>
+        <v>900</v>
       </c>
       <c r="B312" s="3" t="s">
-        <v>900</v>
+        <v>901</v>
       </c>
       <c r="C312" s="3"/>
       <c r="D312" s="3"/>
@@ -15226,10 +15235,10 @@
     </row>
     <row r="313" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A313" s="2" t="s">
-        <v>901</v>
+        <v>902</v>
       </c>
       <c r="B313" s="3" t="s">
-        <v>902</v>
+        <v>903</v>
       </c>
       <c r="C313" s="3"/>
       <c r="D313" s="3"/>
@@ -15258,10 +15267,10 @@
     </row>
     <row r="314" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A314" s="2" t="s">
-        <v>903</v>
+        <v>904</v>
       </c>
       <c r="B314" s="3" t="s">
-        <v>904</v>
+        <v>905</v>
       </c>
       <c r="C314" s="3"/>
       <c r="D314" s="3"/>
@@ -15290,10 +15299,10 @@
     </row>
     <row r="315" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A315" s="2" t="s">
-        <v>905</v>
+        <v>906</v>
       </c>
       <c r="B315" s="3" t="s">
-        <v>906</v>
+        <v>907</v>
       </c>
       <c r="C315" s="3"/>
       <c r="D315" s="3"/>
@@ -15322,10 +15331,10 @@
     </row>
     <row r="316" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A316" s="2" t="s">
-        <v>907</v>
+        <v>908</v>
       </c>
       <c r="B316" s="3" t="s">
-        <v>908</v>
+        <v>909</v>
       </c>
       <c r="C316" s="3"/>
       <c r="D316" s="3"/>
@@ -15354,10 +15363,10 @@
     </row>
     <row r="317" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A317" s="2" t="s">
-        <v>909</v>
+        <v>910</v>
       </c>
       <c r="B317" s="3" t="s">
-        <v>910</v>
+        <v>911</v>
       </c>
       <c r="C317" s="3"/>
       <c r="D317" s="3"/>
@@ -15386,10 +15395,10 @@
     </row>
     <row r="318" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A318" s="2" t="s">
-        <v>911</v>
+        <v>912</v>
       </c>
       <c r="B318" s="3" t="s">
-        <v>912</v>
+        <v>913</v>
       </c>
       <c r="C318" s="3"/>
       <c r="D318" s="3"/>
@@ -15418,10 +15427,10 @@
     </row>
     <row r="319" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A319" s="2" t="s">
-        <v>913</v>
+        <v>914</v>
       </c>
       <c r="B319" s="3" t="s">
-        <v>914</v>
+        <v>915</v>
       </c>
       <c r="C319" s="3"/>
       <c r="D319" s="3"/>
@@ -15450,10 +15459,10 @@
     </row>
     <row r="320" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A320" s="2" t="s">
-        <v>915</v>
+        <v>916</v>
       </c>
       <c r="B320" s="3" t="s">
-        <v>916</v>
+        <v>917</v>
       </c>
       <c r="C320" s="3"/>
       <c r="D320" s="3"/>
@@ -15482,10 +15491,10 @@
     </row>
     <row r="321" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A321" s="2" t="s">
-        <v>917</v>
+        <v>918</v>
       </c>
       <c r="B321" s="3" t="s">
-        <v>918</v>
+        <v>919</v>
       </c>
       <c r="C321" s="3"/>
       <c r="D321" s="3"/>
@@ -15514,10 +15523,10 @@
     </row>
     <row r="322" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A322" s="2" t="s">
-        <v>919</v>
+        <v>920</v>
       </c>
       <c r="B322" s="3" t="s">
-        <v>920</v>
+        <v>921</v>
       </c>
       <c r="C322" s="3"/>
       <c r="D322" s="3"/>
@@ -15546,10 +15555,10 @@
     </row>
     <row r="323" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A323" s="2" t="s">
-        <v>921</v>
+        <v>922</v>
       </c>
       <c r="B323" s="3" t="s">
-        <v>922</v>
+        <v>923</v>
       </c>
       <c r="C323" s="3"/>
       <c r="D323" s="3"/>
@@ -15578,10 +15587,10 @@
     </row>
     <row r="324" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A324" s="2" t="s">
-        <v>923</v>
+        <v>924</v>
       </c>
       <c r="B324" s="3" t="s">
-        <v>924</v>
+        <v>925</v>
       </c>
       <c r="C324" s="3"/>
       <c r="D324" s="3"/>
@@ -15610,10 +15619,10 @@
     </row>
     <row r="325" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A325" s="2" t="s">
-        <v>925</v>
+        <v>926</v>
       </c>
       <c r="B325" s="3" t="s">
-        <v>926</v>
+        <v>927</v>
       </c>
       <c r="C325" s="3"/>
       <c r="D325" s="3"/>
@@ -15642,10 +15651,10 @@
     </row>
     <row r="326" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A326" s="2" t="s">
-        <v>927</v>
+        <v>928</v>
       </c>
       <c r="B326" s="3" t="s">
-        <v>928</v>
+        <v>929</v>
       </c>
       <c r="C326" s="3"/>
       <c r="D326" s="3"/>
@@ -15674,10 +15683,10 @@
     </row>
     <row r="327" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A327" s="2" t="s">
-        <v>929</v>
+        <v>930</v>
       </c>
       <c r="B327" s="3" t="s">
-        <v>930</v>
+        <v>931</v>
       </c>
       <c r="C327" s="3"/>
       <c r="D327" s="3"/>
@@ -15706,10 +15715,10 @@
     </row>
     <row r="328" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A328" s="2" t="s">
-        <v>931</v>
+        <v>932</v>
       </c>
       <c r="B328" s="3" t="s">
-        <v>932</v>
+        <v>933</v>
       </c>
       <c r="C328" s="3"/>
       <c r="D328" s="3"/>
@@ -15738,10 +15747,10 @@
     </row>
     <row r="329" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A329" s="2" t="s">
-        <v>933</v>
+        <v>934</v>
       </c>
       <c r="B329" s="3" t="s">
-        <v>934</v>
+        <v>935</v>
       </c>
       <c r="C329" s="3"/>
       <c r="D329" s="3"/>
@@ -15770,10 +15779,10 @@
     </row>
     <row r="330" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A330" s="2" t="s">
-        <v>935</v>
+        <v>936</v>
       </c>
       <c r="B330" s="3" t="s">
-        <v>936</v>
+        <v>937</v>
       </c>
       <c r="C330" s="3"/>
       <c r="D330" s="3"/>
@@ -15802,10 +15811,10 @@
     </row>
     <row r="331" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A331" s="2" t="s">
-        <v>937</v>
+        <v>938</v>
       </c>
       <c r="B331" s="3" t="s">
-        <v>938</v>
+        <v>939</v>
       </c>
       <c r="C331" s="3"/>
       <c r="D331" s="3"/>
@@ -15834,10 +15843,10 @@
     </row>
     <row r="332" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A332" s="2" t="s">
-        <v>939</v>
+        <v>940</v>
       </c>
       <c r="B332" s="3" t="s">
-        <v>940</v>
+        <v>941</v>
       </c>
       <c r="C332" s="3"/>
       <c r="D332" s="3"/>
@@ -15866,10 +15875,10 @@
     </row>
     <row r="333" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A333" s="2" t="s">
-        <v>941</v>
+        <v>942</v>
       </c>
       <c r="B333" s="3" t="s">
-        <v>942</v>
+        <v>943</v>
       </c>
       <c r="C333" s="3"/>
       <c r="D333" s="3"/>
@@ -15898,10 +15907,10 @@
     </row>
     <row r="334" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A334" s="2" t="s">
-        <v>943</v>
+        <v>944</v>
       </c>
       <c r="B334" s="3" t="s">
-        <v>944</v>
+        <v>945</v>
       </c>
       <c r="C334" s="3"/>
       <c r="D334" s="3"/>
@@ -15930,10 +15939,10 @@
     </row>
     <row r="335" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A335" s="2" t="s">
-        <v>945</v>
+        <v>946</v>
       </c>
       <c r="B335" s="3" t="s">
-        <v>946</v>
+        <v>947</v>
       </c>
       <c r="C335" s="3"/>
       <c r="D335" s="3"/>
@@ -15962,10 +15971,10 @@
     </row>
     <row r="336" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A336" s="2" t="s">
-        <v>947</v>
+        <v>948</v>
       </c>
       <c r="B336" s="3" t="s">
-        <v>948</v>
+        <v>949</v>
       </c>
       <c r="C336" s="3"/>
       <c r="D336" s="3"/>
@@ -15994,10 +16003,10 @@
     </row>
     <row r="337" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A337" s="2" t="s">
-        <v>949</v>
+        <v>950</v>
       </c>
       <c r="B337" s="3" t="s">
-        <v>950</v>
+        <v>951</v>
       </c>
       <c r="C337" s="3"/>
       <c r="D337" s="3"/>
@@ -16026,10 +16035,10 @@
     </row>
     <row r="338" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A338" s="2" t="s">
-        <v>951</v>
+        <v>952</v>
       </c>
       <c r="B338" s="3" t="s">
-        <v>952</v>
+        <v>953</v>
       </c>
       <c r="C338" s="3"/>
       <c r="D338" s="3"/>
@@ -16058,10 +16067,10 @@
     </row>
     <row r="339" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A339" s="2" t="s">
-        <v>953</v>
+        <v>954</v>
       </c>
       <c r="B339" s="3" t="s">
-        <v>954</v>
+        <v>955</v>
       </c>
       <c r="C339" s="3"/>
       <c r="D339" s="3"/>
@@ -16090,10 +16099,10 @@
     </row>
     <row r="340" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A340" s="2" t="s">
-        <v>955</v>
+        <v>956</v>
       </c>
       <c r="B340" s="3" t="s">
-        <v>956</v>
+        <v>957</v>
       </c>
       <c r="C340" s="3"/>
       <c r="D340" s="3"/>
@@ -16122,10 +16131,10 @@
     </row>
     <row r="341" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A341" s="2" t="s">
-        <v>957</v>
+        <v>958</v>
       </c>
       <c r="B341" s="3" t="s">
-        <v>958</v>
+        <v>959</v>
       </c>
       <c r="C341" s="3"/>
       <c r="D341" s="3"/>
@@ -16154,10 +16163,10 @@
     </row>
     <row r="342" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A342" s="2" t="s">
-        <v>959</v>
+        <v>960</v>
       </c>
       <c r="B342" s="3" t="s">
-        <v>960</v>
+        <v>961</v>
       </c>
       <c r="C342" s="3"/>
       <c r="D342" s="3"/>
@@ -16186,10 +16195,10 @@
     </row>
     <row r="343" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A343" s="2" t="s">
-        <v>961</v>
+        <v>962</v>
       </c>
       <c r="B343" s="3" t="s">
-        <v>962</v>
+        <v>963</v>
       </c>
       <c r="C343" s="3"/>
       <c r="D343" s="3"/>
@@ -16218,10 +16227,10 @@
     </row>
     <row r="344" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A344" s="2" t="s">
-        <v>963</v>
+        <v>964</v>
       </c>
       <c r="B344" s="3" t="s">
-        <v>964</v>
+        <v>965</v>
       </c>
       <c r="C344" s="3"/>
       <c r="D344" s="3"/>
@@ -16250,10 +16259,10 @@
     </row>
     <row r="345" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A345" s="2" t="s">
-        <v>965</v>
+        <v>966</v>
       </c>
       <c r="B345" s="3" t="s">
-        <v>966</v>
+        <v>967</v>
       </c>
       <c r="C345" s="3"/>
       <c r="D345" s="3"/>
@@ -16282,10 +16291,10 @@
     </row>
     <row r="346" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A346" s="2" t="s">
-        <v>967</v>
+        <v>968</v>
       </c>
       <c r="B346" s="3" t="s">
-        <v>968</v>
+        <v>969</v>
       </c>
       <c r="C346" s="3"/>
       <c r="D346" s="3"/>
@@ -16314,10 +16323,10 @@
     </row>
     <row r="347" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A347" s="2" t="s">
-        <v>969</v>
+        <v>970</v>
       </c>
       <c r="B347" s="3" t="s">
-        <v>970</v>
+        <v>971</v>
       </c>
       <c r="C347" s="3"/>
       <c r="D347" s="3"/>
@@ -16346,10 +16355,10 @@
     </row>
     <row r="348" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A348" s="2" t="s">
-        <v>971</v>
+        <v>972</v>
       </c>
       <c r="B348" s="3" t="s">
-        <v>972</v>
+        <v>973</v>
       </c>
       <c r="C348" s="3"/>
       <c r="D348" s="3"/>
@@ -16378,10 +16387,10 @@
     </row>
     <row r="349" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A349" s="2" t="s">
-        <v>973</v>
+        <v>974</v>
       </c>
       <c r="B349" s="3" t="s">
-        <v>974</v>
+        <v>975</v>
       </c>
       <c r="C349" s="3"/>
       <c r="D349" s="3"/>
@@ -16410,10 +16419,10 @@
     </row>
     <row r="350" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A350" s="2" t="s">
-        <v>975</v>
+        <v>976</v>
       </c>
       <c r="B350" s="3" t="s">
-        <v>976</v>
+        <v>977</v>
       </c>
       <c r="C350" s="3"/>
       <c r="D350" s="3"/>
@@ -16442,10 +16451,10 @@
     </row>
     <row r="351" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A351" s="2" t="s">
-        <v>977</v>
+        <v>978</v>
       </c>
       <c r="B351" s="3" t="s">
-        <v>978</v>
+        <v>979</v>
       </c>
       <c r="C351" s="3"/>
       <c r="D351" s="3"/>
@@ -16474,10 +16483,10 @@
     </row>
     <row r="352" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A352" s="2" t="s">
-        <v>979</v>
+        <v>980</v>
       </c>
       <c r="B352" s="3" t="s">
-        <v>980</v>
+        <v>981</v>
       </c>
       <c r="C352" s="3"/>
       <c r="D352" s="3"/>
@@ -16506,10 +16515,10 @@
     </row>
     <row r="353" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A353" s="2" t="s">
-        <v>981</v>
+        <v>982</v>
       </c>
       <c r="B353" s="3" t="s">
-        <v>982</v>
+        <v>983</v>
       </c>
       <c r="C353" s="3"/>
       <c r="D353" s="3"/>
@@ -16538,10 +16547,10 @@
     </row>
     <row r="354" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A354" s="2" t="s">
-        <v>983</v>
+        <v>984</v>
       </c>
       <c r="B354" s="3" t="s">
-        <v>984</v>
+        <v>985</v>
       </c>
       <c r="C354" s="3"/>
       <c r="D354" s="3"/>
@@ -16570,10 +16579,10 @@
     </row>
     <row r="355" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A355" s="2" t="s">
-        <v>985</v>
+        <v>986</v>
       </c>
       <c r="B355" s="3" t="s">
-        <v>986</v>
+        <v>987</v>
       </c>
       <c r="C355" s="3"/>
       <c r="D355" s="3"/>
@@ -16602,10 +16611,10 @@
     </row>
     <row r="356" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A356" s="2" t="s">
-        <v>987</v>
+        <v>988</v>
       </c>
       <c r="B356" s="3" t="s">
-        <v>988</v>
+        <v>989</v>
       </c>
       <c r="C356" s="3"/>
       <c r="D356" s="3"/>
@@ -16634,10 +16643,10 @@
     </row>
     <row r="357" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A357" s="2" t="s">
-        <v>989</v>
+        <v>990</v>
       </c>
       <c r="B357" s="3" t="s">
-        <v>990</v>
+        <v>991</v>
       </c>
       <c r="C357" s="3"/>
       <c r="D357" s="3"/>
@@ -16666,10 +16675,10 @@
     </row>
     <row r="358" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A358" s="2" t="s">
-        <v>991</v>
+        <v>992</v>
       </c>
       <c r="B358" s="3" t="s">
-        <v>992</v>
+        <v>993</v>
       </c>
       <c r="C358" s="3"/>
       <c r="D358" s="3"/>
@@ -16698,10 +16707,10 @@
     </row>
     <row r="359" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A359" s="2" t="s">
-        <v>993</v>
+        <v>994</v>
       </c>
       <c r="B359" s="3" t="s">
-        <v>994</v>
+        <v>995</v>
       </c>
       <c r="C359" s="3"/>
       <c r="D359" s="3"/>
@@ -16730,10 +16739,10 @@
     </row>
     <row r="360" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A360" s="2" t="s">
-        <v>995</v>
+        <v>996</v>
       </c>
       <c r="B360" s="3" t="s">
-        <v>996</v>
+        <v>997</v>
       </c>
       <c r="C360" s="3"/>
       <c r="D360" s="3"/>
@@ -16762,10 +16771,10 @@
     </row>
     <row r="361" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A361" s="2" t="s">
-        <v>997</v>
+        <v>998</v>
       </c>
       <c r="B361" s="3" t="s">
-        <v>998</v>
+        <v>999</v>
       </c>
       <c r="C361" s="3"/>
       <c r="D361" s="3"/>
@@ -16794,10 +16803,10 @@
     </row>
     <row r="362" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A362" s="2" t="s">
-        <v>999</v>
+        <v>1000</v>
       </c>
       <c r="B362" s="3" t="s">
-        <v>1000</v>
+        <v>1001</v>
       </c>
       <c r="C362" s="3"/>
       <c r="D362" s="3"/>
@@ -16826,10 +16835,10 @@
     </row>
     <row r="363" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A363" s="2" t="s">
-        <v>1001</v>
+        <v>1002</v>
       </c>
       <c r="B363" s="3" t="s">
-        <v>1002</v>
+        <v>1003</v>
       </c>
       <c r="C363" s="3"/>
       <c r="D363" s="3"/>
@@ -16858,10 +16867,10 @@
     </row>
     <row r="364" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A364" s="2" t="s">
-        <v>1003</v>
+        <v>1004</v>
       </c>
       <c r="B364" s="3" t="s">
-        <v>1004</v>
+        <v>1005</v>
       </c>
       <c r="C364" s="3"/>
       <c r="D364" s="3"/>
@@ -16890,10 +16899,10 @@
     </row>
     <row r="365" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A365" s="2" t="s">
-        <v>1005</v>
+        <v>1006</v>
       </c>
       <c r="B365" s="3" t="s">
-        <v>1006</v>
+        <v>1007</v>
       </c>
       <c r="C365" s="3"/>
       <c r="D365" s="3"/>
@@ -16922,10 +16931,10 @@
     </row>
     <row r="366" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A366" s="2" t="s">
-        <v>1007</v>
+        <v>1008</v>
       </c>
       <c r="B366" s="3" t="s">
-        <v>1008</v>
+        <v>1009</v>
       </c>
       <c r="C366" s="3"/>
       <c r="D366" s="3"/>
@@ -16954,10 +16963,10 @@
     </row>
     <row r="367" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A367" s="2" t="s">
-        <v>1009</v>
+        <v>1010</v>
       </c>
       <c r="B367" s="3" t="s">
-        <v>1010</v>
+        <v>1011</v>
       </c>
       <c r="C367" s="3"/>
       <c r="D367" s="3"/>
@@ -16986,10 +16995,10 @@
     </row>
     <row r="368" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A368" s="2" t="s">
-        <v>1011</v>
+        <v>1012</v>
       </c>
       <c r="B368" s="3" t="s">
-        <v>1012</v>
+        <v>1013</v>
       </c>
       <c r="C368" s="3"/>
       <c r="D368" s="3"/>
@@ -17018,10 +17027,10 @@
     </row>
     <row r="369" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A369" s="2" t="s">
-        <v>1013</v>
+        <v>1014</v>
       </c>
       <c r="B369" s="3" t="s">
-        <v>1014</v>
+        <v>1015</v>
       </c>
       <c r="C369" s="3"/>
       <c r="D369" s="3"/>
@@ -17050,10 +17059,10 @@
     </row>
     <row r="370" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A370" s="2" t="s">
-        <v>1015</v>
+        <v>1016</v>
       </c>
       <c r="B370" s="3" t="s">
-        <v>1016</v>
+        <v>1017</v>
       </c>
       <c r="C370" s="3"/>
       <c r="D370" s="3"/>
@@ -17082,10 +17091,10 @@
     </row>
     <row r="371" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A371" s="2" t="s">
-        <v>1017</v>
+        <v>1018</v>
       </c>
       <c r="B371" s="3" t="s">
-        <v>1018</v>
+        <v>1019</v>
       </c>
       <c r="C371" s="3"/>
       <c r="D371" s="3"/>
@@ -17114,10 +17123,10 @@
     </row>
     <row r="372" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A372" s="2" t="s">
-        <v>1019</v>
+        <v>1020</v>
       </c>
       <c r="B372" s="3" t="s">
-        <v>1020</v>
+        <v>1021</v>
       </c>
       <c r="C372" s="3"/>
       <c r="D372" s="3"/>
@@ -17146,10 +17155,10 @@
     </row>
     <row r="373" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A373" s="2" t="s">
-        <v>1021</v>
+        <v>1022</v>
       </c>
       <c r="B373" s="3" t="s">
-        <v>1022</v>
+        <v>1023</v>
       </c>
       <c r="C373" s="3"/>
       <c r="D373" s="3"/>
@@ -17178,10 +17187,10 @@
     </row>
     <row r="374" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A374" s="2" t="s">
-        <v>1023</v>
+        <v>1024</v>
       </c>
       <c r="B374" s="3" t="s">
-        <v>1024</v>
+        <v>1025</v>
       </c>
       <c r="C374" s="3"/>
       <c r="D374" s="3"/>
@@ -17210,10 +17219,10 @@
     </row>
     <row r="375" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A375" s="2" t="s">
-        <v>1025</v>
+        <v>1026</v>
       </c>
       <c r="B375" s="3" t="s">
-        <v>1026</v>
+        <v>1027</v>
       </c>
       <c r="C375" s="3"/>
       <c r="D375" s="3"/>
@@ -17242,10 +17251,10 @@
     </row>
     <row r="376" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A376" s="2" t="s">
-        <v>1027</v>
+        <v>1028</v>
       </c>
       <c r="B376" s="3" t="s">
-        <v>1028</v>
+        <v>1029</v>
       </c>
       <c r="C376" s="3"/>
       <c r="D376" s="3"/>
@@ -17274,10 +17283,10 @@
     </row>
     <row r="377" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A377" s="2" t="s">
-        <v>1029</v>
+        <v>1030</v>
       </c>
       <c r="B377" s="3" t="s">
-        <v>1030</v>
+        <v>1031</v>
       </c>
       <c r="C377" s="3"/>
       <c r="D377" s="3"/>
@@ -17306,10 +17315,10 @@
     </row>
     <row r="378" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A378" s="2" t="s">
-        <v>1031</v>
+        <v>1032</v>
       </c>
       <c r="B378" s="3" t="s">
-        <v>1032</v>
+        <v>1033</v>
       </c>
       <c r="C378" s="3"/>
       <c r="D378" s="3"/>
@@ -17338,10 +17347,10 @@
     </row>
     <row r="379" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A379" s="2" t="s">
-        <v>1033</v>
+        <v>1034</v>
       </c>
       <c r="B379" s="3" t="s">
-        <v>1034</v>
+        <v>1035</v>
       </c>
       <c r="C379" s="3"/>
       <c r="D379" s="3"/>
@@ -17370,10 +17379,10 @@
     </row>
     <row r="380" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A380" s="2" t="s">
-        <v>1035</v>
+        <v>1036</v>
       </c>
       <c r="B380" s="3" t="s">
-        <v>1036</v>
+        <v>1037</v>
       </c>
       <c r="C380" s="3"/>
       <c r="D380" s="3"/>
@@ -17402,10 +17411,10 @@
     </row>
     <row r="381" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A381" s="2" t="s">
-        <v>1037</v>
+        <v>1038</v>
       </c>
       <c r="B381" s="3" t="s">
-        <v>1038</v>
+        <v>1039</v>
       </c>
       <c r="C381" s="3"/>
       <c r="D381" s="3"/>
@@ -17434,10 +17443,10 @@
     </row>
     <row r="382" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A382" s="2" t="s">
-        <v>1039</v>
+        <v>1040</v>
       </c>
       <c r="B382" s="3" t="s">
-        <v>1040</v>
+        <v>1041</v>
       </c>
       <c r="C382" s="3"/>
       <c r="D382" s="3"/>
@@ -17466,10 +17475,10 @@
     </row>
     <row r="383" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A383" s="2" t="s">
-        <v>1041</v>
+        <v>1042</v>
       </c>
       <c r="B383" s="3" t="s">
-        <v>1042</v>
+        <v>1043</v>
       </c>
       <c r="C383" s="3"/>
       <c r="D383" s="3"/>
@@ -17498,10 +17507,10 @@
     </row>
     <row r="384" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A384" s="2" t="s">
-        <v>1043</v>
+        <v>1044</v>
       </c>
       <c r="B384" s="3" t="s">
-        <v>1044</v>
+        <v>1045</v>
       </c>
       <c r="C384" s="3"/>
       <c r="D384" s="3"/>
@@ -17530,10 +17539,10 @@
     </row>
     <row r="385" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A385" s="2" t="s">
-        <v>1045</v>
+        <v>1046</v>
       </c>
       <c r="B385" s="3" t="s">
-        <v>1046</v>
+        <v>1047</v>
       </c>
       <c r="C385" s="3"/>
       <c r="D385" s="3"/>
@@ -17562,10 +17571,10 @@
     </row>
     <row r="386" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A386" s="2" t="s">
-        <v>1047</v>
+        <v>1048</v>
       </c>
       <c r="B386" s="3" t="s">
-        <v>1048</v>
+        <v>1049</v>
       </c>
       <c r="C386" s="3"/>
       <c r="D386" s="3"/>
@@ -17594,10 +17603,10 @@
     </row>
     <row r="387" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A387" s="2" t="s">
-        <v>1049</v>
+        <v>1050</v>
       </c>
       <c r="B387" s="3" t="s">
-        <v>1050</v>
+        <v>1051</v>
       </c>
       <c r="C387" s="3"/>
       <c r="D387" s="3"/>
@@ -17626,10 +17635,10 @@
     </row>
     <row r="388" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A388" s="2" t="s">
-        <v>1051</v>
+        <v>1052</v>
       </c>
       <c r="B388" s="3" t="s">
-        <v>1052</v>
+        <v>1053</v>
       </c>
       <c r="C388" s="3"/>
       <c r="D388" s="3"/>
@@ -17658,10 +17667,10 @@
     </row>
     <row r="389" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A389" s="2" t="s">
-        <v>1053</v>
+        <v>1054</v>
       </c>
       <c r="B389" s="3" t="s">
-        <v>1054</v>
+        <v>1055</v>
       </c>
       <c r="C389" s="3"/>
       <c r="D389" s="3"/>
@@ -17690,10 +17699,10 @@
     </row>
     <row r="390" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A390" s="2" t="s">
-        <v>1055</v>
+        <v>1056</v>
       </c>
       <c r="B390" s="3" t="s">
-        <v>1056</v>
+        <v>1057</v>
       </c>
       <c r="C390" s="3"/>
       <c r="D390" s="3"/>
@@ -17722,10 +17731,10 @@
     </row>
     <row r="391" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A391" s="2" t="s">
-        <v>1057</v>
+        <v>1058</v>
       </c>
       <c r="B391" s="3" t="s">
-        <v>1058</v>
+        <v>1059</v>
       </c>
       <c r="C391" s="3"/>
       <c r="D391" s="3"/>
@@ -17754,10 +17763,10 @@
     </row>
     <row r="392" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A392" s="2" t="s">
-        <v>1059</v>
+        <v>1060</v>
       </c>
       <c r="B392" s="3" t="s">
-        <v>1060</v>
+        <v>1061</v>
       </c>
       <c r="C392" s="3"/>
       <c r="D392" s="3"/>
@@ -17786,10 +17795,10 @@
     </row>
     <row r="393" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A393" s="2" t="s">
-        <v>1061</v>
+        <v>1062</v>
       </c>
       <c r="B393" s="3" t="s">
-        <v>1062</v>
+        <v>1063</v>
       </c>
       <c r="C393" s="3"/>
       <c r="D393" s="3"/>
@@ -17818,10 +17827,10 @@
     </row>
     <row r="394" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A394" s="2" t="s">
-        <v>1063</v>
+        <v>1064</v>
       </c>
       <c r="B394" s="3" t="s">
-        <v>1064</v>
+        <v>1065</v>
       </c>
       <c r="C394" s="3"/>
       <c r="D394" s="3"/>
@@ -17850,10 +17859,10 @@
     </row>
     <row r="395" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A395" s="2" t="s">
-        <v>1065</v>
+        <v>1066</v>
       </c>
       <c r="B395" s="3" t="s">
-        <v>1066</v>
+        <v>1067</v>
       </c>
       <c r="C395" s="3"/>
       <c r="D395" s="3"/>
@@ -17882,10 +17891,10 @@
     </row>
     <row r="396" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A396" s="2" t="s">
-        <v>1067</v>
+        <v>1068</v>
       </c>
       <c r="B396" s="3" t="s">
-        <v>1068</v>
+        <v>1069</v>
       </c>
       <c r="C396" s="3"/>
       <c r="D396" s="3"/>
@@ -17914,10 +17923,10 @@
     </row>
     <row r="397" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A397" s="2" t="s">
-        <v>1069</v>
+        <v>1070</v>
       </c>
       <c r="B397" s="3" t="s">
-        <v>1070</v>
+        <v>1071</v>
       </c>
       <c r="C397" s="3"/>
       <c r="D397" s="3"/>
@@ -17946,10 +17955,10 @@
     </row>
     <row r="398" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A398" s="2" t="s">
-        <v>1071</v>
+        <v>1072</v>
       </c>
       <c r="B398" s="3" t="s">
-        <v>1072</v>
+        <v>1073</v>
       </c>
       <c r="C398" s="3"/>
       <c r="D398" s="3"/>
@@ -17978,10 +17987,10 @@
     </row>
     <row r="399" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A399" s="2" t="s">
-        <v>1073</v>
+        <v>1074</v>
       </c>
       <c r="B399" s="3" t="s">
-        <v>1074</v>
+        <v>1075</v>
       </c>
       <c r="C399" s="3"/>
       <c r="D399" s="3"/>
@@ -18010,10 +18019,10 @@
     </row>
     <row r="400" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A400" s="2" t="s">
-        <v>1075</v>
+        <v>1076</v>
       </c>
       <c r="B400" s="3" t="s">
-        <v>1076</v>
+        <v>1077</v>
       </c>
       <c r="C400" s="3"/>
       <c r="D400" s="3"/>
@@ -18042,10 +18051,10 @@
     </row>
     <row r="401" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A401" s="2" t="s">
-        <v>1077</v>
+        <v>1078</v>
       </c>
       <c r="B401" s="3" t="s">
-        <v>1078</v>
+        <v>1079</v>
       </c>
       <c r="C401" s="3"/>
       <c r="D401" s="3"/>
@@ -18074,10 +18083,10 @@
     </row>
     <row r="402" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A402" s="2" t="s">
-        <v>1079</v>
+        <v>1080</v>
       </c>
       <c r="B402" s="3" t="s">
-        <v>1080</v>
+        <v>1081</v>
       </c>
       <c r="C402" s="3"/>
       <c r="D402" s="3"/>
@@ -18106,10 +18115,10 @@
     </row>
     <row r="403" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A403" s="2" t="s">
-        <v>1081</v>
+        <v>1082</v>
       </c>
       <c r="B403" s="3" t="s">
-        <v>1082</v>
+        <v>1083</v>
       </c>
       <c r="C403" s="3"/>
       <c r="D403" s="3"/>
@@ -18138,10 +18147,10 @@
     </row>
     <row r="404" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A404" s="2" t="s">
-        <v>1083</v>
+        <v>1084</v>
       </c>
       <c r="B404" s="3" t="s">
-        <v>1084</v>
+        <v>1085</v>
       </c>
       <c r="C404" s="3"/>
       <c r="D404" s="3"/>
@@ -18170,10 +18179,10 @@
     </row>
     <row r="405" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A405" s="2" t="s">
-        <v>1085</v>
+        <v>1086</v>
       </c>
       <c r="B405" s="3" t="s">
-        <v>1086</v>
+        <v>1087</v>
       </c>
       <c r="C405" s="3"/>
       <c r="D405" s="3"/>
@@ -18202,10 +18211,10 @@
     </row>
     <row r="406" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A406" s="2" t="s">
-        <v>1087</v>
+        <v>1088</v>
       </c>
       <c r="B406" s="3" t="s">
-        <v>1088</v>
+        <v>1089</v>
       </c>
       <c r="C406" s="3"/>
       <c r="D406" s="3"/>
@@ -18234,10 +18243,10 @@
     </row>
     <row r="407" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A407" s="2" t="s">
-        <v>1089</v>
+        <v>1090</v>
       </c>
       <c r="B407" s="3" t="s">
-        <v>1090</v>
+        <v>1091</v>
       </c>
       <c r="C407" s="3"/>
       <c r="D407" s="3"/>
@@ -18266,10 +18275,10 @@
     </row>
     <row r="408" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A408" s="2" t="s">
-        <v>1091</v>
+        <v>1092</v>
       </c>
       <c r="B408" s="3" t="s">
-        <v>1092</v>
+        <v>1093</v>
       </c>
       <c r="C408" s="3"/>
       <c r="D408" s="3"/>
@@ -18298,10 +18307,10 @@
     </row>
     <row r="409" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A409" s="2" t="s">
-        <v>1093</v>
+        <v>1094</v>
       </c>
       <c r="B409" s="3" t="s">
-        <v>1094</v>
+        <v>1095</v>
       </c>
       <c r="C409" s="3"/>
       <c r="D409" s="3"/>
@@ -18330,10 +18339,10 @@
     </row>
     <row r="410" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A410" s="2" t="s">
-        <v>1095</v>
+        <v>1096</v>
       </c>
       <c r="B410" s="3" t="s">
-        <v>1096</v>
+        <v>1097</v>
       </c>
       <c r="C410" s="3"/>
       <c r="D410" s="3"/>
@@ -18362,10 +18371,10 @@
     </row>
     <row r="411" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A411" s="2" t="s">
-        <v>1097</v>
+        <v>1098</v>
       </c>
       <c r="B411" s="3" t="s">
-        <v>1098</v>
+        <v>1099</v>
       </c>
       <c r="C411" s="3"/>
       <c r="D411" s="3"/>
@@ -18394,10 +18403,10 @@
     </row>
     <row r="412" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A412" s="2" t="s">
-        <v>1099</v>
+        <v>1100</v>
       </c>
       <c r="B412" s="3" t="s">
-        <v>1100</v>
+        <v>1101</v>
       </c>
       <c r="C412" s="3"/>
       <c r="D412" s="3"/>
@@ -18426,10 +18435,10 @@
     </row>
     <row r="413" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A413" s="2" t="s">
-        <v>1101</v>
+        <v>1102</v>
       </c>
       <c r="B413" s="3" t="s">
-        <v>1102</v>
+        <v>1103</v>
       </c>
       <c r="C413" s="3"/>
       <c r="D413" s="3"/>
@@ -18458,10 +18467,10 @@
     </row>
     <row r="414" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A414" s="2" t="s">
-        <v>1103</v>
+        <v>1104</v>
       </c>
       <c r="B414" s="3" t="s">
-        <v>1104</v>
+        <v>1105</v>
       </c>
       <c r="C414" s="3"/>
       <c r="D414" s="3"/>
@@ -18490,10 +18499,10 @@
     </row>
     <row r="415" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A415" s="2" t="s">
-        <v>1105</v>
+        <v>1106</v>
       </c>
       <c r="B415" s="3" t="s">
-        <v>1106</v>
+        <v>1107</v>
       </c>
       <c r="C415" s="3"/>
       <c r="D415" s="3"/>
@@ -18522,10 +18531,10 @@
     </row>
     <row r="416" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A416" s="2" t="s">
-        <v>1107</v>
+        <v>1108</v>
       </c>
       <c r="B416" s="3" t="s">
-        <v>1108</v>
+        <v>1109</v>
       </c>
       <c r="C416" s="3"/>
       <c r="D416" s="3"/>
@@ -18554,10 +18563,10 @@
     </row>
     <row r="417" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A417" s="2" t="s">
-        <v>1109</v>
+        <v>1110</v>
       </c>
       <c r="B417" s="3" t="s">
-        <v>1110</v>
+        <v>1111</v>
       </c>
       <c r="C417" s="3"/>
       <c r="D417" s="3"/>
@@ -18586,10 +18595,10 @@
     </row>
     <row r="418" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A418" s="2" t="s">
-        <v>1111</v>
+        <v>1112</v>
       </c>
       <c r="B418" s="3" t="s">
-        <v>1112</v>
+        <v>1113</v>
       </c>
       <c r="C418" s="3"/>
       <c r="D418" s="3"/>
@@ -18618,10 +18627,10 @@
     </row>
     <row r="419" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A419" s="2" t="s">
-        <v>1113</v>
+        <v>1114</v>
       </c>
       <c r="B419" s="3" t="s">
-        <v>1114</v>
+        <v>1115</v>
       </c>
       <c r="C419" s="3"/>
       <c r="D419" s="3"/>
@@ -18650,10 +18659,10 @@
     </row>
     <row r="420" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A420" s="2" t="s">
-        <v>1115</v>
+        <v>1116</v>
       </c>
       <c r="B420" s="3" t="s">
-        <v>1116</v>
+        <v>1117</v>
       </c>
       <c r="C420" s="3"/>
       <c r="D420" s="3"/>
@@ -18682,10 +18691,10 @@
     </row>
     <row r="421" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A421" s="2" t="s">
-        <v>1117</v>
+        <v>1118</v>
       </c>
       <c r="B421" s="3" t="s">
-        <v>1118</v>
+        <v>1119</v>
       </c>
       <c r="C421" s="3"/>
       <c r="D421" s="3"/>
@@ -18714,10 +18723,10 @@
     </row>
     <row r="422" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A422" s="2" t="s">
-        <v>1119</v>
+        <v>1120</v>
       </c>
       <c r="B422" s="3" t="s">
-        <v>1120</v>
+        <v>1121</v>
       </c>
       <c r="C422" s="3"/>
       <c r="D422" s="3"/>
@@ -18746,10 +18755,10 @@
     </row>
     <row r="423" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A423" s="2" t="s">
-        <v>1121</v>
+        <v>1122</v>
       </c>
       <c r="B423" s="3" t="s">
-        <v>1122</v>
+        <v>1123</v>
       </c>
       <c r="C423" s="3"/>
       <c r="D423" s="3"/>
@@ -18778,10 +18787,10 @@
     </row>
     <row r="424" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A424" s="2" t="s">
-        <v>1123</v>
+        <v>1124</v>
       </c>
       <c r="B424" s="3" t="s">
-        <v>1124</v>
+        <v>1125</v>
       </c>
       <c r="C424" s="3"/>
       <c r="D424" s="3"/>
@@ -18810,10 +18819,10 @@
     </row>
     <row r="425" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A425" s="2" t="s">
-        <v>1125</v>
+        <v>1126</v>
       </c>
       <c r="B425" s="3" t="s">
-        <v>1126</v>
+        <v>1127</v>
       </c>
       <c r="C425" s="3"/>
       <c r="D425" s="3"/>
@@ -18842,10 +18851,10 @@
     </row>
     <row r="426" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A426" s="2" t="s">
-        <v>1127</v>
+        <v>1128</v>
       </c>
       <c r="B426" s="3" t="s">
-        <v>1128</v>
+        <v>1129</v>
       </c>
       <c r="C426" s="3"/>
       <c r="D426" s="3"/>
@@ -18874,10 +18883,10 @@
     </row>
     <row r="427" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A427" s="2" t="s">
-        <v>1129</v>
+        <v>1130</v>
       </c>
       <c r="B427" s="3" t="s">
-        <v>1130</v>
+        <v>1131</v>
       </c>
       <c r="C427" s="3"/>
       <c r="D427" s="3"/>
@@ -18906,10 +18915,10 @@
     </row>
     <row r="428" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A428" s="2" t="s">
-        <v>1131</v>
+        <v>1132</v>
       </c>
       <c r="B428" s="3" t="s">
-        <v>1132</v>
+        <v>1133</v>
       </c>
       <c r="C428" s="3"/>
       <c r="D428" s="3"/>
@@ -18938,10 +18947,10 @@
     </row>
     <row r="429" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A429" s="2" t="s">
-        <v>1133</v>
+        <v>1134</v>
       </c>
       <c r="B429" s="3" t="s">
-        <v>1134</v>
+        <v>1135</v>
       </c>
       <c r="C429" s="3"/>
       <c r="D429" s="3"/>
@@ -18970,10 +18979,10 @@
     </row>
     <row r="430" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A430" s="2" t="s">
-        <v>1135</v>
+        <v>1136</v>
       </c>
       <c r="B430" s="3" t="s">
-        <v>1136</v>
+        <v>1137</v>
       </c>
       <c r="C430" s="3"/>
       <c r="D430" s="3"/>
@@ -19002,10 +19011,10 @@
     </row>
     <row r="431" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A431" s="2" t="s">
-        <v>1137</v>
+        <v>1138</v>
       </c>
       <c r="B431" s="3" t="s">
-        <v>1138</v>
+        <v>1139</v>
       </c>
       <c r="C431" s="3"/>
       <c r="D431" s="3"/>
@@ -19034,10 +19043,10 @@
     </row>
     <row r="432" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A432" s="2" t="s">
-        <v>1139</v>
+        <v>1140</v>
       </c>
       <c r="B432" s="3" t="s">
-        <v>1140</v>
+        <v>1141</v>
       </c>
       <c r="C432" s="3"/>
       <c r="D432" s="3"/>
@@ -19066,10 +19075,10 @@
     </row>
     <row r="433" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A433" s="2" t="s">
-        <v>1141</v>
+        <v>1142</v>
       </c>
       <c r="B433" s="3" t="s">
-        <v>1142</v>
+        <v>1143</v>
       </c>
       <c r="C433" s="3"/>
       <c r="D433" s="3"/>
@@ -19098,10 +19107,10 @@
     </row>
     <row r="434" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A434" s="2" t="s">
-        <v>1143</v>
+        <v>1144</v>
       </c>
       <c r="B434" s="3" t="s">
-        <v>1144</v>
+        <v>1145</v>
       </c>
       <c r="C434" s="3"/>
       <c r="D434" s="3"/>
@@ -19130,10 +19139,10 @@
     </row>
     <row r="435" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A435" s="2" t="s">
-        <v>1145</v>
+        <v>1146</v>
       </c>
       <c r="B435" s="3" t="s">
-        <v>1146</v>
+        <v>1147</v>
       </c>
       <c r="C435" s="3"/>
       <c r="D435" s="3"/>
@@ -19162,10 +19171,10 @@
     </row>
     <row r="436" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A436" s="2" t="s">
-        <v>1147</v>
+        <v>1148</v>
       </c>
       <c r="B436" s="3" t="s">
-        <v>1148</v>
+        <v>1149</v>
       </c>
       <c r="C436" s="3"/>
       <c r="D436" s="3"/>
@@ -19194,10 +19203,10 @@
     </row>
     <row r="437" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A437" s="2" t="s">
-        <v>1149</v>
+        <v>1150</v>
       </c>
       <c r="B437" s="3" t="s">
-        <v>1150</v>
+        <v>1151</v>
       </c>
       <c r="C437" s="3"/>
       <c r="D437" s="3"/>
@@ -19226,10 +19235,10 @@
     </row>
     <row r="438" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A438" s="2" t="s">
-        <v>1151</v>
+        <v>1152</v>
       </c>
       <c r="B438" s="3" t="s">
-        <v>1152</v>
+        <v>1153</v>
       </c>
       <c r="C438" s="3"/>
       <c r="D438" s="3"/>
@@ -19258,10 +19267,10 @@
     </row>
     <row r="439" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A439" s="2" t="s">
-        <v>1153</v>
+        <v>1154</v>
       </c>
       <c r="B439" s="3" t="s">
-        <v>1154</v>
+        <v>1155</v>
       </c>
       <c r="C439" s="3"/>
       <c r="D439" s="3"/>
@@ -19290,10 +19299,10 @@
     </row>
     <row r="440" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A440" s="2" t="s">
-        <v>1155</v>
+        <v>1156</v>
       </c>
       <c r="B440" s="3" t="s">
-        <v>1156</v>
+        <v>1157</v>
       </c>
       <c r="C440" s="3"/>
       <c r="D440" s="3"/>
@@ -19322,10 +19331,10 @@
     </row>
     <row r="441" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A441" s="2" t="s">
-        <v>1157</v>
+        <v>1158</v>
       </c>
       <c r="B441" s="3" t="s">
-        <v>1158</v>
+        <v>1159</v>
       </c>
       <c r="C441" s="3"/>
       <c r="D441" s="3"/>
@@ -19354,10 +19363,10 @@
     </row>
     <row r="442" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A442" s="2" t="s">
-        <v>1159</v>
+        <v>1160</v>
       </c>
       <c r="B442" s="3" t="s">
-        <v>1160</v>
+        <v>1161</v>
       </c>
       <c r="C442" s="3"/>
       <c r="D442" s="3"/>
@@ -19386,10 +19395,10 @@
     </row>
     <row r="443" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A443" s="2" t="s">
-        <v>1161</v>
+        <v>1162</v>
       </c>
       <c r="B443" s="3" t="s">
-        <v>1162</v>
+        <v>1163</v>
       </c>
       <c r="C443" s="3"/>
       <c r="D443" s="3"/>
@@ -19418,10 +19427,10 @@
     </row>
     <row r="444" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A444" s="2" t="s">
-        <v>1163</v>
+        <v>1164</v>
       </c>
       <c r="B444" s="3" t="s">
-        <v>1164</v>
+        <v>1165</v>
       </c>
       <c r="C444" s="3"/>
       <c r="D444" s="3"/>
@@ -19450,10 +19459,10 @@
     </row>
     <row r="445" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A445" s="2" t="s">
-        <v>1165</v>
+        <v>1166</v>
       </c>
       <c r="B445" s="3" t="s">
-        <v>1166</v>
+        <v>1167</v>
       </c>
       <c r="C445" s="3"/>
       <c r="D445" s="3"/>
@@ -19482,10 +19491,10 @@
     </row>
     <row r="446" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A446" s="2" t="s">
-        <v>1167</v>
+        <v>1168</v>
       </c>
       <c r="B446" s="3" t="s">
-        <v>1168</v>
+        <v>1169</v>
       </c>
       <c r="C446" s="3"/>
       <c r="D446" s="3"/>
@@ -19514,7 +19523,7 @@
     </row>
     <row r="447" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A447" s="2" t="s">
-        <v>1169</v>
+        <v>1170</v>
       </c>
       <c r="B447" s="5"/>
       <c r="C447" s="5"/>
@@ -19544,7 +19553,7 @@
     </row>
     <row r="448" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A448" s="2" t="s">
-        <v>1170</v>
+        <v>1171</v>
       </c>
       <c r="B448" s="5"/>
       <c r="C448" s="5"/>
@@ -19574,7 +19583,7 @@
     </row>
     <row r="449" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A449" s="2" t="s">
-        <v>1171</v>
+        <v>1172</v>
       </c>
       <c r="B449" s="5"/>
       <c r="C449" s="5"/>
@@ -19604,10 +19613,10 @@
     </row>
     <row r="450" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A450" s="2" t="s">
-        <v>1172</v>
+        <v>1173</v>
       </c>
       <c r="B450" s="3" t="s">
-        <v>1173</v>
+        <v>1174</v>
       </c>
       <c r="C450" s="3"/>
       <c r="D450" s="3"/>
@@ -19636,10 +19645,10 @@
     </row>
     <row r="451" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A451" s="2" t="s">
-        <v>1174</v>
+        <v>1175</v>
       </c>
       <c r="B451" s="3" t="s">
-        <v>1175</v>
+        <v>1176</v>
       </c>
       <c r="C451" s="3"/>
       <c r="D451" s="3"/>
@@ -19668,10 +19677,10 @@
     </row>
     <row r="452" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A452" s="2" t="s">
-        <v>1176</v>
+        <v>1177</v>
       </c>
       <c r="B452" s="3" t="s">
-        <v>1177</v>
+        <v>1178</v>
       </c>
       <c r="C452" s="3"/>
       <c r="D452" s="3"/>
@@ -19700,10 +19709,10 @@
     </row>
     <row r="453" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A453" s="2" t="s">
-        <v>1178</v>
+        <v>1179</v>
       </c>
       <c r="B453" s="3" t="s">
-        <v>1179</v>
+        <v>1180</v>
       </c>
       <c r="C453" s="3"/>
       <c r="D453" s="3"/>
@@ -19732,10 +19741,10 @@
     </row>
     <row r="454" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A454" s="2" t="s">
-        <v>1180</v>
+        <v>1181</v>
       </c>
       <c r="B454" s="3" t="s">
-        <v>1181</v>
+        <v>1182</v>
       </c>
       <c r="C454" s="3"/>
       <c r="D454" s="3"/>
@@ -19764,10 +19773,10 @@
     </row>
     <row r="455" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A455" s="2" t="s">
-        <v>1182</v>
+        <v>1183</v>
       </c>
       <c r="B455" s="3" t="s">
-        <v>1183</v>
+        <v>1184</v>
       </c>
       <c r="C455" s="3"/>
       <c r="D455" s="3"/>
@@ -19796,10 +19805,10 @@
     </row>
     <row r="456" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A456" s="2" t="s">
-        <v>1184</v>
+        <v>1185</v>
       </c>
       <c r="B456" s="3" t="s">
-        <v>1185</v>
+        <v>1186</v>
       </c>
       <c r="C456" s="3"/>
       <c r="D456" s="3"/>
@@ -19828,10 +19837,10 @@
     </row>
     <row r="457" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A457" s="2" t="s">
-        <v>1186</v>
+        <v>1187</v>
       </c>
       <c r="B457" s="3" t="s">
-        <v>1187</v>
+        <v>1188</v>
       </c>
       <c r="C457" s="3"/>
       <c r="D457" s="3"/>
@@ -19860,10 +19869,10 @@
     </row>
     <row r="458" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A458" s="2" t="s">
-        <v>1188</v>
+        <v>1189</v>
       </c>
       <c r="B458" s="3" t="s">
-        <v>1189</v>
+        <v>1190</v>
       </c>
       <c r="C458" s="3"/>
       <c r="D458" s="3"/>
@@ -19892,10 +19901,10 @@
     </row>
     <row r="459" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A459" s="2" t="s">
-        <v>1190</v>
+        <v>1191</v>
       </c>
       <c r="B459" s="3" t="s">
-        <v>1191</v>
+        <v>1192</v>
       </c>
       <c r="C459" s="3"/>
       <c r="D459" s="3"/>
@@ -19924,10 +19933,10 @@
     </row>
     <row r="460" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A460" s="2" t="s">
-        <v>1192</v>
+        <v>1193</v>
       </c>
       <c r="B460" s="3" t="s">
-        <v>1193</v>
+        <v>1194</v>
       </c>
       <c r="C460" s="3"/>
       <c r="D460" s="3"/>
@@ -19956,10 +19965,10 @@
     </row>
     <row r="461" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A461" s="2" t="s">
-        <v>1194</v>
+        <v>1195</v>
       </c>
       <c r="B461" s="3" t="s">
-        <v>1195</v>
+        <v>1196</v>
       </c>
       <c r="C461" s="3"/>
       <c r="D461" s="3"/>
@@ -19988,10 +19997,10 @@
     </row>
     <row r="462" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A462" s="2" t="s">
-        <v>1196</v>
+        <v>1197</v>
       </c>
       <c r="B462" s="3" t="s">
-        <v>1197</v>
+        <v>1198</v>
       </c>
       <c r="C462" s="3"/>
       <c r="D462" s="3"/>
@@ -20020,10 +20029,10 @@
     </row>
     <row r="463" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A463" s="2" t="s">
-        <v>1198</v>
+        <v>1199</v>
       </c>
       <c r="B463" s="3" t="s">
-        <v>1199</v>
+        <v>1200</v>
       </c>
       <c r="C463" s="3"/>
       <c r="D463" s="3"/>
@@ -20052,10 +20061,10 @@
     </row>
     <row r="464" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A464" s="2" t="s">
-        <v>1200</v>
+        <v>1201</v>
       </c>
       <c r="B464" s="3" t="s">
-        <v>1201</v>
+        <v>1202</v>
       </c>
       <c r="C464" s="3"/>
       <c r="D464" s="3"/>
@@ -20084,10 +20093,10 @@
     </row>
     <row r="465" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A465" s="2" t="s">
-        <v>1202</v>
+        <v>1203</v>
       </c>
       <c r="B465" s="3" t="s">
-        <v>1203</v>
+        <v>1204</v>
       </c>
       <c r="C465" s="3"/>
       <c r="D465" s="3"/>
@@ -20116,7 +20125,7 @@
     </row>
     <row r="466" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A466" s="2" t="s">
-        <v>1204</v>
+        <v>1205</v>
       </c>
       <c r="B466" s="5"/>
       <c r="C466" s="5"/>
@@ -20146,21 +20155,21 @@
     </row>
     <row r="467" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A467" s="2" t="s">
-        <v>1205</v>
+        <v>1206</v>
       </c>
       <c r="B467" s="5"/>
       <c r="C467" s="5"/>
       <c r="D467" s="5"/>
-      <c r="E467" s="7"/>
-      <c r="F467" s="7"/>
-      <c r="G467" s="7"/>
-      <c r="H467" s="7"/>
-      <c r="I467" s="7"/>
-      <c r="J467" s="7"/>
-      <c r="K467" s="7"/>
-      <c r="L467" s="7"/>
-      <c r="M467" s="7"/>
-      <c r="N467" s="7"/>
+      <c r="E467" s="8"/>
+      <c r="F467" s="8"/>
+      <c r="G467" s="8"/>
+      <c r="H467" s="8"/>
+      <c r="I467" s="8"/>
+      <c r="J467" s="8"/>
+      <c r="K467" s="8"/>
+      <c r="L467" s="8"/>
+      <c r="M467" s="8"/>
+      <c r="N467" s="8"/>
       <c r="O467" s="5"/>
       <c r="P467" s="5"/>
       <c r="Q467" s="5"/>
@@ -20176,21 +20185,21 @@
     </row>
     <row r="468" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A468" s="2" t="s">
-        <v>1206</v>
+        <v>1207</v>
       </c>
       <c r="B468" s="5"/>
       <c r="C468" s="5"/>
       <c r="D468" s="5"/>
-      <c r="E468" s="7"/>
-      <c r="F468" s="7"/>
-      <c r="G468" s="7"/>
-      <c r="H468" s="7"/>
-      <c r="I468" s="7"/>
-      <c r="J468" s="7"/>
-      <c r="K468" s="7"/>
-      <c r="L468" s="7"/>
-      <c r="M468" s="7"/>
-      <c r="N468" s="7"/>
+      <c r="E468" s="8"/>
+      <c r="F468" s="8"/>
+      <c r="G468" s="8"/>
+      <c r="H468" s="8"/>
+      <c r="I468" s="8"/>
+      <c r="J468" s="8"/>
+      <c r="K468" s="8"/>
+      <c r="L468" s="8"/>
+      <c r="M468" s="8"/>
+      <c r="N468" s="8"/>
       <c r="O468" s="5"/>
       <c r="P468" s="5"/>
       <c r="Q468" s="5"/>
@@ -20206,21 +20215,21 @@
     </row>
     <row r="469" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A469" s="2" t="s">
-        <v>1207</v>
+        <v>1208</v>
       </c>
       <c r="B469" s="5"/>
       <c r="C469" s="5"/>
       <c r="D469" s="5"/>
-      <c r="E469" s="7"/>
-      <c r="F469" s="7"/>
-      <c r="G469" s="7"/>
-      <c r="H469" s="7"/>
-      <c r="I469" s="7"/>
-      <c r="J469" s="7"/>
-      <c r="K469" s="7"/>
-      <c r="L469" s="7"/>
-      <c r="M469" s="7"/>
-      <c r="N469" s="7"/>
+      <c r="E469" s="8"/>
+      <c r="F469" s="8"/>
+      <c r="G469" s="8"/>
+      <c r="H469" s="8"/>
+      <c r="I469" s="8"/>
+      <c r="J469" s="8"/>
+      <c r="K469" s="8"/>
+      <c r="L469" s="8"/>
+      <c r="M469" s="8"/>
+      <c r="N469" s="8"/>
       <c r="O469" s="5"/>
       <c r="P469" s="5"/>
       <c r="Q469" s="5"/>
@@ -20236,21 +20245,21 @@
     </row>
     <row r="470" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A470" s="2" t="s">
-        <v>1208</v>
+        <v>1209</v>
       </c>
       <c r="B470" s="5"/>
       <c r="C470" s="5"/>
       <c r="D470" s="5"/>
-      <c r="E470" s="7"/>
-      <c r="F470" s="7"/>
-      <c r="G470" s="7"/>
-      <c r="H470" s="7"/>
-      <c r="I470" s="7"/>
-      <c r="J470" s="7"/>
-      <c r="K470" s="7"/>
-      <c r="L470" s="7"/>
-      <c r="M470" s="7"/>
-      <c r="N470" s="7"/>
+      <c r="E470" s="8"/>
+      <c r="F470" s="8"/>
+      <c r="G470" s="8"/>
+      <c r="H470" s="8"/>
+      <c r="I470" s="8"/>
+      <c r="J470" s="8"/>
+      <c r="K470" s="8"/>
+      <c r="L470" s="8"/>
+      <c r="M470" s="8"/>
+      <c r="N470" s="8"/>
       <c r="O470" s="5"/>
       <c r="P470" s="5"/>
       <c r="Q470" s="5"/>
@@ -20266,21 +20275,21 @@
     </row>
     <row r="471" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A471" s="2" t="s">
-        <v>1209</v>
+        <v>1210</v>
       </c>
       <c r="B471" s="5"/>
       <c r="C471" s="5"/>
       <c r="D471" s="5"/>
-      <c r="E471" s="7"/>
-      <c r="F471" s="7"/>
-      <c r="G471" s="7"/>
-      <c r="H471" s="7"/>
-      <c r="I471" s="7"/>
-      <c r="J471" s="7"/>
-      <c r="K471" s="7"/>
-      <c r="L471" s="7"/>
-      <c r="M471" s="7"/>
-      <c r="N471" s="7"/>
+      <c r="E471" s="8"/>
+      <c r="F471" s="8"/>
+      <c r="G471" s="8"/>
+      <c r="H471" s="8"/>
+      <c r="I471" s="8"/>
+      <c r="J471" s="8"/>
+      <c r="K471" s="8"/>
+      <c r="L471" s="8"/>
+      <c r="M471" s="8"/>
+      <c r="N471" s="8"/>
       <c r="O471" s="5"/>
       <c r="P471" s="5"/>
       <c r="Q471" s="5"/>
@@ -20296,21 +20305,21 @@
     </row>
     <row r="472" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A472" s="2" t="s">
-        <v>1210</v>
+        <v>1211</v>
       </c>
       <c r="B472" s="5"/>
       <c r="C472" s="5"/>
       <c r="D472" s="5"/>
-      <c r="E472" s="7"/>
-      <c r="F472" s="7"/>
-      <c r="G472" s="7"/>
-      <c r="H472" s="7"/>
-      <c r="I472" s="7"/>
-      <c r="J472" s="7"/>
-      <c r="K472" s="7"/>
-      <c r="L472" s="7"/>
-      <c r="M472" s="7"/>
-      <c r="N472" s="7"/>
+      <c r="E472" s="8"/>
+      <c r="F472" s="8"/>
+      <c r="G472" s="8"/>
+      <c r="H472" s="8"/>
+      <c r="I472" s="8"/>
+      <c r="J472" s="8"/>
+      <c r="K472" s="8"/>
+      <c r="L472" s="8"/>
+      <c r="M472" s="8"/>
+      <c r="N472" s="8"/>
       <c r="O472" s="5"/>
       <c r="P472" s="5"/>
       <c r="Q472" s="5"/>
@@ -20326,7 +20335,7 @@
     </row>
     <row r="473" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A473" s="2" t="s">
-        <v>1211</v>
+        <v>1212</v>
       </c>
       <c r="B473" s="5"/>
       <c r="C473" s="5"/>
@@ -20356,7 +20365,7 @@
     </row>
     <row r="474" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A474" s="2" t="s">
-        <v>1212</v>
+        <v>1213</v>
       </c>
       <c r="B474" s="5"/>
       <c r="C474" s="5"/>
@@ -20386,7 +20395,7 @@
     </row>
     <row r="475" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A475" s="2" t="s">
-        <v>1213</v>
+        <v>1214</v>
       </c>
       <c r="B475" s="5"/>
       <c r="C475" s="5"/>
@@ -20416,7 +20425,7 @@
     </row>
     <row r="476" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A476" s="2" t="s">
-        <v>1214</v>
+        <v>1215</v>
       </c>
       <c r="B476" s="5"/>
       <c r="C476" s="5"/>
@@ -20446,7 +20455,7 @@
     </row>
     <row r="477" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A477" s="2" t="s">
-        <v>1215</v>
+        <v>1216</v>
       </c>
       <c r="B477" s="5"/>
       <c r="C477" s="5"/>
@@ -20476,7 +20485,7 @@
     </row>
     <row r="478" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A478" s="2" t="s">
-        <v>1216</v>
+        <v>1217</v>
       </c>
       <c r="B478" s="5"/>
       <c r="C478" s="5"/>
@@ -20506,7 +20515,7 @@
     </row>
     <row r="479" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A479" s="2" t="s">
-        <v>1217</v>
+        <v>1218</v>
       </c>
       <c r="B479" s="5"/>
       <c r="C479" s="5"/>
@@ -20536,7 +20545,7 @@
     </row>
     <row r="480" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A480" s="2" t="s">
-        <v>1218</v>
+        <v>1219</v>
       </c>
       <c r="B480" s="5"/>
       <c r="C480" s="5"/>
@@ -20566,7 +20575,7 @@
     </row>
     <row r="481" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A481" s="2" t="s">
-        <v>1219</v>
+        <v>1220</v>
       </c>
       <c r="B481" s="5"/>
       <c r="C481" s="5"/>
@@ -20595,25 +20604,25 @@
       <c r="Z481" s="1"/>
     </row>
     <row r="482" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A482" s="8"/>
-      <c r="B482" s="9"/>
-      <c r="C482" s="9"/>
-      <c r="D482" s="9"/>
-      <c r="E482" s="9"/>
-      <c r="F482" s="9"/>
-      <c r="G482" s="9"/>
-      <c r="H482" s="9"/>
+      <c r="A482" s="9"/>
+      <c r="B482" s="10"/>
+      <c r="C482" s="10"/>
+      <c r="D482" s="10"/>
+      <c r="E482" s="10"/>
+      <c r="F482" s="10"/>
+      <c r="G482" s="10"/>
+      <c r="H482" s="10"/>
       <c r="I482" s="3" t="s">
-        <v>1220</v>
+        <v>1221</v>
       </c>
       <c r="J482" s="3"/>
-      <c r="K482" s="9"/>
-      <c r="L482" s="9"/>
-      <c r="M482" s="9"/>
-      <c r="N482" s="9"/>
-      <c r="O482" s="9"/>
-      <c r="P482" s="9"/>
-      <c r="Q482" s="9"/>
+      <c r="K482" s="10"/>
+      <c r="L482" s="10"/>
+      <c r="M482" s="10"/>
+      <c r="N482" s="10"/>
+      <c r="O482" s="10"/>
+      <c r="P482" s="10"/>
+      <c r="Q482" s="10"/>
       <c r="R482" s="1"/>
       <c r="S482" s="1"/>
       <c r="T482" s="1"/>
@@ -20626,37 +20635,37 @@
     </row>
     <row r="483" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A483" s="2" t="s">
-        <v>1221</v>
+        <v>1222</v>
       </c>
       <c r="B483" s="4" t="s">
-        <v>1222</v>
+        <v>1223</v>
       </c>
       <c r="C483" s="4" t="s">
-        <v>1223</v>
+        <v>1224</v>
       </c>
       <c r="D483" s="4" t="s">
-        <v>1224</v>
+        <v>1225</v>
       </c>
       <c r="E483" s="4" t="s">
-        <v>1225</v>
+        <v>1226</v>
       </c>
       <c r="F483" s="4" t="s">
-        <v>1226</v>
+        <v>1227</v>
       </c>
       <c r="G483" s="4" t="s">
-        <v>1227</v>
+        <v>1228</v>
       </c>
       <c r="H483" s="4" t="s">
-        <v>1228</v>
+        <v>1229</v>
       </c>
       <c r="I483" s="4" t="s">
-        <v>1229</v>
+        <v>1230</v>
       </c>
       <c r="J483" s="4" t="s">
-        <v>1230</v>
+        <v>1231</v>
       </c>
       <c r="K483" s="4" t="s">
-        <v>1231</v>
+        <v>1232</v>
       </c>
       <c r="L483" s="5"/>
       <c r="M483" s="5"/>
@@ -20676,37 +20685,37 @@
     </row>
     <row r="484" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A484" s="2" t="s">
-        <v>1232</v>
+        <v>1233</v>
       </c>
       <c r="B484" s="4" t="s">
-        <v>1233</v>
+        <v>1234</v>
       </c>
       <c r="C484" s="4" t="s">
-        <v>1234</v>
+        <v>1235</v>
       </c>
       <c r="D484" s="4" t="s">
-        <v>1235</v>
+        <v>1236</v>
       </c>
       <c r="E484" s="4" t="s">
-        <v>1236</v>
+        <v>1237</v>
       </c>
       <c r="F484" s="4" t="s">
-        <v>1237</v>
+        <v>1238</v>
       </c>
       <c r="G484" s="4" t="s">
-        <v>1238</v>
+        <v>1239</v>
       </c>
       <c r="H484" s="4" t="s">
-        <v>1239</v>
+        <v>1240</v>
       </c>
       <c r="I484" s="4" t="s">
-        <v>1240</v>
+        <v>1241</v>
       </c>
       <c r="J484" s="4" t="s">
-        <v>1241</v>
+        <v>1242</v>
       </c>
       <c r="K484" s="4" t="s">
-        <v>1242</v>
+        <v>1243</v>
       </c>
       <c r="L484" s="5"/>
       <c r="M484" s="5"/>
@@ -20726,37 +20735,37 @@
     </row>
     <row r="485" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A485" s="2" t="s">
-        <v>1243</v>
+        <v>1244</v>
       </c>
       <c r="B485" s="4" t="s">
-        <v>1244</v>
+        <v>1245</v>
       </c>
       <c r="C485" s="4" t="s">
-        <v>1245</v>
+        <v>1246</v>
       </c>
       <c r="D485" s="4" t="s">
-        <v>1246</v>
+        <v>1247</v>
       </c>
       <c r="E485" s="4" t="s">
-        <v>1247</v>
+        <v>1248</v>
       </c>
       <c r="F485" s="4" t="s">
-        <v>1248</v>
+        <v>1249</v>
       </c>
       <c r="G485" s="4" t="s">
-        <v>1249</v>
+        <v>1250</v>
       </c>
       <c r="H485" s="4" t="s">
-        <v>1250</v>
+        <v>1251</v>
       </c>
       <c r="I485" s="4" t="s">
-        <v>1251</v>
+        <v>1252</v>
       </c>
       <c r="J485" s="4" t="s">
-        <v>1252</v>
+        <v>1253</v>
       </c>
       <c r="K485" s="4" t="s">
-        <v>1253</v>
+        <v>1254</v>
       </c>
       <c r="L485" s="5"/>
       <c r="M485" s="5"/>
@@ -20776,37 +20785,37 @@
     </row>
     <row r="486" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A486" s="2" t="s">
-        <v>1254</v>
+        <v>1255</v>
       </c>
       <c r="B486" s="4" t="s">
-        <v>1255</v>
+        <v>1256</v>
       </c>
       <c r="C486" s="4" t="s">
-        <v>1256</v>
+        <v>1257</v>
       </c>
       <c r="D486" s="4" t="s">
-        <v>1257</v>
+        <v>1258</v>
       </c>
       <c r="E486" s="4" t="s">
-        <v>1258</v>
+        <v>1259</v>
       </c>
       <c r="F486" s="4" t="s">
-        <v>1259</v>
+        <v>1260</v>
       </c>
       <c r="G486" s="4" t="s">
-        <v>1260</v>
+        <v>1261</v>
       </c>
       <c r="H486" s="4" t="s">
-        <v>1261</v>
+        <v>1262</v>
       </c>
       <c r="I486" s="4" t="s">
-        <v>1262</v>
+        <v>1263</v>
       </c>
       <c r="J486" s="4" t="s">
-        <v>1263</v>
+        <v>1264</v>
       </c>
       <c r="K486" s="4" t="s">
-        <v>1264</v>
+        <v>1265</v>
       </c>
       <c r="L486" s="5"/>
       <c r="M486" s="5"/>
@@ -20826,37 +20835,37 @@
     </row>
     <row r="487" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A487" s="2" t="s">
-        <v>1265</v>
+        <v>1266</v>
       </c>
       <c r="B487" s="4" t="s">
-        <v>1266</v>
+        <v>1267</v>
       </c>
       <c r="C487" s="4" t="s">
-        <v>1267</v>
+        <v>1268</v>
       </c>
       <c r="D487" s="4" t="s">
-        <v>1268</v>
+        <v>1269</v>
       </c>
       <c r="E487" s="4" t="s">
-        <v>1269</v>
+        <v>1270</v>
       </c>
       <c r="F487" s="4" t="s">
-        <v>1270</v>
+        <v>1271</v>
       </c>
       <c r="G487" s="4" t="s">
-        <v>1271</v>
+        <v>1272</v>
       </c>
       <c r="H487" s="4" t="s">
-        <v>1272</v>
+        <v>1273</v>
       </c>
       <c r="I487" s="4" t="s">
-        <v>1273</v>
+        <v>1274</v>
       </c>
       <c r="J487" s="4" t="s">
-        <v>1274</v>
+        <v>1275</v>
       </c>
       <c r="K487" s="4" t="s">
-        <v>1275</v>
+        <v>1276</v>
       </c>
       <c r="L487" s="5"/>
       <c r="M487" s="5"/>
@@ -20876,37 +20885,37 @@
     </row>
     <row r="488" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A488" s="2" t="s">
-        <v>1276</v>
+        <v>1277</v>
       </c>
       <c r="B488" s="4" t="s">
-        <v>1277</v>
+        <v>1278</v>
       </c>
       <c r="C488" s="4" t="s">
-        <v>1278</v>
+        <v>1279</v>
       </c>
       <c r="D488" s="4" t="s">
-        <v>1279</v>
+        <v>1280</v>
       </c>
       <c r="E488" s="4" t="s">
-        <v>1280</v>
+        <v>1281</v>
       </c>
       <c r="F488" s="4" t="s">
-        <v>1281</v>
+        <v>1282</v>
       </c>
       <c r="G488" s="4" t="s">
-        <v>1282</v>
+        <v>1283</v>
       </c>
       <c r="H488" s="4" t="s">
-        <v>1283</v>
+        <v>1284</v>
       </c>
       <c r="I488" s="4" t="s">
-        <v>1284</v>
+        <v>1285</v>
       </c>
       <c r="J488" s="4" t="s">
-        <v>1285</v>
+        <v>1286</v>
       </c>
       <c r="K488" s="4" t="s">
-        <v>1286</v>
+        <v>1287</v>
       </c>
       <c r="L488" s="5"/>
       <c r="M488" s="5"/>
@@ -20926,37 +20935,37 @@
     </row>
     <row r="489" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A489" s="2" t="s">
-        <v>1287</v>
+        <v>1288</v>
       </c>
       <c r="B489" s="4" t="s">
-        <v>1288</v>
+        <v>1289</v>
       </c>
       <c r="C489" s="4" t="s">
-        <v>1289</v>
+        <v>1290</v>
       </c>
       <c r="D489" s="4" t="s">
-        <v>1290</v>
+        <v>1291</v>
       </c>
       <c r="E489" s="4" t="s">
-        <v>1291</v>
+        <v>1292</v>
       </c>
       <c r="F489" s="4" t="s">
-        <v>1292</v>
+        <v>1293</v>
       </c>
       <c r="G489" s="4" t="s">
-        <v>1293</v>
+        <v>1294</v>
       </c>
       <c r="H489" s="4" t="s">
-        <v>1294</v>
+        <v>1295</v>
       </c>
       <c r="I489" s="4" t="s">
-        <v>1295</v>
+        <v>1296</v>
       </c>
       <c r="J489" s="4" t="s">
-        <v>1296</v>
+        <v>1297</v>
       </c>
       <c r="K489" s="4" t="s">
-        <v>1297</v>
+        <v>1298</v>
       </c>
       <c r="L489" s="5"/>
       <c r="M489" s="5"/>
@@ -20976,37 +20985,37 @@
     </row>
     <row r="490" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A490" s="2" t="s">
-        <v>1298</v>
+        <v>1299</v>
       </c>
       <c r="B490" s="4" t="s">
-        <v>1299</v>
+        <v>1300</v>
       </c>
       <c r="C490" s="4" t="s">
-        <v>1300</v>
+        <v>1301</v>
       </c>
       <c r="D490" s="4" t="s">
-        <v>1301</v>
+        <v>1302</v>
       </c>
       <c r="E490" s="4" t="s">
-        <v>1302</v>
+        <v>1303</v>
       </c>
       <c r="F490" s="4" t="s">
-        <v>1303</v>
+        <v>1304</v>
       </c>
       <c r="G490" s="4" t="s">
-        <v>1304</v>
+        <v>1305</v>
       </c>
       <c r="H490" s="4" t="s">
-        <v>1305</v>
+        <v>1306</v>
       </c>
       <c r="I490" s="4" t="s">
-        <v>1306</v>
+        <v>1307</v>
       </c>
       <c r="J490" s="4" t="s">
-        <v>1307</v>
+        <v>1308</v>
       </c>
       <c r="K490" s="4" t="s">
-        <v>1308</v>
+        <v>1309</v>
       </c>
       <c r="L490" s="5"/>
       <c r="M490" s="5"/>
@@ -21026,37 +21035,37 @@
     </row>
     <row r="491" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A491" s="2" t="s">
-        <v>1309</v>
+        <v>1310</v>
       </c>
       <c r="B491" s="4" t="s">
-        <v>1310</v>
+        <v>1311</v>
       </c>
       <c r="C491" s="4" t="s">
-        <v>1311</v>
+        <v>1312</v>
       </c>
       <c r="D491" s="4" t="s">
-        <v>1312</v>
+        <v>1313</v>
       </c>
       <c r="E491" s="4" t="s">
-        <v>1313</v>
+        <v>1314</v>
       </c>
       <c r="F491" s="4" t="s">
-        <v>1314</v>
+        <v>1315</v>
       </c>
       <c r="G491" s="4" t="s">
-        <v>1315</v>
+        <v>1316</v>
       </c>
       <c r="H491" s="4" t="s">
-        <v>1316</v>
+        <v>1317</v>
       </c>
       <c r="I491" s="4" t="s">
-        <v>1317</v>
+        <v>1318</v>
       </c>
       <c r="J491" s="4" t="s">
-        <v>1318</v>
+        <v>1319</v>
       </c>
       <c r="K491" s="4" t="s">
-        <v>1319</v>
+        <v>1320</v>
       </c>
       <c r="L491" s="5"/>
       <c r="M491" s="5"/>
@@ -21076,37 +21085,37 @@
     </row>
     <row r="492" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A492" s="2" t="s">
-        <v>1320</v>
+        <v>1321</v>
       </c>
       <c r="B492" s="4" t="s">
-        <v>1321</v>
+        <v>1322</v>
       </c>
       <c r="C492" s="4" t="s">
-        <v>1322</v>
+        <v>1323</v>
       </c>
       <c r="D492" s="4" t="s">
-        <v>1323</v>
+        <v>1324</v>
       </c>
       <c r="E492" s="4" t="s">
-        <v>1324</v>
+        <v>1325</v>
       </c>
       <c r="F492" s="4" t="s">
-        <v>1325</v>
+        <v>1326</v>
       </c>
       <c r="G492" s="4" t="s">
-        <v>1326</v>
+        <v>1327</v>
       </c>
       <c r="H492" s="4" t="s">
-        <v>1327</v>
+        <v>1328</v>
       </c>
       <c r="I492" s="4" t="s">
-        <v>1328</v>
+        <v>1329</v>
       </c>
       <c r="J492" s="4" t="s">
-        <v>1329</v>
+        <v>1330</v>
       </c>
       <c r="K492" s="4" t="s">
-        <v>1330</v>
+        <v>1331</v>
       </c>
       <c r="L492" s="5"/>
       <c r="M492" s="5"/>
@@ -21126,37 +21135,37 @@
     </row>
     <row r="493" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A493" s="2" t="s">
-        <v>1331</v>
+        <v>1332</v>
       </c>
       <c r="B493" s="4" t="s">
-        <v>1332</v>
+        <v>1333</v>
       </c>
       <c r="C493" s="4" t="s">
-        <v>1333</v>
+        <v>1334</v>
       </c>
       <c r="D493" s="4" t="s">
-        <v>1334</v>
+        <v>1335</v>
       </c>
       <c r="E493" s="4" t="s">
-        <v>1335</v>
+        <v>1336</v>
       </c>
       <c r="F493" s="4" t="s">
-        <v>1336</v>
+        <v>1337</v>
       </c>
       <c r="G493" s="4" t="s">
-        <v>1337</v>
+        <v>1338</v>
       </c>
       <c r="H493" s="4" t="s">
-        <v>1338</v>
+        <v>1339</v>
       </c>
       <c r="I493" s="4" t="s">
-        <v>1339</v>
+        <v>1340</v>
       </c>
       <c r="J493" s="4" t="s">
-        <v>1340</v>
+        <v>1341</v>
       </c>
       <c r="K493" s="4" t="s">
-        <v>1341</v>
+        <v>1342</v>
       </c>
       <c r="L493" s="5"/>
       <c r="M493" s="5"/>
@@ -21176,37 +21185,37 @@
     </row>
     <row r="494" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A494" s="2" t="s">
-        <v>1342</v>
+        <v>1343</v>
       </c>
       <c r="B494" s="4" t="s">
-        <v>1343</v>
+        <v>1344</v>
       </c>
       <c r="C494" s="4" t="s">
-        <v>1344</v>
+        <v>1345</v>
       </c>
       <c r="D494" s="4" t="s">
-        <v>1345</v>
+        <v>1346</v>
       </c>
       <c r="E494" s="4" t="s">
-        <v>1346</v>
+        <v>1347</v>
       </c>
       <c r="F494" s="4" t="s">
-        <v>1347</v>
+        <v>1348</v>
       </c>
       <c r="G494" s="4" t="s">
-        <v>1348</v>
+        <v>1349</v>
       </c>
       <c r="H494" s="4" t="s">
-        <v>1349</v>
+        <v>1350</v>
       </c>
       <c r="I494" s="4" t="s">
-        <v>1350</v>
+        <v>1351</v>
       </c>
       <c r="J494" s="4" t="s">
-        <v>1351</v>
+        <v>1352</v>
       </c>
       <c r="K494" s="4" t="s">
-        <v>1352</v>
+        <v>1353</v>
       </c>
       <c r="L494" s="5"/>
       <c r="M494" s="5"/>
@@ -21226,38 +21235,38 @@
     </row>
     <row r="495" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A495" s="2" t="s">
-        <v>1353</v>
+        <v>1354</v>
       </c>
       <c r="B495" s="3" t="s">
-        <v>1354</v>
+        <v>1355</v>
       </c>
       <c r="C495" s="3"/>
       <c r="D495" s="3" t="s">
-        <v>1355</v>
+        <v>1356</v>
       </c>
       <c r="E495" s="3"/>
       <c r="F495" s="3" t="s">
-        <v>1356</v>
+        <v>1357</v>
       </c>
       <c r="G495" s="3"/>
       <c r="H495" s="3" t="s">
-        <v>1357</v>
+        <v>1358</v>
       </c>
       <c r="I495" s="3"/>
       <c r="J495" s="3" t="s">
-        <v>1358</v>
+        <v>1359</v>
       </c>
       <c r="K495" s="3"/>
       <c r="L495" s="3" t="s">
-        <v>1359</v>
+        <v>1360</v>
       </c>
       <c r="M495" s="3"/>
       <c r="N495" s="3" t="s">
-        <v>1360</v>
+        <v>1361</v>
       </c>
       <c r="O495" s="3"/>
       <c r="P495" s="3" t="s">
-        <v>1361</v>
+        <v>1362</v>
       </c>
       <c r="Q495" s="3"/>
       <c r="R495" s="1"/>
@@ -21272,34 +21281,34 @@
     </row>
     <row r="496" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A496" s="2" t="s">
-        <v>1362</v>
+        <v>1363</v>
       </c>
       <c r="B496" s="4" t="s">
-        <v>1363</v>
+        <v>1364</v>
       </c>
       <c r="C496" s="4" t="s">
-        <v>1364</v>
+        <v>1365</v>
       </c>
       <c r="D496" s="4" t="s">
-        <v>1365</v>
+        <v>1366</v>
       </c>
       <c r="E496" s="4" t="s">
-        <v>1366</v>
+        <v>1367</v>
       </c>
       <c r="F496" s="4" t="s">
-        <v>1367</v>
+        <v>1368</v>
       </c>
       <c r="G496" s="4" t="s">
-        <v>1368</v>
+        <v>1369</v>
       </c>
       <c r="H496" s="4" t="s">
-        <v>1369</v>
+        <v>1370</v>
       </c>
       <c r="I496" s="4" t="s">
-        <v>1370</v>
+        <v>1371</v>
       </c>
       <c r="J496" s="4" t="s">
-        <v>1371</v>
+        <v>1372</v>
       </c>
       <c r="K496" s="5"/>
       <c r="L496" s="5"/>
@@ -21320,34 +21329,34 @@
     </row>
     <row r="497" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A497" s="2" t="s">
-        <v>1372</v>
+        <v>1373</v>
       </c>
       <c r="B497" s="4" t="s">
-        <v>1373</v>
+        <v>1374</v>
       </c>
       <c r="C497" s="4" t="s">
-        <v>1374</v>
+        <v>1375</v>
       </c>
       <c r="D497" s="4" t="s">
-        <v>1375</v>
+        <v>1376</v>
       </c>
       <c r="E497" s="4" t="s">
-        <v>1376</v>
+        <v>1377</v>
       </c>
       <c r="F497" s="4" t="s">
-        <v>1377</v>
+        <v>1378</v>
       </c>
       <c r="G497" s="4" t="s">
-        <v>1378</v>
+        <v>1379</v>
       </c>
       <c r="H497" s="4" t="s">
-        <v>1379</v>
+        <v>1380</v>
       </c>
       <c r="I497" s="4" t="s">
-        <v>1380</v>
+        <v>1381</v>
       </c>
       <c r="J497" s="4" t="s">
-        <v>1381</v>
+        <v>1382</v>
       </c>
       <c r="K497" s="5"/>
       <c r="L497" s="5"/>
@@ -21368,34 +21377,34 @@
     </row>
     <row r="498" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A498" s="2" t="s">
-        <v>1382</v>
+        <v>1383</v>
       </c>
       <c r="B498" s="4" t="s">
-        <v>1383</v>
+        <v>1384</v>
       </c>
       <c r="C498" s="4" t="s">
-        <v>1384</v>
+        <v>1385</v>
       </c>
       <c r="D498" s="4" t="s">
-        <v>1385</v>
+        <v>1386</v>
       </c>
       <c r="E498" s="4" t="s">
-        <v>1386</v>
+        <v>1387</v>
       </c>
       <c r="F498" s="4" t="s">
-        <v>1387</v>
+        <v>1388</v>
       </c>
       <c r="G498" s="4" t="s">
-        <v>1388</v>
+        <v>1389</v>
       </c>
       <c r="H498" s="4" t="s">
-        <v>1389</v>
+        <v>1390</v>
       </c>
       <c r="I498" s="4" t="s">
-        <v>1390</v>
+        <v>1391</v>
       </c>
       <c r="J498" s="4" t="s">
-        <v>1391</v>
+        <v>1392</v>
       </c>
       <c r="K498" s="5"/>
       <c r="L498" s="5"/>
@@ -21416,34 +21425,34 @@
     </row>
     <row r="499" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A499" s="2" t="s">
-        <v>1392</v>
+        <v>1393</v>
       </c>
       <c r="B499" s="4" t="s">
-        <v>1393</v>
+        <v>1394</v>
       </c>
       <c r="C499" s="4" t="s">
-        <v>1394</v>
+        <v>1395</v>
       </c>
       <c r="D499" s="4" t="s">
-        <v>1395</v>
+        <v>1396</v>
       </c>
       <c r="E499" s="4" t="s">
-        <v>1396</v>
+        <v>1397</v>
       </c>
       <c r="F499" s="4" t="s">
-        <v>1397</v>
+        <v>1398</v>
       </c>
       <c r="G499" s="4" t="s">
-        <v>1398</v>
+        <v>1399</v>
       </c>
       <c r="H499" s="4" t="s">
-        <v>1399</v>
+        <v>1400</v>
       </c>
       <c r="I499" s="4" t="s">
-        <v>1400</v>
+        <v>1401</v>
       </c>
       <c r="J499" s="4" t="s">
-        <v>1401</v>
+        <v>1402</v>
       </c>
       <c r="K499" s="5"/>
       <c r="L499" s="5"/>
@@ -21464,34 +21473,34 @@
     </row>
     <row r="500" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A500" s="2" t="s">
-        <v>1402</v>
+        <v>1403</v>
       </c>
       <c r="B500" s="4" t="s">
-        <v>1403</v>
+        <v>1404</v>
       </c>
       <c r="C500" s="4" t="s">
-        <v>1404</v>
+        <v>1405</v>
       </c>
       <c r="D500" s="4" t="s">
-        <v>1405</v>
+        <v>1406</v>
       </c>
       <c r="E500" s="4" t="s">
-        <v>1406</v>
+        <v>1407</v>
       </c>
       <c r="F500" s="4" t="s">
-        <v>1407</v>
+        <v>1408</v>
       </c>
       <c r="G500" s="4" t="s">
-        <v>1408</v>
+        <v>1409</v>
       </c>
       <c r="H500" s="4" t="s">
-        <v>1409</v>
+        <v>1410</v>
       </c>
       <c r="I500" s="4" t="s">
-        <v>1410</v>
+        <v>1411</v>
       </c>
       <c r="J500" s="4" t="s">
-        <v>1411</v>
+        <v>1412</v>
       </c>
       <c r="K500" s="5"/>
       <c r="L500" s="5"/>
@@ -21512,34 +21521,34 @@
     </row>
     <row r="501" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A501" s="2" t="s">
-        <v>1412</v>
+        <v>1413</v>
       </c>
       <c r="B501" s="4" t="s">
-        <v>1413</v>
+        <v>1414</v>
       </c>
       <c r="C501" s="4" t="s">
-        <v>1414</v>
+        <v>1415</v>
       </c>
       <c r="D501" s="4" t="s">
-        <v>1415</v>
+        <v>1416</v>
       </c>
       <c r="E501" s="4" t="s">
-        <v>1416</v>
+        <v>1417</v>
       </c>
       <c r="F501" s="4" t="s">
-        <v>1417</v>
+        <v>1418</v>
       </c>
       <c r="G501" s="4" t="s">
-        <v>1418</v>
+        <v>1419</v>
       </c>
       <c r="H501" s="4" t="s">
-        <v>1419</v>
+        <v>1420</v>
       </c>
       <c r="I501" s="4" t="s">
-        <v>1420</v>
+        <v>1421</v>
       </c>
       <c r="J501" s="4" t="s">
-        <v>1421</v>
+        <v>1422</v>
       </c>
       <c r="K501" s="5"/>
       <c r="L501" s="5"/>
@@ -21560,34 +21569,34 @@
     </row>
     <row r="502" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A502" s="2" t="s">
-        <v>1422</v>
+        <v>1423</v>
       </c>
       <c r="B502" s="4" t="s">
-        <v>1423</v>
+        <v>1424</v>
       </c>
       <c r="C502" s="4" t="s">
-        <v>1424</v>
+        <v>1425</v>
       </c>
       <c r="D502" s="4" t="s">
-        <v>1425</v>
+        <v>1426</v>
       </c>
       <c r="E502" s="4" t="s">
-        <v>1426</v>
+        <v>1427</v>
       </c>
       <c r="F502" s="4" t="s">
-        <v>1427</v>
+        <v>1428</v>
       </c>
       <c r="G502" s="4" t="s">
-        <v>1428</v>
+        <v>1429</v>
       </c>
       <c r="H502" s="4" t="s">
-        <v>1429</v>
+        <v>1430</v>
       </c>
       <c r="I502" s="4" t="s">
-        <v>1430</v>
+        <v>1431</v>
       </c>
       <c r="J502" s="4" t="s">
-        <v>1431</v>
+        <v>1432</v>
       </c>
       <c r="K502" s="5"/>
       <c r="L502" s="5"/>
@@ -21608,30 +21617,30 @@
     </row>
     <row r="503" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A503" s="2" t="s">
-        <v>1432</v>
+        <v>1433</v>
       </c>
       <c r="B503" s="3" t="s">
-        <v>1433</v>
+        <v>1434</v>
       </c>
       <c r="C503" s="3"/>
       <c r="D503" s="3" t="s">
-        <v>1434</v>
+        <v>1435</v>
       </c>
       <c r="E503" s="3"/>
       <c r="F503" s="3" t="s">
-        <v>1435</v>
+        <v>1436</v>
       </c>
       <c r="G503" s="3"/>
       <c r="H503" s="3" t="s">
-        <v>1436</v>
+        <v>1437</v>
       </c>
       <c r="I503" s="3"/>
       <c r="J503" s="3" t="s">
-        <v>1437</v>
+        <v>1438</v>
       </c>
       <c r="K503" s="3"/>
       <c r="L503" s="3" t="s">
-        <v>1438</v>
+        <v>1439</v>
       </c>
       <c r="M503" s="3"/>
       <c r="N503" s="5"/>
@@ -21650,38 +21659,38 @@
     </row>
     <row r="504" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A504" s="2" t="s">
-        <v>1439</v>
+        <v>1440</v>
       </c>
       <c r="B504" s="3" t="s">
-        <v>1440</v>
+        <v>1441</v>
       </c>
       <c r="C504" s="3"/>
       <c r="D504" s="3" t="s">
-        <v>1441</v>
+        <v>1442</v>
       </c>
       <c r="E504" s="3"/>
       <c r="F504" s="3" t="s">
-        <v>1442</v>
+        <v>1443</v>
       </c>
       <c r="G504" s="3"/>
       <c r="H504" s="3" t="s">
-        <v>1443</v>
+        <v>1444</v>
       </c>
       <c r="I504" s="3"/>
       <c r="J504" s="3" t="s">
-        <v>1444</v>
+        <v>1445</v>
       </c>
       <c r="K504" s="3"/>
       <c r="L504" s="3" t="s">
-        <v>1445</v>
+        <v>1446</v>
       </c>
       <c r="M504" s="3"/>
       <c r="N504" s="3" t="s">
-        <v>1446</v>
+        <v>1447</v>
       </c>
       <c r="O504" s="3"/>
       <c r="P504" s="3" t="s">
-        <v>1447</v>
+        <v>1448</v>
       </c>
       <c r="Q504" s="3"/>
       <c r="R504" s="1"/>
@@ -21696,14 +21705,14 @@
     </row>
     <row r="505" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A505" s="2" t="s">
-        <v>1448</v>
+        <v>1449</v>
       </c>
       <c r="B505" s="3" t="s">
-        <v>1449</v>
+        <v>1450</v>
       </c>
       <c r="C505" s="3"/>
       <c r="D505" s="3" t="s">
-        <v>1450</v>
+        <v>1451</v>
       </c>
       <c r="E505" s="3"/>
       <c r="F505" s="5"/>
@@ -21711,19 +21720,19 @@
       <c r="H505" s="5"/>
       <c r="I505" s="5"/>
       <c r="J505" s="3" t="s">
-        <v>1451</v>
+        <v>1452</v>
       </c>
       <c r="K505" s="3"/>
       <c r="L505" s="3" t="s">
-        <v>1452</v>
+        <v>1453</v>
       </c>
       <c r="M505" s="3"/>
       <c r="N505" s="3" t="s">
-        <v>1453</v>
+        <v>1454</v>
       </c>
       <c r="O505" s="3"/>
       <c r="P505" s="3" t="s">
-        <v>1454</v>
+        <v>1455</v>
       </c>
       <c r="Q505" s="3"/>
       <c r="R505" s="1"/>
@@ -21738,30 +21747,30 @@
     </row>
     <row r="506" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A506" s="2" t="s">
-        <v>1455</v>
+        <v>1456</v>
       </c>
       <c r="B506" s="3" t="s">
-        <v>1456</v>
+        <v>1457</v>
       </c>
       <c r="C506" s="3"/>
       <c r="D506" s="3" t="s">
-        <v>1457</v>
+        <v>1458</v>
       </c>
       <c r="E506" s="3"/>
       <c r="F506" s="3" t="s">
-        <v>1458</v>
+        <v>1459</v>
       </c>
       <c r="G506" s="3"/>
       <c r="H506" s="3" t="s">
-        <v>1459</v>
+        <v>1460</v>
       </c>
       <c r="I506" s="3"/>
       <c r="J506" s="3" t="s">
-        <v>1460</v>
+        <v>1461</v>
       </c>
       <c r="K506" s="3"/>
       <c r="L506" s="3" t="s">
-        <v>1461</v>
+        <v>1462</v>
       </c>
       <c r="M506" s="3"/>
       <c r="N506" s="5"/>
@@ -21780,28 +21789,28 @@
     </row>
     <row r="507" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A507" s="2" t="s">
-        <v>1462</v>
+        <v>1463</v>
       </c>
       <c r="B507" s="4" t="s">
-        <v>1463</v>
+        <v>1464</v>
       </c>
       <c r="C507" s="4" t="s">
-        <v>1464</v>
+        <v>1465</v>
       </c>
       <c r="D507" s="4" t="s">
-        <v>1465</v>
+        <v>1466</v>
       </c>
       <c r="E507" s="4" t="s">
-        <v>1466</v>
+        <v>1467</v>
       </c>
       <c r="F507" s="4" t="s">
-        <v>1467</v>
+        <v>1468</v>
       </c>
       <c r="G507" s="5"/>
       <c r="H507" s="5"/>
       <c r="I507" s="5"/>
       <c r="J507" s="3" t="s">
-        <v>1468</v>
+        <v>1469</v>
       </c>
       <c r="K507" s="3"/>
       <c r="L507" s="5"/>
@@ -21809,10 +21818,10 @@
       <c r="N507" s="5"/>
       <c r="O507" s="5"/>
       <c r="P507" s="4" t="s">
-        <v>1469</v>
+        <v>1470</v>
       </c>
       <c r="Q507" s="4" t="s">
-        <v>1470</v>
+        <v>1471</v>
       </c>
       <c r="R507" s="1"/>
       <c r="S507" s="1"/>
@@ -21826,7 +21835,7 @@
     </row>
     <row r="508" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A508" s="2" t="s">
-        <v>1471</v>
+        <v>1472</v>
       </c>
       <c r="B508" s="5"/>
       <c r="C508" s="5"/>
@@ -21856,7 +21865,7 @@
     </row>
     <row r="509" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A509" s="2" t="s">
-        <v>1472</v>
+        <v>1473</v>
       </c>
       <c r="B509" s="5"/>
       <c r="C509" s="5"/>
@@ -21886,7 +21895,7 @@
     </row>
     <row r="510" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A510" s="2" t="s">
-        <v>1473</v>
+        <v>1474</v>
       </c>
       <c r="B510" s="5"/>
       <c r="C510" s="5"/>
@@ -21916,7 +21925,7 @@
     </row>
     <row r="511" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A511" s="2" t="s">
-        <v>1474</v>
+        <v>1475</v>
       </c>
       <c r="B511" s="5"/>
       <c r="C511" s="5"/>
@@ -21946,7 +21955,7 @@
     </row>
     <row r="512" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A512" s="2" t="s">
-        <v>1475</v>
+        <v>1476</v>
       </c>
       <c r="B512" s="5"/>
       <c r="C512" s="5"/>
@@ -21976,7 +21985,7 @@
     </row>
     <row r="513" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A513" s="2" t="s">
-        <v>1476</v>
+        <v>1477</v>
       </c>
       <c r="B513" s="5"/>
       <c r="C513" s="5"/>
@@ -22006,7 +22015,7 @@
     </row>
     <row r="514" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A514" s="2" t="s">
-        <v>1477</v>
+        <v>1478</v>
       </c>
       <c r="B514" s="5"/>
       <c r="C514" s="5"/>

</xml_diff>

<commit_message>
Added RxAGC MENU item.
</commit_message>
<xml_diff>
--- a/docs/UV K5 EEPROM.xlsx
+++ b/docs/UV K5 EEPROM.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1481" uniqueCount="1479">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1482" uniqueCount="1480">
   <si>
     <t xml:space="preserve">00</t>
   </si>
@@ -2189,6 +2189,9 @@
   </si>
   <si>
     <t xml:space="preserve">VOX Delay</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RX_AGC</t>
   </si>
   <si>
     <t xml:space="preserve">AL-MOD</t>
@@ -4559,7 +4562,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -4584,11 +4587,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -4683,11 +4690,11 @@
   </sheetPr>
   <dimension ref="A1:Z1001"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A208" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A212" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="F227" activeCellId="0" sqref="F227"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6796875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.6953125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1"/>
@@ -12575,7 +12582,7 @@
       <c r="I233" s="4" t="s">
         <v>689</v>
       </c>
-      <c r="J233" s="6" t="s">
+      <c r="J233" s="1" t="s">
         <v>690</v>
       </c>
       <c r="K233" s="4" t="s">
@@ -12661,7 +12668,7 @@
       <c r="Y234" s="1"/>
       <c r="Z234" s="1"/>
     </row>
-    <row r="235" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="235" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A235" s="2" t="s">
         <v>710</v>
       </c>
@@ -12695,12 +12702,12 @@
       <c r="K235" s="3"/>
       <c r="L235" s="3"/>
       <c r="M235" s="3"/>
-      <c r="N235" s="7" t="s">
+      <c r="N235" s="3" t="s">
         <v>720</v>
       </c>
-      <c r="O235" s="7"/>
-      <c r="P235" s="7"/>
-      <c r="Q235" s="7"/>
+      <c r="O235" s="3"/>
+      <c r="P235" s="3"/>
+      <c r="Q235" s="3"/>
       <c r="R235" s="1"/>
       <c r="S235" s="1"/>
       <c r="T235" s="1"/>
@@ -12711,31 +12718,33 @@
       <c r="Y235" s="1"/>
       <c r="Z235" s="1"/>
     </row>
-    <row r="236" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="236" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A236" s="2" t="s">
         <v>721</v>
       </c>
       <c r="B236" s="4" t="s">
         <v>722</v>
       </c>
-      <c r="C236" s="5"/>
-      <c r="D236" s="5"/>
-      <c r="E236" s="5"/>
-      <c r="F236" s="5"/>
-      <c r="G236" s="5"/>
+      <c r="C236" s="6" t="s">
+        <v>723</v>
+      </c>
+      <c r="D236" s="7"/>
+      <c r="E236" s="7"/>
+      <c r="F236" s="7"/>
+      <c r="G236" s="8"/>
       <c r="H236" s="5"/>
       <c r="I236" s="5"/>
       <c r="J236" s="4" t="s">
-        <v>723</v>
+        <v>724</v>
       </c>
       <c r="K236" s="4" t="s">
-        <v>724</v>
+        <v>725</v>
       </c>
       <c r="L236" s="4" t="s">
-        <v>725</v>
+        <v>726</v>
       </c>
       <c r="M236" s="4" t="s">
-        <v>726</v>
+        <v>727</v>
       </c>
       <c r="N236" s="5"/>
       <c r="O236" s="5"/>
@@ -12753,10 +12762,10 @@
     </row>
     <row r="237" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A237" s="2" t="s">
-        <v>727</v>
+        <v>728</v>
       </c>
       <c r="B237" s="3" t="s">
-        <v>728</v>
+        <v>729</v>
       </c>
       <c r="C237" s="3"/>
       <c r="D237" s="3"/>
@@ -12785,10 +12794,10 @@
     </row>
     <row r="238" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A238" s="2" t="s">
-        <v>729</v>
+        <v>730</v>
       </c>
       <c r="B238" s="3" t="s">
-        <v>730</v>
+        <v>731</v>
       </c>
       <c r="C238" s="3"/>
       <c r="D238" s="3"/>
@@ -12817,40 +12826,40 @@
     </row>
     <row r="239" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A239" s="2" t="s">
-        <v>731</v>
+        <v>732</v>
       </c>
       <c r="B239" s="4" t="s">
-        <v>732</v>
+        <v>733</v>
       </c>
       <c r="C239" s="4" t="s">
-        <v>733</v>
+        <v>734</v>
       </c>
       <c r="D239" s="4" t="s">
-        <v>734</v>
+        <v>735</v>
       </c>
       <c r="E239" s="4" t="s">
-        <v>735</v>
+        <v>736</v>
       </c>
       <c r="F239" s="4" t="s">
-        <v>736</v>
+        <v>737</v>
       </c>
       <c r="G239" s="4" t="s">
-        <v>737</v>
+        <v>738</v>
       </c>
       <c r="H239" s="4" t="s">
-        <v>738</v>
+        <v>739</v>
       </c>
       <c r="I239" s="4" t="s">
-        <v>739</v>
+        <v>740</v>
       </c>
       <c r="J239" s="4" t="s">
-        <v>740</v>
+        <v>741</v>
       </c>
       <c r="K239" s="4" t="s">
-        <v>741</v>
+        <v>742</v>
       </c>
       <c r="L239" s="4" t="s">
-        <v>742</v>
+        <v>743</v>
       </c>
       <c r="M239" s="5"/>
       <c r="N239" s="5"/>
@@ -12869,10 +12878,10 @@
     </row>
     <row r="240" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A240" s="2" t="s">
-        <v>743</v>
+        <v>744</v>
       </c>
       <c r="B240" s="3" t="s">
-        <v>744</v>
+        <v>745</v>
       </c>
       <c r="C240" s="3"/>
       <c r="D240" s="3"/>
@@ -12882,7 +12891,7 @@
       <c r="H240" s="3"/>
       <c r="I240" s="3"/>
       <c r="J240" s="3" t="s">
-        <v>745</v>
+        <v>746</v>
       </c>
       <c r="K240" s="3"/>
       <c r="L240" s="3"/>
@@ -12903,10 +12912,10 @@
     </row>
     <row r="241" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A241" s="2" t="s">
-        <v>746</v>
+        <v>747</v>
       </c>
       <c r="B241" s="3" t="s">
-        <v>747</v>
+        <v>748</v>
       </c>
       <c r="C241" s="3"/>
       <c r="D241" s="3"/>
@@ -12916,7 +12925,7 @@
       <c r="H241" s="3"/>
       <c r="I241" s="3"/>
       <c r="J241" s="3" t="s">
-        <v>748</v>
+        <v>749</v>
       </c>
       <c r="K241" s="3"/>
       <c r="L241" s="3"/>
@@ -12937,10 +12946,10 @@
     </row>
     <row r="242" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A242" s="2" t="s">
+        <v>750</v>
+      </c>
+      <c r="B242" s="3" t="s">
         <v>749</v>
-      </c>
-      <c r="B242" s="3" t="s">
-        <v>748</v>
       </c>
       <c r="C242" s="3"/>
       <c r="D242" s="3"/>
@@ -12950,7 +12959,7 @@
       <c r="H242" s="3"/>
       <c r="I242" s="3"/>
       <c r="J242" s="3" t="s">
-        <v>750</v>
+        <v>751</v>
       </c>
       <c r="K242" s="3"/>
       <c r="L242" s="3"/>
@@ -12971,10 +12980,10 @@
     </row>
     <row r="243" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A243" s="2" t="s">
+        <v>752</v>
+      </c>
+      <c r="B243" s="3" t="s">
         <v>751</v>
-      </c>
-      <c r="B243" s="3" t="s">
-        <v>750</v>
       </c>
       <c r="C243" s="3"/>
       <c r="D243" s="3"/>
@@ -12984,25 +12993,25 @@
       <c r="H243" s="3"/>
       <c r="I243" s="3"/>
       <c r="J243" s="4" t="s">
-        <v>752</v>
+        <v>753</v>
       </c>
       <c r="K243" s="4" t="s">
-        <v>753</v>
+        <v>754</v>
       </c>
       <c r="L243" s="4" t="s">
-        <v>754</v>
+        <v>755</v>
       </c>
       <c r="M243" s="4" t="s">
-        <v>755</v>
+        <v>756</v>
       </c>
       <c r="N243" s="4" t="s">
-        <v>756</v>
+        <v>757</v>
       </c>
       <c r="O243" s="4" t="s">
-        <v>757</v>
+        <v>758</v>
       </c>
       <c r="P243" s="4" t="s">
-        <v>758</v>
+        <v>759</v>
       </c>
       <c r="Q243" s="5"/>
       <c r="R243" s="1"/>
@@ -13017,7 +13026,7 @@
     </row>
     <row r="244" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A244" s="2" t="s">
-        <v>759</v>
+        <v>760</v>
       </c>
       <c r="B244" s="5"/>
       <c r="C244" s="5"/>
@@ -13047,10 +13056,10 @@
     </row>
     <row r="245" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A245" s="2" t="s">
-        <v>760</v>
+        <v>761</v>
       </c>
       <c r="B245" s="3" t="s">
-        <v>761</v>
+        <v>762</v>
       </c>
       <c r="C245" s="3"/>
       <c r="D245" s="3"/>
@@ -13079,28 +13088,28 @@
     </row>
     <row r="246" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A246" s="2" t="s">
-        <v>762</v>
+        <v>763</v>
       </c>
       <c r="B246" s="4" t="s">
-        <v>763</v>
+        <v>764</v>
       </c>
       <c r="C246" s="4" t="s">
-        <v>764</v>
+        <v>765</v>
       </c>
       <c r="D246" s="4" t="s">
-        <v>765</v>
+        <v>766</v>
       </c>
       <c r="E246" s="4" t="s">
-        <v>766</v>
+        <v>767</v>
       </c>
       <c r="F246" s="4" t="s">
-        <v>767</v>
+        <v>768</v>
       </c>
       <c r="G246" s="4" t="s">
-        <v>768</v>
+        <v>769</v>
       </c>
       <c r="H246" s="4" t="s">
-        <v>769</v>
+        <v>770</v>
       </c>
       <c r="I246" s="5"/>
       <c r="J246" s="5"/>
@@ -13123,10 +13132,10 @@
     </row>
     <row r="247" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A247" s="2" t="s">
-        <v>770</v>
+        <v>771</v>
       </c>
       <c r="B247" s="3" t="s">
-        <v>771</v>
+        <v>772</v>
       </c>
       <c r="C247" s="3"/>
       <c r="D247" s="3"/>
@@ -13155,10 +13164,10 @@
     </row>
     <row r="248" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A248" s="2" t="s">
-        <v>772</v>
+        <v>773</v>
       </c>
       <c r="B248" s="3" t="s">
-        <v>773</v>
+        <v>774</v>
       </c>
       <c r="C248" s="3"/>
       <c r="D248" s="3"/>
@@ -13187,10 +13196,10 @@
     </row>
     <row r="249" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A249" s="2" t="s">
-        <v>774</v>
+        <v>775</v>
       </c>
       <c r="B249" s="3" t="s">
-        <v>775</v>
+        <v>776</v>
       </c>
       <c r="C249" s="3"/>
       <c r="D249" s="3"/>
@@ -13219,10 +13228,10 @@
     </row>
     <row r="250" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A250" s="2" t="s">
-        <v>776</v>
+        <v>777</v>
       </c>
       <c r="B250" s="3" t="s">
-        <v>777</v>
+        <v>778</v>
       </c>
       <c r="C250" s="3"/>
       <c r="D250" s="3"/>
@@ -13251,10 +13260,10 @@
     </row>
     <row r="251" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A251" s="2" t="s">
-        <v>778</v>
+        <v>779</v>
       </c>
       <c r="B251" s="3" t="s">
-        <v>779</v>
+        <v>780</v>
       </c>
       <c r="C251" s="3"/>
       <c r="D251" s="3"/>
@@ -13283,10 +13292,10 @@
     </row>
     <row r="252" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A252" s="2" t="s">
-        <v>780</v>
+        <v>781</v>
       </c>
       <c r="B252" s="3" t="s">
-        <v>781</v>
+        <v>782</v>
       </c>
       <c r="C252" s="3"/>
       <c r="D252" s="3"/>
@@ -13315,10 +13324,10 @@
     </row>
     <row r="253" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A253" s="2" t="s">
-        <v>782</v>
+        <v>783</v>
       </c>
       <c r="B253" s="3" t="s">
-        <v>783</v>
+        <v>784</v>
       </c>
       <c r="C253" s="3"/>
       <c r="D253" s="3"/>
@@ -13347,10 +13356,10 @@
     </row>
     <row r="254" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A254" s="2" t="s">
-        <v>784</v>
+        <v>785</v>
       </c>
       <c r="B254" s="3" t="s">
-        <v>785</v>
+        <v>786</v>
       </c>
       <c r="C254" s="3"/>
       <c r="D254" s="3"/>
@@ -13379,10 +13388,10 @@
     </row>
     <row r="255" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A255" s="2" t="s">
-        <v>786</v>
+        <v>787</v>
       </c>
       <c r="B255" s="3" t="s">
-        <v>787</v>
+        <v>788</v>
       </c>
       <c r="C255" s="3"/>
       <c r="D255" s="3"/>
@@ -13411,10 +13420,10 @@
     </row>
     <row r="256" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A256" s="2" t="s">
-        <v>788</v>
+        <v>789</v>
       </c>
       <c r="B256" s="3" t="s">
-        <v>789</v>
+        <v>790</v>
       </c>
       <c r="C256" s="3"/>
       <c r="D256" s="3"/>
@@ -13443,10 +13452,10 @@
     </row>
     <row r="257" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A257" s="2" t="s">
-        <v>790</v>
+        <v>791</v>
       </c>
       <c r="B257" s="3" t="s">
-        <v>791</v>
+        <v>792</v>
       </c>
       <c r="C257" s="3"/>
       <c r="D257" s="3"/>
@@ -13475,10 +13484,10 @@
     </row>
     <row r="258" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A258" s="2" t="s">
-        <v>792</v>
+        <v>793</v>
       </c>
       <c r="B258" s="3" t="s">
-        <v>793</v>
+        <v>794</v>
       </c>
       <c r="C258" s="3"/>
       <c r="D258" s="3"/>
@@ -13507,10 +13516,10 @@
     </row>
     <row r="259" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A259" s="2" t="s">
-        <v>794</v>
+        <v>795</v>
       </c>
       <c r="B259" s="3" t="s">
-        <v>795</v>
+        <v>796</v>
       </c>
       <c r="C259" s="3"/>
       <c r="D259" s="3"/>
@@ -13539,10 +13548,10 @@
     </row>
     <row r="260" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A260" s="2" t="s">
-        <v>796</v>
+        <v>797</v>
       </c>
       <c r="B260" s="3" t="s">
-        <v>797</v>
+        <v>798</v>
       </c>
       <c r="C260" s="3"/>
       <c r="D260" s="3"/>
@@ -13571,10 +13580,10 @@
     </row>
     <row r="261" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A261" s="2" t="s">
-        <v>798</v>
+        <v>799</v>
       </c>
       <c r="B261" s="3" t="s">
-        <v>799</v>
+        <v>800</v>
       </c>
       <c r="C261" s="3"/>
       <c r="D261" s="3"/>
@@ -13603,10 +13612,10 @@
     </row>
     <row r="262" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A262" s="2" t="s">
-        <v>800</v>
+        <v>801</v>
       </c>
       <c r="B262" s="3" t="s">
-        <v>801</v>
+        <v>802</v>
       </c>
       <c r="C262" s="3"/>
       <c r="D262" s="3"/>
@@ -13635,10 +13644,10 @@
     </row>
     <row r="263" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A263" s="2" t="s">
-        <v>802</v>
+        <v>803</v>
       </c>
       <c r="B263" s="3" t="s">
-        <v>803</v>
+        <v>804</v>
       </c>
       <c r="C263" s="3"/>
       <c r="D263" s="3"/>
@@ -13667,10 +13676,10 @@
     </row>
     <row r="264" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A264" s="2" t="s">
-        <v>804</v>
+        <v>805</v>
       </c>
       <c r="B264" s="3" t="s">
-        <v>805</v>
+        <v>806</v>
       </c>
       <c r="C264" s="3"/>
       <c r="D264" s="3"/>
@@ -13699,10 +13708,10 @@
     </row>
     <row r="265" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A265" s="2" t="s">
-        <v>806</v>
+        <v>807</v>
       </c>
       <c r="B265" s="3" t="s">
-        <v>807</v>
+        <v>808</v>
       </c>
       <c r="C265" s="3"/>
       <c r="D265" s="3"/>
@@ -13731,10 +13740,10 @@
     </row>
     <row r="266" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A266" s="2" t="s">
-        <v>808</v>
+        <v>809</v>
       </c>
       <c r="B266" s="3" t="s">
-        <v>809</v>
+        <v>810</v>
       </c>
       <c r="C266" s="3"/>
       <c r="D266" s="3"/>
@@ -13763,10 +13772,10 @@
     </row>
     <row r="267" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A267" s="2" t="s">
-        <v>810</v>
+        <v>811</v>
       </c>
       <c r="B267" s="3" t="s">
-        <v>811</v>
+        <v>812</v>
       </c>
       <c r="C267" s="3"/>
       <c r="D267" s="3"/>
@@ -13795,10 +13804,10 @@
     </row>
     <row r="268" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A268" s="2" t="s">
-        <v>812</v>
+        <v>813</v>
       </c>
       <c r="B268" s="3" t="s">
-        <v>813</v>
+        <v>814</v>
       </c>
       <c r="C268" s="3"/>
       <c r="D268" s="3"/>
@@ -13827,10 +13836,10 @@
     </row>
     <row r="269" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A269" s="2" t="s">
-        <v>814</v>
+        <v>815</v>
       </c>
       <c r="B269" s="3" t="s">
-        <v>815</v>
+        <v>816</v>
       </c>
       <c r="C269" s="3"/>
       <c r="D269" s="3"/>
@@ -13859,10 +13868,10 @@
     </row>
     <row r="270" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A270" s="2" t="s">
-        <v>816</v>
+        <v>817</v>
       </c>
       <c r="B270" s="3" t="s">
-        <v>817</v>
+        <v>818</v>
       </c>
       <c r="C270" s="3"/>
       <c r="D270" s="3"/>
@@ -13891,10 +13900,10 @@
     </row>
     <row r="271" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A271" s="2" t="s">
-        <v>818</v>
+        <v>819</v>
       </c>
       <c r="B271" s="3" t="s">
-        <v>819</v>
+        <v>820</v>
       </c>
       <c r="C271" s="3"/>
       <c r="D271" s="3"/>
@@ -13923,10 +13932,10 @@
     </row>
     <row r="272" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A272" s="2" t="s">
-        <v>820</v>
+        <v>821</v>
       </c>
       <c r="B272" s="3" t="s">
-        <v>821</v>
+        <v>822</v>
       </c>
       <c r="C272" s="3"/>
       <c r="D272" s="3"/>
@@ -13955,10 +13964,10 @@
     </row>
     <row r="273" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A273" s="2" t="s">
-        <v>822</v>
+        <v>823</v>
       </c>
       <c r="B273" s="3" t="s">
-        <v>823</v>
+        <v>824</v>
       </c>
       <c r="C273" s="3"/>
       <c r="D273" s="3"/>
@@ -13987,10 +13996,10 @@
     </row>
     <row r="274" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A274" s="2" t="s">
-        <v>824</v>
+        <v>825</v>
       </c>
       <c r="B274" s="3" t="s">
-        <v>825</v>
+        <v>826</v>
       </c>
       <c r="C274" s="3"/>
       <c r="D274" s="3"/>
@@ -14019,10 +14028,10 @@
     </row>
     <row r="275" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A275" s="2" t="s">
-        <v>826</v>
+        <v>827</v>
       </c>
       <c r="B275" s="3" t="s">
-        <v>827</v>
+        <v>828</v>
       </c>
       <c r="C275" s="3"/>
       <c r="D275" s="3"/>
@@ -14051,10 +14060,10 @@
     </row>
     <row r="276" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A276" s="2" t="s">
-        <v>828</v>
+        <v>829</v>
       </c>
       <c r="B276" s="3" t="s">
-        <v>829</v>
+        <v>830</v>
       </c>
       <c r="C276" s="3"/>
       <c r="D276" s="3"/>
@@ -14083,10 +14092,10 @@
     </row>
     <row r="277" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A277" s="2" t="s">
-        <v>830</v>
+        <v>831</v>
       </c>
       <c r="B277" s="3" t="s">
-        <v>831</v>
+        <v>832</v>
       </c>
       <c r="C277" s="3"/>
       <c r="D277" s="3"/>
@@ -14115,10 +14124,10 @@
     </row>
     <row r="278" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A278" s="2" t="s">
-        <v>832</v>
+        <v>833</v>
       </c>
       <c r="B278" s="3" t="s">
-        <v>833</v>
+        <v>834</v>
       </c>
       <c r="C278" s="3"/>
       <c r="D278" s="3"/>
@@ -14147,10 +14156,10 @@
     </row>
     <row r="279" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A279" s="2" t="s">
-        <v>834</v>
+        <v>835</v>
       </c>
       <c r="B279" s="3" t="s">
-        <v>835</v>
+        <v>836</v>
       </c>
       <c r="C279" s="3"/>
       <c r="D279" s="3"/>
@@ -14179,10 +14188,10 @@
     </row>
     <row r="280" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A280" s="2" t="s">
-        <v>836</v>
+        <v>837</v>
       </c>
       <c r="B280" s="3" t="s">
-        <v>837</v>
+        <v>838</v>
       </c>
       <c r="C280" s="3"/>
       <c r="D280" s="3"/>
@@ -14211,10 +14220,10 @@
     </row>
     <row r="281" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A281" s="2" t="s">
-        <v>838</v>
+        <v>839</v>
       </c>
       <c r="B281" s="3" t="s">
-        <v>839</v>
+        <v>840</v>
       </c>
       <c r="C281" s="3"/>
       <c r="D281" s="3"/>
@@ -14243,10 +14252,10 @@
     </row>
     <row r="282" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A282" s="2" t="s">
-        <v>840</v>
+        <v>841</v>
       </c>
       <c r="B282" s="3" t="s">
-        <v>841</v>
+        <v>842</v>
       </c>
       <c r="C282" s="3"/>
       <c r="D282" s="3"/>
@@ -14275,10 +14284,10 @@
     </row>
     <row r="283" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A283" s="2" t="s">
-        <v>842</v>
+        <v>843</v>
       </c>
       <c r="B283" s="3" t="s">
-        <v>843</v>
+        <v>844</v>
       </c>
       <c r="C283" s="3"/>
       <c r="D283" s="3"/>
@@ -14307,10 +14316,10 @@
     </row>
     <row r="284" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A284" s="2" t="s">
-        <v>844</v>
+        <v>845</v>
       </c>
       <c r="B284" s="3" t="s">
-        <v>845</v>
+        <v>846</v>
       </c>
       <c r="C284" s="3"/>
       <c r="D284" s="3"/>
@@ -14339,10 +14348,10 @@
     </row>
     <row r="285" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A285" s="2" t="s">
-        <v>846</v>
+        <v>847</v>
       </c>
       <c r="B285" s="3" t="s">
-        <v>847</v>
+        <v>848</v>
       </c>
       <c r="C285" s="3"/>
       <c r="D285" s="3"/>
@@ -14371,10 +14380,10 @@
     </row>
     <row r="286" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A286" s="2" t="s">
-        <v>848</v>
+        <v>849</v>
       </c>
       <c r="B286" s="3" t="s">
-        <v>849</v>
+        <v>850</v>
       </c>
       <c r="C286" s="3"/>
       <c r="D286" s="3"/>
@@ -14403,10 +14412,10 @@
     </row>
     <row r="287" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A287" s="2" t="s">
-        <v>850</v>
+        <v>851</v>
       </c>
       <c r="B287" s="3" t="s">
-        <v>851</v>
+        <v>852</v>
       </c>
       <c r="C287" s="3"/>
       <c r="D287" s="3"/>
@@ -14435,10 +14444,10 @@
     </row>
     <row r="288" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A288" s="2" t="s">
-        <v>852</v>
+        <v>853</v>
       </c>
       <c r="B288" s="3" t="s">
-        <v>853</v>
+        <v>854</v>
       </c>
       <c r="C288" s="3"/>
       <c r="D288" s="3"/>
@@ -14467,10 +14476,10 @@
     </row>
     <row r="289" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A289" s="2" t="s">
-        <v>854</v>
+        <v>855</v>
       </c>
       <c r="B289" s="3" t="s">
-        <v>855</v>
+        <v>856</v>
       </c>
       <c r="C289" s="3"/>
       <c r="D289" s="3"/>
@@ -14499,10 +14508,10 @@
     </row>
     <row r="290" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A290" s="2" t="s">
-        <v>856</v>
+        <v>857</v>
       </c>
       <c r="B290" s="3" t="s">
-        <v>857</v>
+        <v>858</v>
       </c>
       <c r="C290" s="3"/>
       <c r="D290" s="3"/>
@@ -14531,10 +14540,10 @@
     </row>
     <row r="291" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A291" s="2" t="s">
-        <v>858</v>
+        <v>859</v>
       </c>
       <c r="B291" s="3" t="s">
-        <v>859</v>
+        <v>860</v>
       </c>
       <c r="C291" s="3"/>
       <c r="D291" s="3"/>
@@ -14563,10 +14572,10 @@
     </row>
     <row r="292" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A292" s="2" t="s">
-        <v>860</v>
+        <v>861</v>
       </c>
       <c r="B292" s="3" t="s">
-        <v>861</v>
+        <v>862</v>
       </c>
       <c r="C292" s="3"/>
       <c r="D292" s="3"/>
@@ -14595,10 +14604,10 @@
     </row>
     <row r="293" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A293" s="2" t="s">
-        <v>862</v>
+        <v>863</v>
       </c>
       <c r="B293" s="3" t="s">
-        <v>863</v>
+        <v>864</v>
       </c>
       <c r="C293" s="3"/>
       <c r="D293" s="3"/>
@@ -14627,10 +14636,10 @@
     </row>
     <row r="294" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A294" s="2" t="s">
-        <v>864</v>
+        <v>865</v>
       </c>
       <c r="B294" s="3" t="s">
-        <v>865</v>
+        <v>866</v>
       </c>
       <c r="C294" s="3"/>
       <c r="D294" s="3"/>
@@ -14659,10 +14668,10 @@
     </row>
     <row r="295" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A295" s="2" t="s">
-        <v>866</v>
+        <v>867</v>
       </c>
       <c r="B295" s="3" t="s">
-        <v>867</v>
+        <v>868</v>
       </c>
       <c r="C295" s="3"/>
       <c r="D295" s="3"/>
@@ -14691,10 +14700,10 @@
     </row>
     <row r="296" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A296" s="2" t="s">
-        <v>868</v>
+        <v>869</v>
       </c>
       <c r="B296" s="3" t="s">
-        <v>869</v>
+        <v>870</v>
       </c>
       <c r="C296" s="3"/>
       <c r="D296" s="3"/>
@@ -14723,10 +14732,10 @@
     </row>
     <row r="297" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A297" s="2" t="s">
-        <v>870</v>
+        <v>871</v>
       </c>
       <c r="B297" s="3" t="s">
-        <v>871</v>
+        <v>872</v>
       </c>
       <c r="C297" s="3"/>
       <c r="D297" s="3"/>
@@ -14755,10 +14764,10 @@
     </row>
     <row r="298" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A298" s="2" t="s">
-        <v>872</v>
+        <v>873</v>
       </c>
       <c r="B298" s="3" t="s">
-        <v>873</v>
+        <v>874</v>
       </c>
       <c r="C298" s="3"/>
       <c r="D298" s="3"/>
@@ -14787,10 +14796,10 @@
     </row>
     <row r="299" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A299" s="2" t="s">
-        <v>874</v>
+        <v>875</v>
       </c>
       <c r="B299" s="3" t="s">
-        <v>875</v>
+        <v>876</v>
       </c>
       <c r="C299" s="3"/>
       <c r="D299" s="3"/>
@@ -14819,10 +14828,10 @@
     </row>
     <row r="300" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A300" s="2" t="s">
-        <v>876</v>
+        <v>877</v>
       </c>
       <c r="B300" s="3" t="s">
-        <v>877</v>
+        <v>878</v>
       </c>
       <c r="C300" s="3"/>
       <c r="D300" s="3"/>
@@ -14851,10 +14860,10 @@
     </row>
     <row r="301" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A301" s="2" t="s">
-        <v>878</v>
+        <v>879</v>
       </c>
       <c r="B301" s="3" t="s">
-        <v>879</v>
+        <v>880</v>
       </c>
       <c r="C301" s="3"/>
       <c r="D301" s="3"/>
@@ -14883,10 +14892,10 @@
     </row>
     <row r="302" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A302" s="2" t="s">
-        <v>880</v>
+        <v>881</v>
       </c>
       <c r="B302" s="3" t="s">
-        <v>881</v>
+        <v>882</v>
       </c>
       <c r="C302" s="3"/>
       <c r="D302" s="3"/>
@@ -14915,10 +14924,10 @@
     </row>
     <row r="303" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A303" s="2" t="s">
-        <v>882</v>
+        <v>883</v>
       </c>
       <c r="B303" s="3" t="s">
-        <v>883</v>
+        <v>884</v>
       </c>
       <c r="C303" s="3"/>
       <c r="D303" s="3"/>
@@ -14947,10 +14956,10 @@
     </row>
     <row r="304" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A304" s="2" t="s">
-        <v>884</v>
+        <v>885</v>
       </c>
       <c r="B304" s="3" t="s">
-        <v>885</v>
+        <v>886</v>
       </c>
       <c r="C304" s="3"/>
       <c r="D304" s="3"/>
@@ -14979,10 +14988,10 @@
     </row>
     <row r="305" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A305" s="2" t="s">
-        <v>886</v>
+        <v>887</v>
       </c>
       <c r="B305" s="3" t="s">
-        <v>887</v>
+        <v>888</v>
       </c>
       <c r="C305" s="3"/>
       <c r="D305" s="3"/>
@@ -15011,10 +15020,10 @@
     </row>
     <row r="306" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A306" s="2" t="s">
-        <v>888</v>
+        <v>889</v>
       </c>
       <c r="B306" s="3" t="s">
-        <v>889</v>
+        <v>890</v>
       </c>
       <c r="C306" s="3"/>
       <c r="D306" s="3"/>
@@ -15043,10 +15052,10 @@
     </row>
     <row r="307" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A307" s="2" t="s">
-        <v>890</v>
+        <v>891</v>
       </c>
       <c r="B307" s="3" t="s">
-        <v>891</v>
+        <v>892</v>
       </c>
       <c r="C307" s="3"/>
       <c r="D307" s="3"/>
@@ -15075,10 +15084,10 @@
     </row>
     <row r="308" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A308" s="2" t="s">
-        <v>892</v>
+        <v>893</v>
       </c>
       <c r="B308" s="3" t="s">
-        <v>893</v>
+        <v>894</v>
       </c>
       <c r="C308" s="3"/>
       <c r="D308" s="3"/>
@@ -15107,10 +15116,10 @@
     </row>
     <row r="309" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A309" s="2" t="s">
-        <v>894</v>
+        <v>895</v>
       </c>
       <c r="B309" s="3" t="s">
-        <v>895</v>
+        <v>896</v>
       </c>
       <c r="C309" s="3"/>
       <c r="D309" s="3"/>
@@ -15139,10 +15148,10 @@
     </row>
     <row r="310" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A310" s="2" t="s">
-        <v>896</v>
+        <v>897</v>
       </c>
       <c r="B310" s="3" t="s">
-        <v>897</v>
+        <v>898</v>
       </c>
       <c r="C310" s="3"/>
       <c r="D310" s="3"/>
@@ -15171,10 +15180,10 @@
     </row>
     <row r="311" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A311" s="2" t="s">
-        <v>898</v>
+        <v>899</v>
       </c>
       <c r="B311" s="3" t="s">
-        <v>899</v>
+        <v>900</v>
       </c>
       <c r="C311" s="3"/>
       <c r="D311" s="3"/>
@@ -15203,10 +15212,10 @@
     </row>
     <row r="312" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A312" s="2" t="s">
-        <v>900</v>
+        <v>901</v>
       </c>
       <c r="B312" s="3" t="s">
-        <v>901</v>
+        <v>902</v>
       </c>
       <c r="C312" s="3"/>
       <c r="D312" s="3"/>
@@ -15235,10 +15244,10 @@
     </row>
     <row r="313" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A313" s="2" t="s">
-        <v>902</v>
+        <v>903</v>
       </c>
       <c r="B313" s="3" t="s">
-        <v>903</v>
+        <v>904</v>
       </c>
       <c r="C313" s="3"/>
       <c r="D313" s="3"/>
@@ -15267,10 +15276,10 @@
     </row>
     <row r="314" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A314" s="2" t="s">
-        <v>904</v>
+        <v>905</v>
       </c>
       <c r="B314" s="3" t="s">
-        <v>905</v>
+        <v>906</v>
       </c>
       <c r="C314" s="3"/>
       <c r="D314" s="3"/>
@@ -15299,10 +15308,10 @@
     </row>
     <row r="315" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A315" s="2" t="s">
-        <v>906</v>
+        <v>907</v>
       </c>
       <c r="B315" s="3" t="s">
-        <v>907</v>
+        <v>908</v>
       </c>
       <c r="C315" s="3"/>
       <c r="D315" s="3"/>
@@ -15331,10 +15340,10 @@
     </row>
     <row r="316" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A316" s="2" t="s">
-        <v>908</v>
+        <v>909</v>
       </c>
       <c r="B316" s="3" t="s">
-        <v>909</v>
+        <v>910</v>
       </c>
       <c r="C316" s="3"/>
       <c r="D316" s="3"/>
@@ -15363,10 +15372,10 @@
     </row>
     <row r="317" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A317" s="2" t="s">
-        <v>910</v>
+        <v>911</v>
       </c>
       <c r="B317" s="3" t="s">
-        <v>911</v>
+        <v>912</v>
       </c>
       <c r="C317" s="3"/>
       <c r="D317" s="3"/>
@@ -15395,10 +15404,10 @@
     </row>
     <row r="318" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A318" s="2" t="s">
-        <v>912</v>
+        <v>913</v>
       </c>
       <c r="B318" s="3" t="s">
-        <v>913</v>
+        <v>914</v>
       </c>
       <c r="C318" s="3"/>
       <c r="D318" s="3"/>
@@ -15427,10 +15436,10 @@
     </row>
     <row r="319" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A319" s="2" t="s">
-        <v>914</v>
+        <v>915</v>
       </c>
       <c r="B319" s="3" t="s">
-        <v>915</v>
+        <v>916</v>
       </c>
       <c r="C319" s="3"/>
       <c r="D319" s="3"/>
@@ -15459,10 +15468,10 @@
     </row>
     <row r="320" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A320" s="2" t="s">
-        <v>916</v>
+        <v>917</v>
       </c>
       <c r="B320" s="3" t="s">
-        <v>917</v>
+        <v>918</v>
       </c>
       <c r="C320" s="3"/>
       <c r="D320" s="3"/>
@@ -15491,10 +15500,10 @@
     </row>
     <row r="321" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A321" s="2" t="s">
-        <v>918</v>
+        <v>919</v>
       </c>
       <c r="B321" s="3" t="s">
-        <v>919</v>
+        <v>920</v>
       </c>
       <c r="C321" s="3"/>
       <c r="D321" s="3"/>
@@ -15523,10 +15532,10 @@
     </row>
     <row r="322" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A322" s="2" t="s">
-        <v>920</v>
+        <v>921</v>
       </c>
       <c r="B322" s="3" t="s">
-        <v>921</v>
+        <v>922</v>
       </c>
       <c r="C322" s="3"/>
       <c r="D322" s="3"/>
@@ -15555,10 +15564,10 @@
     </row>
     <row r="323" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A323" s="2" t="s">
-        <v>922</v>
+        <v>923</v>
       </c>
       <c r="B323" s="3" t="s">
-        <v>923</v>
+        <v>924</v>
       </c>
       <c r="C323" s="3"/>
       <c r="D323" s="3"/>
@@ -15587,10 +15596,10 @@
     </row>
     <row r="324" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A324" s="2" t="s">
-        <v>924</v>
+        <v>925</v>
       </c>
       <c r="B324" s="3" t="s">
-        <v>925</v>
+        <v>926</v>
       </c>
       <c r="C324" s="3"/>
       <c r="D324" s="3"/>
@@ -15619,10 +15628,10 @@
     </row>
     <row r="325" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A325" s="2" t="s">
-        <v>926</v>
+        <v>927</v>
       </c>
       <c r="B325" s="3" t="s">
-        <v>927</v>
+        <v>928</v>
       </c>
       <c r="C325" s="3"/>
       <c r="D325" s="3"/>
@@ -15651,10 +15660,10 @@
     </row>
     <row r="326" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A326" s="2" t="s">
-        <v>928</v>
+        <v>929</v>
       </c>
       <c r="B326" s="3" t="s">
-        <v>929</v>
+        <v>930</v>
       </c>
       <c r="C326" s="3"/>
       <c r="D326" s="3"/>
@@ -15683,10 +15692,10 @@
     </row>
     <row r="327" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A327" s="2" t="s">
-        <v>930</v>
+        <v>931</v>
       </c>
       <c r="B327" s="3" t="s">
-        <v>931</v>
+        <v>932</v>
       </c>
       <c r="C327" s="3"/>
       <c r="D327" s="3"/>
@@ -15715,10 +15724,10 @@
     </row>
     <row r="328" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A328" s="2" t="s">
-        <v>932</v>
+        <v>933</v>
       </c>
       <c r="B328" s="3" t="s">
-        <v>933</v>
+        <v>934</v>
       </c>
       <c r="C328" s="3"/>
       <c r="D328" s="3"/>
@@ -15747,10 +15756,10 @@
     </row>
     <row r="329" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A329" s="2" t="s">
-        <v>934</v>
+        <v>935</v>
       </c>
       <c r="B329" s="3" t="s">
-        <v>935</v>
+        <v>936</v>
       </c>
       <c r="C329" s="3"/>
       <c r="D329" s="3"/>
@@ -15779,10 +15788,10 @@
     </row>
     <row r="330" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A330" s="2" t="s">
-        <v>936</v>
+        <v>937</v>
       </c>
       <c r="B330" s="3" t="s">
-        <v>937</v>
+        <v>938</v>
       </c>
       <c r="C330" s="3"/>
       <c r="D330" s="3"/>
@@ -15811,10 +15820,10 @@
     </row>
     <row r="331" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A331" s="2" t="s">
-        <v>938</v>
+        <v>939</v>
       </c>
       <c r="B331" s="3" t="s">
-        <v>939</v>
+        <v>940</v>
       </c>
       <c r="C331" s="3"/>
       <c r="D331" s="3"/>
@@ -15843,10 +15852,10 @@
     </row>
     <row r="332" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A332" s="2" t="s">
-        <v>940</v>
+        <v>941</v>
       </c>
       <c r="B332" s="3" t="s">
-        <v>941</v>
+        <v>942</v>
       </c>
       <c r="C332" s="3"/>
       <c r="D332" s="3"/>
@@ -15875,10 +15884,10 @@
     </row>
     <row r="333" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A333" s="2" t="s">
-        <v>942</v>
+        <v>943</v>
       </c>
       <c r="B333" s="3" t="s">
-        <v>943</v>
+        <v>944</v>
       </c>
       <c r="C333" s="3"/>
       <c r="D333" s="3"/>
@@ -15907,10 +15916,10 @@
     </row>
     <row r="334" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A334" s="2" t="s">
-        <v>944</v>
+        <v>945</v>
       </c>
       <c r="B334" s="3" t="s">
-        <v>945</v>
+        <v>946</v>
       </c>
       <c r="C334" s="3"/>
       <c r="D334" s="3"/>
@@ -15939,10 +15948,10 @@
     </row>
     <row r="335" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A335" s="2" t="s">
-        <v>946</v>
+        <v>947</v>
       </c>
       <c r="B335" s="3" t="s">
-        <v>947</v>
+        <v>948</v>
       </c>
       <c r="C335" s="3"/>
       <c r="D335" s="3"/>
@@ -15971,10 +15980,10 @@
     </row>
     <row r="336" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A336" s="2" t="s">
-        <v>948</v>
+        <v>949</v>
       </c>
       <c r="B336" s="3" t="s">
-        <v>949</v>
+        <v>950</v>
       </c>
       <c r="C336" s="3"/>
       <c r="D336" s="3"/>
@@ -16003,10 +16012,10 @@
     </row>
     <row r="337" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A337" s="2" t="s">
-        <v>950</v>
+        <v>951</v>
       </c>
       <c r="B337" s="3" t="s">
-        <v>951</v>
+        <v>952</v>
       </c>
       <c r="C337" s="3"/>
       <c r="D337" s="3"/>
@@ -16035,10 +16044,10 @@
     </row>
     <row r="338" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A338" s="2" t="s">
-        <v>952</v>
+        <v>953</v>
       </c>
       <c r="B338" s="3" t="s">
-        <v>953</v>
+        <v>954</v>
       </c>
       <c r="C338" s="3"/>
       <c r="D338" s="3"/>
@@ -16067,10 +16076,10 @@
     </row>
     <row r="339" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A339" s="2" t="s">
-        <v>954</v>
+        <v>955</v>
       </c>
       <c r="B339" s="3" t="s">
-        <v>955</v>
+        <v>956</v>
       </c>
       <c r="C339" s="3"/>
       <c r="D339" s="3"/>
@@ -16099,10 +16108,10 @@
     </row>
     <row r="340" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A340" s="2" t="s">
-        <v>956</v>
+        <v>957</v>
       </c>
       <c r="B340" s="3" t="s">
-        <v>957</v>
+        <v>958</v>
       </c>
       <c r="C340" s="3"/>
       <c r="D340" s="3"/>
@@ -16131,10 +16140,10 @@
     </row>
     <row r="341" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A341" s="2" t="s">
-        <v>958</v>
+        <v>959</v>
       </c>
       <c r="B341" s="3" t="s">
-        <v>959</v>
+        <v>960</v>
       </c>
       <c r="C341" s="3"/>
       <c r="D341" s="3"/>
@@ -16163,10 +16172,10 @@
     </row>
     <row r="342" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A342" s="2" t="s">
-        <v>960</v>
+        <v>961</v>
       </c>
       <c r="B342" s="3" t="s">
-        <v>961</v>
+        <v>962</v>
       </c>
       <c r="C342" s="3"/>
       <c r="D342" s="3"/>
@@ -16195,10 +16204,10 @@
     </row>
     <row r="343" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A343" s="2" t="s">
-        <v>962</v>
+        <v>963</v>
       </c>
       <c r="B343" s="3" t="s">
-        <v>963</v>
+        <v>964</v>
       </c>
       <c r="C343" s="3"/>
       <c r="D343" s="3"/>
@@ -16227,10 +16236,10 @@
     </row>
     <row r="344" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A344" s="2" t="s">
-        <v>964</v>
+        <v>965</v>
       </c>
       <c r="B344" s="3" t="s">
-        <v>965</v>
+        <v>966</v>
       </c>
       <c r="C344" s="3"/>
       <c r="D344" s="3"/>
@@ -16259,10 +16268,10 @@
     </row>
     <row r="345" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A345" s="2" t="s">
-        <v>966</v>
+        <v>967</v>
       </c>
       <c r="B345" s="3" t="s">
-        <v>967</v>
+        <v>968</v>
       </c>
       <c r="C345" s="3"/>
       <c r="D345" s="3"/>
@@ -16291,10 +16300,10 @@
     </row>
     <row r="346" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A346" s="2" t="s">
-        <v>968</v>
+        <v>969</v>
       </c>
       <c r="B346" s="3" t="s">
-        <v>969</v>
+        <v>970</v>
       </c>
       <c r="C346" s="3"/>
       <c r="D346" s="3"/>
@@ -16323,10 +16332,10 @@
     </row>
     <row r="347" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A347" s="2" t="s">
-        <v>970</v>
+        <v>971</v>
       </c>
       <c r="B347" s="3" t="s">
-        <v>971</v>
+        <v>972</v>
       </c>
       <c r="C347" s="3"/>
       <c r="D347" s="3"/>
@@ -16355,10 +16364,10 @@
     </row>
     <row r="348" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A348" s="2" t="s">
-        <v>972</v>
+        <v>973</v>
       </c>
       <c r="B348" s="3" t="s">
-        <v>973</v>
+        <v>974</v>
       </c>
       <c r="C348" s="3"/>
       <c r="D348" s="3"/>
@@ -16387,10 +16396,10 @@
     </row>
     <row r="349" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A349" s="2" t="s">
-        <v>974</v>
+        <v>975</v>
       </c>
       <c r="B349" s="3" t="s">
-        <v>975</v>
+        <v>976</v>
       </c>
       <c r="C349" s="3"/>
       <c r="D349" s="3"/>
@@ -16419,10 +16428,10 @@
     </row>
     <row r="350" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A350" s="2" t="s">
-        <v>976</v>
+        <v>977</v>
       </c>
       <c r="B350" s="3" t="s">
-        <v>977</v>
+        <v>978</v>
       </c>
       <c r="C350" s="3"/>
       <c r="D350" s="3"/>
@@ -16451,10 +16460,10 @@
     </row>
     <row r="351" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A351" s="2" t="s">
-        <v>978</v>
+        <v>979</v>
       </c>
       <c r="B351" s="3" t="s">
-        <v>979</v>
+        <v>980</v>
       </c>
       <c r="C351" s="3"/>
       <c r="D351" s="3"/>
@@ -16483,10 +16492,10 @@
     </row>
     <row r="352" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A352" s="2" t="s">
-        <v>980</v>
+        <v>981</v>
       </c>
       <c r="B352" s="3" t="s">
-        <v>981</v>
+        <v>982</v>
       </c>
       <c r="C352" s="3"/>
       <c r="D352" s="3"/>
@@ -16515,10 +16524,10 @@
     </row>
     <row r="353" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A353" s="2" t="s">
-        <v>982</v>
+        <v>983</v>
       </c>
       <c r="B353" s="3" t="s">
-        <v>983</v>
+        <v>984</v>
       </c>
       <c r="C353" s="3"/>
       <c r="D353" s="3"/>
@@ -16547,10 +16556,10 @@
     </row>
     <row r="354" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A354" s="2" t="s">
-        <v>984</v>
+        <v>985</v>
       </c>
       <c r="B354" s="3" t="s">
-        <v>985</v>
+        <v>986</v>
       </c>
       <c r="C354" s="3"/>
       <c r="D354" s="3"/>
@@ -16579,10 +16588,10 @@
     </row>
     <row r="355" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A355" s="2" t="s">
-        <v>986</v>
+        <v>987</v>
       </c>
       <c r="B355" s="3" t="s">
-        <v>987</v>
+        <v>988</v>
       </c>
       <c r="C355" s="3"/>
       <c r="D355" s="3"/>
@@ -16611,10 +16620,10 @@
     </row>
     <row r="356" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A356" s="2" t="s">
-        <v>988</v>
+        <v>989</v>
       </c>
       <c r="B356" s="3" t="s">
-        <v>989</v>
+        <v>990</v>
       </c>
       <c r="C356" s="3"/>
       <c r="D356" s="3"/>
@@ -16643,10 +16652,10 @@
     </row>
     <row r="357" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A357" s="2" t="s">
-        <v>990</v>
+        <v>991</v>
       </c>
       <c r="B357" s="3" t="s">
-        <v>991</v>
+        <v>992</v>
       </c>
       <c r="C357" s="3"/>
       <c r="D357" s="3"/>
@@ -16675,10 +16684,10 @@
     </row>
     <row r="358" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A358" s="2" t="s">
-        <v>992</v>
+        <v>993</v>
       </c>
       <c r="B358" s="3" t="s">
-        <v>993</v>
+        <v>994</v>
       </c>
       <c r="C358" s="3"/>
       <c r="D358" s="3"/>
@@ -16707,10 +16716,10 @@
     </row>
     <row r="359" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A359" s="2" t="s">
-        <v>994</v>
+        <v>995</v>
       </c>
       <c r="B359" s="3" t="s">
-        <v>995</v>
+        <v>996</v>
       </c>
       <c r="C359" s="3"/>
       <c r="D359" s="3"/>
@@ -16739,10 +16748,10 @@
     </row>
     <row r="360" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A360" s="2" t="s">
-        <v>996</v>
+        <v>997</v>
       </c>
       <c r="B360" s="3" t="s">
-        <v>997</v>
+        <v>998</v>
       </c>
       <c r="C360" s="3"/>
       <c r="D360" s="3"/>
@@ -16771,10 +16780,10 @@
     </row>
     <row r="361" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A361" s="2" t="s">
-        <v>998</v>
+        <v>999</v>
       </c>
       <c r="B361" s="3" t="s">
-        <v>999</v>
+        <v>1000</v>
       </c>
       <c r="C361" s="3"/>
       <c r="D361" s="3"/>
@@ -16803,10 +16812,10 @@
     </row>
     <row r="362" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A362" s="2" t="s">
-        <v>1000</v>
+        <v>1001</v>
       </c>
       <c r="B362" s="3" t="s">
-        <v>1001</v>
+        <v>1002</v>
       </c>
       <c r="C362" s="3"/>
       <c r="D362" s="3"/>
@@ -16835,10 +16844,10 @@
     </row>
     <row r="363" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A363" s="2" t="s">
-        <v>1002</v>
+        <v>1003</v>
       </c>
       <c r="B363" s="3" t="s">
-        <v>1003</v>
+        <v>1004</v>
       </c>
       <c r="C363" s="3"/>
       <c r="D363" s="3"/>
@@ -16867,10 +16876,10 @@
     </row>
     <row r="364" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A364" s="2" t="s">
-        <v>1004</v>
+        <v>1005</v>
       </c>
       <c r="B364" s="3" t="s">
-        <v>1005</v>
+        <v>1006</v>
       </c>
       <c r="C364" s="3"/>
       <c r="D364" s="3"/>
@@ -16899,10 +16908,10 @@
     </row>
     <row r="365" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A365" s="2" t="s">
-        <v>1006</v>
+        <v>1007</v>
       </c>
       <c r="B365" s="3" t="s">
-        <v>1007</v>
+        <v>1008</v>
       </c>
       <c r="C365" s="3"/>
       <c r="D365" s="3"/>
@@ -16931,10 +16940,10 @@
     </row>
     <row r="366" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A366" s="2" t="s">
-        <v>1008</v>
+        <v>1009</v>
       </c>
       <c r="B366" s="3" t="s">
-        <v>1009</v>
+        <v>1010</v>
       </c>
       <c r="C366" s="3"/>
       <c r="D366" s="3"/>
@@ -16963,10 +16972,10 @@
     </row>
     <row r="367" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A367" s="2" t="s">
-        <v>1010</v>
+        <v>1011</v>
       </c>
       <c r="B367" s="3" t="s">
-        <v>1011</v>
+        <v>1012</v>
       </c>
       <c r="C367" s="3"/>
       <c r="D367" s="3"/>
@@ -16995,10 +17004,10 @@
     </row>
     <row r="368" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A368" s="2" t="s">
-        <v>1012</v>
+        <v>1013</v>
       </c>
       <c r="B368" s="3" t="s">
-        <v>1013</v>
+        <v>1014</v>
       </c>
       <c r="C368" s="3"/>
       <c r="D368" s="3"/>
@@ -17027,10 +17036,10 @@
     </row>
     <row r="369" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A369" s="2" t="s">
-        <v>1014</v>
+        <v>1015</v>
       </c>
       <c r="B369" s="3" t="s">
-        <v>1015</v>
+        <v>1016</v>
       </c>
       <c r="C369" s="3"/>
       <c r="D369" s="3"/>
@@ -17059,10 +17068,10 @@
     </row>
     <row r="370" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A370" s="2" t="s">
-        <v>1016</v>
+        <v>1017</v>
       </c>
       <c r="B370" s="3" t="s">
-        <v>1017</v>
+        <v>1018</v>
       </c>
       <c r="C370" s="3"/>
       <c r="D370" s="3"/>
@@ -17091,10 +17100,10 @@
     </row>
     <row r="371" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A371" s="2" t="s">
-        <v>1018</v>
+        <v>1019</v>
       </c>
       <c r="B371" s="3" t="s">
-        <v>1019</v>
+        <v>1020</v>
       </c>
       <c r="C371" s="3"/>
       <c r="D371" s="3"/>
@@ -17123,10 +17132,10 @@
     </row>
     <row r="372" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A372" s="2" t="s">
-        <v>1020</v>
+        <v>1021</v>
       </c>
       <c r="B372" s="3" t="s">
-        <v>1021</v>
+        <v>1022</v>
       </c>
       <c r="C372" s="3"/>
       <c r="D372" s="3"/>
@@ -17155,10 +17164,10 @@
     </row>
     <row r="373" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A373" s="2" t="s">
-        <v>1022</v>
+        <v>1023</v>
       </c>
       <c r="B373" s="3" t="s">
-        <v>1023</v>
+        <v>1024</v>
       </c>
       <c r="C373" s="3"/>
       <c r="D373" s="3"/>
@@ -17187,10 +17196,10 @@
     </row>
     <row r="374" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A374" s="2" t="s">
-        <v>1024</v>
+        <v>1025</v>
       </c>
       <c r="B374" s="3" t="s">
-        <v>1025</v>
+        <v>1026</v>
       </c>
       <c r="C374" s="3"/>
       <c r="D374" s="3"/>
@@ -17219,10 +17228,10 @@
     </row>
     <row r="375" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A375" s="2" t="s">
-        <v>1026</v>
+        <v>1027</v>
       </c>
       <c r="B375" s="3" t="s">
-        <v>1027</v>
+        <v>1028</v>
       </c>
       <c r="C375" s="3"/>
       <c r="D375" s="3"/>
@@ -17251,10 +17260,10 @@
     </row>
     <row r="376" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A376" s="2" t="s">
-        <v>1028</v>
+        <v>1029</v>
       </c>
       <c r="B376" s="3" t="s">
-        <v>1029</v>
+        <v>1030</v>
       </c>
       <c r="C376" s="3"/>
       <c r="D376" s="3"/>
@@ -17283,10 +17292,10 @@
     </row>
     <row r="377" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A377" s="2" t="s">
-        <v>1030</v>
+        <v>1031</v>
       </c>
       <c r="B377" s="3" t="s">
-        <v>1031</v>
+        <v>1032</v>
       </c>
       <c r="C377" s="3"/>
       <c r="D377" s="3"/>
@@ -17315,10 +17324,10 @@
     </row>
     <row r="378" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A378" s="2" t="s">
-        <v>1032</v>
+        <v>1033</v>
       </c>
       <c r="B378" s="3" t="s">
-        <v>1033</v>
+        <v>1034</v>
       </c>
       <c r="C378" s="3"/>
       <c r="D378" s="3"/>
@@ -17347,10 +17356,10 @@
     </row>
     <row r="379" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A379" s="2" t="s">
-        <v>1034</v>
+        <v>1035</v>
       </c>
       <c r="B379" s="3" t="s">
-        <v>1035</v>
+        <v>1036</v>
       </c>
       <c r="C379" s="3"/>
       <c r="D379" s="3"/>
@@ -17379,10 +17388,10 @@
     </row>
     <row r="380" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A380" s="2" t="s">
-        <v>1036</v>
+        <v>1037</v>
       </c>
       <c r="B380" s="3" t="s">
-        <v>1037</v>
+        <v>1038</v>
       </c>
       <c r="C380" s="3"/>
       <c r="D380" s="3"/>
@@ -17411,10 +17420,10 @@
     </row>
     <row r="381" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A381" s="2" t="s">
-        <v>1038</v>
+        <v>1039</v>
       </c>
       <c r="B381" s="3" t="s">
-        <v>1039</v>
+        <v>1040</v>
       </c>
       <c r="C381" s="3"/>
       <c r="D381" s="3"/>
@@ -17443,10 +17452,10 @@
     </row>
     <row r="382" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A382" s="2" t="s">
-        <v>1040</v>
+        <v>1041</v>
       </c>
       <c r="B382" s="3" t="s">
-        <v>1041</v>
+        <v>1042</v>
       </c>
       <c r="C382" s="3"/>
       <c r="D382" s="3"/>
@@ -17475,10 +17484,10 @@
     </row>
     <row r="383" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A383" s="2" t="s">
-        <v>1042</v>
+        <v>1043</v>
       </c>
       <c r="B383" s="3" t="s">
-        <v>1043</v>
+        <v>1044</v>
       </c>
       <c r="C383" s="3"/>
       <c r="D383" s="3"/>
@@ -17507,10 +17516,10 @@
     </row>
     <row r="384" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A384" s="2" t="s">
-        <v>1044</v>
+        <v>1045</v>
       </c>
       <c r="B384" s="3" t="s">
-        <v>1045</v>
+        <v>1046</v>
       </c>
       <c r="C384" s="3"/>
       <c r="D384" s="3"/>
@@ -17539,10 +17548,10 @@
     </row>
     <row r="385" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A385" s="2" t="s">
-        <v>1046</v>
+        <v>1047</v>
       </c>
       <c r="B385" s="3" t="s">
-        <v>1047</v>
+        <v>1048</v>
       </c>
       <c r="C385" s="3"/>
       <c r="D385" s="3"/>
@@ -17571,10 +17580,10 @@
     </row>
     <row r="386" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A386" s="2" t="s">
-        <v>1048</v>
+        <v>1049</v>
       </c>
       <c r="B386" s="3" t="s">
-        <v>1049</v>
+        <v>1050</v>
       </c>
       <c r="C386" s="3"/>
       <c r="D386" s="3"/>
@@ -17603,10 +17612,10 @@
     </row>
     <row r="387" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A387" s="2" t="s">
-        <v>1050</v>
+        <v>1051</v>
       </c>
       <c r="B387" s="3" t="s">
-        <v>1051</v>
+        <v>1052</v>
       </c>
       <c r="C387" s="3"/>
       <c r="D387" s="3"/>
@@ -17635,10 +17644,10 @@
     </row>
     <row r="388" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A388" s="2" t="s">
-        <v>1052</v>
+        <v>1053</v>
       </c>
       <c r="B388" s="3" t="s">
-        <v>1053</v>
+        <v>1054</v>
       </c>
       <c r="C388" s="3"/>
       <c r="D388" s="3"/>
@@ -17667,10 +17676,10 @@
     </row>
     <row r="389" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A389" s="2" t="s">
-        <v>1054</v>
+        <v>1055</v>
       </c>
       <c r="B389" s="3" t="s">
-        <v>1055</v>
+        <v>1056</v>
       </c>
       <c r="C389" s="3"/>
       <c r="D389" s="3"/>
@@ -17699,10 +17708,10 @@
     </row>
     <row r="390" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A390" s="2" t="s">
-        <v>1056</v>
+        <v>1057</v>
       </c>
       <c r="B390" s="3" t="s">
-        <v>1057</v>
+        <v>1058</v>
       </c>
       <c r="C390" s="3"/>
       <c r="D390" s="3"/>
@@ -17731,10 +17740,10 @@
     </row>
     <row r="391" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A391" s="2" t="s">
-        <v>1058</v>
+        <v>1059</v>
       </c>
       <c r="B391" s="3" t="s">
-        <v>1059</v>
+        <v>1060</v>
       </c>
       <c r="C391" s="3"/>
       <c r="D391" s="3"/>
@@ -17763,10 +17772,10 @@
     </row>
     <row r="392" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A392" s="2" t="s">
-        <v>1060</v>
+        <v>1061</v>
       </c>
       <c r="B392" s="3" t="s">
-        <v>1061</v>
+        <v>1062</v>
       </c>
       <c r="C392" s="3"/>
       <c r="D392" s="3"/>
@@ -17795,10 +17804,10 @@
     </row>
     <row r="393" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A393" s="2" t="s">
-        <v>1062</v>
+        <v>1063</v>
       </c>
       <c r="B393" s="3" t="s">
-        <v>1063</v>
+        <v>1064</v>
       </c>
       <c r="C393" s="3"/>
       <c r="D393" s="3"/>
@@ -17827,10 +17836,10 @@
     </row>
     <row r="394" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A394" s="2" t="s">
-        <v>1064</v>
+        <v>1065</v>
       </c>
       <c r="B394" s="3" t="s">
-        <v>1065</v>
+        <v>1066</v>
       </c>
       <c r="C394" s="3"/>
       <c r="D394" s="3"/>
@@ -17859,10 +17868,10 @@
     </row>
     <row r="395" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A395" s="2" t="s">
-        <v>1066</v>
+        <v>1067</v>
       </c>
       <c r="B395" s="3" t="s">
-        <v>1067</v>
+        <v>1068</v>
       </c>
       <c r="C395" s="3"/>
       <c r="D395" s="3"/>
@@ -17891,10 +17900,10 @@
     </row>
     <row r="396" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A396" s="2" t="s">
-        <v>1068</v>
+        <v>1069</v>
       </c>
       <c r="B396" s="3" t="s">
-        <v>1069</v>
+        <v>1070</v>
       </c>
       <c r="C396" s="3"/>
       <c r="D396" s="3"/>
@@ -17923,10 +17932,10 @@
     </row>
     <row r="397" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A397" s="2" t="s">
-        <v>1070</v>
+        <v>1071</v>
       </c>
       <c r="B397" s="3" t="s">
-        <v>1071</v>
+        <v>1072</v>
       </c>
       <c r="C397" s="3"/>
       <c r="D397" s="3"/>
@@ -17955,10 +17964,10 @@
     </row>
     <row r="398" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A398" s="2" t="s">
-        <v>1072</v>
+        <v>1073</v>
       </c>
       <c r="B398" s="3" t="s">
-        <v>1073</v>
+        <v>1074</v>
       </c>
       <c r="C398" s="3"/>
       <c r="D398" s="3"/>
@@ -17987,10 +17996,10 @@
     </row>
     <row r="399" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A399" s="2" t="s">
-        <v>1074</v>
+        <v>1075</v>
       </c>
       <c r="B399" s="3" t="s">
-        <v>1075</v>
+        <v>1076</v>
       </c>
       <c r="C399" s="3"/>
       <c r="D399" s="3"/>
@@ -18019,10 +18028,10 @@
     </row>
     <row r="400" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A400" s="2" t="s">
-        <v>1076</v>
+        <v>1077</v>
       </c>
       <c r="B400" s="3" t="s">
-        <v>1077</v>
+        <v>1078</v>
       </c>
       <c r="C400" s="3"/>
       <c r="D400" s="3"/>
@@ -18051,10 +18060,10 @@
     </row>
     <row r="401" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A401" s="2" t="s">
-        <v>1078</v>
+        <v>1079</v>
       </c>
       <c r="B401" s="3" t="s">
-        <v>1079</v>
+        <v>1080</v>
       </c>
       <c r="C401" s="3"/>
       <c r="D401" s="3"/>
@@ -18083,10 +18092,10 @@
     </row>
     <row r="402" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A402" s="2" t="s">
-        <v>1080</v>
+        <v>1081</v>
       </c>
       <c r="B402" s="3" t="s">
-        <v>1081</v>
+        <v>1082</v>
       </c>
       <c r="C402" s="3"/>
       <c r="D402" s="3"/>
@@ -18115,10 +18124,10 @@
     </row>
     <row r="403" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A403" s="2" t="s">
-        <v>1082</v>
+        <v>1083</v>
       </c>
       <c r="B403" s="3" t="s">
-        <v>1083</v>
+        <v>1084</v>
       </c>
       <c r="C403" s="3"/>
       <c r="D403" s="3"/>
@@ -18147,10 +18156,10 @@
     </row>
     <row r="404" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A404" s="2" t="s">
-        <v>1084</v>
+        <v>1085</v>
       </c>
       <c r="B404" s="3" t="s">
-        <v>1085</v>
+        <v>1086</v>
       </c>
       <c r="C404" s="3"/>
       <c r="D404" s="3"/>
@@ -18179,10 +18188,10 @@
     </row>
     <row r="405" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A405" s="2" t="s">
-        <v>1086</v>
+        <v>1087</v>
       </c>
       <c r="B405" s="3" t="s">
-        <v>1087</v>
+        <v>1088</v>
       </c>
       <c r="C405" s="3"/>
       <c r="D405" s="3"/>
@@ -18211,10 +18220,10 @@
     </row>
     <row r="406" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A406" s="2" t="s">
-        <v>1088</v>
+        <v>1089</v>
       </c>
       <c r="B406" s="3" t="s">
-        <v>1089</v>
+        <v>1090</v>
       </c>
       <c r="C406" s="3"/>
       <c r="D406" s="3"/>
@@ -18243,10 +18252,10 @@
     </row>
     <row r="407" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A407" s="2" t="s">
-        <v>1090</v>
+        <v>1091</v>
       </c>
       <c r="B407" s="3" t="s">
-        <v>1091</v>
+        <v>1092</v>
       </c>
       <c r="C407" s="3"/>
       <c r="D407" s="3"/>
@@ -18275,10 +18284,10 @@
     </row>
     <row r="408" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A408" s="2" t="s">
-        <v>1092</v>
+        <v>1093</v>
       </c>
       <c r="B408" s="3" t="s">
-        <v>1093</v>
+        <v>1094</v>
       </c>
       <c r="C408" s="3"/>
       <c r="D408" s="3"/>
@@ -18307,10 +18316,10 @@
     </row>
     <row r="409" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A409" s="2" t="s">
-        <v>1094</v>
+        <v>1095</v>
       </c>
       <c r="B409" s="3" t="s">
-        <v>1095</v>
+        <v>1096</v>
       </c>
       <c r="C409" s="3"/>
       <c r="D409" s="3"/>
@@ -18339,10 +18348,10 @@
     </row>
     <row r="410" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A410" s="2" t="s">
-        <v>1096</v>
+        <v>1097</v>
       </c>
       <c r="B410" s="3" t="s">
-        <v>1097</v>
+        <v>1098</v>
       </c>
       <c r="C410" s="3"/>
       <c r="D410" s="3"/>
@@ -18371,10 +18380,10 @@
     </row>
     <row r="411" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A411" s="2" t="s">
-        <v>1098</v>
+        <v>1099</v>
       </c>
       <c r="B411" s="3" t="s">
-        <v>1099</v>
+        <v>1100</v>
       </c>
       <c r="C411" s="3"/>
       <c r="D411" s="3"/>
@@ -18403,10 +18412,10 @@
     </row>
     <row r="412" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A412" s="2" t="s">
-        <v>1100</v>
+        <v>1101</v>
       </c>
       <c r="B412" s="3" t="s">
-        <v>1101</v>
+        <v>1102</v>
       </c>
       <c r="C412" s="3"/>
       <c r="D412" s="3"/>
@@ -18435,10 +18444,10 @@
     </row>
     <row r="413" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A413" s="2" t="s">
-        <v>1102</v>
+        <v>1103</v>
       </c>
       <c r="B413" s="3" t="s">
-        <v>1103</v>
+        <v>1104</v>
       </c>
       <c r="C413" s="3"/>
       <c r="D413" s="3"/>
@@ -18467,10 +18476,10 @@
     </row>
     <row r="414" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A414" s="2" t="s">
-        <v>1104</v>
+        <v>1105</v>
       </c>
       <c r="B414" s="3" t="s">
-        <v>1105</v>
+        <v>1106</v>
       </c>
       <c r="C414" s="3"/>
       <c r="D414" s="3"/>
@@ -18499,10 +18508,10 @@
     </row>
     <row r="415" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A415" s="2" t="s">
-        <v>1106</v>
+        <v>1107</v>
       </c>
       <c r="B415" s="3" t="s">
-        <v>1107</v>
+        <v>1108</v>
       </c>
       <c r="C415" s="3"/>
       <c r="D415" s="3"/>
@@ -18531,10 +18540,10 @@
     </row>
     <row r="416" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A416" s="2" t="s">
-        <v>1108</v>
+        <v>1109</v>
       </c>
       <c r="B416" s="3" t="s">
-        <v>1109</v>
+        <v>1110</v>
       </c>
       <c r="C416" s="3"/>
       <c r="D416" s="3"/>
@@ -18563,10 +18572,10 @@
     </row>
     <row r="417" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A417" s="2" t="s">
-        <v>1110</v>
+        <v>1111</v>
       </c>
       <c r="B417" s="3" t="s">
-        <v>1111</v>
+        <v>1112</v>
       </c>
       <c r="C417" s="3"/>
       <c r="D417" s="3"/>
@@ -18595,10 +18604,10 @@
     </row>
     <row r="418" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A418" s="2" t="s">
-        <v>1112</v>
+        <v>1113</v>
       </c>
       <c r="B418" s="3" t="s">
-        <v>1113</v>
+        <v>1114</v>
       </c>
       <c r="C418" s="3"/>
       <c r="D418" s="3"/>
@@ -18627,10 +18636,10 @@
     </row>
     <row r="419" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A419" s="2" t="s">
-        <v>1114</v>
+        <v>1115</v>
       </c>
       <c r="B419" s="3" t="s">
-        <v>1115</v>
+        <v>1116</v>
       </c>
       <c r="C419" s="3"/>
       <c r="D419" s="3"/>
@@ -18659,10 +18668,10 @@
     </row>
     <row r="420" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A420" s="2" t="s">
-        <v>1116</v>
+        <v>1117</v>
       </c>
       <c r="B420" s="3" t="s">
-        <v>1117</v>
+        <v>1118</v>
       </c>
       <c r="C420" s="3"/>
       <c r="D420" s="3"/>
@@ -18691,10 +18700,10 @@
     </row>
     <row r="421" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A421" s="2" t="s">
-        <v>1118</v>
+        <v>1119</v>
       </c>
       <c r="B421" s="3" t="s">
-        <v>1119</v>
+        <v>1120</v>
       </c>
       <c r="C421" s="3"/>
       <c r="D421" s="3"/>
@@ -18723,10 +18732,10 @@
     </row>
     <row r="422" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A422" s="2" t="s">
-        <v>1120</v>
+        <v>1121</v>
       </c>
       <c r="B422" s="3" t="s">
-        <v>1121</v>
+        <v>1122</v>
       </c>
       <c r="C422" s="3"/>
       <c r="D422" s="3"/>
@@ -18755,10 +18764,10 @@
     </row>
     <row r="423" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A423" s="2" t="s">
-        <v>1122</v>
+        <v>1123</v>
       </c>
       <c r="B423" s="3" t="s">
-        <v>1123</v>
+        <v>1124</v>
       </c>
       <c r="C423" s="3"/>
       <c r="D423" s="3"/>
@@ -18787,10 +18796,10 @@
     </row>
     <row r="424" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A424" s="2" t="s">
-        <v>1124</v>
+        <v>1125</v>
       </c>
       <c r="B424" s="3" t="s">
-        <v>1125</v>
+        <v>1126</v>
       </c>
       <c r="C424" s="3"/>
       <c r="D424" s="3"/>
@@ -18819,10 +18828,10 @@
     </row>
     <row r="425" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A425" s="2" t="s">
-        <v>1126</v>
+        <v>1127</v>
       </c>
       <c r="B425" s="3" t="s">
-        <v>1127</v>
+        <v>1128</v>
       </c>
       <c r="C425" s="3"/>
       <c r="D425" s="3"/>
@@ -18851,10 +18860,10 @@
     </row>
     <row r="426" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A426" s="2" t="s">
-        <v>1128</v>
+        <v>1129</v>
       </c>
       <c r="B426" s="3" t="s">
-        <v>1129</v>
+        <v>1130</v>
       </c>
       <c r="C426" s="3"/>
       <c r="D426" s="3"/>
@@ -18883,10 +18892,10 @@
     </row>
     <row r="427" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A427" s="2" t="s">
-        <v>1130</v>
+        <v>1131</v>
       </c>
       <c r="B427" s="3" t="s">
-        <v>1131</v>
+        <v>1132</v>
       </c>
       <c r="C427" s="3"/>
       <c r="D427" s="3"/>
@@ -18915,10 +18924,10 @@
     </row>
     <row r="428" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A428" s="2" t="s">
-        <v>1132</v>
+        <v>1133</v>
       </c>
       <c r="B428" s="3" t="s">
-        <v>1133</v>
+        <v>1134</v>
       </c>
       <c r="C428" s="3"/>
       <c r="D428" s="3"/>
@@ -18947,10 +18956,10 @@
     </row>
     <row r="429" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A429" s="2" t="s">
-        <v>1134</v>
+        <v>1135</v>
       </c>
       <c r="B429" s="3" t="s">
-        <v>1135</v>
+        <v>1136</v>
       </c>
       <c r="C429" s="3"/>
       <c r="D429" s="3"/>
@@ -18979,10 +18988,10 @@
     </row>
     <row r="430" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A430" s="2" t="s">
-        <v>1136</v>
+        <v>1137</v>
       </c>
       <c r="B430" s="3" t="s">
-        <v>1137</v>
+        <v>1138</v>
       </c>
       <c r="C430" s="3"/>
       <c r="D430" s="3"/>
@@ -19011,10 +19020,10 @@
     </row>
     <row r="431" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A431" s="2" t="s">
-        <v>1138</v>
+        <v>1139</v>
       </c>
       <c r="B431" s="3" t="s">
-        <v>1139</v>
+        <v>1140</v>
       </c>
       <c r="C431" s="3"/>
       <c r="D431" s="3"/>
@@ -19043,10 +19052,10 @@
     </row>
     <row r="432" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A432" s="2" t="s">
-        <v>1140</v>
+        <v>1141</v>
       </c>
       <c r="B432" s="3" t="s">
-        <v>1141</v>
+        <v>1142</v>
       </c>
       <c r="C432" s="3"/>
       <c r="D432" s="3"/>
@@ -19075,10 +19084,10 @@
     </row>
     <row r="433" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A433" s="2" t="s">
-        <v>1142</v>
+        <v>1143</v>
       </c>
       <c r="B433" s="3" t="s">
-        <v>1143</v>
+        <v>1144</v>
       </c>
       <c r="C433" s="3"/>
       <c r="D433" s="3"/>
@@ -19107,10 +19116,10 @@
     </row>
     <row r="434" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A434" s="2" t="s">
-        <v>1144</v>
+        <v>1145</v>
       </c>
       <c r="B434" s="3" t="s">
-        <v>1145</v>
+        <v>1146</v>
       </c>
       <c r="C434" s="3"/>
       <c r="D434" s="3"/>
@@ -19139,10 +19148,10 @@
     </row>
     <row r="435" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A435" s="2" t="s">
-        <v>1146</v>
+        <v>1147</v>
       </c>
       <c r="B435" s="3" t="s">
-        <v>1147</v>
+        <v>1148</v>
       </c>
       <c r="C435" s="3"/>
       <c r="D435" s="3"/>
@@ -19171,10 +19180,10 @@
     </row>
     <row r="436" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A436" s="2" t="s">
-        <v>1148</v>
+        <v>1149</v>
       </c>
       <c r="B436" s="3" t="s">
-        <v>1149</v>
+        <v>1150</v>
       </c>
       <c r="C436" s="3"/>
       <c r="D436" s="3"/>
@@ -19203,10 +19212,10 @@
     </row>
     <row r="437" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A437" s="2" t="s">
-        <v>1150</v>
+        <v>1151</v>
       </c>
       <c r="B437" s="3" t="s">
-        <v>1151</v>
+        <v>1152</v>
       </c>
       <c r="C437" s="3"/>
       <c r="D437" s="3"/>
@@ -19235,10 +19244,10 @@
     </row>
     <row r="438" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A438" s="2" t="s">
-        <v>1152</v>
+        <v>1153</v>
       </c>
       <c r="B438" s="3" t="s">
-        <v>1153</v>
+        <v>1154</v>
       </c>
       <c r="C438" s="3"/>
       <c r="D438" s="3"/>
@@ -19267,10 +19276,10 @@
     </row>
     <row r="439" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A439" s="2" t="s">
-        <v>1154</v>
+        <v>1155</v>
       </c>
       <c r="B439" s="3" t="s">
-        <v>1155</v>
+        <v>1156</v>
       </c>
       <c r="C439" s="3"/>
       <c r="D439" s="3"/>
@@ -19299,10 +19308,10 @@
     </row>
     <row r="440" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A440" s="2" t="s">
-        <v>1156</v>
+        <v>1157</v>
       </c>
       <c r="B440" s="3" t="s">
-        <v>1157</v>
+        <v>1158</v>
       </c>
       <c r="C440" s="3"/>
       <c r="D440" s="3"/>
@@ -19331,10 +19340,10 @@
     </row>
     <row r="441" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A441" s="2" t="s">
-        <v>1158</v>
+        <v>1159</v>
       </c>
       <c r="B441" s="3" t="s">
-        <v>1159</v>
+        <v>1160</v>
       </c>
       <c r="C441" s="3"/>
       <c r="D441" s="3"/>
@@ -19363,10 +19372,10 @@
     </row>
     <row r="442" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A442" s="2" t="s">
-        <v>1160</v>
+        <v>1161</v>
       </c>
       <c r="B442" s="3" t="s">
-        <v>1161</v>
+        <v>1162</v>
       </c>
       <c r="C442" s="3"/>
       <c r="D442" s="3"/>
@@ -19395,10 +19404,10 @@
     </row>
     <row r="443" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A443" s="2" t="s">
-        <v>1162</v>
+        <v>1163</v>
       </c>
       <c r="B443" s="3" t="s">
-        <v>1163</v>
+        <v>1164</v>
       </c>
       <c r="C443" s="3"/>
       <c r="D443" s="3"/>
@@ -19427,10 +19436,10 @@
     </row>
     <row r="444" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A444" s="2" t="s">
-        <v>1164</v>
+        <v>1165</v>
       </c>
       <c r="B444" s="3" t="s">
-        <v>1165</v>
+        <v>1166</v>
       </c>
       <c r="C444" s="3"/>
       <c r="D444" s="3"/>
@@ -19459,10 +19468,10 @@
     </row>
     <row r="445" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A445" s="2" t="s">
-        <v>1166</v>
+        <v>1167</v>
       </c>
       <c r="B445" s="3" t="s">
-        <v>1167</v>
+        <v>1168</v>
       </c>
       <c r="C445" s="3"/>
       <c r="D445" s="3"/>
@@ -19491,10 +19500,10 @@
     </row>
     <row r="446" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A446" s="2" t="s">
-        <v>1168</v>
+        <v>1169</v>
       </c>
       <c r="B446" s="3" t="s">
-        <v>1169</v>
+        <v>1170</v>
       </c>
       <c r="C446" s="3"/>
       <c r="D446" s="3"/>
@@ -19523,7 +19532,7 @@
     </row>
     <row r="447" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A447" s="2" t="s">
-        <v>1170</v>
+        <v>1171</v>
       </c>
       <c r="B447" s="5"/>
       <c r="C447" s="5"/>
@@ -19553,7 +19562,7 @@
     </row>
     <row r="448" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A448" s="2" t="s">
-        <v>1171</v>
+        <v>1172</v>
       </c>
       <c r="B448" s="5"/>
       <c r="C448" s="5"/>
@@ -19583,7 +19592,7 @@
     </row>
     <row r="449" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A449" s="2" t="s">
-        <v>1172</v>
+        <v>1173</v>
       </c>
       <c r="B449" s="5"/>
       <c r="C449" s="5"/>
@@ -19613,10 +19622,10 @@
     </row>
     <row r="450" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A450" s="2" t="s">
-        <v>1173</v>
+        <v>1174</v>
       </c>
       <c r="B450" s="3" t="s">
-        <v>1174</v>
+        <v>1175</v>
       </c>
       <c r="C450" s="3"/>
       <c r="D450" s="3"/>
@@ -19645,10 +19654,10 @@
     </row>
     <row r="451" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A451" s="2" t="s">
-        <v>1175</v>
+        <v>1176</v>
       </c>
       <c r="B451" s="3" t="s">
-        <v>1176</v>
+        <v>1177</v>
       </c>
       <c r="C451" s="3"/>
       <c r="D451" s="3"/>
@@ -19677,10 +19686,10 @@
     </row>
     <row r="452" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A452" s="2" t="s">
-        <v>1177</v>
+        <v>1178</v>
       </c>
       <c r="B452" s="3" t="s">
-        <v>1178</v>
+        <v>1179</v>
       </c>
       <c r="C452" s="3"/>
       <c r="D452" s="3"/>
@@ -19709,10 +19718,10 @@
     </row>
     <row r="453" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A453" s="2" t="s">
-        <v>1179</v>
+        <v>1180</v>
       </c>
       <c r="B453" s="3" t="s">
-        <v>1180</v>
+        <v>1181</v>
       </c>
       <c r="C453" s="3"/>
       <c r="D453" s="3"/>
@@ -19741,10 +19750,10 @@
     </row>
     <row r="454" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A454" s="2" t="s">
-        <v>1181</v>
+        <v>1182</v>
       </c>
       <c r="B454" s="3" t="s">
-        <v>1182</v>
+        <v>1183</v>
       </c>
       <c r="C454" s="3"/>
       <c r="D454" s="3"/>
@@ -19773,10 +19782,10 @@
     </row>
     <row r="455" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A455" s="2" t="s">
-        <v>1183</v>
+        <v>1184</v>
       </c>
       <c r="B455" s="3" t="s">
-        <v>1184</v>
+        <v>1185</v>
       </c>
       <c r="C455" s="3"/>
       <c r="D455" s="3"/>
@@ -19805,10 +19814,10 @@
     </row>
     <row r="456" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A456" s="2" t="s">
-        <v>1185</v>
+        <v>1186</v>
       </c>
       <c r="B456" s="3" t="s">
-        <v>1186</v>
+        <v>1187</v>
       </c>
       <c r="C456" s="3"/>
       <c r="D456" s="3"/>
@@ -19837,10 +19846,10 @@
     </row>
     <row r="457" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A457" s="2" t="s">
-        <v>1187</v>
+        <v>1188</v>
       </c>
       <c r="B457" s="3" t="s">
-        <v>1188</v>
+        <v>1189</v>
       </c>
       <c r="C457" s="3"/>
       <c r="D457" s="3"/>
@@ -19869,10 +19878,10 @@
     </row>
     <row r="458" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A458" s="2" t="s">
-        <v>1189</v>
+        <v>1190</v>
       </c>
       <c r="B458" s="3" t="s">
-        <v>1190</v>
+        <v>1191</v>
       </c>
       <c r="C458" s="3"/>
       <c r="D458" s="3"/>
@@ -19901,10 +19910,10 @@
     </row>
     <row r="459" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A459" s="2" t="s">
-        <v>1191</v>
+        <v>1192</v>
       </c>
       <c r="B459" s="3" t="s">
-        <v>1192</v>
+        <v>1193</v>
       </c>
       <c r="C459" s="3"/>
       <c r="D459" s="3"/>
@@ -19933,10 +19942,10 @@
     </row>
     <row r="460" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A460" s="2" t="s">
-        <v>1193</v>
+        <v>1194</v>
       </c>
       <c r="B460" s="3" t="s">
-        <v>1194</v>
+        <v>1195</v>
       </c>
       <c r="C460" s="3"/>
       <c r="D460" s="3"/>
@@ -19965,10 +19974,10 @@
     </row>
     <row r="461" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A461" s="2" t="s">
-        <v>1195</v>
+        <v>1196</v>
       </c>
       <c r="B461" s="3" t="s">
-        <v>1196</v>
+        <v>1197</v>
       </c>
       <c r="C461" s="3"/>
       <c r="D461" s="3"/>
@@ -19997,10 +20006,10 @@
     </row>
     <row r="462" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A462" s="2" t="s">
-        <v>1197</v>
+        <v>1198</v>
       </c>
       <c r="B462" s="3" t="s">
-        <v>1198</v>
+        <v>1199</v>
       </c>
       <c r="C462" s="3"/>
       <c r="D462" s="3"/>
@@ -20029,10 +20038,10 @@
     </row>
     <row r="463" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A463" s="2" t="s">
-        <v>1199</v>
+        <v>1200</v>
       </c>
       <c r="B463" s="3" t="s">
-        <v>1200</v>
+        <v>1201</v>
       </c>
       <c r="C463" s="3"/>
       <c r="D463" s="3"/>
@@ -20061,10 +20070,10 @@
     </row>
     <row r="464" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A464" s="2" t="s">
-        <v>1201</v>
+        <v>1202</v>
       </c>
       <c r="B464" s="3" t="s">
-        <v>1202</v>
+        <v>1203</v>
       </c>
       <c r="C464" s="3"/>
       <c r="D464" s="3"/>
@@ -20093,10 +20102,10 @@
     </row>
     <row r="465" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A465" s="2" t="s">
-        <v>1203</v>
+        <v>1204</v>
       </c>
       <c r="B465" s="3" t="s">
-        <v>1204</v>
+        <v>1205</v>
       </c>
       <c r="C465" s="3"/>
       <c r="D465" s="3"/>
@@ -20125,7 +20134,7 @@
     </row>
     <row r="466" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A466" s="2" t="s">
-        <v>1205</v>
+        <v>1206</v>
       </c>
       <c r="B466" s="5"/>
       <c r="C466" s="5"/>
@@ -20155,21 +20164,21 @@
     </row>
     <row r="467" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A467" s="2" t="s">
-        <v>1206</v>
+        <v>1207</v>
       </c>
       <c r="B467" s="5"/>
       <c r="C467" s="5"/>
       <c r="D467" s="5"/>
-      <c r="E467" s="8"/>
-      <c r="F467" s="8"/>
-      <c r="G467" s="8"/>
-      <c r="H467" s="8"/>
-      <c r="I467" s="8"/>
-      <c r="J467" s="8"/>
-      <c r="K467" s="8"/>
-      <c r="L467" s="8"/>
-      <c r="M467" s="8"/>
-      <c r="N467" s="8"/>
+      <c r="E467" s="9"/>
+      <c r="F467" s="9"/>
+      <c r="G467" s="9"/>
+      <c r="H467" s="9"/>
+      <c r="I467" s="9"/>
+      <c r="J467" s="9"/>
+      <c r="K467" s="9"/>
+      <c r="L467" s="9"/>
+      <c r="M467" s="9"/>
+      <c r="N467" s="9"/>
       <c r="O467" s="5"/>
       <c r="P467" s="5"/>
       <c r="Q467" s="5"/>
@@ -20185,21 +20194,21 @@
     </row>
     <row r="468" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A468" s="2" t="s">
-        <v>1207</v>
+        <v>1208</v>
       </c>
       <c r="B468" s="5"/>
       <c r="C468" s="5"/>
       <c r="D468" s="5"/>
-      <c r="E468" s="8"/>
-      <c r="F468" s="8"/>
-      <c r="G468" s="8"/>
-      <c r="H468" s="8"/>
-      <c r="I468" s="8"/>
-      <c r="J468" s="8"/>
-      <c r="K468" s="8"/>
-      <c r="L468" s="8"/>
-      <c r="M468" s="8"/>
-      <c r="N468" s="8"/>
+      <c r="E468" s="9"/>
+      <c r="F468" s="9"/>
+      <c r="G468" s="9"/>
+      <c r="H468" s="9"/>
+      <c r="I468" s="9"/>
+      <c r="J468" s="9"/>
+      <c r="K468" s="9"/>
+      <c r="L468" s="9"/>
+      <c r="M468" s="9"/>
+      <c r="N468" s="9"/>
       <c r="O468" s="5"/>
       <c r="P468" s="5"/>
       <c r="Q468" s="5"/>
@@ -20215,21 +20224,21 @@
     </row>
     <row r="469" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A469" s="2" t="s">
-        <v>1208</v>
+        <v>1209</v>
       </c>
       <c r="B469" s="5"/>
       <c r="C469" s="5"/>
       <c r="D469" s="5"/>
-      <c r="E469" s="8"/>
-      <c r="F469" s="8"/>
-      <c r="G469" s="8"/>
-      <c r="H469" s="8"/>
-      <c r="I469" s="8"/>
-      <c r="J469" s="8"/>
-      <c r="K469" s="8"/>
-      <c r="L469" s="8"/>
-      <c r="M469" s="8"/>
-      <c r="N469" s="8"/>
+      <c r="E469" s="9"/>
+      <c r="F469" s="9"/>
+      <c r="G469" s="9"/>
+      <c r="H469" s="9"/>
+      <c r="I469" s="9"/>
+      <c r="J469" s="9"/>
+      <c r="K469" s="9"/>
+      <c r="L469" s="9"/>
+      <c r="M469" s="9"/>
+      <c r="N469" s="9"/>
       <c r="O469" s="5"/>
       <c r="P469" s="5"/>
       <c r="Q469" s="5"/>
@@ -20245,21 +20254,21 @@
     </row>
     <row r="470" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A470" s="2" t="s">
-        <v>1209</v>
+        <v>1210</v>
       </c>
       <c r="B470" s="5"/>
       <c r="C470" s="5"/>
       <c r="D470" s="5"/>
-      <c r="E470" s="8"/>
-      <c r="F470" s="8"/>
-      <c r="G470" s="8"/>
-      <c r="H470" s="8"/>
-      <c r="I470" s="8"/>
-      <c r="J470" s="8"/>
-      <c r="K470" s="8"/>
-      <c r="L470" s="8"/>
-      <c r="M470" s="8"/>
-      <c r="N470" s="8"/>
+      <c r="E470" s="9"/>
+      <c r="F470" s="9"/>
+      <c r="G470" s="9"/>
+      <c r="H470" s="9"/>
+      <c r="I470" s="9"/>
+      <c r="J470" s="9"/>
+      <c r="K470" s="9"/>
+      <c r="L470" s="9"/>
+      <c r="M470" s="9"/>
+      <c r="N470" s="9"/>
       <c r="O470" s="5"/>
       <c r="P470" s="5"/>
       <c r="Q470" s="5"/>
@@ -20275,21 +20284,21 @@
     </row>
     <row r="471" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A471" s="2" t="s">
-        <v>1210</v>
+        <v>1211</v>
       </c>
       <c r="B471" s="5"/>
       <c r="C471" s="5"/>
       <c r="D471" s="5"/>
-      <c r="E471" s="8"/>
-      <c r="F471" s="8"/>
-      <c r="G471" s="8"/>
-      <c r="H471" s="8"/>
-      <c r="I471" s="8"/>
-      <c r="J471" s="8"/>
-      <c r="K471" s="8"/>
-      <c r="L471" s="8"/>
-      <c r="M471" s="8"/>
-      <c r="N471" s="8"/>
+      <c r="E471" s="9"/>
+      <c r="F471" s="9"/>
+      <c r="G471" s="9"/>
+      <c r="H471" s="9"/>
+      <c r="I471" s="9"/>
+      <c r="J471" s="9"/>
+      <c r="K471" s="9"/>
+      <c r="L471" s="9"/>
+      <c r="M471" s="9"/>
+      <c r="N471" s="9"/>
       <c r="O471" s="5"/>
       <c r="P471" s="5"/>
       <c r="Q471" s="5"/>
@@ -20305,21 +20314,21 @@
     </row>
     <row r="472" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A472" s="2" t="s">
-        <v>1211</v>
+        <v>1212</v>
       </c>
       <c r="B472" s="5"/>
       <c r="C472" s="5"/>
       <c r="D472" s="5"/>
-      <c r="E472" s="8"/>
-      <c r="F472" s="8"/>
-      <c r="G472" s="8"/>
-      <c r="H472" s="8"/>
-      <c r="I472" s="8"/>
-      <c r="J472" s="8"/>
-      <c r="K472" s="8"/>
-      <c r="L472" s="8"/>
-      <c r="M472" s="8"/>
-      <c r="N472" s="8"/>
+      <c r="E472" s="9"/>
+      <c r="F472" s="9"/>
+      <c r="G472" s="9"/>
+      <c r="H472" s="9"/>
+      <c r="I472" s="9"/>
+      <c r="J472" s="9"/>
+      <c r="K472" s="9"/>
+      <c r="L472" s="9"/>
+      <c r="M472" s="9"/>
+      <c r="N472" s="9"/>
       <c r="O472" s="5"/>
       <c r="P472" s="5"/>
       <c r="Q472" s="5"/>
@@ -20335,7 +20344,7 @@
     </row>
     <row r="473" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A473" s="2" t="s">
-        <v>1212</v>
+        <v>1213</v>
       </c>
       <c r="B473" s="5"/>
       <c r="C473" s="5"/>
@@ -20365,7 +20374,7 @@
     </row>
     <row r="474" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A474" s="2" t="s">
-        <v>1213</v>
+        <v>1214</v>
       </c>
       <c r="B474" s="5"/>
       <c r="C474" s="5"/>
@@ -20395,7 +20404,7 @@
     </row>
     <row r="475" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A475" s="2" t="s">
-        <v>1214</v>
+        <v>1215</v>
       </c>
       <c r="B475" s="5"/>
       <c r="C475" s="5"/>
@@ -20425,7 +20434,7 @@
     </row>
     <row r="476" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A476" s="2" t="s">
-        <v>1215</v>
+        <v>1216</v>
       </c>
       <c r="B476" s="5"/>
       <c r="C476" s="5"/>
@@ -20455,7 +20464,7 @@
     </row>
     <row r="477" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A477" s="2" t="s">
-        <v>1216</v>
+        <v>1217</v>
       </c>
       <c r="B477" s="5"/>
       <c r="C477" s="5"/>
@@ -20485,7 +20494,7 @@
     </row>
     <row r="478" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A478" s="2" t="s">
-        <v>1217</v>
+        <v>1218</v>
       </c>
       <c r="B478" s="5"/>
       <c r="C478" s="5"/>
@@ -20515,7 +20524,7 @@
     </row>
     <row r="479" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A479" s="2" t="s">
-        <v>1218</v>
+        <v>1219</v>
       </c>
       <c r="B479" s="5"/>
       <c r="C479" s="5"/>
@@ -20545,7 +20554,7 @@
     </row>
     <row r="480" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A480" s="2" t="s">
-        <v>1219</v>
+        <v>1220</v>
       </c>
       <c r="B480" s="5"/>
       <c r="C480" s="5"/>
@@ -20575,7 +20584,7 @@
     </row>
     <row r="481" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A481" s="2" t="s">
-        <v>1220</v>
+        <v>1221</v>
       </c>
       <c r="B481" s="5"/>
       <c r="C481" s="5"/>
@@ -20604,25 +20613,25 @@
       <c r="Z481" s="1"/>
     </row>
     <row r="482" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A482" s="9"/>
-      <c r="B482" s="10"/>
-      <c r="C482" s="10"/>
-      <c r="D482" s="10"/>
-      <c r="E482" s="10"/>
-      <c r="F482" s="10"/>
-      <c r="G482" s="10"/>
-      <c r="H482" s="10"/>
+      <c r="A482" s="10"/>
+      <c r="B482" s="11"/>
+      <c r="C482" s="11"/>
+      <c r="D482" s="11"/>
+      <c r="E482" s="11"/>
+      <c r="F482" s="11"/>
+      <c r="G482" s="11"/>
+      <c r="H482" s="11"/>
       <c r="I482" s="3" t="s">
-        <v>1221</v>
+        <v>1222</v>
       </c>
       <c r="J482" s="3"/>
-      <c r="K482" s="10"/>
-      <c r="L482" s="10"/>
-      <c r="M482" s="10"/>
-      <c r="N482" s="10"/>
-      <c r="O482" s="10"/>
-      <c r="P482" s="10"/>
-      <c r="Q482" s="10"/>
+      <c r="K482" s="11"/>
+      <c r="L482" s="11"/>
+      <c r="M482" s="11"/>
+      <c r="N482" s="11"/>
+      <c r="O482" s="11"/>
+      <c r="P482" s="11"/>
+      <c r="Q482" s="11"/>
       <c r="R482" s="1"/>
       <c r="S482" s="1"/>
       <c r="T482" s="1"/>
@@ -20635,37 +20644,37 @@
     </row>
     <row r="483" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A483" s="2" t="s">
-        <v>1222</v>
+        <v>1223</v>
       </c>
       <c r="B483" s="4" t="s">
-        <v>1223</v>
+        <v>1224</v>
       </c>
       <c r="C483" s="4" t="s">
-        <v>1224</v>
+        <v>1225</v>
       </c>
       <c r="D483" s="4" t="s">
-        <v>1225</v>
+        <v>1226</v>
       </c>
       <c r="E483" s="4" t="s">
-        <v>1226</v>
+        <v>1227</v>
       </c>
       <c r="F483" s="4" t="s">
-        <v>1227</v>
+        <v>1228</v>
       </c>
       <c r="G483" s="4" t="s">
-        <v>1228</v>
+        <v>1229</v>
       </c>
       <c r="H483" s="4" t="s">
-        <v>1229</v>
+        <v>1230</v>
       </c>
       <c r="I483" s="4" t="s">
-        <v>1230</v>
+        <v>1231</v>
       </c>
       <c r="J483" s="4" t="s">
-        <v>1231</v>
+        <v>1232</v>
       </c>
       <c r="K483" s="4" t="s">
-        <v>1232</v>
+        <v>1233</v>
       </c>
       <c r="L483" s="5"/>
       <c r="M483" s="5"/>
@@ -20685,37 +20694,37 @@
     </row>
     <row r="484" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A484" s="2" t="s">
-        <v>1233</v>
+        <v>1234</v>
       </c>
       <c r="B484" s="4" t="s">
-        <v>1234</v>
+        <v>1235</v>
       </c>
       <c r="C484" s="4" t="s">
-        <v>1235</v>
+        <v>1236</v>
       </c>
       <c r="D484" s="4" t="s">
-        <v>1236</v>
+        <v>1237</v>
       </c>
       <c r="E484" s="4" t="s">
-        <v>1237</v>
+        <v>1238</v>
       </c>
       <c r="F484" s="4" t="s">
-        <v>1238</v>
+        <v>1239</v>
       </c>
       <c r="G484" s="4" t="s">
-        <v>1239</v>
+        <v>1240</v>
       </c>
       <c r="H484" s="4" t="s">
-        <v>1240</v>
+        <v>1241</v>
       </c>
       <c r="I484" s="4" t="s">
-        <v>1241</v>
+        <v>1242</v>
       </c>
       <c r="J484" s="4" t="s">
-        <v>1242</v>
+        <v>1243</v>
       </c>
       <c r="K484" s="4" t="s">
-        <v>1243</v>
+        <v>1244</v>
       </c>
       <c r="L484" s="5"/>
       <c r="M484" s="5"/>
@@ -20735,37 +20744,37 @@
     </row>
     <row r="485" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A485" s="2" t="s">
-        <v>1244</v>
+        <v>1245</v>
       </c>
       <c r="B485" s="4" t="s">
-        <v>1245</v>
+        <v>1246</v>
       </c>
       <c r="C485" s="4" t="s">
-        <v>1246</v>
+        <v>1247</v>
       </c>
       <c r="D485" s="4" t="s">
-        <v>1247</v>
+        <v>1248</v>
       </c>
       <c r="E485" s="4" t="s">
-        <v>1248</v>
+        <v>1249</v>
       </c>
       <c r="F485" s="4" t="s">
-        <v>1249</v>
+        <v>1250</v>
       </c>
       <c r="G485" s="4" t="s">
-        <v>1250</v>
+        <v>1251</v>
       </c>
       <c r="H485" s="4" t="s">
-        <v>1251</v>
+        <v>1252</v>
       </c>
       <c r="I485" s="4" t="s">
-        <v>1252</v>
+        <v>1253</v>
       </c>
       <c r="J485" s="4" t="s">
-        <v>1253</v>
+        <v>1254</v>
       </c>
       <c r="K485" s="4" t="s">
-        <v>1254</v>
+        <v>1255</v>
       </c>
       <c r="L485" s="5"/>
       <c r="M485" s="5"/>
@@ -20785,37 +20794,37 @@
     </row>
     <row r="486" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A486" s="2" t="s">
-        <v>1255</v>
+        <v>1256</v>
       </c>
       <c r="B486" s="4" t="s">
-        <v>1256</v>
+        <v>1257</v>
       </c>
       <c r="C486" s="4" t="s">
-        <v>1257</v>
+        <v>1258</v>
       </c>
       <c r="D486" s="4" t="s">
-        <v>1258</v>
+        <v>1259</v>
       </c>
       <c r="E486" s="4" t="s">
-        <v>1259</v>
+        <v>1260</v>
       </c>
       <c r="F486" s="4" t="s">
-        <v>1260</v>
+        <v>1261</v>
       </c>
       <c r="G486" s="4" t="s">
-        <v>1261</v>
+        <v>1262</v>
       </c>
       <c r="H486" s="4" t="s">
-        <v>1262</v>
+        <v>1263</v>
       </c>
       <c r="I486" s="4" t="s">
-        <v>1263</v>
+        <v>1264</v>
       </c>
       <c r="J486" s="4" t="s">
-        <v>1264</v>
+        <v>1265</v>
       </c>
       <c r="K486" s="4" t="s">
-        <v>1265</v>
+        <v>1266</v>
       </c>
       <c r="L486" s="5"/>
       <c r="M486" s="5"/>
@@ -20835,37 +20844,37 @@
     </row>
     <row r="487" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A487" s="2" t="s">
-        <v>1266</v>
+        <v>1267</v>
       </c>
       <c r="B487" s="4" t="s">
-        <v>1267</v>
+        <v>1268</v>
       </c>
       <c r="C487" s="4" t="s">
-        <v>1268</v>
+        <v>1269</v>
       </c>
       <c r="D487" s="4" t="s">
-        <v>1269</v>
+        <v>1270</v>
       </c>
       <c r="E487" s="4" t="s">
-        <v>1270</v>
+        <v>1271</v>
       </c>
       <c r="F487" s="4" t="s">
-        <v>1271</v>
+        <v>1272</v>
       </c>
       <c r="G487" s="4" t="s">
-        <v>1272</v>
+        <v>1273</v>
       </c>
       <c r="H487" s="4" t="s">
-        <v>1273</v>
+        <v>1274</v>
       </c>
       <c r="I487" s="4" t="s">
-        <v>1274</v>
+        <v>1275</v>
       </c>
       <c r="J487" s="4" t="s">
-        <v>1275</v>
+        <v>1276</v>
       </c>
       <c r="K487" s="4" t="s">
-        <v>1276</v>
+        <v>1277</v>
       </c>
       <c r="L487" s="5"/>
       <c r="M487" s="5"/>
@@ -20885,37 +20894,37 @@
     </row>
     <row r="488" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A488" s="2" t="s">
-        <v>1277</v>
+        <v>1278</v>
       </c>
       <c r="B488" s="4" t="s">
-        <v>1278</v>
+        <v>1279</v>
       </c>
       <c r="C488" s="4" t="s">
-        <v>1279</v>
+        <v>1280</v>
       </c>
       <c r="D488" s="4" t="s">
-        <v>1280</v>
+        <v>1281</v>
       </c>
       <c r="E488" s="4" t="s">
-        <v>1281</v>
+        <v>1282</v>
       </c>
       <c r="F488" s="4" t="s">
-        <v>1282</v>
+        <v>1283</v>
       </c>
       <c r="G488" s="4" t="s">
-        <v>1283</v>
+        <v>1284</v>
       </c>
       <c r="H488" s="4" t="s">
-        <v>1284</v>
+        <v>1285</v>
       </c>
       <c r="I488" s="4" t="s">
-        <v>1285</v>
+        <v>1286</v>
       </c>
       <c r="J488" s="4" t="s">
-        <v>1286</v>
+        <v>1287</v>
       </c>
       <c r="K488" s="4" t="s">
-        <v>1287</v>
+        <v>1288</v>
       </c>
       <c r="L488" s="5"/>
       <c r="M488" s="5"/>
@@ -20935,37 +20944,37 @@
     </row>
     <row r="489" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A489" s="2" t="s">
-        <v>1288</v>
+        <v>1289</v>
       </c>
       <c r="B489" s="4" t="s">
-        <v>1289</v>
+        <v>1290</v>
       </c>
       <c r="C489" s="4" t="s">
-        <v>1290</v>
+        <v>1291</v>
       </c>
       <c r="D489" s="4" t="s">
-        <v>1291</v>
+        <v>1292</v>
       </c>
       <c r="E489" s="4" t="s">
-        <v>1292</v>
+        <v>1293</v>
       </c>
       <c r="F489" s="4" t="s">
-        <v>1293</v>
+        <v>1294</v>
       </c>
       <c r="G489" s="4" t="s">
-        <v>1294</v>
+        <v>1295</v>
       </c>
       <c r="H489" s="4" t="s">
-        <v>1295</v>
+        <v>1296</v>
       </c>
       <c r="I489" s="4" t="s">
-        <v>1296</v>
+        <v>1297</v>
       </c>
       <c r="J489" s="4" t="s">
-        <v>1297</v>
+        <v>1298</v>
       </c>
       <c r="K489" s="4" t="s">
-        <v>1298</v>
+        <v>1299</v>
       </c>
       <c r="L489" s="5"/>
       <c r="M489" s="5"/>
@@ -20985,37 +20994,37 @@
     </row>
     <row r="490" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A490" s="2" t="s">
-        <v>1299</v>
+        <v>1300</v>
       </c>
       <c r="B490" s="4" t="s">
-        <v>1300</v>
+        <v>1301</v>
       </c>
       <c r="C490" s="4" t="s">
-        <v>1301</v>
+        <v>1302</v>
       </c>
       <c r="D490" s="4" t="s">
-        <v>1302</v>
+        <v>1303</v>
       </c>
       <c r="E490" s="4" t="s">
-        <v>1303</v>
+        <v>1304</v>
       </c>
       <c r="F490" s="4" t="s">
-        <v>1304</v>
+        <v>1305</v>
       </c>
       <c r="G490" s="4" t="s">
-        <v>1305</v>
+        <v>1306</v>
       </c>
       <c r="H490" s="4" t="s">
-        <v>1306</v>
+        <v>1307</v>
       </c>
       <c r="I490" s="4" t="s">
-        <v>1307</v>
+        <v>1308</v>
       </c>
       <c r="J490" s="4" t="s">
-        <v>1308</v>
+        <v>1309</v>
       </c>
       <c r="K490" s="4" t="s">
-        <v>1309</v>
+        <v>1310</v>
       </c>
       <c r="L490" s="5"/>
       <c r="M490" s="5"/>
@@ -21035,37 +21044,37 @@
     </row>
     <row r="491" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A491" s="2" t="s">
-        <v>1310</v>
+        <v>1311</v>
       </c>
       <c r="B491" s="4" t="s">
-        <v>1311</v>
+        <v>1312</v>
       </c>
       <c r="C491" s="4" t="s">
-        <v>1312</v>
+        <v>1313</v>
       </c>
       <c r="D491" s="4" t="s">
-        <v>1313</v>
+        <v>1314</v>
       </c>
       <c r="E491" s="4" t="s">
-        <v>1314</v>
+        <v>1315</v>
       </c>
       <c r="F491" s="4" t="s">
-        <v>1315</v>
+        <v>1316</v>
       </c>
       <c r="G491" s="4" t="s">
-        <v>1316</v>
+        <v>1317</v>
       </c>
       <c r="H491" s="4" t="s">
-        <v>1317</v>
+        <v>1318</v>
       </c>
       <c r="I491" s="4" t="s">
-        <v>1318</v>
+        <v>1319</v>
       </c>
       <c r="J491" s="4" t="s">
-        <v>1319</v>
+        <v>1320</v>
       </c>
       <c r="K491" s="4" t="s">
-        <v>1320</v>
+        <v>1321</v>
       </c>
       <c r="L491" s="5"/>
       <c r="M491" s="5"/>
@@ -21085,37 +21094,37 @@
     </row>
     <row r="492" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A492" s="2" t="s">
-        <v>1321</v>
+        <v>1322</v>
       </c>
       <c r="B492" s="4" t="s">
-        <v>1322</v>
+        <v>1323</v>
       </c>
       <c r="C492" s="4" t="s">
-        <v>1323</v>
+        <v>1324</v>
       </c>
       <c r="D492" s="4" t="s">
-        <v>1324</v>
+        <v>1325</v>
       </c>
       <c r="E492" s="4" t="s">
-        <v>1325</v>
+        <v>1326</v>
       </c>
       <c r="F492" s="4" t="s">
-        <v>1326</v>
+        <v>1327</v>
       </c>
       <c r="G492" s="4" t="s">
-        <v>1327</v>
+        <v>1328</v>
       </c>
       <c r="H492" s="4" t="s">
-        <v>1328</v>
+        <v>1329</v>
       </c>
       <c r="I492" s="4" t="s">
-        <v>1329</v>
+        <v>1330</v>
       </c>
       <c r="J492" s="4" t="s">
-        <v>1330</v>
+        <v>1331</v>
       </c>
       <c r="K492" s="4" t="s">
-        <v>1331</v>
+        <v>1332</v>
       </c>
       <c r="L492" s="5"/>
       <c r="M492" s="5"/>
@@ -21135,37 +21144,37 @@
     </row>
     <row r="493" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A493" s="2" t="s">
-        <v>1332</v>
+        <v>1333</v>
       </c>
       <c r="B493" s="4" t="s">
-        <v>1333</v>
+        <v>1334</v>
       </c>
       <c r="C493" s="4" t="s">
-        <v>1334</v>
+        <v>1335</v>
       </c>
       <c r="D493" s="4" t="s">
-        <v>1335</v>
+        <v>1336</v>
       </c>
       <c r="E493" s="4" t="s">
-        <v>1336</v>
+        <v>1337</v>
       </c>
       <c r="F493" s="4" t="s">
-        <v>1337</v>
+        <v>1338</v>
       </c>
       <c r="G493" s="4" t="s">
-        <v>1338</v>
+        <v>1339</v>
       </c>
       <c r="H493" s="4" t="s">
-        <v>1339</v>
+        <v>1340</v>
       </c>
       <c r="I493" s="4" t="s">
-        <v>1340</v>
+        <v>1341</v>
       </c>
       <c r="J493" s="4" t="s">
-        <v>1341</v>
+        <v>1342</v>
       </c>
       <c r="K493" s="4" t="s">
-        <v>1342</v>
+        <v>1343</v>
       </c>
       <c r="L493" s="5"/>
       <c r="M493" s="5"/>
@@ -21185,37 +21194,37 @@
     </row>
     <row r="494" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A494" s="2" t="s">
-        <v>1343</v>
+        <v>1344</v>
       </c>
       <c r="B494" s="4" t="s">
-        <v>1344</v>
+        <v>1345</v>
       </c>
       <c r="C494" s="4" t="s">
-        <v>1345</v>
+        <v>1346</v>
       </c>
       <c r="D494" s="4" t="s">
-        <v>1346</v>
+        <v>1347</v>
       </c>
       <c r="E494" s="4" t="s">
-        <v>1347</v>
+        <v>1348</v>
       </c>
       <c r="F494" s="4" t="s">
-        <v>1348</v>
+        <v>1349</v>
       </c>
       <c r="G494" s="4" t="s">
-        <v>1349</v>
+        <v>1350</v>
       </c>
       <c r="H494" s="4" t="s">
-        <v>1350</v>
+        <v>1351</v>
       </c>
       <c r="I494" s="4" t="s">
-        <v>1351</v>
+        <v>1352</v>
       </c>
       <c r="J494" s="4" t="s">
-        <v>1352</v>
+        <v>1353</v>
       </c>
       <c r="K494" s="4" t="s">
-        <v>1353</v>
+        <v>1354</v>
       </c>
       <c r="L494" s="5"/>
       <c r="M494" s="5"/>
@@ -21235,38 +21244,38 @@
     </row>
     <row r="495" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A495" s="2" t="s">
-        <v>1354</v>
+        <v>1355</v>
       </c>
       <c r="B495" s="3" t="s">
-        <v>1355</v>
+        <v>1356</v>
       </c>
       <c r="C495" s="3"/>
       <c r="D495" s="3" t="s">
-        <v>1356</v>
+        <v>1357</v>
       </c>
       <c r="E495" s="3"/>
       <c r="F495" s="3" t="s">
-        <v>1357</v>
+        <v>1358</v>
       </c>
       <c r="G495" s="3"/>
       <c r="H495" s="3" t="s">
-        <v>1358</v>
+        <v>1359</v>
       </c>
       <c r="I495" s="3"/>
       <c r="J495" s="3" t="s">
-        <v>1359</v>
+        <v>1360</v>
       </c>
       <c r="K495" s="3"/>
       <c r="L495" s="3" t="s">
-        <v>1360</v>
+        <v>1361</v>
       </c>
       <c r="M495" s="3"/>
       <c r="N495" s="3" t="s">
-        <v>1361</v>
+        <v>1362</v>
       </c>
       <c r="O495" s="3"/>
       <c r="P495" s="3" t="s">
-        <v>1362</v>
+        <v>1363</v>
       </c>
       <c r="Q495" s="3"/>
       <c r="R495" s="1"/>
@@ -21281,34 +21290,34 @@
     </row>
     <row r="496" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A496" s="2" t="s">
-        <v>1363</v>
+        <v>1364</v>
       </c>
       <c r="B496" s="4" t="s">
-        <v>1364</v>
+        <v>1365</v>
       </c>
       <c r="C496" s="4" t="s">
-        <v>1365</v>
+        <v>1366</v>
       </c>
       <c r="D496" s="4" t="s">
-        <v>1366</v>
+        <v>1367</v>
       </c>
       <c r="E496" s="4" t="s">
-        <v>1367</v>
+        <v>1368</v>
       </c>
       <c r="F496" s="4" t="s">
-        <v>1368</v>
+        <v>1369</v>
       </c>
       <c r="G496" s="4" t="s">
-        <v>1369</v>
+        <v>1370</v>
       </c>
       <c r="H496" s="4" t="s">
-        <v>1370</v>
+        <v>1371</v>
       </c>
       <c r="I496" s="4" t="s">
-        <v>1371</v>
+        <v>1372</v>
       </c>
       <c r="J496" s="4" t="s">
-        <v>1372</v>
+        <v>1373</v>
       </c>
       <c r="K496" s="5"/>
       <c r="L496" s="5"/>
@@ -21329,34 +21338,34 @@
     </row>
     <row r="497" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A497" s="2" t="s">
-        <v>1373</v>
+        <v>1374</v>
       </c>
       <c r="B497" s="4" t="s">
-        <v>1374</v>
+        <v>1375</v>
       </c>
       <c r="C497" s="4" t="s">
-        <v>1375</v>
+        <v>1376</v>
       </c>
       <c r="D497" s="4" t="s">
-        <v>1376</v>
+        <v>1377</v>
       </c>
       <c r="E497" s="4" t="s">
-        <v>1377</v>
+        <v>1378</v>
       </c>
       <c r="F497" s="4" t="s">
-        <v>1378</v>
+        <v>1379</v>
       </c>
       <c r="G497" s="4" t="s">
-        <v>1379</v>
+        <v>1380</v>
       </c>
       <c r="H497" s="4" t="s">
-        <v>1380</v>
+        <v>1381</v>
       </c>
       <c r="I497" s="4" t="s">
-        <v>1381</v>
+        <v>1382</v>
       </c>
       <c r="J497" s="4" t="s">
-        <v>1382</v>
+        <v>1383</v>
       </c>
       <c r="K497" s="5"/>
       <c r="L497" s="5"/>
@@ -21377,34 +21386,34 @@
     </row>
     <row r="498" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A498" s="2" t="s">
-        <v>1383</v>
+        <v>1384</v>
       </c>
       <c r="B498" s="4" t="s">
-        <v>1384</v>
+        <v>1385</v>
       </c>
       <c r="C498" s="4" t="s">
-        <v>1385</v>
+        <v>1386</v>
       </c>
       <c r="D498" s="4" t="s">
-        <v>1386</v>
+        <v>1387</v>
       </c>
       <c r="E498" s="4" t="s">
-        <v>1387</v>
+        <v>1388</v>
       </c>
       <c r="F498" s="4" t="s">
-        <v>1388</v>
+        <v>1389</v>
       </c>
       <c r="G498" s="4" t="s">
-        <v>1389</v>
+        <v>1390</v>
       </c>
       <c r="H498" s="4" t="s">
-        <v>1390</v>
+        <v>1391</v>
       </c>
       <c r="I498" s="4" t="s">
-        <v>1391</v>
+        <v>1392</v>
       </c>
       <c r="J498" s="4" t="s">
-        <v>1392</v>
+        <v>1393</v>
       </c>
       <c r="K498" s="5"/>
       <c r="L498" s="5"/>
@@ -21425,34 +21434,34 @@
     </row>
     <row r="499" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A499" s="2" t="s">
-        <v>1393</v>
+        <v>1394</v>
       </c>
       <c r="B499" s="4" t="s">
-        <v>1394</v>
+        <v>1395</v>
       </c>
       <c r="C499" s="4" t="s">
-        <v>1395</v>
+        <v>1396</v>
       </c>
       <c r="D499" s="4" t="s">
-        <v>1396</v>
+        <v>1397</v>
       </c>
       <c r="E499" s="4" t="s">
-        <v>1397</v>
+        <v>1398</v>
       </c>
       <c r="F499" s="4" t="s">
-        <v>1398</v>
+        <v>1399</v>
       </c>
       <c r="G499" s="4" t="s">
-        <v>1399</v>
+        <v>1400</v>
       </c>
       <c r="H499" s="4" t="s">
-        <v>1400</v>
+        <v>1401</v>
       </c>
       <c r="I499" s="4" t="s">
-        <v>1401</v>
+        <v>1402</v>
       </c>
       <c r="J499" s="4" t="s">
-        <v>1402</v>
+        <v>1403</v>
       </c>
       <c r="K499" s="5"/>
       <c r="L499" s="5"/>
@@ -21473,34 +21482,34 @@
     </row>
     <row r="500" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A500" s="2" t="s">
-        <v>1403</v>
+        <v>1404</v>
       </c>
       <c r="B500" s="4" t="s">
-        <v>1404</v>
+        <v>1405</v>
       </c>
       <c r="C500" s="4" t="s">
-        <v>1405</v>
+        <v>1406</v>
       </c>
       <c r="D500" s="4" t="s">
-        <v>1406</v>
+        <v>1407</v>
       </c>
       <c r="E500" s="4" t="s">
-        <v>1407</v>
+        <v>1408</v>
       </c>
       <c r="F500" s="4" t="s">
-        <v>1408</v>
+        <v>1409</v>
       </c>
       <c r="G500" s="4" t="s">
-        <v>1409</v>
+        <v>1410</v>
       </c>
       <c r="H500" s="4" t="s">
-        <v>1410</v>
+        <v>1411</v>
       </c>
       <c r="I500" s="4" t="s">
-        <v>1411</v>
+        <v>1412</v>
       </c>
       <c r="J500" s="4" t="s">
-        <v>1412</v>
+        <v>1413</v>
       </c>
       <c r="K500" s="5"/>
       <c r="L500" s="5"/>
@@ -21521,34 +21530,34 @@
     </row>
     <row r="501" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A501" s="2" t="s">
-        <v>1413</v>
+        <v>1414</v>
       </c>
       <c r="B501" s="4" t="s">
-        <v>1414</v>
+        <v>1415</v>
       </c>
       <c r="C501" s="4" t="s">
-        <v>1415</v>
+        <v>1416</v>
       </c>
       <c r="D501" s="4" t="s">
-        <v>1416</v>
+        <v>1417</v>
       </c>
       <c r="E501" s="4" t="s">
-        <v>1417</v>
+        <v>1418</v>
       </c>
       <c r="F501" s="4" t="s">
-        <v>1418</v>
+        <v>1419</v>
       </c>
       <c r="G501" s="4" t="s">
-        <v>1419</v>
+        <v>1420</v>
       </c>
       <c r="H501" s="4" t="s">
-        <v>1420</v>
+        <v>1421</v>
       </c>
       <c r="I501" s="4" t="s">
-        <v>1421</v>
+        <v>1422</v>
       </c>
       <c r="J501" s="4" t="s">
-        <v>1422</v>
+        <v>1423</v>
       </c>
       <c r="K501" s="5"/>
       <c r="L501" s="5"/>
@@ -21569,34 +21578,34 @@
     </row>
     <row r="502" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A502" s="2" t="s">
-        <v>1423</v>
+        <v>1424</v>
       </c>
       <c r="B502" s="4" t="s">
-        <v>1424</v>
+        <v>1425</v>
       </c>
       <c r="C502" s="4" t="s">
-        <v>1425</v>
+        <v>1426</v>
       </c>
       <c r="D502" s="4" t="s">
-        <v>1426</v>
+        <v>1427</v>
       </c>
       <c r="E502" s="4" t="s">
-        <v>1427</v>
+        <v>1428</v>
       </c>
       <c r="F502" s="4" t="s">
-        <v>1428</v>
+        <v>1429</v>
       </c>
       <c r="G502" s="4" t="s">
-        <v>1429</v>
+        <v>1430</v>
       </c>
       <c r="H502" s="4" t="s">
-        <v>1430</v>
+        <v>1431</v>
       </c>
       <c r="I502" s="4" t="s">
-        <v>1431</v>
+        <v>1432</v>
       </c>
       <c r="J502" s="4" t="s">
-        <v>1432</v>
+        <v>1433</v>
       </c>
       <c r="K502" s="5"/>
       <c r="L502" s="5"/>
@@ -21617,30 +21626,30 @@
     </row>
     <row r="503" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A503" s="2" t="s">
-        <v>1433</v>
+        <v>1434</v>
       </c>
       <c r="B503" s="3" t="s">
-        <v>1434</v>
+        <v>1435</v>
       </c>
       <c r="C503" s="3"/>
       <c r="D503" s="3" t="s">
-        <v>1435</v>
+        <v>1436</v>
       </c>
       <c r="E503" s="3"/>
       <c r="F503" s="3" t="s">
-        <v>1436</v>
+        <v>1437</v>
       </c>
       <c r="G503" s="3"/>
       <c r="H503" s="3" t="s">
-        <v>1437</v>
+        <v>1438</v>
       </c>
       <c r="I503" s="3"/>
       <c r="J503" s="3" t="s">
-        <v>1438</v>
+        <v>1439</v>
       </c>
       <c r="K503" s="3"/>
       <c r="L503" s="3" t="s">
-        <v>1439</v>
+        <v>1440</v>
       </c>
       <c r="M503" s="3"/>
       <c r="N503" s="5"/>
@@ -21659,38 +21668,38 @@
     </row>
     <row r="504" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A504" s="2" t="s">
-        <v>1440</v>
+        <v>1441</v>
       </c>
       <c r="B504" s="3" t="s">
-        <v>1441</v>
+        <v>1442</v>
       </c>
       <c r="C504" s="3"/>
       <c r="D504" s="3" t="s">
-        <v>1442</v>
+        <v>1443</v>
       </c>
       <c r="E504" s="3"/>
       <c r="F504" s="3" t="s">
-        <v>1443</v>
+        <v>1444</v>
       </c>
       <c r="G504" s="3"/>
       <c r="H504" s="3" t="s">
-        <v>1444</v>
+        <v>1445</v>
       </c>
       <c r="I504" s="3"/>
       <c r="J504" s="3" t="s">
-        <v>1445</v>
+        <v>1446</v>
       </c>
       <c r="K504" s="3"/>
       <c r="L504" s="3" t="s">
-        <v>1446</v>
+        <v>1447</v>
       </c>
       <c r="M504" s="3"/>
       <c r="N504" s="3" t="s">
-        <v>1447</v>
+        <v>1448</v>
       </c>
       <c r="O504" s="3"/>
       <c r="P504" s="3" t="s">
-        <v>1448</v>
+        <v>1449</v>
       </c>
       <c r="Q504" s="3"/>
       <c r="R504" s="1"/>
@@ -21705,14 +21714,14 @@
     </row>
     <row r="505" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A505" s="2" t="s">
-        <v>1449</v>
+        <v>1450</v>
       </c>
       <c r="B505" s="3" t="s">
-        <v>1450</v>
+        <v>1451</v>
       </c>
       <c r="C505" s="3"/>
       <c r="D505" s="3" t="s">
-        <v>1451</v>
+        <v>1452</v>
       </c>
       <c r="E505" s="3"/>
       <c r="F505" s="5"/>
@@ -21720,19 +21729,19 @@
       <c r="H505" s="5"/>
       <c r="I505" s="5"/>
       <c r="J505" s="3" t="s">
-        <v>1452</v>
+        <v>1453</v>
       </c>
       <c r="K505" s="3"/>
       <c r="L505" s="3" t="s">
-        <v>1453</v>
+        <v>1454</v>
       </c>
       <c r="M505" s="3"/>
       <c r="N505" s="3" t="s">
-        <v>1454</v>
+        <v>1455</v>
       </c>
       <c r="O505" s="3"/>
       <c r="P505" s="3" t="s">
-        <v>1455</v>
+        <v>1456</v>
       </c>
       <c r="Q505" s="3"/>
       <c r="R505" s="1"/>
@@ -21747,30 +21756,30 @@
     </row>
     <row r="506" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A506" s="2" t="s">
-        <v>1456</v>
+        <v>1457</v>
       </c>
       <c r="B506" s="3" t="s">
-        <v>1457</v>
+        <v>1458</v>
       </c>
       <c r="C506" s="3"/>
       <c r="D506" s="3" t="s">
-        <v>1458</v>
+        <v>1459</v>
       </c>
       <c r="E506" s="3"/>
       <c r="F506" s="3" t="s">
-        <v>1459</v>
+        <v>1460</v>
       </c>
       <c r="G506" s="3"/>
       <c r="H506" s="3" t="s">
-        <v>1460</v>
+        <v>1461</v>
       </c>
       <c r="I506" s="3"/>
       <c r="J506" s="3" t="s">
-        <v>1461</v>
+        <v>1462</v>
       </c>
       <c r="K506" s="3"/>
       <c r="L506" s="3" t="s">
-        <v>1462</v>
+        <v>1463</v>
       </c>
       <c r="M506" s="3"/>
       <c r="N506" s="5"/>
@@ -21789,28 +21798,28 @@
     </row>
     <row r="507" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A507" s="2" t="s">
-        <v>1463</v>
+        <v>1464</v>
       </c>
       <c r="B507" s="4" t="s">
-        <v>1464</v>
+        <v>1465</v>
       </c>
       <c r="C507" s="4" t="s">
-        <v>1465</v>
+        <v>1466</v>
       </c>
       <c r="D507" s="4" t="s">
-        <v>1466</v>
+        <v>1467</v>
       </c>
       <c r="E507" s="4" t="s">
-        <v>1467</v>
+        <v>1468</v>
       </c>
       <c r="F507" s="4" t="s">
-        <v>1468</v>
+        <v>1469</v>
       </c>
       <c r="G507" s="5"/>
       <c r="H507" s="5"/>
       <c r="I507" s="5"/>
       <c r="J507" s="3" t="s">
-        <v>1469</v>
+        <v>1470</v>
       </c>
       <c r="K507" s="3"/>
       <c r="L507" s="5"/>
@@ -21818,10 +21827,10 @@
       <c r="N507" s="5"/>
       <c r="O507" s="5"/>
       <c r="P507" s="4" t="s">
-        <v>1470</v>
+        <v>1471</v>
       </c>
       <c r="Q507" s="4" t="s">
-        <v>1471</v>
+        <v>1472</v>
       </c>
       <c r="R507" s="1"/>
       <c r="S507" s="1"/>
@@ -21835,7 +21844,7 @@
     </row>
     <row r="508" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A508" s="2" t="s">
-        <v>1472</v>
+        <v>1473</v>
       </c>
       <c r="B508" s="5"/>
       <c r="C508" s="5"/>
@@ -21865,7 +21874,7 @@
     </row>
     <row r="509" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A509" s="2" t="s">
-        <v>1473</v>
+        <v>1474</v>
       </c>
       <c r="B509" s="5"/>
       <c r="C509" s="5"/>
@@ -21895,7 +21904,7 @@
     </row>
     <row r="510" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A510" s="2" t="s">
-        <v>1474</v>
+        <v>1475</v>
       </c>
       <c r="B510" s="5"/>
       <c r="C510" s="5"/>
@@ -21925,7 +21934,7 @@
     </row>
     <row r="511" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A511" s="2" t="s">
-        <v>1475</v>
+        <v>1476</v>
       </c>
       <c r="B511" s="5"/>
       <c r="C511" s="5"/>
@@ -21955,7 +21964,7 @@
     </row>
     <row r="512" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A512" s="2" t="s">
-        <v>1476</v>
+        <v>1477</v>
       </c>
       <c r="B512" s="5"/>
       <c r="C512" s="5"/>
@@ -21985,7 +21994,7 @@
     </row>
     <row r="513" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A513" s="2" t="s">
-        <v>1477</v>
+        <v>1478</v>
       </c>
       <c r="B513" s="5"/>
       <c r="C513" s="5"/>
@@ -22015,7 +22024,7 @@
     </row>
     <row r="514" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A514" s="2" t="s">
-        <v>1478</v>
+        <v>1479</v>
       </c>
       <c r="B514" s="5"/>
       <c r="C514" s="5"/>

</xml_diff>

<commit_message>
password wrong attempts stored in eeprom
</commit_message>
<xml_diff>
--- a/docs/UV K5 EEPROM.xlsx
+++ b/docs/UV K5 EEPROM.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1460" uniqueCount="1458">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1461" uniqueCount="1459">
   <si>
     <t xml:space="preserve">00</t>
   </si>
@@ -2126,6 +2126,9 @@
   </si>
   <si>
     <t xml:space="preserve">RX_AGC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PASSWORD_WRONG_ATTEMPTS</t>
   </si>
   <si>
     <t xml:space="preserve">AL-MOD</t>
@@ -4496,7 +4499,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -4526,6 +4529,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -4625,10 +4632,10 @@
   <dimension ref="A1:Z1001"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A214" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="M232" activeCellId="0" sqref="M232"/>
+      <selection pane="topLeft" activeCell="G220" activeCellId="0" sqref="G220"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.71484375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.73046875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1"/>
@@ -12618,23 +12625,25 @@
       <c r="C236" s="4" t="s">
         <v>701</v>
       </c>
-      <c r="D236" s="7"/>
+      <c r="D236" s="8" t="s">
+        <v>702</v>
+      </c>
       <c r="E236" s="7"/>
       <c r="F236" s="7"/>
-      <c r="G236" s="8"/>
+      <c r="G236" s="9"/>
       <c r="H236" s="5"/>
       <c r="I236" s="5"/>
       <c r="J236" s="4" t="s">
-        <v>702</v>
+        <v>703</v>
       </c>
       <c r="K236" s="4" t="s">
-        <v>703</v>
+        <v>704</v>
       </c>
       <c r="L236" s="4" t="s">
-        <v>704</v>
+        <v>705</v>
       </c>
       <c r="M236" s="4" t="s">
-        <v>705</v>
+        <v>706</v>
       </c>
       <c r="N236" s="5"/>
       <c r="O236" s="5"/>
@@ -12652,10 +12661,10 @@
     </row>
     <row r="237" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A237" s="2" t="s">
-        <v>706</v>
+        <v>707</v>
       </c>
       <c r="B237" s="3" t="s">
-        <v>707</v>
+        <v>708</v>
       </c>
       <c r="C237" s="3"/>
       <c r="D237" s="3"/>
@@ -12684,10 +12693,10 @@
     </row>
     <row r="238" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A238" s="2" t="s">
-        <v>708</v>
+        <v>709</v>
       </c>
       <c r="B238" s="3" t="s">
-        <v>709</v>
+        <v>710</v>
       </c>
       <c r="C238" s="3"/>
       <c r="D238" s="3"/>
@@ -12716,40 +12725,40 @@
     </row>
     <row r="239" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A239" s="2" t="s">
-        <v>710</v>
+        <v>711</v>
       </c>
       <c r="B239" s="4" t="s">
-        <v>711</v>
+        <v>712</v>
       </c>
       <c r="C239" s="4" t="s">
-        <v>712</v>
+        <v>713</v>
       </c>
       <c r="D239" s="4" t="s">
-        <v>713</v>
+        <v>714</v>
       </c>
       <c r="E239" s="4" t="s">
-        <v>714</v>
+        <v>715</v>
       </c>
       <c r="F239" s="4" t="s">
-        <v>715</v>
+        <v>716</v>
       </c>
       <c r="G239" s="4" t="s">
-        <v>716</v>
+        <v>717</v>
       </c>
       <c r="H239" s="4" t="s">
-        <v>717</v>
+        <v>718</v>
       </c>
       <c r="I239" s="4" t="s">
-        <v>718</v>
+        <v>719</v>
       </c>
       <c r="J239" s="4" t="s">
-        <v>719</v>
+        <v>720</v>
       </c>
       <c r="K239" s="4" t="s">
-        <v>720</v>
+        <v>721</v>
       </c>
       <c r="L239" s="4" t="s">
-        <v>721</v>
+        <v>722</v>
       </c>
       <c r="M239" s="5"/>
       <c r="N239" s="5"/>
@@ -12768,10 +12777,10 @@
     </row>
     <row r="240" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A240" s="2" t="s">
-        <v>722</v>
+        <v>723</v>
       </c>
       <c r="B240" s="3" t="s">
-        <v>723</v>
+        <v>724</v>
       </c>
       <c r="C240" s="3"/>
       <c r="D240" s="3"/>
@@ -12781,7 +12790,7 @@
       <c r="H240" s="3"/>
       <c r="I240" s="3"/>
       <c r="J240" s="3" t="s">
-        <v>724</v>
+        <v>725</v>
       </c>
       <c r="K240" s="3"/>
       <c r="L240" s="3"/>
@@ -12802,10 +12811,10 @@
     </row>
     <row r="241" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A241" s="2" t="s">
-        <v>725</v>
+        <v>726</v>
       </c>
       <c r="B241" s="3" t="s">
-        <v>726</v>
+        <v>727</v>
       </c>
       <c r="C241" s="3"/>
       <c r="D241" s="3"/>
@@ -12815,7 +12824,7 @@
       <c r="H241" s="3"/>
       <c r="I241" s="3"/>
       <c r="J241" s="3" t="s">
-        <v>727</v>
+        <v>728</v>
       </c>
       <c r="K241" s="3"/>
       <c r="L241" s="3"/>
@@ -12836,10 +12845,10 @@
     </row>
     <row r="242" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A242" s="2" t="s">
+        <v>729</v>
+      </c>
+      <c r="B242" s="3" t="s">
         <v>728</v>
-      </c>
-      <c r="B242" s="3" t="s">
-        <v>727</v>
       </c>
       <c r="C242" s="3"/>
       <c r="D242" s="3"/>
@@ -12849,7 +12858,7 @@
       <c r="H242" s="3"/>
       <c r="I242" s="3"/>
       <c r="J242" s="3" t="s">
-        <v>729</v>
+        <v>730</v>
       </c>
       <c r="K242" s="3"/>
       <c r="L242" s="3"/>
@@ -12870,10 +12879,10 @@
     </row>
     <row r="243" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A243" s="2" t="s">
+        <v>731</v>
+      </c>
+      <c r="B243" s="3" t="s">
         <v>730</v>
-      </c>
-      <c r="B243" s="3" t="s">
-        <v>729</v>
       </c>
       <c r="C243" s="3"/>
       <c r="D243" s="3"/>
@@ -12883,25 +12892,25 @@
       <c r="H243" s="3"/>
       <c r="I243" s="3"/>
       <c r="J243" s="4" t="s">
-        <v>731</v>
+        <v>732</v>
       </c>
       <c r="K243" s="4" t="s">
-        <v>732</v>
+        <v>733</v>
       </c>
       <c r="L243" s="4" t="s">
-        <v>733</v>
+        <v>734</v>
       </c>
       <c r="M243" s="4" t="s">
-        <v>734</v>
+        <v>735</v>
       </c>
       <c r="N243" s="4" t="s">
-        <v>735</v>
+        <v>736</v>
       </c>
       <c r="O243" s="4" t="s">
-        <v>736</v>
+        <v>737</v>
       </c>
       <c r="P243" s="4" t="s">
-        <v>737</v>
+        <v>738</v>
       </c>
       <c r="Q243" s="5"/>
       <c r="R243" s="1"/>
@@ -12916,7 +12925,7 @@
     </row>
     <row r="244" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A244" s="2" t="s">
-        <v>738</v>
+        <v>739</v>
       </c>
       <c r="B244" s="5"/>
       <c r="C244" s="5"/>
@@ -12946,10 +12955,10 @@
     </row>
     <row r="245" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A245" s="2" t="s">
-        <v>739</v>
+        <v>740</v>
       </c>
       <c r="B245" s="3" t="s">
-        <v>740</v>
+        <v>741</v>
       </c>
       <c r="C245" s="3"/>
       <c r="D245" s="3"/>
@@ -12978,28 +12987,28 @@
     </row>
     <row r="246" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A246" s="2" t="s">
-        <v>741</v>
+        <v>742</v>
       </c>
       <c r="B246" s="4" t="s">
-        <v>742</v>
+        <v>743</v>
       </c>
       <c r="C246" s="4" t="s">
-        <v>743</v>
+        <v>744</v>
       </c>
       <c r="D246" s="4" t="s">
-        <v>744</v>
+        <v>745</v>
       </c>
       <c r="E246" s="4" t="s">
-        <v>745</v>
+        <v>746</v>
       </c>
       <c r="F246" s="4" t="s">
-        <v>746</v>
+        <v>747</v>
       </c>
       <c r="G246" s="4" t="s">
-        <v>747</v>
+        <v>748</v>
       </c>
       <c r="H246" s="4" t="s">
-        <v>748</v>
+        <v>749</v>
       </c>
       <c r="I246" s="5"/>
       <c r="J246" s="5"/>
@@ -13022,10 +13031,10 @@
     </row>
     <row r="247" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A247" s="2" t="s">
-        <v>749</v>
+        <v>750</v>
       </c>
       <c r="B247" s="3" t="s">
-        <v>750</v>
+        <v>751</v>
       </c>
       <c r="C247" s="3"/>
       <c r="D247" s="3"/>
@@ -13054,10 +13063,10 @@
     </row>
     <row r="248" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A248" s="2" t="s">
-        <v>751</v>
+        <v>752</v>
       </c>
       <c r="B248" s="3" t="s">
-        <v>752</v>
+        <v>753</v>
       </c>
       <c r="C248" s="3"/>
       <c r="D248" s="3"/>
@@ -13086,10 +13095,10 @@
     </row>
     <row r="249" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A249" s="2" t="s">
-        <v>753</v>
+        <v>754</v>
       </c>
       <c r="B249" s="3" t="s">
-        <v>754</v>
+        <v>755</v>
       </c>
       <c r="C249" s="3"/>
       <c r="D249" s="3"/>
@@ -13118,10 +13127,10 @@
     </row>
     <row r="250" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A250" s="2" t="s">
-        <v>755</v>
+        <v>756</v>
       </c>
       <c r="B250" s="3" t="s">
-        <v>756</v>
+        <v>757</v>
       </c>
       <c r="C250" s="3"/>
       <c r="D250" s="3"/>
@@ -13150,10 +13159,10 @@
     </row>
     <row r="251" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A251" s="2" t="s">
-        <v>757</v>
+        <v>758</v>
       </c>
       <c r="B251" s="3" t="s">
-        <v>758</v>
+        <v>759</v>
       </c>
       <c r="C251" s="3"/>
       <c r="D251" s="3"/>
@@ -13182,10 +13191,10 @@
     </row>
     <row r="252" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A252" s="2" t="s">
-        <v>759</v>
+        <v>760</v>
       </c>
       <c r="B252" s="3" t="s">
-        <v>760</v>
+        <v>761</v>
       </c>
       <c r="C252" s="3"/>
       <c r="D252" s="3"/>
@@ -13214,10 +13223,10 @@
     </row>
     <row r="253" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A253" s="2" t="s">
-        <v>761</v>
+        <v>762</v>
       </c>
       <c r="B253" s="3" t="s">
-        <v>762</v>
+        <v>763</v>
       </c>
       <c r="C253" s="3"/>
       <c r="D253" s="3"/>
@@ -13246,10 +13255,10 @@
     </row>
     <row r="254" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A254" s="2" t="s">
-        <v>763</v>
+        <v>764</v>
       </c>
       <c r="B254" s="3" t="s">
-        <v>764</v>
+        <v>765</v>
       </c>
       <c r="C254" s="3"/>
       <c r="D254" s="3"/>
@@ -13278,10 +13287,10 @@
     </row>
     <row r="255" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A255" s="2" t="s">
-        <v>765</v>
+        <v>766</v>
       </c>
       <c r="B255" s="3" t="s">
-        <v>766</v>
+        <v>767</v>
       </c>
       <c r="C255" s="3"/>
       <c r="D255" s="3"/>
@@ -13310,10 +13319,10 @@
     </row>
     <row r="256" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A256" s="2" t="s">
-        <v>767</v>
+        <v>768</v>
       </c>
       <c r="B256" s="3" t="s">
-        <v>768</v>
+        <v>769</v>
       </c>
       <c r="C256" s="3"/>
       <c r="D256" s="3"/>
@@ -13342,10 +13351,10 @@
     </row>
     <row r="257" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A257" s="2" t="s">
-        <v>769</v>
+        <v>770</v>
       </c>
       <c r="B257" s="3" t="s">
-        <v>770</v>
+        <v>771</v>
       </c>
       <c r="C257" s="3"/>
       <c r="D257" s="3"/>
@@ -13374,10 +13383,10 @@
     </row>
     <row r="258" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A258" s="2" t="s">
-        <v>771</v>
+        <v>772</v>
       </c>
       <c r="B258" s="3" t="s">
-        <v>772</v>
+        <v>773</v>
       </c>
       <c r="C258" s="3"/>
       <c r="D258" s="3"/>
@@ -13406,10 +13415,10 @@
     </row>
     <row r="259" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A259" s="2" t="s">
-        <v>773</v>
+        <v>774</v>
       </c>
       <c r="B259" s="3" t="s">
-        <v>774</v>
+        <v>775</v>
       </c>
       <c r="C259" s="3"/>
       <c r="D259" s="3"/>
@@ -13438,10 +13447,10 @@
     </row>
     <row r="260" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A260" s="2" t="s">
-        <v>775</v>
+        <v>776</v>
       </c>
       <c r="B260" s="3" t="s">
-        <v>776</v>
+        <v>777</v>
       </c>
       <c r="C260" s="3"/>
       <c r="D260" s="3"/>
@@ -13470,10 +13479,10 @@
     </row>
     <row r="261" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A261" s="2" t="s">
-        <v>777</v>
+        <v>778</v>
       </c>
       <c r="B261" s="3" t="s">
-        <v>778</v>
+        <v>779</v>
       </c>
       <c r="C261" s="3"/>
       <c r="D261" s="3"/>
@@ -13502,10 +13511,10 @@
     </row>
     <row r="262" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A262" s="2" t="s">
-        <v>779</v>
+        <v>780</v>
       </c>
       <c r="B262" s="3" t="s">
-        <v>780</v>
+        <v>781</v>
       </c>
       <c r="C262" s="3"/>
       <c r="D262" s="3"/>
@@ -13534,10 +13543,10 @@
     </row>
     <row r="263" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A263" s="2" t="s">
-        <v>781</v>
+        <v>782</v>
       </c>
       <c r="B263" s="3" t="s">
-        <v>782</v>
+        <v>783</v>
       </c>
       <c r="C263" s="3"/>
       <c r="D263" s="3"/>
@@ -13566,10 +13575,10 @@
     </row>
     <row r="264" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A264" s="2" t="s">
-        <v>783</v>
+        <v>784</v>
       </c>
       <c r="B264" s="3" t="s">
-        <v>784</v>
+        <v>785</v>
       </c>
       <c r="C264" s="3"/>
       <c r="D264" s="3"/>
@@ -13598,10 +13607,10 @@
     </row>
     <row r="265" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A265" s="2" t="s">
-        <v>785</v>
+        <v>786</v>
       </c>
       <c r="B265" s="3" t="s">
-        <v>786</v>
+        <v>787</v>
       </c>
       <c r="C265" s="3"/>
       <c r="D265" s="3"/>
@@ -13630,10 +13639,10 @@
     </row>
     <row r="266" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A266" s="2" t="s">
-        <v>787</v>
+        <v>788</v>
       </c>
       <c r="B266" s="3" t="s">
-        <v>788</v>
+        <v>789</v>
       </c>
       <c r="C266" s="3"/>
       <c r="D266" s="3"/>
@@ -13662,10 +13671,10 @@
     </row>
     <row r="267" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A267" s="2" t="s">
-        <v>789</v>
+        <v>790</v>
       </c>
       <c r="B267" s="3" t="s">
-        <v>790</v>
+        <v>791</v>
       </c>
       <c r="C267" s="3"/>
       <c r="D267" s="3"/>
@@ -13694,10 +13703,10 @@
     </row>
     <row r="268" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A268" s="2" t="s">
-        <v>791</v>
+        <v>792</v>
       </c>
       <c r="B268" s="3" t="s">
-        <v>792</v>
+        <v>793</v>
       </c>
       <c r="C268" s="3"/>
       <c r="D268" s="3"/>
@@ -13726,10 +13735,10 @@
     </row>
     <row r="269" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A269" s="2" t="s">
-        <v>793</v>
+        <v>794</v>
       </c>
       <c r="B269" s="3" t="s">
-        <v>794</v>
+        <v>795</v>
       </c>
       <c r="C269" s="3"/>
       <c r="D269" s="3"/>
@@ -13758,10 +13767,10 @@
     </row>
     <row r="270" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A270" s="2" t="s">
-        <v>795</v>
+        <v>796</v>
       </c>
       <c r="B270" s="3" t="s">
-        <v>796</v>
+        <v>797</v>
       </c>
       <c r="C270" s="3"/>
       <c r="D270" s="3"/>
@@ -13790,10 +13799,10 @@
     </row>
     <row r="271" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A271" s="2" t="s">
-        <v>797</v>
+        <v>798</v>
       </c>
       <c r="B271" s="3" t="s">
-        <v>798</v>
+        <v>799</v>
       </c>
       <c r="C271" s="3"/>
       <c r="D271" s="3"/>
@@ -13822,10 +13831,10 @@
     </row>
     <row r="272" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A272" s="2" t="s">
-        <v>799</v>
+        <v>800</v>
       </c>
       <c r="B272" s="3" t="s">
-        <v>800</v>
+        <v>801</v>
       </c>
       <c r="C272" s="3"/>
       <c r="D272" s="3"/>
@@ -13854,10 +13863,10 @@
     </row>
     <row r="273" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A273" s="2" t="s">
-        <v>801</v>
+        <v>802</v>
       </c>
       <c r="B273" s="3" t="s">
-        <v>802</v>
+        <v>803</v>
       </c>
       <c r="C273" s="3"/>
       <c r="D273" s="3"/>
@@ -13886,10 +13895,10 @@
     </row>
     <row r="274" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A274" s="2" t="s">
-        <v>803</v>
+        <v>804</v>
       </c>
       <c r="B274" s="3" t="s">
-        <v>804</v>
+        <v>805</v>
       </c>
       <c r="C274" s="3"/>
       <c r="D274" s="3"/>
@@ -13918,10 +13927,10 @@
     </row>
     <row r="275" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A275" s="2" t="s">
-        <v>805</v>
+        <v>806</v>
       </c>
       <c r="B275" s="3" t="s">
-        <v>806</v>
+        <v>807</v>
       </c>
       <c r="C275" s="3"/>
       <c r="D275" s="3"/>
@@ -13950,10 +13959,10 @@
     </row>
     <row r="276" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A276" s="2" t="s">
-        <v>807</v>
+        <v>808</v>
       </c>
       <c r="B276" s="3" t="s">
-        <v>808</v>
+        <v>809</v>
       </c>
       <c r="C276" s="3"/>
       <c r="D276" s="3"/>
@@ -13982,10 +13991,10 @@
     </row>
     <row r="277" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A277" s="2" t="s">
-        <v>809</v>
+        <v>810</v>
       </c>
       <c r="B277" s="3" t="s">
-        <v>810</v>
+        <v>811</v>
       </c>
       <c r="C277" s="3"/>
       <c r="D277" s="3"/>
@@ -14014,10 +14023,10 @@
     </row>
     <row r="278" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A278" s="2" t="s">
-        <v>811</v>
+        <v>812</v>
       </c>
       <c r="B278" s="3" t="s">
-        <v>812</v>
+        <v>813</v>
       </c>
       <c r="C278" s="3"/>
       <c r="D278" s="3"/>
@@ -14046,10 +14055,10 @@
     </row>
     <row r="279" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A279" s="2" t="s">
-        <v>813</v>
+        <v>814</v>
       </c>
       <c r="B279" s="3" t="s">
-        <v>814</v>
+        <v>815</v>
       </c>
       <c r="C279" s="3"/>
       <c r="D279" s="3"/>
@@ -14078,10 +14087,10 @@
     </row>
     <row r="280" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A280" s="2" t="s">
-        <v>815</v>
+        <v>816</v>
       </c>
       <c r="B280" s="3" t="s">
-        <v>816</v>
+        <v>817</v>
       </c>
       <c r="C280" s="3"/>
       <c r="D280" s="3"/>
@@ -14110,10 +14119,10 @@
     </row>
     <row r="281" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A281" s="2" t="s">
-        <v>817</v>
+        <v>818</v>
       </c>
       <c r="B281" s="3" t="s">
-        <v>818</v>
+        <v>819</v>
       </c>
       <c r="C281" s="3"/>
       <c r="D281" s="3"/>
@@ -14142,10 +14151,10 @@
     </row>
     <row r="282" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A282" s="2" t="s">
-        <v>819</v>
+        <v>820</v>
       </c>
       <c r="B282" s="3" t="s">
-        <v>820</v>
+        <v>821</v>
       </c>
       <c r="C282" s="3"/>
       <c r="D282" s="3"/>
@@ -14174,10 +14183,10 @@
     </row>
     <row r="283" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A283" s="2" t="s">
-        <v>821</v>
+        <v>822</v>
       </c>
       <c r="B283" s="3" t="s">
-        <v>822</v>
+        <v>823</v>
       </c>
       <c r="C283" s="3"/>
       <c r="D283" s="3"/>
@@ -14206,10 +14215,10 @@
     </row>
     <row r="284" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A284" s="2" t="s">
-        <v>823</v>
+        <v>824</v>
       </c>
       <c r="B284" s="3" t="s">
-        <v>824</v>
+        <v>825</v>
       </c>
       <c r="C284" s="3"/>
       <c r="D284" s="3"/>
@@ -14238,10 +14247,10 @@
     </row>
     <row r="285" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A285" s="2" t="s">
-        <v>825</v>
+        <v>826</v>
       </c>
       <c r="B285" s="3" t="s">
-        <v>826</v>
+        <v>827</v>
       </c>
       <c r="C285" s="3"/>
       <c r="D285" s="3"/>
@@ -14270,10 +14279,10 @@
     </row>
     <row r="286" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A286" s="2" t="s">
-        <v>827</v>
+        <v>828</v>
       </c>
       <c r="B286" s="3" t="s">
-        <v>828</v>
+        <v>829</v>
       </c>
       <c r="C286" s="3"/>
       <c r="D286" s="3"/>
@@ -14302,10 +14311,10 @@
     </row>
     <row r="287" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A287" s="2" t="s">
-        <v>829</v>
+        <v>830</v>
       </c>
       <c r="B287" s="3" t="s">
-        <v>830</v>
+        <v>831</v>
       </c>
       <c r="C287" s="3"/>
       <c r="D287" s="3"/>
@@ -14334,10 +14343,10 @@
     </row>
     <row r="288" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A288" s="2" t="s">
-        <v>831</v>
+        <v>832</v>
       </c>
       <c r="B288" s="3" t="s">
-        <v>832</v>
+        <v>833</v>
       </c>
       <c r="C288" s="3"/>
       <c r="D288" s="3"/>
@@ -14366,10 +14375,10 @@
     </row>
     <row r="289" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A289" s="2" t="s">
-        <v>833</v>
+        <v>834</v>
       </c>
       <c r="B289" s="3" t="s">
-        <v>834</v>
+        <v>835</v>
       </c>
       <c r="C289" s="3"/>
       <c r="D289" s="3"/>
@@ -14398,10 +14407,10 @@
     </row>
     <row r="290" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A290" s="2" t="s">
-        <v>835</v>
+        <v>836</v>
       </c>
       <c r="B290" s="3" t="s">
-        <v>836</v>
+        <v>837</v>
       </c>
       <c r="C290" s="3"/>
       <c r="D290" s="3"/>
@@ -14430,10 +14439,10 @@
     </row>
     <row r="291" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A291" s="2" t="s">
-        <v>837</v>
+        <v>838</v>
       </c>
       <c r="B291" s="3" t="s">
-        <v>838</v>
+        <v>839</v>
       </c>
       <c r="C291" s="3"/>
       <c r="D291" s="3"/>
@@ -14462,10 +14471,10 @@
     </row>
     <row r="292" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A292" s="2" t="s">
-        <v>839</v>
+        <v>840</v>
       </c>
       <c r="B292" s="3" t="s">
-        <v>840</v>
+        <v>841</v>
       </c>
       <c r="C292" s="3"/>
       <c r="D292" s="3"/>
@@ -14494,10 +14503,10 @@
     </row>
     <row r="293" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A293" s="2" t="s">
-        <v>841</v>
+        <v>842</v>
       </c>
       <c r="B293" s="3" t="s">
-        <v>842</v>
+        <v>843</v>
       </c>
       <c r="C293" s="3"/>
       <c r="D293" s="3"/>
@@ -14526,10 +14535,10 @@
     </row>
     <row r="294" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A294" s="2" t="s">
-        <v>843</v>
+        <v>844</v>
       </c>
       <c r="B294" s="3" t="s">
-        <v>844</v>
+        <v>845</v>
       </c>
       <c r="C294" s="3"/>
       <c r="D294" s="3"/>
@@ -14558,10 +14567,10 @@
     </row>
     <row r="295" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A295" s="2" t="s">
-        <v>845</v>
+        <v>846</v>
       </c>
       <c r="B295" s="3" t="s">
-        <v>846</v>
+        <v>847</v>
       </c>
       <c r="C295" s="3"/>
       <c r="D295" s="3"/>
@@ -14590,10 +14599,10 @@
     </row>
     <row r="296" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A296" s="2" t="s">
-        <v>847</v>
+        <v>848</v>
       </c>
       <c r="B296" s="3" t="s">
-        <v>848</v>
+        <v>849</v>
       </c>
       <c r="C296" s="3"/>
       <c r="D296" s="3"/>
@@ -14622,10 +14631,10 @@
     </row>
     <row r="297" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A297" s="2" t="s">
-        <v>849</v>
+        <v>850</v>
       </c>
       <c r="B297" s="3" t="s">
-        <v>850</v>
+        <v>851</v>
       </c>
       <c r="C297" s="3"/>
       <c r="D297" s="3"/>
@@ -14654,10 +14663,10 @@
     </row>
     <row r="298" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A298" s="2" t="s">
-        <v>851</v>
+        <v>852</v>
       </c>
       <c r="B298" s="3" t="s">
-        <v>852</v>
+        <v>853</v>
       </c>
       <c r="C298" s="3"/>
       <c r="D298" s="3"/>
@@ -14686,10 +14695,10 @@
     </row>
     <row r="299" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A299" s="2" t="s">
-        <v>853</v>
+        <v>854</v>
       </c>
       <c r="B299" s="3" t="s">
-        <v>854</v>
+        <v>855</v>
       </c>
       <c r="C299" s="3"/>
       <c r="D299" s="3"/>
@@ -14718,10 +14727,10 @@
     </row>
     <row r="300" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A300" s="2" t="s">
-        <v>855</v>
+        <v>856</v>
       </c>
       <c r="B300" s="3" t="s">
-        <v>856</v>
+        <v>857</v>
       </c>
       <c r="C300" s="3"/>
       <c r="D300" s="3"/>
@@ -14750,10 +14759,10 @@
     </row>
     <row r="301" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A301" s="2" t="s">
-        <v>857</v>
+        <v>858</v>
       </c>
       <c r="B301" s="3" t="s">
-        <v>858</v>
+        <v>859</v>
       </c>
       <c r="C301" s="3"/>
       <c r="D301" s="3"/>
@@ -14782,10 +14791,10 @@
     </row>
     <row r="302" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A302" s="2" t="s">
-        <v>859</v>
+        <v>860</v>
       </c>
       <c r="B302" s="3" t="s">
-        <v>860</v>
+        <v>861</v>
       </c>
       <c r="C302" s="3"/>
       <c r="D302" s="3"/>
@@ -14814,10 +14823,10 @@
     </row>
     <row r="303" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A303" s="2" t="s">
-        <v>861</v>
+        <v>862</v>
       </c>
       <c r="B303" s="3" t="s">
-        <v>862</v>
+        <v>863</v>
       </c>
       <c r="C303" s="3"/>
       <c r="D303" s="3"/>
@@ -14846,10 +14855,10 @@
     </row>
     <row r="304" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A304" s="2" t="s">
-        <v>863</v>
+        <v>864</v>
       </c>
       <c r="B304" s="3" t="s">
-        <v>864</v>
+        <v>865</v>
       </c>
       <c r="C304" s="3"/>
       <c r="D304" s="3"/>
@@ -14878,10 +14887,10 @@
     </row>
     <row r="305" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A305" s="2" t="s">
-        <v>865</v>
+        <v>866</v>
       </c>
       <c r="B305" s="3" t="s">
-        <v>866</v>
+        <v>867</v>
       </c>
       <c r="C305" s="3"/>
       <c r="D305" s="3"/>
@@ -14910,10 +14919,10 @@
     </row>
     <row r="306" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A306" s="2" t="s">
-        <v>867</v>
+        <v>868</v>
       </c>
       <c r="B306" s="3" t="s">
-        <v>868</v>
+        <v>869</v>
       </c>
       <c r="C306" s="3"/>
       <c r="D306" s="3"/>
@@ -14942,10 +14951,10 @@
     </row>
     <row r="307" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A307" s="2" t="s">
-        <v>869</v>
+        <v>870</v>
       </c>
       <c r="B307" s="3" t="s">
-        <v>870</v>
+        <v>871</v>
       </c>
       <c r="C307" s="3"/>
       <c r="D307" s="3"/>
@@ -14974,10 +14983,10 @@
     </row>
     <row r="308" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A308" s="2" t="s">
-        <v>871</v>
+        <v>872</v>
       </c>
       <c r="B308" s="3" t="s">
-        <v>872</v>
+        <v>873</v>
       </c>
       <c r="C308" s="3"/>
       <c r="D308" s="3"/>
@@ -15006,10 +15015,10 @@
     </row>
     <row r="309" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A309" s="2" t="s">
-        <v>873</v>
+        <v>874</v>
       </c>
       <c r="B309" s="3" t="s">
-        <v>874</v>
+        <v>875</v>
       </c>
       <c r="C309" s="3"/>
       <c r="D309" s="3"/>
@@ -15038,10 +15047,10 @@
     </row>
     <row r="310" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A310" s="2" t="s">
-        <v>875</v>
+        <v>876</v>
       </c>
       <c r="B310" s="3" t="s">
-        <v>876</v>
+        <v>877</v>
       </c>
       <c r="C310" s="3"/>
       <c r="D310" s="3"/>
@@ -15070,10 +15079,10 @@
     </row>
     <row r="311" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A311" s="2" t="s">
-        <v>877</v>
+        <v>878</v>
       </c>
       <c r="B311" s="3" t="s">
-        <v>878</v>
+        <v>879</v>
       </c>
       <c r="C311" s="3"/>
       <c r="D311" s="3"/>
@@ -15102,10 +15111,10 @@
     </row>
     <row r="312" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A312" s="2" t="s">
-        <v>879</v>
+        <v>880</v>
       </c>
       <c r="B312" s="3" t="s">
-        <v>880</v>
+        <v>881</v>
       </c>
       <c r="C312" s="3"/>
       <c r="D312" s="3"/>
@@ -15134,10 +15143,10 @@
     </row>
     <row r="313" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A313" s="2" t="s">
-        <v>881</v>
+        <v>882</v>
       </c>
       <c r="B313" s="3" t="s">
-        <v>882</v>
+        <v>883</v>
       </c>
       <c r="C313" s="3"/>
       <c r="D313" s="3"/>
@@ -15166,10 +15175,10 @@
     </row>
     <row r="314" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A314" s="2" t="s">
-        <v>883</v>
+        <v>884</v>
       </c>
       <c r="B314" s="3" t="s">
-        <v>884</v>
+        <v>885</v>
       </c>
       <c r="C314" s="3"/>
       <c r="D314" s="3"/>
@@ -15198,10 +15207,10 @@
     </row>
     <row r="315" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A315" s="2" t="s">
-        <v>885</v>
+        <v>886</v>
       </c>
       <c r="B315" s="3" t="s">
-        <v>886</v>
+        <v>887</v>
       </c>
       <c r="C315" s="3"/>
       <c r="D315" s="3"/>
@@ -15230,10 +15239,10 @@
     </row>
     <row r="316" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A316" s="2" t="s">
-        <v>887</v>
+        <v>888</v>
       </c>
       <c r="B316" s="3" t="s">
-        <v>888</v>
+        <v>889</v>
       </c>
       <c r="C316" s="3"/>
       <c r="D316" s="3"/>
@@ -15262,10 +15271,10 @@
     </row>
     <row r="317" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A317" s="2" t="s">
-        <v>889</v>
+        <v>890</v>
       </c>
       <c r="B317" s="3" t="s">
-        <v>890</v>
+        <v>891</v>
       </c>
       <c r="C317" s="3"/>
       <c r="D317" s="3"/>
@@ -15294,10 +15303,10 @@
     </row>
     <row r="318" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A318" s="2" t="s">
-        <v>891</v>
+        <v>892</v>
       </c>
       <c r="B318" s="3" t="s">
-        <v>892</v>
+        <v>893</v>
       </c>
       <c r="C318" s="3"/>
       <c r="D318" s="3"/>
@@ -15326,10 +15335,10 @@
     </row>
     <row r="319" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A319" s="2" t="s">
-        <v>893</v>
+        <v>894</v>
       </c>
       <c r="B319" s="3" t="s">
-        <v>894</v>
+        <v>895</v>
       </c>
       <c r="C319" s="3"/>
       <c r="D319" s="3"/>
@@ -15358,10 +15367,10 @@
     </row>
     <row r="320" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A320" s="2" t="s">
-        <v>895</v>
+        <v>896</v>
       </c>
       <c r="B320" s="3" t="s">
-        <v>896</v>
+        <v>897</v>
       </c>
       <c r="C320" s="3"/>
       <c r="D320" s="3"/>
@@ -15390,10 +15399,10 @@
     </row>
     <row r="321" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A321" s="2" t="s">
-        <v>897</v>
+        <v>898</v>
       </c>
       <c r="B321" s="3" t="s">
-        <v>898</v>
+        <v>899</v>
       </c>
       <c r="C321" s="3"/>
       <c r="D321" s="3"/>
@@ -15422,10 +15431,10 @@
     </row>
     <row r="322" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A322" s="2" t="s">
-        <v>899</v>
+        <v>900</v>
       </c>
       <c r="B322" s="3" t="s">
-        <v>900</v>
+        <v>901</v>
       </c>
       <c r="C322" s="3"/>
       <c r="D322" s="3"/>
@@ -15454,10 +15463,10 @@
     </row>
     <row r="323" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A323" s="2" t="s">
-        <v>901</v>
+        <v>902</v>
       </c>
       <c r="B323" s="3" t="s">
-        <v>902</v>
+        <v>903</v>
       </c>
       <c r="C323" s="3"/>
       <c r="D323" s="3"/>
@@ -15486,10 +15495,10 @@
     </row>
     <row r="324" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A324" s="2" t="s">
-        <v>903</v>
+        <v>904</v>
       </c>
       <c r="B324" s="3" t="s">
-        <v>904</v>
+        <v>905</v>
       </c>
       <c r="C324" s="3"/>
       <c r="D324" s="3"/>
@@ -15518,10 +15527,10 @@
     </row>
     <row r="325" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A325" s="2" t="s">
-        <v>905</v>
+        <v>906</v>
       </c>
       <c r="B325" s="3" t="s">
-        <v>906</v>
+        <v>907</v>
       </c>
       <c r="C325" s="3"/>
       <c r="D325" s="3"/>
@@ -15550,10 +15559,10 @@
     </row>
     <row r="326" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A326" s="2" t="s">
-        <v>907</v>
+        <v>908</v>
       </c>
       <c r="B326" s="3" t="s">
-        <v>908</v>
+        <v>909</v>
       </c>
       <c r="C326" s="3"/>
       <c r="D326" s="3"/>
@@ -15582,10 +15591,10 @@
     </row>
     <row r="327" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A327" s="2" t="s">
-        <v>909</v>
+        <v>910</v>
       </c>
       <c r="B327" s="3" t="s">
-        <v>910</v>
+        <v>911</v>
       </c>
       <c r="C327" s="3"/>
       <c r="D327" s="3"/>
@@ -15614,10 +15623,10 @@
     </row>
     <row r="328" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A328" s="2" t="s">
-        <v>911</v>
+        <v>912</v>
       </c>
       <c r="B328" s="3" t="s">
-        <v>912</v>
+        <v>913</v>
       </c>
       <c r="C328" s="3"/>
       <c r="D328" s="3"/>
@@ -15646,10 +15655,10 @@
     </row>
     <row r="329" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A329" s="2" t="s">
-        <v>913</v>
+        <v>914</v>
       </c>
       <c r="B329" s="3" t="s">
-        <v>914</v>
+        <v>915</v>
       </c>
       <c r="C329" s="3"/>
       <c r="D329" s="3"/>
@@ -15678,10 +15687,10 @@
     </row>
     <row r="330" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A330" s="2" t="s">
-        <v>915</v>
+        <v>916</v>
       </c>
       <c r="B330" s="3" t="s">
-        <v>916</v>
+        <v>917</v>
       </c>
       <c r="C330" s="3"/>
       <c r="D330" s="3"/>
@@ -15710,10 +15719,10 @@
     </row>
     <row r="331" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A331" s="2" t="s">
-        <v>917</v>
+        <v>918</v>
       </c>
       <c r="B331" s="3" t="s">
-        <v>918</v>
+        <v>919</v>
       </c>
       <c r="C331" s="3"/>
       <c r="D331" s="3"/>
@@ -15742,10 +15751,10 @@
     </row>
     <row r="332" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A332" s="2" t="s">
-        <v>919</v>
+        <v>920</v>
       </c>
       <c r="B332" s="3" t="s">
-        <v>920</v>
+        <v>921</v>
       </c>
       <c r="C332" s="3"/>
       <c r="D332" s="3"/>
@@ -15774,10 +15783,10 @@
     </row>
     <row r="333" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A333" s="2" t="s">
-        <v>921</v>
+        <v>922</v>
       </c>
       <c r="B333" s="3" t="s">
-        <v>922</v>
+        <v>923</v>
       </c>
       <c r="C333" s="3"/>
       <c r="D333" s="3"/>
@@ -15806,10 +15815,10 @@
     </row>
     <row r="334" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A334" s="2" t="s">
-        <v>923</v>
+        <v>924</v>
       </c>
       <c r="B334" s="3" t="s">
-        <v>924</v>
+        <v>925</v>
       </c>
       <c r="C334" s="3"/>
       <c r="D334" s="3"/>
@@ -15838,10 +15847,10 @@
     </row>
     <row r="335" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A335" s="2" t="s">
-        <v>925</v>
+        <v>926</v>
       </c>
       <c r="B335" s="3" t="s">
-        <v>926</v>
+        <v>927</v>
       </c>
       <c r="C335" s="3"/>
       <c r="D335" s="3"/>
@@ -15870,10 +15879,10 @@
     </row>
     <row r="336" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A336" s="2" t="s">
-        <v>927</v>
+        <v>928</v>
       </c>
       <c r="B336" s="3" t="s">
-        <v>928</v>
+        <v>929</v>
       </c>
       <c r="C336" s="3"/>
       <c r="D336" s="3"/>
@@ -15902,10 +15911,10 @@
     </row>
     <row r="337" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A337" s="2" t="s">
-        <v>929</v>
+        <v>930</v>
       </c>
       <c r="B337" s="3" t="s">
-        <v>930</v>
+        <v>931</v>
       </c>
       <c r="C337" s="3"/>
       <c r="D337" s="3"/>
@@ -15934,10 +15943,10 @@
     </row>
     <row r="338" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A338" s="2" t="s">
-        <v>931</v>
+        <v>932</v>
       </c>
       <c r="B338" s="3" t="s">
-        <v>932</v>
+        <v>933</v>
       </c>
       <c r="C338" s="3"/>
       <c r="D338" s="3"/>
@@ -15966,10 +15975,10 @@
     </row>
     <row r="339" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A339" s="2" t="s">
-        <v>933</v>
+        <v>934</v>
       </c>
       <c r="B339" s="3" t="s">
-        <v>934</v>
+        <v>935</v>
       </c>
       <c r="C339" s="3"/>
       <c r="D339" s="3"/>
@@ -15998,10 +16007,10 @@
     </row>
     <row r="340" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A340" s="2" t="s">
-        <v>935</v>
+        <v>936</v>
       </c>
       <c r="B340" s="3" t="s">
-        <v>936</v>
+        <v>937</v>
       </c>
       <c r="C340" s="3"/>
       <c r="D340" s="3"/>
@@ -16030,10 +16039,10 @@
     </row>
     <row r="341" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A341" s="2" t="s">
-        <v>937</v>
+        <v>938</v>
       </c>
       <c r="B341" s="3" t="s">
-        <v>938</v>
+        <v>939</v>
       </c>
       <c r="C341" s="3"/>
       <c r="D341" s="3"/>
@@ -16062,10 +16071,10 @@
     </row>
     <row r="342" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A342" s="2" t="s">
-        <v>939</v>
+        <v>940</v>
       </c>
       <c r="B342" s="3" t="s">
-        <v>940</v>
+        <v>941</v>
       </c>
       <c r="C342" s="3"/>
       <c r="D342" s="3"/>
@@ -16094,10 +16103,10 @@
     </row>
     <row r="343" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A343" s="2" t="s">
-        <v>941</v>
+        <v>942</v>
       </c>
       <c r="B343" s="3" t="s">
-        <v>942</v>
+        <v>943</v>
       </c>
       <c r="C343" s="3"/>
       <c r="D343" s="3"/>
@@ -16126,10 +16135,10 @@
     </row>
     <row r="344" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A344" s="2" t="s">
-        <v>943</v>
+        <v>944</v>
       </c>
       <c r="B344" s="3" t="s">
-        <v>944</v>
+        <v>945</v>
       </c>
       <c r="C344" s="3"/>
       <c r="D344" s="3"/>
@@ -16158,10 +16167,10 @@
     </row>
     <row r="345" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A345" s="2" t="s">
-        <v>945</v>
+        <v>946</v>
       </c>
       <c r="B345" s="3" t="s">
-        <v>946</v>
+        <v>947</v>
       </c>
       <c r="C345" s="3"/>
       <c r="D345" s="3"/>
@@ -16190,10 +16199,10 @@
     </row>
     <row r="346" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A346" s="2" t="s">
-        <v>947</v>
+        <v>948</v>
       </c>
       <c r="B346" s="3" t="s">
-        <v>948</v>
+        <v>949</v>
       </c>
       <c r="C346" s="3"/>
       <c r="D346" s="3"/>
@@ -16222,10 +16231,10 @@
     </row>
     <row r="347" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A347" s="2" t="s">
-        <v>949</v>
+        <v>950</v>
       </c>
       <c r="B347" s="3" t="s">
-        <v>950</v>
+        <v>951</v>
       </c>
       <c r="C347" s="3"/>
       <c r="D347" s="3"/>
@@ -16254,10 +16263,10 @@
     </row>
     <row r="348" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A348" s="2" t="s">
-        <v>951</v>
+        <v>952</v>
       </c>
       <c r="B348" s="3" t="s">
-        <v>952</v>
+        <v>953</v>
       </c>
       <c r="C348" s="3"/>
       <c r="D348" s="3"/>
@@ -16286,10 +16295,10 @@
     </row>
     <row r="349" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A349" s="2" t="s">
-        <v>953</v>
+        <v>954</v>
       </c>
       <c r="B349" s="3" t="s">
-        <v>954</v>
+        <v>955</v>
       </c>
       <c r="C349" s="3"/>
       <c r="D349" s="3"/>
@@ -16318,10 +16327,10 @@
     </row>
     <row r="350" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A350" s="2" t="s">
-        <v>955</v>
+        <v>956</v>
       </c>
       <c r="B350" s="3" t="s">
-        <v>956</v>
+        <v>957</v>
       </c>
       <c r="C350" s="3"/>
       <c r="D350" s="3"/>
@@ -16350,10 +16359,10 @@
     </row>
     <row r="351" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A351" s="2" t="s">
-        <v>957</v>
+        <v>958</v>
       </c>
       <c r="B351" s="3" t="s">
-        <v>958</v>
+        <v>959</v>
       </c>
       <c r="C351" s="3"/>
       <c r="D351" s="3"/>
@@ -16382,10 +16391,10 @@
     </row>
     <row r="352" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A352" s="2" t="s">
-        <v>959</v>
+        <v>960</v>
       </c>
       <c r="B352" s="3" t="s">
-        <v>960</v>
+        <v>961</v>
       </c>
       <c r="C352" s="3"/>
       <c r="D352" s="3"/>
@@ -16414,10 +16423,10 @@
     </row>
     <row r="353" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A353" s="2" t="s">
-        <v>961</v>
+        <v>962</v>
       </c>
       <c r="B353" s="3" t="s">
-        <v>962</v>
+        <v>963</v>
       </c>
       <c r="C353" s="3"/>
       <c r="D353" s="3"/>
@@ -16446,10 +16455,10 @@
     </row>
     <row r="354" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A354" s="2" t="s">
-        <v>963</v>
+        <v>964</v>
       </c>
       <c r="B354" s="3" t="s">
-        <v>964</v>
+        <v>965</v>
       </c>
       <c r="C354" s="3"/>
       <c r="D354" s="3"/>
@@ -16478,10 +16487,10 @@
     </row>
     <row r="355" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A355" s="2" t="s">
-        <v>965</v>
+        <v>966</v>
       </c>
       <c r="B355" s="3" t="s">
-        <v>966</v>
+        <v>967</v>
       </c>
       <c r="C355" s="3"/>
       <c r="D355" s="3"/>
@@ -16510,10 +16519,10 @@
     </row>
     <row r="356" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A356" s="2" t="s">
-        <v>967</v>
+        <v>968</v>
       </c>
       <c r="B356" s="3" t="s">
-        <v>968</v>
+        <v>969</v>
       </c>
       <c r="C356" s="3"/>
       <c r="D356" s="3"/>
@@ -16542,10 +16551,10 @@
     </row>
     <row r="357" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A357" s="2" t="s">
-        <v>969</v>
+        <v>970</v>
       </c>
       <c r="B357" s="3" t="s">
-        <v>970</v>
+        <v>971</v>
       </c>
       <c r="C357" s="3"/>
       <c r="D357" s="3"/>
@@ -16574,10 +16583,10 @@
     </row>
     <row r="358" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A358" s="2" t="s">
-        <v>971</v>
+        <v>972</v>
       </c>
       <c r="B358" s="3" t="s">
-        <v>972</v>
+        <v>973</v>
       </c>
       <c r="C358" s="3"/>
       <c r="D358" s="3"/>
@@ -16606,10 +16615,10 @@
     </row>
     <row r="359" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A359" s="2" t="s">
-        <v>973</v>
+        <v>974</v>
       </c>
       <c r="B359" s="3" t="s">
-        <v>974</v>
+        <v>975</v>
       </c>
       <c r="C359" s="3"/>
       <c r="D359" s="3"/>
@@ -16638,10 +16647,10 @@
     </row>
     <row r="360" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A360" s="2" t="s">
-        <v>975</v>
+        <v>976</v>
       </c>
       <c r="B360" s="3" t="s">
-        <v>976</v>
+        <v>977</v>
       </c>
       <c r="C360" s="3"/>
       <c r="D360" s="3"/>
@@ -16670,10 +16679,10 @@
     </row>
     <row r="361" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A361" s="2" t="s">
-        <v>977</v>
+        <v>978</v>
       </c>
       <c r="B361" s="3" t="s">
-        <v>978</v>
+        <v>979</v>
       </c>
       <c r="C361" s="3"/>
       <c r="D361" s="3"/>
@@ -16702,10 +16711,10 @@
     </row>
     <row r="362" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A362" s="2" t="s">
-        <v>979</v>
+        <v>980</v>
       </c>
       <c r="B362" s="3" t="s">
-        <v>980</v>
+        <v>981</v>
       </c>
       <c r="C362" s="3"/>
       <c r="D362" s="3"/>
@@ -16734,10 +16743,10 @@
     </row>
     <row r="363" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A363" s="2" t="s">
-        <v>981</v>
+        <v>982</v>
       </c>
       <c r="B363" s="3" t="s">
-        <v>982</v>
+        <v>983</v>
       </c>
       <c r="C363" s="3"/>
       <c r="D363" s="3"/>
@@ -16766,10 +16775,10 @@
     </row>
     <row r="364" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A364" s="2" t="s">
-        <v>983</v>
+        <v>984</v>
       </c>
       <c r="B364" s="3" t="s">
-        <v>984</v>
+        <v>985</v>
       </c>
       <c r="C364" s="3"/>
       <c r="D364" s="3"/>
@@ -16798,10 +16807,10 @@
     </row>
     <row r="365" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A365" s="2" t="s">
-        <v>985</v>
+        <v>986</v>
       </c>
       <c r="B365" s="3" t="s">
-        <v>986</v>
+        <v>987</v>
       </c>
       <c r="C365" s="3"/>
       <c r="D365" s="3"/>
@@ -16830,10 +16839,10 @@
     </row>
     <row r="366" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A366" s="2" t="s">
-        <v>987</v>
+        <v>988</v>
       </c>
       <c r="B366" s="3" t="s">
-        <v>988</v>
+        <v>989</v>
       </c>
       <c r="C366" s="3"/>
       <c r="D366" s="3"/>
@@ -16862,10 +16871,10 @@
     </row>
     <row r="367" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A367" s="2" t="s">
-        <v>989</v>
+        <v>990</v>
       </c>
       <c r="B367" s="3" t="s">
-        <v>990</v>
+        <v>991</v>
       </c>
       <c r="C367" s="3"/>
       <c r="D367" s="3"/>
@@ -16894,10 +16903,10 @@
     </row>
     <row r="368" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A368" s="2" t="s">
-        <v>991</v>
+        <v>992</v>
       </c>
       <c r="B368" s="3" t="s">
-        <v>992</v>
+        <v>993</v>
       </c>
       <c r="C368" s="3"/>
       <c r="D368" s="3"/>
@@ -16926,10 +16935,10 @@
     </row>
     <row r="369" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A369" s="2" t="s">
-        <v>993</v>
+        <v>994</v>
       </c>
       <c r="B369" s="3" t="s">
-        <v>994</v>
+        <v>995</v>
       </c>
       <c r="C369" s="3"/>
       <c r="D369" s="3"/>
@@ -16958,10 +16967,10 @@
     </row>
     <row r="370" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A370" s="2" t="s">
-        <v>995</v>
+        <v>996</v>
       </c>
       <c r="B370" s="3" t="s">
-        <v>996</v>
+        <v>997</v>
       </c>
       <c r="C370" s="3"/>
       <c r="D370" s="3"/>
@@ -16990,10 +16999,10 @@
     </row>
     <row r="371" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A371" s="2" t="s">
-        <v>997</v>
+        <v>998</v>
       </c>
       <c r="B371" s="3" t="s">
-        <v>998</v>
+        <v>999</v>
       </c>
       <c r="C371" s="3"/>
       <c r="D371" s="3"/>
@@ -17022,10 +17031,10 @@
     </row>
     <row r="372" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A372" s="2" t="s">
-        <v>999</v>
+        <v>1000</v>
       </c>
       <c r="B372" s="3" t="s">
-        <v>1000</v>
+        <v>1001</v>
       </c>
       <c r="C372" s="3"/>
       <c r="D372" s="3"/>
@@ -17054,10 +17063,10 @@
     </row>
     <row r="373" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A373" s="2" t="s">
-        <v>1001</v>
+        <v>1002</v>
       </c>
       <c r="B373" s="3" t="s">
-        <v>1002</v>
+        <v>1003</v>
       </c>
       <c r="C373" s="3"/>
       <c r="D373" s="3"/>
@@ -17086,10 +17095,10 @@
     </row>
     <row r="374" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A374" s="2" t="s">
-        <v>1003</v>
+        <v>1004</v>
       </c>
       <c r="B374" s="3" t="s">
-        <v>1004</v>
+        <v>1005</v>
       </c>
       <c r="C374" s="3"/>
       <c r="D374" s="3"/>
@@ -17118,10 +17127,10 @@
     </row>
     <row r="375" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A375" s="2" t="s">
-        <v>1005</v>
+        <v>1006</v>
       </c>
       <c r="B375" s="3" t="s">
-        <v>1006</v>
+        <v>1007</v>
       </c>
       <c r="C375" s="3"/>
       <c r="D375" s="3"/>
@@ -17150,10 +17159,10 @@
     </row>
     <row r="376" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A376" s="2" t="s">
-        <v>1007</v>
+        <v>1008</v>
       </c>
       <c r="B376" s="3" t="s">
-        <v>1008</v>
+        <v>1009</v>
       </c>
       <c r="C376" s="3"/>
       <c r="D376" s="3"/>
@@ -17182,10 +17191,10 @@
     </row>
     <row r="377" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A377" s="2" t="s">
-        <v>1009</v>
+        <v>1010</v>
       </c>
       <c r="B377" s="3" t="s">
-        <v>1010</v>
+        <v>1011</v>
       </c>
       <c r="C377" s="3"/>
       <c r="D377" s="3"/>
@@ -17214,10 +17223,10 @@
     </row>
     <row r="378" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A378" s="2" t="s">
-        <v>1011</v>
+        <v>1012</v>
       </c>
       <c r="B378" s="3" t="s">
-        <v>1012</v>
+        <v>1013</v>
       </c>
       <c r="C378" s="3"/>
       <c r="D378" s="3"/>
@@ -17246,10 +17255,10 @@
     </row>
     <row r="379" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A379" s="2" t="s">
-        <v>1013</v>
+        <v>1014</v>
       </c>
       <c r="B379" s="3" t="s">
-        <v>1014</v>
+        <v>1015</v>
       </c>
       <c r="C379" s="3"/>
       <c r="D379" s="3"/>
@@ -17278,10 +17287,10 @@
     </row>
     <row r="380" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A380" s="2" t="s">
-        <v>1015</v>
+        <v>1016</v>
       </c>
       <c r="B380" s="3" t="s">
-        <v>1016</v>
+        <v>1017</v>
       </c>
       <c r="C380" s="3"/>
       <c r="D380" s="3"/>
@@ -17310,10 +17319,10 @@
     </row>
     <row r="381" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A381" s="2" t="s">
-        <v>1017</v>
+        <v>1018</v>
       </c>
       <c r="B381" s="3" t="s">
-        <v>1018</v>
+        <v>1019</v>
       </c>
       <c r="C381" s="3"/>
       <c r="D381" s="3"/>
@@ -17342,10 +17351,10 @@
     </row>
     <row r="382" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A382" s="2" t="s">
-        <v>1019</v>
+        <v>1020</v>
       </c>
       <c r="B382" s="3" t="s">
-        <v>1020</v>
+        <v>1021</v>
       </c>
       <c r="C382" s="3"/>
       <c r="D382" s="3"/>
@@ -17374,10 +17383,10 @@
     </row>
     <row r="383" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A383" s="2" t="s">
-        <v>1021</v>
+        <v>1022</v>
       </c>
       <c r="B383" s="3" t="s">
-        <v>1022</v>
+        <v>1023</v>
       </c>
       <c r="C383" s="3"/>
       <c r="D383" s="3"/>
@@ -17406,10 +17415,10 @@
     </row>
     <row r="384" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A384" s="2" t="s">
-        <v>1023</v>
+        <v>1024</v>
       </c>
       <c r="B384" s="3" t="s">
-        <v>1024</v>
+        <v>1025</v>
       </c>
       <c r="C384" s="3"/>
       <c r="D384" s="3"/>
@@ -17438,10 +17447,10 @@
     </row>
     <row r="385" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A385" s="2" t="s">
-        <v>1025</v>
+        <v>1026</v>
       </c>
       <c r="B385" s="3" t="s">
-        <v>1026</v>
+        <v>1027</v>
       </c>
       <c r="C385" s="3"/>
       <c r="D385" s="3"/>
@@ -17470,10 +17479,10 @@
     </row>
     <row r="386" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A386" s="2" t="s">
-        <v>1027</v>
+        <v>1028</v>
       </c>
       <c r="B386" s="3" t="s">
-        <v>1028</v>
+        <v>1029</v>
       </c>
       <c r="C386" s="3"/>
       <c r="D386" s="3"/>
@@ -17502,10 +17511,10 @@
     </row>
     <row r="387" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A387" s="2" t="s">
-        <v>1029</v>
+        <v>1030</v>
       </c>
       <c r="B387" s="3" t="s">
-        <v>1030</v>
+        <v>1031</v>
       </c>
       <c r="C387" s="3"/>
       <c r="D387" s="3"/>
@@ -17534,10 +17543,10 @@
     </row>
     <row r="388" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A388" s="2" t="s">
-        <v>1031</v>
+        <v>1032</v>
       </c>
       <c r="B388" s="3" t="s">
-        <v>1032</v>
+        <v>1033</v>
       </c>
       <c r="C388" s="3"/>
       <c r="D388" s="3"/>
@@ -17566,10 +17575,10 @@
     </row>
     <row r="389" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A389" s="2" t="s">
-        <v>1033</v>
+        <v>1034</v>
       </c>
       <c r="B389" s="3" t="s">
-        <v>1034</v>
+        <v>1035</v>
       </c>
       <c r="C389" s="3"/>
       <c r="D389" s="3"/>
@@ -17598,10 +17607,10 @@
     </row>
     <row r="390" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A390" s="2" t="s">
-        <v>1035</v>
+        <v>1036</v>
       </c>
       <c r="B390" s="3" t="s">
-        <v>1036</v>
+        <v>1037</v>
       </c>
       <c r="C390" s="3"/>
       <c r="D390" s="3"/>
@@ -17630,10 +17639,10 @@
     </row>
     <row r="391" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A391" s="2" t="s">
-        <v>1037</v>
+        <v>1038</v>
       </c>
       <c r="B391" s="3" t="s">
-        <v>1038</v>
+        <v>1039</v>
       </c>
       <c r="C391" s="3"/>
       <c r="D391" s="3"/>
@@ -17662,10 +17671,10 @@
     </row>
     <row r="392" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A392" s="2" t="s">
-        <v>1039</v>
+        <v>1040</v>
       </c>
       <c r="B392" s="3" t="s">
-        <v>1040</v>
+        <v>1041</v>
       </c>
       <c r="C392" s="3"/>
       <c r="D392" s="3"/>
@@ -17694,10 +17703,10 @@
     </row>
     <row r="393" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A393" s="2" t="s">
-        <v>1041</v>
+        <v>1042</v>
       </c>
       <c r="B393" s="3" t="s">
-        <v>1042</v>
+        <v>1043</v>
       </c>
       <c r="C393" s="3"/>
       <c r="D393" s="3"/>
@@ -17726,10 +17735,10 @@
     </row>
     <row r="394" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A394" s="2" t="s">
-        <v>1043</v>
+        <v>1044</v>
       </c>
       <c r="B394" s="3" t="s">
-        <v>1044</v>
+        <v>1045</v>
       </c>
       <c r="C394" s="3"/>
       <c r="D394" s="3"/>
@@ -17758,10 +17767,10 @@
     </row>
     <row r="395" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A395" s="2" t="s">
-        <v>1045</v>
+        <v>1046</v>
       </c>
       <c r="B395" s="3" t="s">
-        <v>1046</v>
+        <v>1047</v>
       </c>
       <c r="C395" s="3"/>
       <c r="D395" s="3"/>
@@ -17790,10 +17799,10 @@
     </row>
     <row r="396" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A396" s="2" t="s">
-        <v>1047</v>
+        <v>1048</v>
       </c>
       <c r="B396" s="3" t="s">
-        <v>1048</v>
+        <v>1049</v>
       </c>
       <c r="C396" s="3"/>
       <c r="D396" s="3"/>
@@ -17822,10 +17831,10 @@
     </row>
     <row r="397" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A397" s="2" t="s">
-        <v>1049</v>
+        <v>1050</v>
       </c>
       <c r="B397" s="3" t="s">
-        <v>1050</v>
+        <v>1051</v>
       </c>
       <c r="C397" s="3"/>
       <c r="D397" s="3"/>
@@ -17854,10 +17863,10 @@
     </row>
     <row r="398" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A398" s="2" t="s">
-        <v>1051</v>
+        <v>1052</v>
       </c>
       <c r="B398" s="3" t="s">
-        <v>1052</v>
+        <v>1053</v>
       </c>
       <c r="C398" s="3"/>
       <c r="D398" s="3"/>
@@ -17886,10 +17895,10 @@
     </row>
     <row r="399" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A399" s="2" t="s">
-        <v>1053</v>
+        <v>1054</v>
       </c>
       <c r="B399" s="3" t="s">
-        <v>1054</v>
+        <v>1055</v>
       </c>
       <c r="C399" s="3"/>
       <c r="D399" s="3"/>
@@ -17918,10 +17927,10 @@
     </row>
     <row r="400" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A400" s="2" t="s">
-        <v>1055</v>
+        <v>1056</v>
       </c>
       <c r="B400" s="3" t="s">
-        <v>1056</v>
+        <v>1057</v>
       </c>
       <c r="C400" s="3"/>
       <c r="D400" s="3"/>
@@ -17950,10 +17959,10 @@
     </row>
     <row r="401" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A401" s="2" t="s">
-        <v>1057</v>
+        <v>1058</v>
       </c>
       <c r="B401" s="3" t="s">
-        <v>1058</v>
+        <v>1059</v>
       </c>
       <c r="C401" s="3"/>
       <c r="D401" s="3"/>
@@ -17982,10 +17991,10 @@
     </row>
     <row r="402" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A402" s="2" t="s">
-        <v>1059</v>
+        <v>1060</v>
       </c>
       <c r="B402" s="3" t="s">
-        <v>1060</v>
+        <v>1061</v>
       </c>
       <c r="C402" s="3"/>
       <c r="D402" s="3"/>
@@ -18014,10 +18023,10 @@
     </row>
     <row r="403" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A403" s="2" t="s">
-        <v>1061</v>
+        <v>1062</v>
       </c>
       <c r="B403" s="3" t="s">
-        <v>1062</v>
+        <v>1063</v>
       </c>
       <c r="C403" s="3"/>
       <c r="D403" s="3"/>
@@ -18046,10 +18055,10 @@
     </row>
     <row r="404" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A404" s="2" t="s">
-        <v>1063</v>
+        <v>1064</v>
       </c>
       <c r="B404" s="3" t="s">
-        <v>1064</v>
+        <v>1065</v>
       </c>
       <c r="C404" s="3"/>
       <c r="D404" s="3"/>
@@ -18078,10 +18087,10 @@
     </row>
     <row r="405" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A405" s="2" t="s">
-        <v>1065</v>
+        <v>1066</v>
       </c>
       <c r="B405" s="3" t="s">
-        <v>1066</v>
+        <v>1067</v>
       </c>
       <c r="C405" s="3"/>
       <c r="D405" s="3"/>
@@ -18110,10 +18119,10 @@
     </row>
     <row r="406" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A406" s="2" t="s">
-        <v>1067</v>
+        <v>1068</v>
       </c>
       <c r="B406" s="3" t="s">
-        <v>1068</v>
+        <v>1069</v>
       </c>
       <c r="C406" s="3"/>
       <c r="D406" s="3"/>
@@ -18142,10 +18151,10 @@
     </row>
     <row r="407" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A407" s="2" t="s">
-        <v>1069</v>
+        <v>1070</v>
       </c>
       <c r="B407" s="3" t="s">
-        <v>1070</v>
+        <v>1071</v>
       </c>
       <c r="C407" s="3"/>
       <c r="D407" s="3"/>
@@ -18174,10 +18183,10 @@
     </row>
     <row r="408" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A408" s="2" t="s">
-        <v>1071</v>
+        <v>1072</v>
       </c>
       <c r="B408" s="3" t="s">
-        <v>1072</v>
+        <v>1073</v>
       </c>
       <c r="C408" s="3"/>
       <c r="D408" s="3"/>
@@ -18206,10 +18215,10 @@
     </row>
     <row r="409" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A409" s="2" t="s">
-        <v>1073</v>
+        <v>1074</v>
       </c>
       <c r="B409" s="3" t="s">
-        <v>1074</v>
+        <v>1075</v>
       </c>
       <c r="C409" s="3"/>
       <c r="D409" s="3"/>
@@ -18238,10 +18247,10 @@
     </row>
     <row r="410" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A410" s="2" t="s">
-        <v>1075</v>
+        <v>1076</v>
       </c>
       <c r="B410" s="3" t="s">
-        <v>1076</v>
+        <v>1077</v>
       </c>
       <c r="C410" s="3"/>
       <c r="D410" s="3"/>
@@ -18270,10 +18279,10 @@
     </row>
     <row r="411" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A411" s="2" t="s">
-        <v>1077</v>
+        <v>1078</v>
       </c>
       <c r="B411" s="3" t="s">
-        <v>1078</v>
+        <v>1079</v>
       </c>
       <c r="C411" s="3"/>
       <c r="D411" s="3"/>
@@ -18302,10 +18311,10 @@
     </row>
     <row r="412" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A412" s="2" t="s">
-        <v>1079</v>
+        <v>1080</v>
       </c>
       <c r="B412" s="3" t="s">
-        <v>1080</v>
+        <v>1081</v>
       </c>
       <c r="C412" s="3"/>
       <c r="D412" s="3"/>
@@ -18334,10 +18343,10 @@
     </row>
     <row r="413" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A413" s="2" t="s">
-        <v>1081</v>
+        <v>1082</v>
       </c>
       <c r="B413" s="3" t="s">
-        <v>1082</v>
+        <v>1083</v>
       </c>
       <c r="C413" s="3"/>
       <c r="D413" s="3"/>
@@ -18366,10 +18375,10 @@
     </row>
     <row r="414" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A414" s="2" t="s">
-        <v>1083</v>
+        <v>1084</v>
       </c>
       <c r="B414" s="3" t="s">
-        <v>1084</v>
+        <v>1085</v>
       </c>
       <c r="C414" s="3"/>
       <c r="D414" s="3"/>
@@ -18398,10 +18407,10 @@
     </row>
     <row r="415" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A415" s="2" t="s">
-        <v>1085</v>
+        <v>1086</v>
       </c>
       <c r="B415" s="3" t="s">
-        <v>1086</v>
+        <v>1087</v>
       </c>
       <c r="C415" s="3"/>
       <c r="D415" s="3"/>
@@ -18430,10 +18439,10 @@
     </row>
     <row r="416" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A416" s="2" t="s">
-        <v>1087</v>
+        <v>1088</v>
       </c>
       <c r="B416" s="3" t="s">
-        <v>1088</v>
+        <v>1089</v>
       </c>
       <c r="C416" s="3"/>
       <c r="D416" s="3"/>
@@ -18462,10 +18471,10 @@
     </row>
     <row r="417" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A417" s="2" t="s">
-        <v>1089</v>
+        <v>1090</v>
       </c>
       <c r="B417" s="3" t="s">
-        <v>1090</v>
+        <v>1091</v>
       </c>
       <c r="C417" s="3"/>
       <c r="D417" s="3"/>
@@ -18494,10 +18503,10 @@
     </row>
     <row r="418" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A418" s="2" t="s">
-        <v>1091</v>
+        <v>1092</v>
       </c>
       <c r="B418" s="3" t="s">
-        <v>1092</v>
+        <v>1093</v>
       </c>
       <c r="C418" s="3"/>
       <c r="D418" s="3"/>
@@ -18526,10 +18535,10 @@
     </row>
     <row r="419" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A419" s="2" t="s">
-        <v>1093</v>
+        <v>1094</v>
       </c>
       <c r="B419" s="3" t="s">
-        <v>1094</v>
+        <v>1095</v>
       </c>
       <c r="C419" s="3"/>
       <c r="D419" s="3"/>
@@ -18558,10 +18567,10 @@
     </row>
     <row r="420" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A420" s="2" t="s">
-        <v>1095</v>
+        <v>1096</v>
       </c>
       <c r="B420" s="3" t="s">
-        <v>1096</v>
+        <v>1097</v>
       </c>
       <c r="C420" s="3"/>
       <c r="D420" s="3"/>
@@ -18590,10 +18599,10 @@
     </row>
     <row r="421" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A421" s="2" t="s">
-        <v>1097</v>
+        <v>1098</v>
       </c>
       <c r="B421" s="3" t="s">
-        <v>1098</v>
+        <v>1099</v>
       </c>
       <c r="C421" s="3"/>
       <c r="D421" s="3"/>
@@ -18622,10 +18631,10 @@
     </row>
     <row r="422" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A422" s="2" t="s">
-        <v>1099</v>
+        <v>1100</v>
       </c>
       <c r="B422" s="3" t="s">
-        <v>1100</v>
+        <v>1101</v>
       </c>
       <c r="C422" s="3"/>
       <c r="D422" s="3"/>
@@ -18654,10 +18663,10 @@
     </row>
     <row r="423" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A423" s="2" t="s">
-        <v>1101</v>
+        <v>1102</v>
       </c>
       <c r="B423" s="3" t="s">
-        <v>1102</v>
+        <v>1103</v>
       </c>
       <c r="C423" s="3"/>
       <c r="D423" s="3"/>
@@ -18686,10 +18695,10 @@
     </row>
     <row r="424" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A424" s="2" t="s">
-        <v>1103</v>
+        <v>1104</v>
       </c>
       <c r="B424" s="3" t="s">
-        <v>1104</v>
+        <v>1105</v>
       </c>
       <c r="C424" s="3"/>
       <c r="D424" s="3"/>
@@ -18718,10 +18727,10 @@
     </row>
     <row r="425" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A425" s="2" t="s">
-        <v>1105</v>
+        <v>1106</v>
       </c>
       <c r="B425" s="3" t="s">
-        <v>1106</v>
+        <v>1107</v>
       </c>
       <c r="C425" s="3"/>
       <c r="D425" s="3"/>
@@ -18750,10 +18759,10 @@
     </row>
     <row r="426" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A426" s="2" t="s">
-        <v>1107</v>
+        <v>1108</v>
       </c>
       <c r="B426" s="3" t="s">
-        <v>1108</v>
+        <v>1109</v>
       </c>
       <c r="C426" s="3"/>
       <c r="D426" s="3"/>
@@ -18782,10 +18791,10 @@
     </row>
     <row r="427" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A427" s="2" t="s">
-        <v>1109</v>
+        <v>1110</v>
       </c>
       <c r="B427" s="3" t="s">
-        <v>1110</v>
+        <v>1111</v>
       </c>
       <c r="C427" s="3"/>
       <c r="D427" s="3"/>
@@ -18814,10 +18823,10 @@
     </row>
     <row r="428" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A428" s="2" t="s">
-        <v>1111</v>
+        <v>1112</v>
       </c>
       <c r="B428" s="3" t="s">
-        <v>1112</v>
+        <v>1113</v>
       </c>
       <c r="C428" s="3"/>
       <c r="D428" s="3"/>
@@ -18846,10 +18855,10 @@
     </row>
     <row r="429" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A429" s="2" t="s">
-        <v>1113</v>
+        <v>1114</v>
       </c>
       <c r="B429" s="3" t="s">
-        <v>1114</v>
+        <v>1115</v>
       </c>
       <c r="C429" s="3"/>
       <c r="D429" s="3"/>
@@ -18878,10 +18887,10 @@
     </row>
     <row r="430" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A430" s="2" t="s">
-        <v>1115</v>
+        <v>1116</v>
       </c>
       <c r="B430" s="3" t="s">
-        <v>1116</v>
+        <v>1117</v>
       </c>
       <c r="C430" s="3"/>
       <c r="D430" s="3"/>
@@ -18910,10 +18919,10 @@
     </row>
     <row r="431" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A431" s="2" t="s">
-        <v>1117</v>
+        <v>1118</v>
       </c>
       <c r="B431" s="3" t="s">
-        <v>1118</v>
+        <v>1119</v>
       </c>
       <c r="C431" s="3"/>
       <c r="D431" s="3"/>
@@ -18942,10 +18951,10 @@
     </row>
     <row r="432" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A432" s="2" t="s">
-        <v>1119</v>
+        <v>1120</v>
       </c>
       <c r="B432" s="3" t="s">
-        <v>1120</v>
+        <v>1121</v>
       </c>
       <c r="C432" s="3"/>
       <c r="D432" s="3"/>
@@ -18974,10 +18983,10 @@
     </row>
     <row r="433" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A433" s="2" t="s">
-        <v>1121</v>
+        <v>1122</v>
       </c>
       <c r="B433" s="3" t="s">
-        <v>1122</v>
+        <v>1123</v>
       </c>
       <c r="C433" s="3"/>
       <c r="D433" s="3"/>
@@ -19006,10 +19015,10 @@
     </row>
     <row r="434" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A434" s="2" t="s">
-        <v>1123</v>
+        <v>1124</v>
       </c>
       <c r="B434" s="3" t="s">
-        <v>1124</v>
+        <v>1125</v>
       </c>
       <c r="C434" s="3"/>
       <c r="D434" s="3"/>
@@ -19038,10 +19047,10 @@
     </row>
     <row r="435" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A435" s="2" t="s">
-        <v>1125</v>
+        <v>1126</v>
       </c>
       <c r="B435" s="3" t="s">
-        <v>1126</v>
+        <v>1127</v>
       </c>
       <c r="C435" s="3"/>
       <c r="D435" s="3"/>
@@ -19070,10 +19079,10 @@
     </row>
     <row r="436" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A436" s="2" t="s">
-        <v>1127</v>
+        <v>1128</v>
       </c>
       <c r="B436" s="3" t="s">
-        <v>1128</v>
+        <v>1129</v>
       </c>
       <c r="C436" s="3"/>
       <c r="D436" s="3"/>
@@ -19102,10 +19111,10 @@
     </row>
     <row r="437" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A437" s="2" t="s">
-        <v>1129</v>
+        <v>1130</v>
       </c>
       <c r="B437" s="3" t="s">
-        <v>1130</v>
+        <v>1131</v>
       </c>
       <c r="C437" s="3"/>
       <c r="D437" s="3"/>
@@ -19134,10 +19143,10 @@
     </row>
     <row r="438" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A438" s="2" t="s">
-        <v>1131</v>
+        <v>1132</v>
       </c>
       <c r="B438" s="3" t="s">
-        <v>1132</v>
+        <v>1133</v>
       </c>
       <c r="C438" s="3"/>
       <c r="D438" s="3"/>
@@ -19166,10 +19175,10 @@
     </row>
     <row r="439" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A439" s="2" t="s">
-        <v>1133</v>
+        <v>1134</v>
       </c>
       <c r="B439" s="3" t="s">
-        <v>1134</v>
+        <v>1135</v>
       </c>
       <c r="C439" s="3"/>
       <c r="D439" s="3"/>
@@ -19198,10 +19207,10 @@
     </row>
     <row r="440" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A440" s="2" t="s">
-        <v>1135</v>
+        <v>1136</v>
       </c>
       <c r="B440" s="3" t="s">
-        <v>1136</v>
+        <v>1137</v>
       </c>
       <c r="C440" s="3"/>
       <c r="D440" s="3"/>
@@ -19230,10 +19239,10 @@
     </row>
     <row r="441" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A441" s="2" t="s">
-        <v>1137</v>
+        <v>1138</v>
       </c>
       <c r="B441" s="3" t="s">
-        <v>1138</v>
+        <v>1139</v>
       </c>
       <c r="C441" s="3"/>
       <c r="D441" s="3"/>
@@ -19262,10 +19271,10 @@
     </row>
     <row r="442" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A442" s="2" t="s">
-        <v>1139</v>
+        <v>1140</v>
       </c>
       <c r="B442" s="3" t="s">
-        <v>1140</v>
+        <v>1141</v>
       </c>
       <c r="C442" s="3"/>
       <c r="D442" s="3"/>
@@ -19294,10 +19303,10 @@
     </row>
     <row r="443" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A443" s="2" t="s">
-        <v>1141</v>
+        <v>1142</v>
       </c>
       <c r="B443" s="3" t="s">
-        <v>1142</v>
+        <v>1143</v>
       </c>
       <c r="C443" s="3"/>
       <c r="D443" s="3"/>
@@ -19326,10 +19335,10 @@
     </row>
     <row r="444" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A444" s="2" t="s">
-        <v>1143</v>
+        <v>1144</v>
       </c>
       <c r="B444" s="3" t="s">
-        <v>1144</v>
+        <v>1145</v>
       </c>
       <c r="C444" s="3"/>
       <c r="D444" s="3"/>
@@ -19358,10 +19367,10 @@
     </row>
     <row r="445" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A445" s="2" t="s">
-        <v>1145</v>
+        <v>1146</v>
       </c>
       <c r="B445" s="3" t="s">
-        <v>1146</v>
+        <v>1147</v>
       </c>
       <c r="C445" s="3"/>
       <c r="D445" s="3"/>
@@ -19390,10 +19399,10 @@
     </row>
     <row r="446" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A446" s="2" t="s">
-        <v>1147</v>
+        <v>1148</v>
       </c>
       <c r="B446" s="3" t="s">
-        <v>1148</v>
+        <v>1149</v>
       </c>
       <c r="C446" s="3"/>
       <c r="D446" s="3"/>
@@ -19422,7 +19431,7 @@
     </row>
     <row r="447" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A447" s="2" t="s">
-        <v>1149</v>
+        <v>1150</v>
       </c>
       <c r="B447" s="5"/>
       <c r="C447" s="5"/>
@@ -19452,7 +19461,7 @@
     </row>
     <row r="448" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A448" s="2" t="s">
-        <v>1150</v>
+        <v>1151</v>
       </c>
       <c r="B448" s="5"/>
       <c r="C448" s="5"/>
@@ -19482,7 +19491,7 @@
     </row>
     <row r="449" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A449" s="2" t="s">
-        <v>1151</v>
+        <v>1152</v>
       </c>
       <c r="B449" s="5"/>
       <c r="C449" s="5"/>
@@ -19512,10 +19521,10 @@
     </row>
     <row r="450" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A450" s="2" t="s">
-        <v>1152</v>
+        <v>1153</v>
       </c>
       <c r="B450" s="3" t="s">
-        <v>1153</v>
+        <v>1154</v>
       </c>
       <c r="C450" s="3"/>
       <c r="D450" s="3"/>
@@ -19544,10 +19553,10 @@
     </row>
     <row r="451" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A451" s="2" t="s">
-        <v>1154</v>
+        <v>1155</v>
       </c>
       <c r="B451" s="3" t="s">
-        <v>1155</v>
+        <v>1156</v>
       </c>
       <c r="C451" s="3"/>
       <c r="D451" s="3"/>
@@ -19576,10 +19585,10 @@
     </row>
     <row r="452" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A452" s="2" t="s">
-        <v>1156</v>
+        <v>1157</v>
       </c>
       <c r="B452" s="3" t="s">
-        <v>1157</v>
+        <v>1158</v>
       </c>
       <c r="C452" s="3"/>
       <c r="D452" s="3"/>
@@ -19608,10 +19617,10 @@
     </row>
     <row r="453" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A453" s="2" t="s">
-        <v>1158</v>
+        <v>1159</v>
       </c>
       <c r="B453" s="3" t="s">
-        <v>1159</v>
+        <v>1160</v>
       </c>
       <c r="C453" s="3"/>
       <c r="D453" s="3"/>
@@ -19640,10 +19649,10 @@
     </row>
     <row r="454" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A454" s="2" t="s">
-        <v>1160</v>
+        <v>1161</v>
       </c>
       <c r="B454" s="3" t="s">
-        <v>1161</v>
+        <v>1162</v>
       </c>
       <c r="C454" s="3"/>
       <c r="D454" s="3"/>
@@ -19672,10 +19681,10 @@
     </row>
     <row r="455" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A455" s="2" t="s">
-        <v>1162</v>
+        <v>1163</v>
       </c>
       <c r="B455" s="3" t="s">
-        <v>1163</v>
+        <v>1164</v>
       </c>
       <c r="C455" s="3"/>
       <c r="D455" s="3"/>
@@ -19704,10 +19713,10 @@
     </row>
     <row r="456" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A456" s="2" t="s">
-        <v>1164</v>
+        <v>1165</v>
       </c>
       <c r="B456" s="3" t="s">
-        <v>1165</v>
+        <v>1166</v>
       </c>
       <c r="C456" s="3"/>
       <c r="D456" s="3"/>
@@ -19736,10 +19745,10 @@
     </row>
     <row r="457" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A457" s="2" t="s">
-        <v>1166</v>
+        <v>1167</v>
       </c>
       <c r="B457" s="3" t="s">
-        <v>1167</v>
+        <v>1168</v>
       </c>
       <c r="C457" s="3"/>
       <c r="D457" s="3"/>
@@ -19768,10 +19777,10 @@
     </row>
     <row r="458" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A458" s="2" t="s">
-        <v>1168</v>
+        <v>1169</v>
       </c>
       <c r="B458" s="3" t="s">
-        <v>1169</v>
+        <v>1170</v>
       </c>
       <c r="C458" s="3"/>
       <c r="D458" s="3"/>
@@ -19800,10 +19809,10 @@
     </row>
     <row r="459" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A459" s="2" t="s">
-        <v>1170</v>
+        <v>1171</v>
       </c>
       <c r="B459" s="3" t="s">
-        <v>1171</v>
+        <v>1172</v>
       </c>
       <c r="C459" s="3"/>
       <c r="D459" s="3"/>
@@ -19832,10 +19841,10 @@
     </row>
     <row r="460" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A460" s="2" t="s">
-        <v>1172</v>
+        <v>1173</v>
       </c>
       <c r="B460" s="3" t="s">
-        <v>1173</v>
+        <v>1174</v>
       </c>
       <c r="C460" s="3"/>
       <c r="D460" s="3"/>
@@ -19864,10 +19873,10 @@
     </row>
     <row r="461" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A461" s="2" t="s">
-        <v>1174</v>
+        <v>1175</v>
       </c>
       <c r="B461" s="3" t="s">
-        <v>1175</v>
+        <v>1176</v>
       </c>
       <c r="C461" s="3"/>
       <c r="D461" s="3"/>
@@ -19896,10 +19905,10 @@
     </row>
     <row r="462" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A462" s="2" t="s">
-        <v>1176</v>
+        <v>1177</v>
       </c>
       <c r="B462" s="3" t="s">
-        <v>1177</v>
+        <v>1178</v>
       </c>
       <c r="C462" s="3"/>
       <c r="D462" s="3"/>
@@ -19928,10 +19937,10 @@
     </row>
     <row r="463" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A463" s="2" t="s">
-        <v>1178</v>
+        <v>1179</v>
       </c>
       <c r="B463" s="3" t="s">
-        <v>1179</v>
+        <v>1180</v>
       </c>
       <c r="C463" s="3"/>
       <c r="D463" s="3"/>
@@ -19960,10 +19969,10 @@
     </row>
     <row r="464" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A464" s="2" t="s">
-        <v>1180</v>
+        <v>1181</v>
       </c>
       <c r="B464" s="3" t="s">
-        <v>1181</v>
+        <v>1182</v>
       </c>
       <c r="C464" s="3"/>
       <c r="D464" s="3"/>
@@ -19992,10 +20001,10 @@
     </row>
     <row r="465" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A465" s="2" t="s">
-        <v>1182</v>
+        <v>1183</v>
       </c>
       <c r="B465" s="3" t="s">
-        <v>1183</v>
+        <v>1184</v>
       </c>
       <c r="C465" s="3"/>
       <c r="D465" s="3"/>
@@ -20024,7 +20033,7 @@
     </row>
     <row r="466" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A466" s="2" t="s">
-        <v>1184</v>
+        <v>1185</v>
       </c>
       <c r="B466" s="5"/>
       <c r="C466" s="5"/>
@@ -20054,21 +20063,21 @@
     </row>
     <row r="467" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A467" s="2" t="s">
-        <v>1185</v>
+        <v>1186</v>
       </c>
       <c r="B467" s="5"/>
       <c r="C467" s="5"/>
       <c r="D467" s="5"/>
-      <c r="E467" s="9"/>
-      <c r="F467" s="9"/>
-      <c r="G467" s="9"/>
-      <c r="H467" s="9"/>
-      <c r="I467" s="9"/>
-      <c r="J467" s="9"/>
-      <c r="K467" s="9"/>
-      <c r="L467" s="9"/>
-      <c r="M467" s="9"/>
-      <c r="N467" s="9"/>
+      <c r="E467" s="10"/>
+      <c r="F467" s="10"/>
+      <c r="G467" s="10"/>
+      <c r="H467" s="10"/>
+      <c r="I467" s="10"/>
+      <c r="J467" s="10"/>
+      <c r="K467" s="10"/>
+      <c r="L467" s="10"/>
+      <c r="M467" s="10"/>
+      <c r="N467" s="10"/>
       <c r="O467" s="5"/>
       <c r="P467" s="5"/>
       <c r="Q467" s="5"/>
@@ -20084,21 +20093,21 @@
     </row>
     <row r="468" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A468" s="2" t="s">
-        <v>1186</v>
+        <v>1187</v>
       </c>
       <c r="B468" s="5"/>
       <c r="C468" s="5"/>
       <c r="D468" s="5"/>
-      <c r="E468" s="9"/>
-      <c r="F468" s="9"/>
-      <c r="G468" s="9"/>
-      <c r="H468" s="9"/>
-      <c r="I468" s="9"/>
-      <c r="J468" s="9"/>
-      <c r="K468" s="9"/>
-      <c r="L468" s="9"/>
-      <c r="M468" s="9"/>
-      <c r="N468" s="9"/>
+      <c r="E468" s="10"/>
+      <c r="F468" s="10"/>
+      <c r="G468" s="10"/>
+      <c r="H468" s="10"/>
+      <c r="I468" s="10"/>
+      <c r="J468" s="10"/>
+      <c r="K468" s="10"/>
+      <c r="L468" s="10"/>
+      <c r="M468" s="10"/>
+      <c r="N468" s="10"/>
       <c r="O468" s="5"/>
       <c r="P468" s="5"/>
       <c r="Q468" s="5"/>
@@ -20114,21 +20123,21 @@
     </row>
     <row r="469" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A469" s="2" t="s">
-        <v>1187</v>
+        <v>1188</v>
       </c>
       <c r="B469" s="5"/>
       <c r="C469" s="5"/>
       <c r="D469" s="5"/>
-      <c r="E469" s="9"/>
-      <c r="F469" s="9"/>
-      <c r="G469" s="9"/>
-      <c r="H469" s="9"/>
-      <c r="I469" s="9"/>
-      <c r="J469" s="9"/>
-      <c r="K469" s="9"/>
-      <c r="L469" s="9"/>
-      <c r="M469" s="9"/>
-      <c r="N469" s="9"/>
+      <c r="E469" s="10"/>
+      <c r="F469" s="10"/>
+      <c r="G469" s="10"/>
+      <c r="H469" s="10"/>
+      <c r="I469" s="10"/>
+      <c r="J469" s="10"/>
+      <c r="K469" s="10"/>
+      <c r="L469" s="10"/>
+      <c r="M469" s="10"/>
+      <c r="N469" s="10"/>
       <c r="O469" s="5"/>
       <c r="P469" s="5"/>
       <c r="Q469" s="5"/>
@@ -20144,21 +20153,21 @@
     </row>
     <row r="470" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A470" s="2" t="s">
-        <v>1188</v>
+        <v>1189</v>
       </c>
       <c r="B470" s="5"/>
       <c r="C470" s="5"/>
       <c r="D470" s="5"/>
-      <c r="E470" s="9"/>
-      <c r="F470" s="9"/>
-      <c r="G470" s="9"/>
-      <c r="H470" s="9"/>
-      <c r="I470" s="9"/>
-      <c r="J470" s="9"/>
-      <c r="K470" s="9"/>
-      <c r="L470" s="9"/>
-      <c r="M470" s="9"/>
-      <c r="N470" s="9"/>
+      <c r="E470" s="10"/>
+      <c r="F470" s="10"/>
+      <c r="G470" s="10"/>
+      <c r="H470" s="10"/>
+      <c r="I470" s="10"/>
+      <c r="J470" s="10"/>
+      <c r="K470" s="10"/>
+      <c r="L470" s="10"/>
+      <c r="M470" s="10"/>
+      <c r="N470" s="10"/>
       <c r="O470" s="5"/>
       <c r="P470" s="5"/>
       <c r="Q470" s="5"/>
@@ -20174,21 +20183,21 @@
     </row>
     <row r="471" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A471" s="2" t="s">
-        <v>1189</v>
+        <v>1190</v>
       </c>
       <c r="B471" s="5"/>
       <c r="C471" s="5"/>
       <c r="D471" s="5"/>
-      <c r="E471" s="9"/>
-      <c r="F471" s="9"/>
-      <c r="G471" s="9"/>
-      <c r="H471" s="9"/>
-      <c r="I471" s="9"/>
-      <c r="J471" s="9"/>
-      <c r="K471" s="9"/>
-      <c r="L471" s="9"/>
-      <c r="M471" s="9"/>
-      <c r="N471" s="9"/>
+      <c r="E471" s="10"/>
+      <c r="F471" s="10"/>
+      <c r="G471" s="10"/>
+      <c r="H471" s="10"/>
+      <c r="I471" s="10"/>
+      <c r="J471" s="10"/>
+      <c r="K471" s="10"/>
+      <c r="L471" s="10"/>
+      <c r="M471" s="10"/>
+      <c r="N471" s="10"/>
       <c r="O471" s="5"/>
       <c r="P471" s="5"/>
       <c r="Q471" s="5"/>
@@ -20204,21 +20213,21 @@
     </row>
     <row r="472" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A472" s="2" t="s">
-        <v>1190</v>
+        <v>1191</v>
       </c>
       <c r="B472" s="5"/>
       <c r="C472" s="5"/>
       <c r="D472" s="5"/>
-      <c r="E472" s="9"/>
-      <c r="F472" s="9"/>
-      <c r="G472" s="9"/>
-      <c r="H472" s="9"/>
-      <c r="I472" s="9"/>
-      <c r="J472" s="9"/>
-      <c r="K472" s="9"/>
-      <c r="L472" s="9"/>
-      <c r="M472" s="9"/>
-      <c r="N472" s="9"/>
+      <c r="E472" s="10"/>
+      <c r="F472" s="10"/>
+      <c r="G472" s="10"/>
+      <c r="H472" s="10"/>
+      <c r="I472" s="10"/>
+      <c r="J472" s="10"/>
+      <c r="K472" s="10"/>
+      <c r="L472" s="10"/>
+      <c r="M472" s="10"/>
+      <c r="N472" s="10"/>
       <c r="O472" s="5"/>
       <c r="P472" s="5"/>
       <c r="Q472" s="5"/>
@@ -20234,7 +20243,7 @@
     </row>
     <row r="473" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A473" s="2" t="s">
-        <v>1191</v>
+        <v>1192</v>
       </c>
       <c r="B473" s="5"/>
       <c r="C473" s="5"/>
@@ -20264,7 +20273,7 @@
     </row>
     <row r="474" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A474" s="2" t="s">
-        <v>1192</v>
+        <v>1193</v>
       </c>
       <c r="B474" s="5"/>
       <c r="C474" s="5"/>
@@ -20294,7 +20303,7 @@
     </row>
     <row r="475" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A475" s="2" t="s">
-        <v>1193</v>
+        <v>1194</v>
       </c>
       <c r="B475" s="5"/>
       <c r="C475" s="5"/>
@@ -20324,7 +20333,7 @@
     </row>
     <row r="476" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A476" s="2" t="s">
-        <v>1194</v>
+        <v>1195</v>
       </c>
       <c r="B476" s="5"/>
       <c r="C476" s="5"/>
@@ -20354,7 +20363,7 @@
     </row>
     <row r="477" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A477" s="2" t="s">
-        <v>1195</v>
+        <v>1196</v>
       </c>
       <c r="B477" s="5"/>
       <c r="C477" s="5"/>
@@ -20384,7 +20393,7 @@
     </row>
     <row r="478" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A478" s="2" t="s">
-        <v>1196</v>
+        <v>1197</v>
       </c>
       <c r="B478" s="5"/>
       <c r="C478" s="5"/>
@@ -20414,7 +20423,7 @@
     </row>
     <row r="479" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A479" s="2" t="s">
-        <v>1197</v>
+        <v>1198</v>
       </c>
       <c r="B479" s="5"/>
       <c r="C479" s="5"/>
@@ -20444,7 +20453,7 @@
     </row>
     <row r="480" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A480" s="2" t="s">
-        <v>1198</v>
+        <v>1199</v>
       </c>
       <c r="B480" s="5"/>
       <c r="C480" s="5"/>
@@ -20474,7 +20483,7 @@
     </row>
     <row r="481" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A481" s="2" t="s">
-        <v>1199</v>
+        <v>1200</v>
       </c>
       <c r="B481" s="5"/>
       <c r="C481" s="5"/>
@@ -20503,25 +20512,25 @@
       <c r="Z481" s="1"/>
     </row>
     <row r="482" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A482" s="10"/>
-      <c r="B482" s="11"/>
-      <c r="C482" s="11"/>
-      <c r="D482" s="11"/>
-      <c r="E482" s="11"/>
-      <c r="F482" s="11"/>
-      <c r="G482" s="11"/>
-      <c r="H482" s="11"/>
+      <c r="A482" s="11"/>
+      <c r="B482" s="12"/>
+      <c r="C482" s="12"/>
+      <c r="D482" s="12"/>
+      <c r="E482" s="12"/>
+      <c r="F482" s="12"/>
+      <c r="G482" s="12"/>
+      <c r="H482" s="12"/>
       <c r="I482" s="3" t="s">
-        <v>1200</v>
+        <v>1201</v>
       </c>
       <c r="J482" s="3"/>
-      <c r="K482" s="11"/>
-      <c r="L482" s="11"/>
-      <c r="M482" s="11"/>
-      <c r="N482" s="11"/>
-      <c r="O482" s="11"/>
-      <c r="P482" s="11"/>
-      <c r="Q482" s="11"/>
+      <c r="K482" s="12"/>
+      <c r="L482" s="12"/>
+      <c r="M482" s="12"/>
+      <c r="N482" s="12"/>
+      <c r="O482" s="12"/>
+      <c r="P482" s="12"/>
+      <c r="Q482" s="12"/>
       <c r="R482" s="1"/>
       <c r="S482" s="1"/>
       <c r="T482" s="1"/>
@@ -20534,37 +20543,37 @@
     </row>
     <row r="483" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A483" s="2" t="s">
-        <v>1201</v>
+        <v>1202</v>
       </c>
       <c r="B483" s="4" t="s">
-        <v>1202</v>
+        <v>1203</v>
       </c>
       <c r="C483" s="4" t="s">
-        <v>1203</v>
+        <v>1204</v>
       </c>
       <c r="D483" s="4" t="s">
-        <v>1204</v>
+        <v>1205</v>
       </c>
       <c r="E483" s="4" t="s">
-        <v>1205</v>
+        <v>1206</v>
       </c>
       <c r="F483" s="4" t="s">
-        <v>1206</v>
+        <v>1207</v>
       </c>
       <c r="G483" s="4" t="s">
-        <v>1207</v>
+        <v>1208</v>
       </c>
       <c r="H483" s="4" t="s">
-        <v>1208</v>
+        <v>1209</v>
       </c>
       <c r="I483" s="4" t="s">
-        <v>1209</v>
+        <v>1210</v>
       </c>
       <c r="J483" s="4" t="s">
-        <v>1210</v>
+        <v>1211</v>
       </c>
       <c r="K483" s="4" t="s">
-        <v>1211</v>
+        <v>1212</v>
       </c>
       <c r="L483" s="5"/>
       <c r="M483" s="5"/>
@@ -20584,37 +20593,37 @@
     </row>
     <row r="484" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A484" s="2" t="s">
-        <v>1212</v>
+        <v>1213</v>
       </c>
       <c r="B484" s="4" t="s">
-        <v>1213</v>
+        <v>1214</v>
       </c>
       <c r="C484" s="4" t="s">
-        <v>1214</v>
+        <v>1215</v>
       </c>
       <c r="D484" s="4" t="s">
-        <v>1215</v>
+        <v>1216</v>
       </c>
       <c r="E484" s="4" t="s">
-        <v>1216</v>
+        <v>1217</v>
       </c>
       <c r="F484" s="4" t="s">
-        <v>1217</v>
+        <v>1218</v>
       </c>
       <c r="G484" s="4" t="s">
-        <v>1218</v>
+        <v>1219</v>
       </c>
       <c r="H484" s="4" t="s">
-        <v>1219</v>
+        <v>1220</v>
       </c>
       <c r="I484" s="4" t="s">
-        <v>1220</v>
+        <v>1221</v>
       </c>
       <c r="J484" s="4" t="s">
-        <v>1221</v>
+        <v>1222</v>
       </c>
       <c r="K484" s="4" t="s">
-        <v>1222</v>
+        <v>1223</v>
       </c>
       <c r="L484" s="5"/>
       <c r="M484" s="5"/>
@@ -20634,37 +20643,37 @@
     </row>
     <row r="485" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A485" s="2" t="s">
-        <v>1223</v>
+        <v>1224</v>
       </c>
       <c r="B485" s="4" t="s">
-        <v>1224</v>
+        <v>1225</v>
       </c>
       <c r="C485" s="4" t="s">
-        <v>1225</v>
+        <v>1226</v>
       </c>
       <c r="D485" s="4" t="s">
-        <v>1226</v>
+        <v>1227</v>
       </c>
       <c r="E485" s="4" t="s">
-        <v>1227</v>
+        <v>1228</v>
       </c>
       <c r="F485" s="4" t="s">
-        <v>1228</v>
+        <v>1229</v>
       </c>
       <c r="G485" s="4" t="s">
-        <v>1229</v>
+        <v>1230</v>
       </c>
       <c r="H485" s="4" t="s">
-        <v>1230</v>
+        <v>1231</v>
       </c>
       <c r="I485" s="4" t="s">
-        <v>1231</v>
+        <v>1232</v>
       </c>
       <c r="J485" s="4" t="s">
-        <v>1232</v>
+        <v>1233</v>
       </c>
       <c r="K485" s="4" t="s">
-        <v>1233</v>
+        <v>1234</v>
       </c>
       <c r="L485" s="5"/>
       <c r="M485" s="5"/>
@@ -20684,37 +20693,37 @@
     </row>
     <row r="486" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A486" s="2" t="s">
-        <v>1234</v>
+        <v>1235</v>
       </c>
       <c r="B486" s="4" t="s">
-        <v>1235</v>
+        <v>1236</v>
       </c>
       <c r="C486" s="4" t="s">
-        <v>1236</v>
+        <v>1237</v>
       </c>
       <c r="D486" s="4" t="s">
-        <v>1237</v>
+        <v>1238</v>
       </c>
       <c r="E486" s="4" t="s">
-        <v>1238</v>
+        <v>1239</v>
       </c>
       <c r="F486" s="4" t="s">
-        <v>1239</v>
+        <v>1240</v>
       </c>
       <c r="G486" s="4" t="s">
-        <v>1240</v>
+        <v>1241</v>
       </c>
       <c r="H486" s="4" t="s">
-        <v>1241</v>
+        <v>1242</v>
       </c>
       <c r="I486" s="4" t="s">
-        <v>1242</v>
+        <v>1243</v>
       </c>
       <c r="J486" s="4" t="s">
-        <v>1243</v>
+        <v>1244</v>
       </c>
       <c r="K486" s="4" t="s">
-        <v>1244</v>
+        <v>1245</v>
       </c>
       <c r="L486" s="5"/>
       <c r="M486" s="5"/>
@@ -20734,37 +20743,37 @@
     </row>
     <row r="487" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A487" s="2" t="s">
-        <v>1245</v>
+        <v>1246</v>
       </c>
       <c r="B487" s="4" t="s">
-        <v>1246</v>
+        <v>1247</v>
       </c>
       <c r="C487" s="4" t="s">
-        <v>1247</v>
+        <v>1248</v>
       </c>
       <c r="D487" s="4" t="s">
-        <v>1248</v>
+        <v>1249</v>
       </c>
       <c r="E487" s="4" t="s">
-        <v>1249</v>
+        <v>1250</v>
       </c>
       <c r="F487" s="4" t="s">
-        <v>1250</v>
+        <v>1251</v>
       </c>
       <c r="G487" s="4" t="s">
-        <v>1251</v>
+        <v>1252</v>
       </c>
       <c r="H487" s="4" t="s">
-        <v>1252</v>
+        <v>1253</v>
       </c>
       <c r="I487" s="4" t="s">
-        <v>1253</v>
+        <v>1254</v>
       </c>
       <c r="J487" s="4" t="s">
-        <v>1254</v>
+        <v>1255</v>
       </c>
       <c r="K487" s="4" t="s">
-        <v>1255</v>
+        <v>1256</v>
       </c>
       <c r="L487" s="5"/>
       <c r="M487" s="5"/>
@@ -20784,37 +20793,37 @@
     </row>
     <row r="488" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A488" s="2" t="s">
-        <v>1256</v>
+        <v>1257</v>
       </c>
       <c r="B488" s="4" t="s">
-        <v>1257</v>
+        <v>1258</v>
       </c>
       <c r="C488" s="4" t="s">
-        <v>1258</v>
+        <v>1259</v>
       </c>
       <c r="D488" s="4" t="s">
-        <v>1259</v>
+        <v>1260</v>
       </c>
       <c r="E488" s="4" t="s">
-        <v>1260</v>
+        <v>1261</v>
       </c>
       <c r="F488" s="4" t="s">
-        <v>1261</v>
+        <v>1262</v>
       </c>
       <c r="G488" s="4" t="s">
-        <v>1262</v>
+        <v>1263</v>
       </c>
       <c r="H488" s="4" t="s">
-        <v>1263</v>
+        <v>1264</v>
       </c>
       <c r="I488" s="4" t="s">
-        <v>1264</v>
+        <v>1265</v>
       </c>
       <c r="J488" s="4" t="s">
-        <v>1265</v>
+        <v>1266</v>
       </c>
       <c r="K488" s="4" t="s">
-        <v>1266</v>
+        <v>1267</v>
       </c>
       <c r="L488" s="5"/>
       <c r="M488" s="5"/>
@@ -20834,37 +20843,37 @@
     </row>
     <row r="489" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A489" s="2" t="s">
-        <v>1267</v>
+        <v>1268</v>
       </c>
       <c r="B489" s="4" t="s">
-        <v>1268</v>
+        <v>1269</v>
       </c>
       <c r="C489" s="4" t="s">
-        <v>1269</v>
+        <v>1270</v>
       </c>
       <c r="D489" s="4" t="s">
-        <v>1270</v>
+        <v>1271</v>
       </c>
       <c r="E489" s="4" t="s">
-        <v>1271</v>
+        <v>1272</v>
       </c>
       <c r="F489" s="4" t="s">
-        <v>1272</v>
+        <v>1273</v>
       </c>
       <c r="G489" s="4" t="s">
-        <v>1273</v>
+        <v>1274</v>
       </c>
       <c r="H489" s="4" t="s">
-        <v>1274</v>
+        <v>1275</v>
       </c>
       <c r="I489" s="4" t="s">
-        <v>1275</v>
+        <v>1276</v>
       </c>
       <c r="J489" s="4" t="s">
-        <v>1276</v>
+        <v>1277</v>
       </c>
       <c r="K489" s="4" t="s">
-        <v>1277</v>
+        <v>1278</v>
       </c>
       <c r="L489" s="5"/>
       <c r="M489" s="5"/>
@@ -20884,37 +20893,37 @@
     </row>
     <row r="490" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A490" s="2" t="s">
-        <v>1278</v>
+        <v>1279</v>
       </c>
       <c r="B490" s="4" t="s">
-        <v>1279</v>
+        <v>1280</v>
       </c>
       <c r="C490" s="4" t="s">
-        <v>1280</v>
+        <v>1281</v>
       </c>
       <c r="D490" s="4" t="s">
-        <v>1281</v>
+        <v>1282</v>
       </c>
       <c r="E490" s="4" t="s">
-        <v>1282</v>
+        <v>1283</v>
       </c>
       <c r="F490" s="4" t="s">
-        <v>1283</v>
+        <v>1284</v>
       </c>
       <c r="G490" s="4" t="s">
-        <v>1284</v>
+        <v>1285</v>
       </c>
       <c r="H490" s="4" t="s">
-        <v>1285</v>
+        <v>1286</v>
       </c>
       <c r="I490" s="4" t="s">
-        <v>1286</v>
+        <v>1287</v>
       </c>
       <c r="J490" s="4" t="s">
-        <v>1287</v>
+        <v>1288</v>
       </c>
       <c r="K490" s="4" t="s">
-        <v>1288</v>
+        <v>1289</v>
       </c>
       <c r="L490" s="5"/>
       <c r="M490" s="5"/>
@@ -20934,37 +20943,37 @@
     </row>
     <row r="491" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A491" s="2" t="s">
-        <v>1289</v>
+        <v>1290</v>
       </c>
       <c r="B491" s="4" t="s">
-        <v>1290</v>
+        <v>1291</v>
       </c>
       <c r="C491" s="4" t="s">
-        <v>1291</v>
+        <v>1292</v>
       </c>
       <c r="D491" s="4" t="s">
-        <v>1292</v>
+        <v>1293</v>
       </c>
       <c r="E491" s="4" t="s">
-        <v>1293</v>
+        <v>1294</v>
       </c>
       <c r="F491" s="4" t="s">
-        <v>1294</v>
+        <v>1295</v>
       </c>
       <c r="G491" s="4" t="s">
-        <v>1295</v>
+        <v>1296</v>
       </c>
       <c r="H491" s="4" t="s">
-        <v>1296</v>
+        <v>1297</v>
       </c>
       <c r="I491" s="4" t="s">
-        <v>1297</v>
+        <v>1298</v>
       </c>
       <c r="J491" s="4" t="s">
-        <v>1298</v>
+        <v>1299</v>
       </c>
       <c r="K491" s="4" t="s">
-        <v>1299</v>
+        <v>1300</v>
       </c>
       <c r="L491" s="5"/>
       <c r="M491" s="5"/>
@@ -20984,37 +20993,37 @@
     </row>
     <row r="492" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A492" s="2" t="s">
-        <v>1300</v>
+        <v>1301</v>
       </c>
       <c r="B492" s="4" t="s">
-        <v>1301</v>
+        <v>1302</v>
       </c>
       <c r="C492" s="4" t="s">
-        <v>1302</v>
+        <v>1303</v>
       </c>
       <c r="D492" s="4" t="s">
-        <v>1303</v>
+        <v>1304</v>
       </c>
       <c r="E492" s="4" t="s">
-        <v>1304</v>
+        <v>1305</v>
       </c>
       <c r="F492" s="4" t="s">
-        <v>1305</v>
+        <v>1306</v>
       </c>
       <c r="G492" s="4" t="s">
-        <v>1306</v>
+        <v>1307</v>
       </c>
       <c r="H492" s="4" t="s">
-        <v>1307</v>
+        <v>1308</v>
       </c>
       <c r="I492" s="4" t="s">
-        <v>1308</v>
+        <v>1309</v>
       </c>
       <c r="J492" s="4" t="s">
-        <v>1309</v>
+        <v>1310</v>
       </c>
       <c r="K492" s="4" t="s">
-        <v>1310</v>
+        <v>1311</v>
       </c>
       <c r="L492" s="5"/>
       <c r="M492" s="5"/>
@@ -21034,37 +21043,37 @@
     </row>
     <row r="493" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A493" s="2" t="s">
-        <v>1311</v>
+        <v>1312</v>
       </c>
       <c r="B493" s="4" t="s">
-        <v>1312</v>
+        <v>1313</v>
       </c>
       <c r="C493" s="4" t="s">
-        <v>1313</v>
+        <v>1314</v>
       </c>
       <c r="D493" s="4" t="s">
-        <v>1314</v>
+        <v>1315</v>
       </c>
       <c r="E493" s="4" t="s">
-        <v>1315</v>
+        <v>1316</v>
       </c>
       <c r="F493" s="4" t="s">
-        <v>1316</v>
+        <v>1317</v>
       </c>
       <c r="G493" s="4" t="s">
-        <v>1317</v>
+        <v>1318</v>
       </c>
       <c r="H493" s="4" t="s">
-        <v>1318</v>
+        <v>1319</v>
       </c>
       <c r="I493" s="4" t="s">
-        <v>1319</v>
+        <v>1320</v>
       </c>
       <c r="J493" s="4" t="s">
-        <v>1320</v>
+        <v>1321</v>
       </c>
       <c r="K493" s="4" t="s">
-        <v>1321</v>
+        <v>1322</v>
       </c>
       <c r="L493" s="5"/>
       <c r="M493" s="5"/>
@@ -21084,37 +21093,37 @@
     </row>
     <row r="494" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A494" s="2" t="s">
-        <v>1322</v>
+        <v>1323</v>
       </c>
       <c r="B494" s="4" t="s">
-        <v>1323</v>
+        <v>1324</v>
       </c>
       <c r="C494" s="4" t="s">
-        <v>1324</v>
+        <v>1325</v>
       </c>
       <c r="D494" s="4" t="s">
-        <v>1325</v>
+        <v>1326</v>
       </c>
       <c r="E494" s="4" t="s">
-        <v>1326</v>
+        <v>1327</v>
       </c>
       <c r="F494" s="4" t="s">
-        <v>1327</v>
+        <v>1328</v>
       </c>
       <c r="G494" s="4" t="s">
-        <v>1328</v>
+        <v>1329</v>
       </c>
       <c r="H494" s="4" t="s">
-        <v>1329</v>
+        <v>1330</v>
       </c>
       <c r="I494" s="4" t="s">
-        <v>1330</v>
+        <v>1331</v>
       </c>
       <c r="J494" s="4" t="s">
-        <v>1331</v>
+        <v>1332</v>
       </c>
       <c r="K494" s="4" t="s">
-        <v>1332</v>
+        <v>1333</v>
       </c>
       <c r="L494" s="5"/>
       <c r="M494" s="5"/>
@@ -21134,38 +21143,38 @@
     </row>
     <row r="495" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A495" s="2" t="s">
-        <v>1333</v>
+        <v>1334</v>
       </c>
       <c r="B495" s="3" t="s">
-        <v>1334</v>
+        <v>1335</v>
       </c>
       <c r="C495" s="3"/>
       <c r="D495" s="3" t="s">
-        <v>1335</v>
+        <v>1336</v>
       </c>
       <c r="E495" s="3"/>
       <c r="F495" s="3" t="s">
-        <v>1336</v>
+        <v>1337</v>
       </c>
       <c r="G495" s="3"/>
       <c r="H495" s="3" t="s">
-        <v>1337</v>
+        <v>1338</v>
       </c>
       <c r="I495" s="3"/>
       <c r="J495" s="3" t="s">
-        <v>1338</v>
+        <v>1339</v>
       </c>
       <c r="K495" s="3"/>
       <c r="L495" s="3" t="s">
-        <v>1339</v>
+        <v>1340</v>
       </c>
       <c r="M495" s="3"/>
       <c r="N495" s="3" t="s">
-        <v>1340</v>
+        <v>1341</v>
       </c>
       <c r="O495" s="3"/>
       <c r="P495" s="3" t="s">
-        <v>1341</v>
+        <v>1342</v>
       </c>
       <c r="Q495" s="3"/>
       <c r="R495" s="1"/>
@@ -21180,34 +21189,34 @@
     </row>
     <row r="496" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A496" s="2" t="s">
-        <v>1342</v>
+        <v>1343</v>
       </c>
       <c r="B496" s="4" t="s">
-        <v>1343</v>
+        <v>1344</v>
       </c>
       <c r="C496" s="4" t="s">
-        <v>1344</v>
+        <v>1345</v>
       </c>
       <c r="D496" s="4" t="s">
-        <v>1345</v>
+        <v>1346</v>
       </c>
       <c r="E496" s="4" t="s">
-        <v>1346</v>
+        <v>1347</v>
       </c>
       <c r="F496" s="4" t="s">
-        <v>1347</v>
+        <v>1348</v>
       </c>
       <c r="G496" s="4" t="s">
-        <v>1348</v>
+        <v>1349</v>
       </c>
       <c r="H496" s="4" t="s">
-        <v>1349</v>
+        <v>1350</v>
       </c>
       <c r="I496" s="4" t="s">
-        <v>1350</v>
+        <v>1351</v>
       </c>
       <c r="J496" s="4" t="s">
-        <v>1351</v>
+        <v>1352</v>
       </c>
       <c r="K496" s="5"/>
       <c r="L496" s="5"/>
@@ -21228,34 +21237,34 @@
     </row>
     <row r="497" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A497" s="2" t="s">
-        <v>1352</v>
+        <v>1353</v>
       </c>
       <c r="B497" s="4" t="s">
-        <v>1353</v>
+        <v>1354</v>
       </c>
       <c r="C497" s="4" t="s">
-        <v>1354</v>
+        <v>1355</v>
       </c>
       <c r="D497" s="4" t="s">
-        <v>1355</v>
+        <v>1356</v>
       </c>
       <c r="E497" s="4" t="s">
-        <v>1356</v>
+        <v>1357</v>
       </c>
       <c r="F497" s="4" t="s">
-        <v>1357</v>
+        <v>1358</v>
       </c>
       <c r="G497" s="4" t="s">
-        <v>1358</v>
+        <v>1359</v>
       </c>
       <c r="H497" s="4" t="s">
-        <v>1359</v>
+        <v>1360</v>
       </c>
       <c r="I497" s="4" t="s">
-        <v>1360</v>
+        <v>1361</v>
       </c>
       <c r="J497" s="4" t="s">
-        <v>1361</v>
+        <v>1362</v>
       </c>
       <c r="K497" s="5"/>
       <c r="L497" s="5"/>
@@ -21276,34 +21285,34 @@
     </row>
     <row r="498" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A498" s="2" t="s">
-        <v>1362</v>
+        <v>1363</v>
       </c>
       <c r="B498" s="4" t="s">
-        <v>1363</v>
+        <v>1364</v>
       </c>
       <c r="C498" s="4" t="s">
-        <v>1364</v>
+        <v>1365</v>
       </c>
       <c r="D498" s="4" t="s">
-        <v>1365</v>
+        <v>1366</v>
       </c>
       <c r="E498" s="4" t="s">
-        <v>1366</v>
+        <v>1367</v>
       </c>
       <c r="F498" s="4" t="s">
-        <v>1367</v>
+        <v>1368</v>
       </c>
       <c r="G498" s="4" t="s">
-        <v>1368</v>
+        <v>1369</v>
       </c>
       <c r="H498" s="4" t="s">
-        <v>1369</v>
+        <v>1370</v>
       </c>
       <c r="I498" s="4" t="s">
-        <v>1370</v>
+        <v>1371</v>
       </c>
       <c r="J498" s="4" t="s">
-        <v>1371</v>
+        <v>1372</v>
       </c>
       <c r="K498" s="5"/>
       <c r="L498" s="5"/>
@@ -21324,34 +21333,34 @@
     </row>
     <row r="499" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A499" s="2" t="s">
-        <v>1372</v>
+        <v>1373</v>
       </c>
       <c r="B499" s="4" t="s">
-        <v>1373</v>
+        <v>1374</v>
       </c>
       <c r="C499" s="4" t="s">
-        <v>1374</v>
+        <v>1375</v>
       </c>
       <c r="D499" s="4" t="s">
-        <v>1375</v>
+        <v>1376</v>
       </c>
       <c r="E499" s="4" t="s">
-        <v>1376</v>
+        <v>1377</v>
       </c>
       <c r="F499" s="4" t="s">
-        <v>1377</v>
+        <v>1378</v>
       </c>
       <c r="G499" s="4" t="s">
-        <v>1378</v>
+        <v>1379</v>
       </c>
       <c r="H499" s="4" t="s">
-        <v>1379</v>
+        <v>1380</v>
       </c>
       <c r="I499" s="4" t="s">
-        <v>1380</v>
+        <v>1381</v>
       </c>
       <c r="J499" s="4" t="s">
-        <v>1381</v>
+        <v>1382</v>
       </c>
       <c r="K499" s="5"/>
       <c r="L499" s="5"/>
@@ -21372,34 +21381,34 @@
     </row>
     <row r="500" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A500" s="2" t="s">
-        <v>1382</v>
+        <v>1383</v>
       </c>
       <c r="B500" s="4" t="s">
-        <v>1383</v>
+        <v>1384</v>
       </c>
       <c r="C500" s="4" t="s">
-        <v>1384</v>
+        <v>1385</v>
       </c>
       <c r="D500" s="4" t="s">
-        <v>1385</v>
+        <v>1386</v>
       </c>
       <c r="E500" s="4" t="s">
-        <v>1386</v>
+        <v>1387</v>
       </c>
       <c r="F500" s="4" t="s">
-        <v>1387</v>
+        <v>1388</v>
       </c>
       <c r="G500" s="4" t="s">
-        <v>1388</v>
+        <v>1389</v>
       </c>
       <c r="H500" s="4" t="s">
-        <v>1389</v>
+        <v>1390</v>
       </c>
       <c r="I500" s="4" t="s">
-        <v>1390</v>
+        <v>1391</v>
       </c>
       <c r="J500" s="4" t="s">
-        <v>1391</v>
+        <v>1392</v>
       </c>
       <c r="K500" s="5"/>
       <c r="L500" s="5"/>
@@ -21420,34 +21429,34 @@
     </row>
     <row r="501" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A501" s="2" t="s">
-        <v>1392</v>
+        <v>1393</v>
       </c>
       <c r="B501" s="4" t="s">
-        <v>1393</v>
+        <v>1394</v>
       </c>
       <c r="C501" s="4" t="s">
-        <v>1394</v>
+        <v>1395</v>
       </c>
       <c r="D501" s="4" t="s">
-        <v>1395</v>
+        <v>1396</v>
       </c>
       <c r="E501" s="4" t="s">
-        <v>1396</v>
+        <v>1397</v>
       </c>
       <c r="F501" s="4" t="s">
-        <v>1397</v>
+        <v>1398</v>
       </c>
       <c r="G501" s="4" t="s">
-        <v>1398</v>
+        <v>1399</v>
       </c>
       <c r="H501" s="4" t="s">
-        <v>1399</v>
+        <v>1400</v>
       </c>
       <c r="I501" s="4" t="s">
-        <v>1400</v>
+        <v>1401</v>
       </c>
       <c r="J501" s="4" t="s">
-        <v>1401</v>
+        <v>1402</v>
       </c>
       <c r="K501" s="5"/>
       <c r="L501" s="5"/>
@@ -21468,34 +21477,34 @@
     </row>
     <row r="502" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A502" s="2" t="s">
-        <v>1402</v>
+        <v>1403</v>
       </c>
       <c r="B502" s="4" t="s">
-        <v>1403</v>
+        <v>1404</v>
       </c>
       <c r="C502" s="4" t="s">
-        <v>1404</v>
+        <v>1405</v>
       </c>
       <c r="D502" s="4" t="s">
-        <v>1405</v>
+        <v>1406</v>
       </c>
       <c r="E502" s="4" t="s">
-        <v>1406</v>
+        <v>1407</v>
       </c>
       <c r="F502" s="4" t="s">
-        <v>1407</v>
+        <v>1408</v>
       </c>
       <c r="G502" s="4" t="s">
-        <v>1408</v>
+        <v>1409</v>
       </c>
       <c r="H502" s="4" t="s">
-        <v>1409</v>
+        <v>1410</v>
       </c>
       <c r="I502" s="4" t="s">
-        <v>1410</v>
+        <v>1411</v>
       </c>
       <c r="J502" s="4" t="s">
-        <v>1411</v>
+        <v>1412</v>
       </c>
       <c r="K502" s="5"/>
       <c r="L502" s="5"/>
@@ -21516,30 +21525,30 @@
     </row>
     <row r="503" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A503" s="2" t="s">
-        <v>1412</v>
+        <v>1413</v>
       </c>
       <c r="B503" s="3" t="s">
-        <v>1413</v>
+        <v>1414</v>
       </c>
       <c r="C503" s="3"/>
       <c r="D503" s="3" t="s">
-        <v>1414</v>
+        <v>1415</v>
       </c>
       <c r="E503" s="3"/>
       <c r="F503" s="3" t="s">
-        <v>1415</v>
+        <v>1416</v>
       </c>
       <c r="G503" s="3"/>
       <c r="H503" s="3" t="s">
-        <v>1416</v>
+        <v>1417</v>
       </c>
       <c r="I503" s="3"/>
       <c r="J503" s="3" t="s">
-        <v>1417</v>
+        <v>1418</v>
       </c>
       <c r="K503" s="3"/>
       <c r="L503" s="3" t="s">
-        <v>1418</v>
+        <v>1419</v>
       </c>
       <c r="M503" s="3"/>
       <c r="N503" s="5"/>
@@ -21558,38 +21567,38 @@
     </row>
     <row r="504" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A504" s="2" t="s">
-        <v>1419</v>
+        <v>1420</v>
       </c>
       <c r="B504" s="3" t="s">
-        <v>1420</v>
+        <v>1421</v>
       </c>
       <c r="C504" s="3"/>
       <c r="D504" s="3" t="s">
-        <v>1421</v>
+        <v>1422</v>
       </c>
       <c r="E504" s="3"/>
       <c r="F504" s="3" t="s">
-        <v>1422</v>
+        <v>1423</v>
       </c>
       <c r="G504" s="3"/>
       <c r="H504" s="3" t="s">
-        <v>1423</v>
+        <v>1424</v>
       </c>
       <c r="I504" s="3"/>
       <c r="J504" s="3" t="s">
-        <v>1424</v>
+        <v>1425</v>
       </c>
       <c r="K504" s="3"/>
       <c r="L504" s="3" t="s">
-        <v>1425</v>
+        <v>1426</v>
       </c>
       <c r="M504" s="3"/>
       <c r="N504" s="3" t="s">
-        <v>1426</v>
+        <v>1427</v>
       </c>
       <c r="O504" s="3"/>
       <c r="P504" s="3" t="s">
-        <v>1427</v>
+        <v>1428</v>
       </c>
       <c r="Q504" s="3"/>
       <c r="R504" s="1"/>
@@ -21604,14 +21613,14 @@
     </row>
     <row r="505" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A505" s="2" t="s">
-        <v>1428</v>
+        <v>1429</v>
       </c>
       <c r="B505" s="3" t="s">
-        <v>1429</v>
+        <v>1430</v>
       </c>
       <c r="C505" s="3"/>
       <c r="D505" s="3" t="s">
-        <v>1430</v>
+        <v>1431</v>
       </c>
       <c r="E505" s="3"/>
       <c r="F505" s="5"/>
@@ -21619,19 +21628,19 @@
       <c r="H505" s="5"/>
       <c r="I505" s="5"/>
       <c r="J505" s="3" t="s">
-        <v>1431</v>
+        <v>1432</v>
       </c>
       <c r="K505" s="3"/>
       <c r="L505" s="3" t="s">
-        <v>1432</v>
+        <v>1433</v>
       </c>
       <c r="M505" s="3"/>
       <c r="N505" s="3" t="s">
-        <v>1433</v>
+        <v>1434</v>
       </c>
       <c r="O505" s="3"/>
       <c r="P505" s="3" t="s">
-        <v>1434</v>
+        <v>1435</v>
       </c>
       <c r="Q505" s="3"/>
       <c r="R505" s="1"/>
@@ -21646,30 +21655,30 @@
     </row>
     <row r="506" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A506" s="2" t="s">
-        <v>1435</v>
+        <v>1436</v>
       </c>
       <c r="B506" s="3" t="s">
-        <v>1436</v>
+        <v>1437</v>
       </c>
       <c r="C506" s="3"/>
       <c r="D506" s="3" t="s">
-        <v>1437</v>
+        <v>1438</v>
       </c>
       <c r="E506" s="3"/>
       <c r="F506" s="3" t="s">
-        <v>1438</v>
+        <v>1439</v>
       </c>
       <c r="G506" s="3"/>
       <c r="H506" s="3" t="s">
-        <v>1439</v>
+        <v>1440</v>
       </c>
       <c r="I506" s="3"/>
       <c r="J506" s="3" t="s">
-        <v>1440</v>
+        <v>1441</v>
       </c>
       <c r="K506" s="3"/>
       <c r="L506" s="3" t="s">
-        <v>1441</v>
+        <v>1442</v>
       </c>
       <c r="M506" s="3"/>
       <c r="N506" s="5"/>
@@ -21688,28 +21697,28 @@
     </row>
     <row r="507" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A507" s="2" t="s">
-        <v>1442</v>
+        <v>1443</v>
       </c>
       <c r="B507" s="4" t="s">
-        <v>1443</v>
+        <v>1444</v>
       </c>
       <c r="C507" s="4" t="s">
-        <v>1444</v>
+        <v>1445</v>
       </c>
       <c r="D507" s="4" t="s">
-        <v>1445</v>
+        <v>1446</v>
       </c>
       <c r="E507" s="4" t="s">
-        <v>1446</v>
+        <v>1447</v>
       </c>
       <c r="F507" s="4" t="s">
-        <v>1447</v>
+        <v>1448</v>
       </c>
       <c r="G507" s="5"/>
       <c r="H507" s="5"/>
       <c r="I507" s="5"/>
       <c r="J507" s="3" t="s">
-        <v>1448</v>
+        <v>1449</v>
       </c>
       <c r="K507" s="3"/>
       <c r="L507" s="5"/>
@@ -21717,10 +21726,10 @@
       <c r="N507" s="5"/>
       <c r="O507" s="5"/>
       <c r="P507" s="4" t="s">
-        <v>1449</v>
+        <v>1450</v>
       </c>
       <c r="Q507" s="4" t="s">
-        <v>1450</v>
+        <v>1451</v>
       </c>
       <c r="R507" s="1"/>
       <c r="S507" s="1"/>
@@ -21734,7 +21743,7 @@
     </row>
     <row r="508" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A508" s="2" t="s">
-        <v>1451</v>
+        <v>1452</v>
       </c>
       <c r="B508" s="5"/>
       <c r="C508" s="5"/>
@@ -21764,7 +21773,7 @@
     </row>
     <row r="509" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A509" s="2" t="s">
-        <v>1452</v>
+        <v>1453</v>
       </c>
       <c r="B509" s="5"/>
       <c r="C509" s="5"/>
@@ -21794,7 +21803,7 @@
     </row>
     <row r="510" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A510" s="2" t="s">
-        <v>1453</v>
+        <v>1454</v>
       </c>
       <c r="B510" s="5"/>
       <c r="C510" s="5"/>
@@ -21824,7 +21833,7 @@
     </row>
     <row r="511" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A511" s="2" t="s">
-        <v>1454</v>
+        <v>1455</v>
       </c>
       <c r="B511" s="5"/>
       <c r="C511" s="5"/>
@@ -21854,7 +21863,7 @@
     </row>
     <row r="512" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A512" s="2" t="s">
-        <v>1455</v>
+        <v>1456</v>
       </c>
       <c r="B512" s="5"/>
       <c r="C512" s="5"/>
@@ -21884,7 +21893,7 @@
     </row>
     <row r="513" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A513" s="2" t="s">
-        <v>1456</v>
+        <v>1457</v>
       </c>
       <c r="B513" s="5"/>
       <c r="C513" s="5"/>
@@ -21914,7 +21923,7 @@
     </row>
     <row r="514" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A514" s="2" t="s">
-        <v>1457</v>
+        <v>1458</v>
       </c>
       <c r="B514" s="5"/>
       <c r="C514" s="5"/>

</xml_diff>

<commit_message>
SQLTone saving and loading from eeprom.
</commit_message>
<xml_diff>
--- a/docs/UV K5 EEPROM.xlsx
+++ b/docs/UV K5 EEPROM.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1460" uniqueCount="1458">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1462" uniqueCount="1460">
   <si>
     <t xml:space="preserve">00</t>
   </si>
@@ -2138,6 +2138,12 @@
   </si>
   <si>
     <t xml:space="preserve">???TX CH???</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BATTERY_TYPE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SQTONE</t>
   </si>
   <si>
     <t xml:space="preserve">0x0EB0</t>
@@ -4496,7 +4502,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -4530,6 +4536,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -4625,7 +4635,7 @@
   <dimension ref="A1:Z1001"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A214" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="S234" activeCellId="0" sqref="S234"/>
+      <selection pane="topLeft" activeCell="B237" activeCellId="0" sqref="B237"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.7421875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -12636,8 +12646,12 @@
       <c r="M236" s="4" t="s">
         <v>705</v>
       </c>
-      <c r="N236" s="5"/>
-      <c r="O236" s="5"/>
+      <c r="N236" s="0" t="s">
+        <v>706</v>
+      </c>
+      <c r="O236" s="9" t="s">
+        <v>707</v>
+      </c>
       <c r="P236" s="5"/>
       <c r="Q236" s="5"/>
       <c r="R236" s="1"/>
@@ -12652,10 +12666,10 @@
     </row>
     <row r="237" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A237" s="2" t="s">
-        <v>706</v>
+        <v>708</v>
       </c>
       <c r="B237" s="3" t="s">
-        <v>707</v>
+        <v>709</v>
       </c>
       <c r="C237" s="3"/>
       <c r="D237" s="3"/>
@@ -12684,10 +12698,10 @@
     </row>
     <row r="238" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A238" s="2" t="s">
-        <v>708</v>
+        <v>710</v>
       </c>
       <c r="B238" s="3" t="s">
-        <v>709</v>
+        <v>711</v>
       </c>
       <c r="C238" s="3"/>
       <c r="D238" s="3"/>
@@ -12716,40 +12730,40 @@
     </row>
     <row r="239" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A239" s="2" t="s">
-        <v>710</v>
+        <v>712</v>
       </c>
       <c r="B239" s="4" t="s">
-        <v>711</v>
+        <v>713</v>
       </c>
       <c r="C239" s="4" t="s">
-        <v>712</v>
+        <v>714</v>
       </c>
       <c r="D239" s="4" t="s">
-        <v>713</v>
+        <v>715</v>
       </c>
       <c r="E239" s="4" t="s">
-        <v>714</v>
+        <v>716</v>
       </c>
       <c r="F239" s="4" t="s">
-        <v>715</v>
+        <v>717</v>
       </c>
       <c r="G239" s="4" t="s">
-        <v>716</v>
+        <v>718</v>
       </c>
       <c r="H239" s="4" t="s">
-        <v>717</v>
+        <v>719</v>
       </c>
       <c r="I239" s="4" t="s">
-        <v>718</v>
+        <v>720</v>
       </c>
       <c r="J239" s="4" t="s">
-        <v>719</v>
+        <v>721</v>
       </c>
       <c r="K239" s="4" t="s">
-        <v>720</v>
+        <v>722</v>
       </c>
       <c r="L239" s="4" t="s">
-        <v>721</v>
+        <v>723</v>
       </c>
       <c r="M239" s="5"/>
       <c r="N239" s="5"/>
@@ -12768,10 +12782,10 @@
     </row>
     <row r="240" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A240" s="2" t="s">
-        <v>722</v>
+        <v>724</v>
       </c>
       <c r="B240" s="3" t="s">
-        <v>723</v>
+        <v>725</v>
       </c>
       <c r="C240" s="3"/>
       <c r="D240" s="3"/>
@@ -12781,7 +12795,7 @@
       <c r="H240" s="3"/>
       <c r="I240" s="3"/>
       <c r="J240" s="3" t="s">
-        <v>724</v>
+        <v>726</v>
       </c>
       <c r="K240" s="3"/>
       <c r="L240" s="3"/>
@@ -12802,10 +12816,10 @@
     </row>
     <row r="241" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A241" s="2" t="s">
-        <v>725</v>
+        <v>727</v>
       </c>
       <c r="B241" s="3" t="s">
-        <v>726</v>
+        <v>728</v>
       </c>
       <c r="C241" s="3"/>
       <c r="D241" s="3"/>
@@ -12815,7 +12829,7 @@
       <c r="H241" s="3"/>
       <c r="I241" s="3"/>
       <c r="J241" s="3" t="s">
-        <v>727</v>
+        <v>729</v>
       </c>
       <c r="K241" s="3"/>
       <c r="L241" s="3"/>
@@ -12836,10 +12850,10 @@
     </row>
     <row r="242" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A242" s="2" t="s">
-        <v>728</v>
+        <v>730</v>
       </c>
       <c r="B242" s="3" t="s">
-        <v>727</v>
+        <v>729</v>
       </c>
       <c r="C242" s="3"/>
       <c r="D242" s="3"/>
@@ -12849,7 +12863,7 @@
       <c r="H242" s="3"/>
       <c r="I242" s="3"/>
       <c r="J242" s="3" t="s">
-        <v>729</v>
+        <v>731</v>
       </c>
       <c r="K242" s="3"/>
       <c r="L242" s="3"/>
@@ -12870,10 +12884,10 @@
     </row>
     <row r="243" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A243" s="2" t="s">
-        <v>730</v>
+        <v>732</v>
       </c>
       <c r="B243" s="3" t="s">
-        <v>729</v>
+        <v>731</v>
       </c>
       <c r="C243" s="3"/>
       <c r="D243" s="3"/>
@@ -12883,25 +12897,25 @@
       <c r="H243" s="3"/>
       <c r="I243" s="3"/>
       <c r="J243" s="4" t="s">
-        <v>731</v>
+        <v>733</v>
       </c>
       <c r="K243" s="4" t="s">
-        <v>732</v>
+        <v>734</v>
       </c>
       <c r="L243" s="4" t="s">
-        <v>733</v>
+        <v>735</v>
       </c>
       <c r="M243" s="4" t="s">
-        <v>734</v>
+        <v>736</v>
       </c>
       <c r="N243" s="4" t="s">
-        <v>735</v>
+        <v>737</v>
       </c>
       <c r="O243" s="4" t="s">
-        <v>736</v>
+        <v>738</v>
       </c>
       <c r="P243" s="4" t="s">
-        <v>737</v>
+        <v>739</v>
       </c>
       <c r="Q243" s="5"/>
       <c r="R243" s="1"/>
@@ -12916,7 +12930,7 @@
     </row>
     <row r="244" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A244" s="2" t="s">
-        <v>738</v>
+        <v>740</v>
       </c>
       <c r="B244" s="5"/>
       <c r="C244" s="5"/>
@@ -12946,10 +12960,10 @@
     </row>
     <row r="245" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A245" s="2" t="s">
-        <v>739</v>
+        <v>741</v>
       </c>
       <c r="B245" s="3" t="s">
-        <v>740</v>
+        <v>742</v>
       </c>
       <c r="C245" s="3"/>
       <c r="D245" s="3"/>
@@ -12978,28 +12992,28 @@
     </row>
     <row r="246" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A246" s="2" t="s">
-        <v>741</v>
+        <v>743</v>
       </c>
       <c r="B246" s="4" t="s">
-        <v>742</v>
+        <v>744</v>
       </c>
       <c r="C246" s="4" t="s">
-        <v>743</v>
+        <v>745</v>
       </c>
       <c r="D246" s="4" t="s">
-        <v>744</v>
+        <v>746</v>
       </c>
       <c r="E246" s="4" t="s">
-        <v>745</v>
+        <v>747</v>
       </c>
       <c r="F246" s="4" t="s">
-        <v>746</v>
+        <v>748</v>
       </c>
       <c r="G246" s="4" t="s">
-        <v>747</v>
+        <v>749</v>
       </c>
       <c r="H246" s="4" t="s">
-        <v>748</v>
+        <v>750</v>
       </c>
       <c r="I246" s="5"/>
       <c r="J246" s="5"/>
@@ -13022,10 +13036,10 @@
     </row>
     <row r="247" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A247" s="2" t="s">
-        <v>749</v>
+        <v>751</v>
       </c>
       <c r="B247" s="3" t="s">
-        <v>750</v>
+        <v>752</v>
       </c>
       <c r="C247" s="3"/>
       <c r="D247" s="3"/>
@@ -13054,10 +13068,10 @@
     </row>
     <row r="248" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A248" s="2" t="s">
-        <v>751</v>
+        <v>753</v>
       </c>
       <c r="B248" s="3" t="s">
-        <v>752</v>
+        <v>754</v>
       </c>
       <c r="C248" s="3"/>
       <c r="D248" s="3"/>
@@ -13086,10 +13100,10 @@
     </row>
     <row r="249" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A249" s="2" t="s">
-        <v>753</v>
+        <v>755</v>
       </c>
       <c r="B249" s="3" t="s">
-        <v>754</v>
+        <v>756</v>
       </c>
       <c r="C249" s="3"/>
       <c r="D249" s="3"/>
@@ -13118,10 +13132,10 @@
     </row>
     <row r="250" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A250" s="2" t="s">
-        <v>755</v>
+        <v>757</v>
       </c>
       <c r="B250" s="3" t="s">
-        <v>756</v>
+        <v>758</v>
       </c>
       <c r="C250" s="3"/>
       <c r="D250" s="3"/>
@@ -13150,10 +13164,10 @@
     </row>
     <row r="251" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A251" s="2" t="s">
-        <v>757</v>
+        <v>759</v>
       </c>
       <c r="B251" s="3" t="s">
-        <v>758</v>
+        <v>760</v>
       </c>
       <c r="C251" s="3"/>
       <c r="D251" s="3"/>
@@ -13182,10 +13196,10 @@
     </row>
     <row r="252" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A252" s="2" t="s">
-        <v>759</v>
+        <v>761</v>
       </c>
       <c r="B252" s="3" t="s">
-        <v>760</v>
+        <v>762</v>
       </c>
       <c r="C252" s="3"/>
       <c r="D252" s="3"/>
@@ -13214,10 +13228,10 @@
     </row>
     <row r="253" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A253" s="2" t="s">
-        <v>761</v>
+        <v>763</v>
       </c>
       <c r="B253" s="3" t="s">
-        <v>762</v>
+        <v>764</v>
       </c>
       <c r="C253" s="3"/>
       <c r="D253" s="3"/>
@@ -13246,10 +13260,10 @@
     </row>
     <row r="254" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A254" s="2" t="s">
-        <v>763</v>
+        <v>765</v>
       </c>
       <c r="B254" s="3" t="s">
-        <v>764</v>
+        <v>766</v>
       </c>
       <c r="C254" s="3"/>
       <c r="D254" s="3"/>
@@ -13278,10 +13292,10 @@
     </row>
     <row r="255" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A255" s="2" t="s">
-        <v>765</v>
+        <v>767</v>
       </c>
       <c r="B255" s="3" t="s">
-        <v>766</v>
+        <v>768</v>
       </c>
       <c r="C255" s="3"/>
       <c r="D255" s="3"/>
@@ -13310,10 +13324,10 @@
     </row>
     <row r="256" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A256" s="2" t="s">
-        <v>767</v>
+        <v>769</v>
       </c>
       <c r="B256" s="3" t="s">
-        <v>768</v>
+        <v>770</v>
       </c>
       <c r="C256" s="3"/>
       <c r="D256" s="3"/>
@@ -13342,10 +13356,10 @@
     </row>
     <row r="257" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A257" s="2" t="s">
-        <v>769</v>
+        <v>771</v>
       </c>
       <c r="B257" s="3" t="s">
-        <v>770</v>
+        <v>772</v>
       </c>
       <c r="C257" s="3"/>
       <c r="D257" s="3"/>
@@ -13374,10 +13388,10 @@
     </row>
     <row r="258" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A258" s="2" t="s">
-        <v>771</v>
+        <v>773</v>
       </c>
       <c r="B258" s="3" t="s">
-        <v>772</v>
+        <v>774</v>
       </c>
       <c r="C258" s="3"/>
       <c r="D258" s="3"/>
@@ -13406,10 +13420,10 @@
     </row>
     <row r="259" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A259" s="2" t="s">
-        <v>773</v>
+        <v>775</v>
       </c>
       <c r="B259" s="3" t="s">
-        <v>774</v>
+        <v>776</v>
       </c>
       <c r="C259" s="3"/>
       <c r="D259" s="3"/>
@@ -13438,10 +13452,10 @@
     </row>
     <row r="260" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A260" s="2" t="s">
-        <v>775</v>
+        <v>777</v>
       </c>
       <c r="B260" s="3" t="s">
-        <v>776</v>
+        <v>778</v>
       </c>
       <c r="C260" s="3"/>
       <c r="D260" s="3"/>
@@ -13470,10 +13484,10 @@
     </row>
     <row r="261" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A261" s="2" t="s">
-        <v>777</v>
+        <v>779</v>
       </c>
       <c r="B261" s="3" t="s">
-        <v>778</v>
+        <v>780</v>
       </c>
       <c r="C261" s="3"/>
       <c r="D261" s="3"/>
@@ -13502,10 +13516,10 @@
     </row>
     <row r="262" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A262" s="2" t="s">
-        <v>779</v>
+        <v>781</v>
       </c>
       <c r="B262" s="3" t="s">
-        <v>780</v>
+        <v>782</v>
       </c>
       <c r="C262" s="3"/>
       <c r="D262" s="3"/>
@@ -13534,10 +13548,10 @@
     </row>
     <row r="263" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A263" s="2" t="s">
-        <v>781</v>
+        <v>783</v>
       </c>
       <c r="B263" s="3" t="s">
-        <v>782</v>
+        <v>784</v>
       </c>
       <c r="C263" s="3"/>
       <c r="D263" s="3"/>
@@ -13566,10 +13580,10 @@
     </row>
     <row r="264" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A264" s="2" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="B264" s="3" t="s">
-        <v>784</v>
+        <v>786</v>
       </c>
       <c r="C264" s="3"/>
       <c r="D264" s="3"/>
@@ -13598,10 +13612,10 @@
     </row>
     <row r="265" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A265" s="2" t="s">
-        <v>785</v>
+        <v>787</v>
       </c>
       <c r="B265" s="3" t="s">
-        <v>786</v>
+        <v>788</v>
       </c>
       <c r="C265" s="3"/>
       <c r="D265" s="3"/>
@@ -13630,10 +13644,10 @@
     </row>
     <row r="266" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A266" s="2" t="s">
-        <v>787</v>
+        <v>789</v>
       </c>
       <c r="B266" s="3" t="s">
-        <v>788</v>
+        <v>790</v>
       </c>
       <c r="C266" s="3"/>
       <c r="D266" s="3"/>
@@ -13662,10 +13676,10 @@
     </row>
     <row r="267" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A267" s="2" t="s">
-        <v>789</v>
+        <v>791</v>
       </c>
       <c r="B267" s="3" t="s">
-        <v>790</v>
+        <v>792</v>
       </c>
       <c r="C267" s="3"/>
       <c r="D267" s="3"/>
@@ -13694,10 +13708,10 @@
     </row>
     <row r="268" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A268" s="2" t="s">
-        <v>791</v>
+        <v>793</v>
       </c>
       <c r="B268" s="3" t="s">
-        <v>792</v>
+        <v>794</v>
       </c>
       <c r="C268" s="3"/>
       <c r="D268" s="3"/>
@@ -13726,10 +13740,10 @@
     </row>
     <row r="269" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A269" s="2" t="s">
-        <v>793</v>
+        <v>795</v>
       </c>
       <c r="B269" s="3" t="s">
-        <v>794</v>
+        <v>796</v>
       </c>
       <c r="C269" s="3"/>
       <c r="D269" s="3"/>
@@ -13758,10 +13772,10 @@
     </row>
     <row r="270" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A270" s="2" t="s">
-        <v>795</v>
+        <v>797</v>
       </c>
       <c r="B270" s="3" t="s">
-        <v>796</v>
+        <v>798</v>
       </c>
       <c r="C270" s="3"/>
       <c r="D270" s="3"/>
@@ -13790,10 +13804,10 @@
     </row>
     <row r="271" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A271" s="2" t="s">
-        <v>797</v>
+        <v>799</v>
       </c>
       <c r="B271" s="3" t="s">
-        <v>798</v>
+        <v>800</v>
       </c>
       <c r="C271" s="3"/>
       <c r="D271" s="3"/>
@@ -13822,10 +13836,10 @@
     </row>
     <row r="272" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A272" s="2" t="s">
-        <v>799</v>
+        <v>801</v>
       </c>
       <c r="B272" s="3" t="s">
-        <v>800</v>
+        <v>802</v>
       </c>
       <c r="C272" s="3"/>
       <c r="D272" s="3"/>
@@ -13854,10 +13868,10 @@
     </row>
     <row r="273" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A273" s="2" t="s">
-        <v>801</v>
+        <v>803</v>
       </c>
       <c r="B273" s="3" t="s">
-        <v>802</v>
+        <v>804</v>
       </c>
       <c r="C273" s="3"/>
       <c r="D273" s="3"/>
@@ -13886,10 +13900,10 @@
     </row>
     <row r="274" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A274" s="2" t="s">
-        <v>803</v>
+        <v>805</v>
       </c>
       <c r="B274" s="3" t="s">
-        <v>804</v>
+        <v>806</v>
       </c>
       <c r="C274" s="3"/>
       <c r="D274" s="3"/>
@@ -13918,10 +13932,10 @@
     </row>
     <row r="275" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A275" s="2" t="s">
-        <v>805</v>
+        <v>807</v>
       </c>
       <c r="B275" s="3" t="s">
-        <v>806</v>
+        <v>808</v>
       </c>
       <c r="C275" s="3"/>
       <c r="D275" s="3"/>
@@ -13950,10 +13964,10 @@
     </row>
     <row r="276" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A276" s="2" t="s">
-        <v>807</v>
+        <v>809</v>
       </c>
       <c r="B276" s="3" t="s">
-        <v>808</v>
+        <v>810</v>
       </c>
       <c r="C276" s="3"/>
       <c r="D276" s="3"/>
@@ -13982,10 +13996,10 @@
     </row>
     <row r="277" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A277" s="2" t="s">
-        <v>809</v>
+        <v>811</v>
       </c>
       <c r="B277" s="3" t="s">
-        <v>810</v>
+        <v>812</v>
       </c>
       <c r="C277" s="3"/>
       <c r="D277" s="3"/>
@@ -14014,10 +14028,10 @@
     </row>
     <row r="278" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A278" s="2" t="s">
-        <v>811</v>
+        <v>813</v>
       </c>
       <c r="B278" s="3" t="s">
-        <v>812</v>
+        <v>814</v>
       </c>
       <c r="C278" s="3"/>
       <c r="D278" s="3"/>
@@ -14046,10 +14060,10 @@
     </row>
     <row r="279" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A279" s="2" t="s">
-        <v>813</v>
+        <v>815</v>
       </c>
       <c r="B279" s="3" t="s">
-        <v>814</v>
+        <v>816</v>
       </c>
       <c r="C279" s="3"/>
       <c r="D279" s="3"/>
@@ -14078,10 +14092,10 @@
     </row>
     <row r="280" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A280" s="2" t="s">
-        <v>815</v>
+        <v>817</v>
       </c>
       <c r="B280" s="3" t="s">
-        <v>816</v>
+        <v>818</v>
       </c>
       <c r="C280" s="3"/>
       <c r="D280" s="3"/>
@@ -14110,10 +14124,10 @@
     </row>
     <row r="281" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A281" s="2" t="s">
-        <v>817</v>
+        <v>819</v>
       </c>
       <c r="B281" s="3" t="s">
-        <v>818</v>
+        <v>820</v>
       </c>
       <c r="C281" s="3"/>
       <c r="D281" s="3"/>
@@ -14142,10 +14156,10 @@
     </row>
     <row r="282" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A282" s="2" t="s">
-        <v>819</v>
+        <v>821</v>
       </c>
       <c r="B282" s="3" t="s">
-        <v>820</v>
+        <v>822</v>
       </c>
       <c r="C282" s="3"/>
       <c r="D282" s="3"/>
@@ -14174,10 +14188,10 @@
     </row>
     <row r="283" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A283" s="2" t="s">
-        <v>821</v>
+        <v>823</v>
       </c>
       <c r="B283" s="3" t="s">
-        <v>822</v>
+        <v>824</v>
       </c>
       <c r="C283" s="3"/>
       <c r="D283" s="3"/>
@@ -14206,10 +14220,10 @@
     </row>
     <row r="284" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A284" s="2" t="s">
-        <v>823</v>
+        <v>825</v>
       </c>
       <c r="B284" s="3" t="s">
-        <v>824</v>
+        <v>826</v>
       </c>
       <c r="C284" s="3"/>
       <c r="D284" s="3"/>
@@ -14238,10 +14252,10 @@
     </row>
     <row r="285" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A285" s="2" t="s">
-        <v>825</v>
+        <v>827</v>
       </c>
       <c r="B285" s="3" t="s">
-        <v>826</v>
+        <v>828</v>
       </c>
       <c r="C285" s="3"/>
       <c r="D285" s="3"/>
@@ -14270,10 +14284,10 @@
     </row>
     <row r="286" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A286" s="2" t="s">
-        <v>827</v>
+        <v>829</v>
       </c>
       <c r="B286" s="3" t="s">
-        <v>828</v>
+        <v>830</v>
       </c>
       <c r="C286" s="3"/>
       <c r="D286" s="3"/>
@@ -14302,10 +14316,10 @@
     </row>
     <row r="287" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A287" s="2" t="s">
-        <v>829</v>
+        <v>831</v>
       </c>
       <c r="B287" s="3" t="s">
-        <v>830</v>
+        <v>832</v>
       </c>
       <c r="C287" s="3"/>
       <c r="D287" s="3"/>
@@ -14334,10 +14348,10 @@
     </row>
     <row r="288" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A288" s="2" t="s">
-        <v>831</v>
+        <v>833</v>
       </c>
       <c r="B288" s="3" t="s">
-        <v>832</v>
+        <v>834</v>
       </c>
       <c r="C288" s="3"/>
       <c r="D288" s="3"/>
@@ -14366,10 +14380,10 @@
     </row>
     <row r="289" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A289" s="2" t="s">
-        <v>833</v>
+        <v>835</v>
       </c>
       <c r="B289" s="3" t="s">
-        <v>834</v>
+        <v>836</v>
       </c>
       <c r="C289" s="3"/>
       <c r="D289" s="3"/>
@@ -14398,10 +14412,10 @@
     </row>
     <row r="290" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A290" s="2" t="s">
-        <v>835</v>
+        <v>837</v>
       </c>
       <c r="B290" s="3" t="s">
-        <v>836</v>
+        <v>838</v>
       </c>
       <c r="C290" s="3"/>
       <c r="D290" s="3"/>
@@ -14430,10 +14444,10 @@
     </row>
     <row r="291" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A291" s="2" t="s">
-        <v>837</v>
+        <v>839</v>
       </c>
       <c r="B291" s="3" t="s">
-        <v>838</v>
+        <v>840</v>
       </c>
       <c r="C291" s="3"/>
       <c r="D291" s="3"/>
@@ -14462,10 +14476,10 @@
     </row>
     <row r="292" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A292" s="2" t="s">
-        <v>839</v>
+        <v>841</v>
       </c>
       <c r="B292" s="3" t="s">
-        <v>840</v>
+        <v>842</v>
       </c>
       <c r="C292" s="3"/>
       <c r="D292" s="3"/>
@@ -14494,10 +14508,10 @@
     </row>
     <row r="293" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A293" s="2" t="s">
-        <v>841</v>
+        <v>843</v>
       </c>
       <c r="B293" s="3" t="s">
-        <v>842</v>
+        <v>844</v>
       </c>
       <c r="C293" s="3"/>
       <c r="D293" s="3"/>
@@ -14526,10 +14540,10 @@
     </row>
     <row r="294" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A294" s="2" t="s">
-        <v>843</v>
+        <v>845</v>
       </c>
       <c r="B294" s="3" t="s">
-        <v>844</v>
+        <v>846</v>
       </c>
       <c r="C294" s="3"/>
       <c r="D294" s="3"/>
@@ -14558,10 +14572,10 @@
     </row>
     <row r="295" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A295" s="2" t="s">
-        <v>845</v>
+        <v>847</v>
       </c>
       <c r="B295" s="3" t="s">
-        <v>846</v>
+        <v>848</v>
       </c>
       <c r="C295" s="3"/>
       <c r="D295" s="3"/>
@@ -14590,10 +14604,10 @@
     </row>
     <row r="296" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A296" s="2" t="s">
-        <v>847</v>
+        <v>849</v>
       </c>
       <c r="B296" s="3" t="s">
-        <v>848</v>
+        <v>850</v>
       </c>
       <c r="C296" s="3"/>
       <c r="D296" s="3"/>
@@ -14622,10 +14636,10 @@
     </row>
     <row r="297" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A297" s="2" t="s">
-        <v>849</v>
+        <v>851</v>
       </c>
       <c r="B297" s="3" t="s">
-        <v>850</v>
+        <v>852</v>
       </c>
       <c r="C297" s="3"/>
       <c r="D297" s="3"/>
@@ -14654,10 +14668,10 @@
     </row>
     <row r="298" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A298" s="2" t="s">
-        <v>851</v>
+        <v>853</v>
       </c>
       <c r="B298" s="3" t="s">
-        <v>852</v>
+        <v>854</v>
       </c>
       <c r="C298" s="3"/>
       <c r="D298" s="3"/>
@@ -14686,10 +14700,10 @@
     </row>
     <row r="299" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A299" s="2" t="s">
-        <v>853</v>
+        <v>855</v>
       </c>
       <c r="B299" s="3" t="s">
-        <v>854</v>
+        <v>856</v>
       </c>
       <c r="C299" s="3"/>
       <c r="D299" s="3"/>
@@ -14718,10 +14732,10 @@
     </row>
     <row r="300" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A300" s="2" t="s">
-        <v>855</v>
+        <v>857</v>
       </c>
       <c r="B300" s="3" t="s">
-        <v>856</v>
+        <v>858</v>
       </c>
       <c r="C300" s="3"/>
       <c r="D300" s="3"/>
@@ -14750,10 +14764,10 @@
     </row>
     <row r="301" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A301" s="2" t="s">
-        <v>857</v>
+        <v>859</v>
       </c>
       <c r="B301" s="3" t="s">
-        <v>858</v>
+        <v>860</v>
       </c>
       <c r="C301" s="3"/>
       <c r="D301" s="3"/>
@@ -14782,10 +14796,10 @@
     </row>
     <row r="302" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A302" s="2" t="s">
-        <v>859</v>
+        <v>861</v>
       </c>
       <c r="B302" s="3" t="s">
-        <v>860</v>
+        <v>862</v>
       </c>
       <c r="C302" s="3"/>
       <c r="D302" s="3"/>
@@ -14814,10 +14828,10 @@
     </row>
     <row r="303" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A303" s="2" t="s">
-        <v>861</v>
+        <v>863</v>
       </c>
       <c r="B303" s="3" t="s">
-        <v>862</v>
+        <v>864</v>
       </c>
       <c r="C303" s="3"/>
       <c r="D303" s="3"/>
@@ -14846,10 +14860,10 @@
     </row>
     <row r="304" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A304" s="2" t="s">
-        <v>863</v>
+        <v>865</v>
       </c>
       <c r="B304" s="3" t="s">
-        <v>864</v>
+        <v>866</v>
       </c>
       <c r="C304" s="3"/>
       <c r="D304" s="3"/>
@@ -14878,10 +14892,10 @@
     </row>
     <row r="305" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A305" s="2" t="s">
-        <v>865</v>
+        <v>867</v>
       </c>
       <c r="B305" s="3" t="s">
-        <v>866</v>
+        <v>868</v>
       </c>
       <c r="C305" s="3"/>
       <c r="D305" s="3"/>
@@ -14910,10 +14924,10 @@
     </row>
     <row r="306" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A306" s="2" t="s">
-        <v>867</v>
+        <v>869</v>
       </c>
       <c r="B306" s="3" t="s">
-        <v>868</v>
+        <v>870</v>
       </c>
       <c r="C306" s="3"/>
       <c r="D306" s="3"/>
@@ -14942,10 +14956,10 @@
     </row>
     <row r="307" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A307" s="2" t="s">
-        <v>869</v>
+        <v>871</v>
       </c>
       <c r="B307" s="3" t="s">
-        <v>870</v>
+        <v>872</v>
       </c>
       <c r="C307" s="3"/>
       <c r="D307" s="3"/>
@@ -14974,10 +14988,10 @@
     </row>
     <row r="308" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A308" s="2" t="s">
-        <v>871</v>
+        <v>873</v>
       </c>
       <c r="B308" s="3" t="s">
-        <v>872</v>
+        <v>874</v>
       </c>
       <c r="C308" s="3"/>
       <c r="D308" s="3"/>
@@ -15006,10 +15020,10 @@
     </row>
     <row r="309" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A309" s="2" t="s">
-        <v>873</v>
+        <v>875</v>
       </c>
       <c r="B309" s="3" t="s">
-        <v>874</v>
+        <v>876</v>
       </c>
       <c r="C309" s="3"/>
       <c r="D309" s="3"/>
@@ -15038,10 +15052,10 @@
     </row>
     <row r="310" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A310" s="2" t="s">
-        <v>875</v>
+        <v>877</v>
       </c>
       <c r="B310" s="3" t="s">
-        <v>876</v>
+        <v>878</v>
       </c>
       <c r="C310" s="3"/>
       <c r="D310" s="3"/>
@@ -15070,10 +15084,10 @@
     </row>
     <row r="311" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A311" s="2" t="s">
-        <v>877</v>
+        <v>879</v>
       </c>
       <c r="B311" s="3" t="s">
-        <v>878</v>
+        <v>880</v>
       </c>
       <c r="C311" s="3"/>
       <c r="D311" s="3"/>
@@ -15102,10 +15116,10 @@
     </row>
     <row r="312" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A312" s="2" t="s">
-        <v>879</v>
+        <v>881</v>
       </c>
       <c r="B312" s="3" t="s">
-        <v>880</v>
+        <v>882</v>
       </c>
       <c r="C312" s="3"/>
       <c r="D312" s="3"/>
@@ -15134,10 +15148,10 @@
     </row>
     <row r="313" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A313" s="2" t="s">
-        <v>881</v>
+        <v>883</v>
       </c>
       <c r="B313" s="3" t="s">
-        <v>882</v>
+        <v>884</v>
       </c>
       <c r="C313" s="3"/>
       <c r="D313" s="3"/>
@@ -15166,10 +15180,10 @@
     </row>
     <row r="314" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A314" s="2" t="s">
-        <v>883</v>
+        <v>885</v>
       </c>
       <c r="B314" s="3" t="s">
-        <v>884</v>
+        <v>886</v>
       </c>
       <c r="C314" s="3"/>
       <c r="D314" s="3"/>
@@ -15198,10 +15212,10 @@
     </row>
     <row r="315" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A315" s="2" t="s">
-        <v>885</v>
+        <v>887</v>
       </c>
       <c r="B315" s="3" t="s">
-        <v>886</v>
+        <v>888</v>
       </c>
       <c r="C315" s="3"/>
       <c r="D315" s="3"/>
@@ -15230,10 +15244,10 @@
     </row>
     <row r="316" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A316" s="2" t="s">
-        <v>887</v>
+        <v>889</v>
       </c>
       <c r="B316" s="3" t="s">
-        <v>888</v>
+        <v>890</v>
       </c>
       <c r="C316" s="3"/>
       <c r="D316" s="3"/>
@@ -15262,10 +15276,10 @@
     </row>
     <row r="317" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A317" s="2" t="s">
-        <v>889</v>
+        <v>891</v>
       </c>
       <c r="B317" s="3" t="s">
-        <v>890</v>
+        <v>892</v>
       </c>
       <c r="C317" s="3"/>
       <c r="D317" s="3"/>
@@ -15294,10 +15308,10 @@
     </row>
     <row r="318" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A318" s="2" t="s">
-        <v>891</v>
+        <v>893</v>
       </c>
       <c r="B318" s="3" t="s">
-        <v>892</v>
+        <v>894</v>
       </c>
       <c r="C318" s="3"/>
       <c r="D318" s="3"/>
@@ -15326,10 +15340,10 @@
     </row>
     <row r="319" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A319" s="2" t="s">
-        <v>893</v>
+        <v>895</v>
       </c>
       <c r="B319" s="3" t="s">
-        <v>894</v>
+        <v>896</v>
       </c>
       <c r="C319" s="3"/>
       <c r="D319" s="3"/>
@@ -15358,10 +15372,10 @@
     </row>
     <row r="320" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A320" s="2" t="s">
-        <v>895</v>
+        <v>897</v>
       </c>
       <c r="B320" s="3" t="s">
-        <v>896</v>
+        <v>898</v>
       </c>
       <c r="C320" s="3"/>
       <c r="D320" s="3"/>
@@ -15390,10 +15404,10 @@
     </row>
     <row r="321" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A321" s="2" t="s">
-        <v>897</v>
+        <v>899</v>
       </c>
       <c r="B321" s="3" t="s">
-        <v>898</v>
+        <v>900</v>
       </c>
       <c r="C321" s="3"/>
       <c r="D321" s="3"/>
@@ -15422,10 +15436,10 @@
     </row>
     <row r="322" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A322" s="2" t="s">
-        <v>899</v>
+        <v>901</v>
       </c>
       <c r="B322" s="3" t="s">
-        <v>900</v>
+        <v>902</v>
       </c>
       <c r="C322" s="3"/>
       <c r="D322" s="3"/>
@@ -15454,10 +15468,10 @@
     </row>
     <row r="323" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A323" s="2" t="s">
-        <v>901</v>
+        <v>903</v>
       </c>
       <c r="B323" s="3" t="s">
-        <v>902</v>
+        <v>904</v>
       </c>
       <c r="C323" s="3"/>
       <c r="D323" s="3"/>
@@ -15486,10 +15500,10 @@
     </row>
     <row r="324" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A324" s="2" t="s">
-        <v>903</v>
+        <v>905</v>
       </c>
       <c r="B324" s="3" t="s">
-        <v>904</v>
+        <v>906</v>
       </c>
       <c r="C324" s="3"/>
       <c r="D324" s="3"/>
@@ -15518,10 +15532,10 @@
     </row>
     <row r="325" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A325" s="2" t="s">
-        <v>905</v>
+        <v>907</v>
       </c>
       <c r="B325" s="3" t="s">
-        <v>906</v>
+        <v>908</v>
       </c>
       <c r="C325" s="3"/>
       <c r="D325" s="3"/>
@@ -15550,10 +15564,10 @@
     </row>
     <row r="326" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A326" s="2" t="s">
-        <v>907</v>
+        <v>909</v>
       </c>
       <c r="B326" s="3" t="s">
-        <v>908</v>
+        <v>910</v>
       </c>
       <c r="C326" s="3"/>
       <c r="D326" s="3"/>
@@ -15582,10 +15596,10 @@
     </row>
     <row r="327" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A327" s="2" t="s">
-        <v>909</v>
+        <v>911</v>
       </c>
       <c r="B327" s="3" t="s">
-        <v>910</v>
+        <v>912</v>
       </c>
       <c r="C327" s="3"/>
       <c r="D327" s="3"/>
@@ -15614,10 +15628,10 @@
     </row>
     <row r="328" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A328" s="2" t="s">
-        <v>911</v>
+        <v>913</v>
       </c>
       <c r="B328" s="3" t="s">
-        <v>912</v>
+        <v>914</v>
       </c>
       <c r="C328" s="3"/>
       <c r="D328" s="3"/>
@@ -15646,10 +15660,10 @@
     </row>
     <row r="329" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A329" s="2" t="s">
-        <v>913</v>
+        <v>915</v>
       </c>
       <c r="B329" s="3" t="s">
-        <v>914</v>
+        <v>916</v>
       </c>
       <c r="C329" s="3"/>
       <c r="D329" s="3"/>
@@ -15678,10 +15692,10 @@
     </row>
     <row r="330" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A330" s="2" t="s">
-        <v>915</v>
+        <v>917</v>
       </c>
       <c r="B330" s="3" t="s">
-        <v>916</v>
+        <v>918</v>
       </c>
       <c r="C330" s="3"/>
       <c r="D330" s="3"/>
@@ -15710,10 +15724,10 @@
     </row>
     <row r="331" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A331" s="2" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
       <c r="B331" s="3" t="s">
-        <v>918</v>
+        <v>920</v>
       </c>
       <c r="C331" s="3"/>
       <c r="D331" s="3"/>
@@ -15742,10 +15756,10 @@
     </row>
     <row r="332" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A332" s="2" t="s">
-        <v>919</v>
+        <v>921</v>
       </c>
       <c r="B332" s="3" t="s">
-        <v>920</v>
+        <v>922</v>
       </c>
       <c r="C332" s="3"/>
       <c r="D332" s="3"/>
@@ -15774,10 +15788,10 @@
     </row>
     <row r="333" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A333" s="2" t="s">
-        <v>921</v>
+        <v>923</v>
       </c>
       <c r="B333" s="3" t="s">
-        <v>922</v>
+        <v>924</v>
       </c>
       <c r="C333" s="3"/>
       <c r="D333" s="3"/>
@@ -15806,10 +15820,10 @@
     </row>
     <row r="334" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A334" s="2" t="s">
-        <v>923</v>
+        <v>925</v>
       </c>
       <c r="B334" s="3" t="s">
-        <v>924</v>
+        <v>926</v>
       </c>
       <c r="C334" s="3"/>
       <c r="D334" s="3"/>
@@ -15838,10 +15852,10 @@
     </row>
     <row r="335" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A335" s="2" t="s">
-        <v>925</v>
+        <v>927</v>
       </c>
       <c r="B335" s="3" t="s">
-        <v>926</v>
+        <v>928</v>
       </c>
       <c r="C335" s="3"/>
       <c r="D335" s="3"/>
@@ -15870,10 +15884,10 @@
     </row>
     <row r="336" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A336" s="2" t="s">
-        <v>927</v>
+        <v>929</v>
       </c>
       <c r="B336" s="3" t="s">
-        <v>928</v>
+        <v>930</v>
       </c>
       <c r="C336" s="3"/>
       <c r="D336" s="3"/>
@@ -15902,10 +15916,10 @@
     </row>
     <row r="337" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A337" s="2" t="s">
-        <v>929</v>
+        <v>931</v>
       </c>
       <c r="B337" s="3" t="s">
-        <v>930</v>
+        <v>932</v>
       </c>
       <c r="C337" s="3"/>
       <c r="D337" s="3"/>
@@ -15934,10 +15948,10 @@
     </row>
     <row r="338" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A338" s="2" t="s">
-        <v>931</v>
+        <v>933</v>
       </c>
       <c r="B338" s="3" t="s">
-        <v>932</v>
+        <v>934</v>
       </c>
       <c r="C338" s="3"/>
       <c r="D338" s="3"/>
@@ -15966,10 +15980,10 @@
     </row>
     <row r="339" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A339" s="2" t="s">
-        <v>933</v>
+        <v>935</v>
       </c>
       <c r="B339" s="3" t="s">
-        <v>934</v>
+        <v>936</v>
       </c>
       <c r="C339" s="3"/>
       <c r="D339" s="3"/>
@@ -15998,10 +16012,10 @@
     </row>
     <row r="340" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A340" s="2" t="s">
-        <v>935</v>
+        <v>937</v>
       </c>
       <c r="B340" s="3" t="s">
-        <v>936</v>
+        <v>938</v>
       </c>
       <c r="C340" s="3"/>
       <c r="D340" s="3"/>
@@ -16030,10 +16044,10 @@
     </row>
     <row r="341" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A341" s="2" t="s">
-        <v>937</v>
+        <v>939</v>
       </c>
       <c r="B341" s="3" t="s">
-        <v>938</v>
+        <v>940</v>
       </c>
       <c r="C341" s="3"/>
       <c r="D341" s="3"/>
@@ -16062,10 +16076,10 @@
     </row>
     <row r="342" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A342" s="2" t="s">
-        <v>939</v>
+        <v>941</v>
       </c>
       <c r="B342" s="3" t="s">
-        <v>940</v>
+        <v>942</v>
       </c>
       <c r="C342" s="3"/>
       <c r="D342" s="3"/>
@@ -16094,10 +16108,10 @@
     </row>
     <row r="343" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A343" s="2" t="s">
-        <v>941</v>
+        <v>943</v>
       </c>
       <c r="B343" s="3" t="s">
-        <v>942</v>
+        <v>944</v>
       </c>
       <c r="C343" s="3"/>
       <c r="D343" s="3"/>
@@ -16126,10 +16140,10 @@
     </row>
     <row r="344" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A344" s="2" t="s">
-        <v>943</v>
+        <v>945</v>
       </c>
       <c r="B344" s="3" t="s">
-        <v>944</v>
+        <v>946</v>
       </c>
       <c r="C344" s="3"/>
       <c r="D344" s="3"/>
@@ -16158,10 +16172,10 @@
     </row>
     <row r="345" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A345" s="2" t="s">
-        <v>945</v>
+        <v>947</v>
       </c>
       <c r="B345" s="3" t="s">
-        <v>946</v>
+        <v>948</v>
       </c>
       <c r="C345" s="3"/>
       <c r="D345" s="3"/>
@@ -16190,10 +16204,10 @@
     </row>
     <row r="346" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A346" s="2" t="s">
-        <v>947</v>
+        <v>949</v>
       </c>
       <c r="B346" s="3" t="s">
-        <v>948</v>
+        <v>950</v>
       </c>
       <c r="C346" s="3"/>
       <c r="D346" s="3"/>
@@ -16222,10 +16236,10 @@
     </row>
     <row r="347" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A347" s="2" t="s">
-        <v>949</v>
+        <v>951</v>
       </c>
       <c r="B347" s="3" t="s">
-        <v>950</v>
+        <v>952</v>
       </c>
       <c r="C347" s="3"/>
       <c r="D347" s="3"/>
@@ -16254,10 +16268,10 @@
     </row>
     <row r="348" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A348" s="2" t="s">
-        <v>951</v>
+        <v>953</v>
       </c>
       <c r="B348" s="3" t="s">
-        <v>952</v>
+        <v>954</v>
       </c>
       <c r="C348" s="3"/>
       <c r="D348" s="3"/>
@@ -16286,10 +16300,10 @@
     </row>
     <row r="349" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A349" s="2" t="s">
-        <v>953</v>
+        <v>955</v>
       </c>
       <c r="B349" s="3" t="s">
-        <v>954</v>
+        <v>956</v>
       </c>
       <c r="C349" s="3"/>
       <c r="D349" s="3"/>
@@ -16318,10 +16332,10 @@
     </row>
     <row r="350" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A350" s="2" t="s">
-        <v>955</v>
+        <v>957</v>
       </c>
       <c r="B350" s="3" t="s">
-        <v>956</v>
+        <v>958</v>
       </c>
       <c r="C350" s="3"/>
       <c r="D350" s="3"/>
@@ -16350,10 +16364,10 @@
     </row>
     <row r="351" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A351" s="2" t="s">
-        <v>957</v>
+        <v>959</v>
       </c>
       <c r="B351" s="3" t="s">
-        <v>958</v>
+        <v>960</v>
       </c>
       <c r="C351" s="3"/>
       <c r="D351" s="3"/>
@@ -16382,10 +16396,10 @@
     </row>
     <row r="352" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A352" s="2" t="s">
-        <v>959</v>
+        <v>961</v>
       </c>
       <c r="B352" s="3" t="s">
-        <v>960</v>
+        <v>962</v>
       </c>
       <c r="C352" s="3"/>
       <c r="D352" s="3"/>
@@ -16414,10 +16428,10 @@
     </row>
     <row r="353" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A353" s="2" t="s">
-        <v>961</v>
+        <v>963</v>
       </c>
       <c r="B353" s="3" t="s">
-        <v>962</v>
+        <v>964</v>
       </c>
       <c r="C353" s="3"/>
       <c r="D353" s="3"/>
@@ -16446,10 +16460,10 @@
     </row>
     <row r="354" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A354" s="2" t="s">
-        <v>963</v>
+        <v>965</v>
       </c>
       <c r="B354" s="3" t="s">
-        <v>964</v>
+        <v>966</v>
       </c>
       <c r="C354" s="3"/>
       <c r="D354" s="3"/>
@@ -16478,10 +16492,10 @@
     </row>
     <row r="355" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A355" s="2" t="s">
-        <v>965</v>
+        <v>967</v>
       </c>
       <c r="B355" s="3" t="s">
-        <v>966</v>
+        <v>968</v>
       </c>
       <c r="C355" s="3"/>
       <c r="D355" s="3"/>
@@ -16510,10 +16524,10 @@
     </row>
     <row r="356" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A356" s="2" t="s">
-        <v>967</v>
+        <v>969</v>
       </c>
       <c r="B356" s="3" t="s">
-        <v>968</v>
+        <v>970</v>
       </c>
       <c r="C356" s="3"/>
       <c r="D356" s="3"/>
@@ -16542,10 +16556,10 @@
     </row>
     <row r="357" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A357" s="2" t="s">
-        <v>969</v>
+        <v>971</v>
       </c>
       <c r="B357" s="3" t="s">
-        <v>970</v>
+        <v>972</v>
       </c>
       <c r="C357" s="3"/>
       <c r="D357" s="3"/>
@@ -16574,10 +16588,10 @@
     </row>
     <row r="358" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A358" s="2" t="s">
-        <v>971</v>
+        <v>973</v>
       </c>
       <c r="B358" s="3" t="s">
-        <v>972</v>
+        <v>974</v>
       </c>
       <c r="C358" s="3"/>
       <c r="D358" s="3"/>
@@ -16606,10 +16620,10 @@
     </row>
     <row r="359" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A359" s="2" t="s">
-        <v>973</v>
+        <v>975</v>
       </c>
       <c r="B359" s="3" t="s">
-        <v>974</v>
+        <v>976</v>
       </c>
       <c r="C359" s="3"/>
       <c r="D359" s="3"/>
@@ -16638,10 +16652,10 @@
     </row>
     <row r="360" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A360" s="2" t="s">
-        <v>975</v>
+        <v>977</v>
       </c>
       <c r="B360" s="3" t="s">
-        <v>976</v>
+        <v>978</v>
       </c>
       <c r="C360" s="3"/>
       <c r="D360" s="3"/>
@@ -16670,10 +16684,10 @@
     </row>
     <row r="361" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A361" s="2" t="s">
-        <v>977</v>
+        <v>979</v>
       </c>
       <c r="B361" s="3" t="s">
-        <v>978</v>
+        <v>980</v>
       </c>
       <c r="C361" s="3"/>
       <c r="D361" s="3"/>
@@ -16702,10 +16716,10 @@
     </row>
     <row r="362" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A362" s="2" t="s">
-        <v>979</v>
+        <v>981</v>
       </c>
       <c r="B362" s="3" t="s">
-        <v>980</v>
+        <v>982</v>
       </c>
       <c r="C362" s="3"/>
       <c r="D362" s="3"/>
@@ -16734,10 +16748,10 @@
     </row>
     <row r="363" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A363" s="2" t="s">
-        <v>981</v>
+        <v>983</v>
       </c>
       <c r="B363" s="3" t="s">
-        <v>982</v>
+        <v>984</v>
       </c>
       <c r="C363" s="3"/>
       <c r="D363" s="3"/>
@@ -16766,10 +16780,10 @@
     </row>
     <row r="364" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A364" s="2" t="s">
-        <v>983</v>
+        <v>985</v>
       </c>
       <c r="B364" s="3" t="s">
-        <v>984</v>
+        <v>986</v>
       </c>
       <c r="C364" s="3"/>
       <c r="D364" s="3"/>
@@ -16798,10 +16812,10 @@
     </row>
     <row r="365" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A365" s="2" t="s">
-        <v>985</v>
+        <v>987</v>
       </c>
       <c r="B365" s="3" t="s">
-        <v>986</v>
+        <v>988</v>
       </c>
       <c r="C365" s="3"/>
       <c r="D365" s="3"/>
@@ -16830,10 +16844,10 @@
     </row>
     <row r="366" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A366" s="2" t="s">
-        <v>987</v>
+        <v>989</v>
       </c>
       <c r="B366" s="3" t="s">
-        <v>988</v>
+        <v>990</v>
       </c>
       <c r="C366" s="3"/>
       <c r="D366" s="3"/>
@@ -16862,10 +16876,10 @@
     </row>
     <row r="367" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A367" s="2" t="s">
-        <v>989</v>
+        <v>991</v>
       </c>
       <c r="B367" s="3" t="s">
-        <v>990</v>
+        <v>992</v>
       </c>
       <c r="C367" s="3"/>
       <c r="D367" s="3"/>
@@ -16894,10 +16908,10 @@
     </row>
     <row r="368" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A368" s="2" t="s">
-        <v>991</v>
+        <v>993</v>
       </c>
       <c r="B368" s="3" t="s">
-        <v>992</v>
+        <v>994</v>
       </c>
       <c r="C368" s="3"/>
       <c r="D368" s="3"/>
@@ -16926,10 +16940,10 @@
     </row>
     <row r="369" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A369" s="2" t="s">
-        <v>993</v>
+        <v>995</v>
       </c>
       <c r="B369" s="3" t="s">
-        <v>994</v>
+        <v>996</v>
       </c>
       <c r="C369" s="3"/>
       <c r="D369" s="3"/>
@@ -16958,10 +16972,10 @@
     </row>
     <row r="370" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A370" s="2" t="s">
-        <v>995</v>
+        <v>997</v>
       </c>
       <c r="B370" s="3" t="s">
-        <v>996</v>
+        <v>998</v>
       </c>
       <c r="C370" s="3"/>
       <c r="D370" s="3"/>
@@ -16990,10 +17004,10 @@
     </row>
     <row r="371" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A371" s="2" t="s">
-        <v>997</v>
+        <v>999</v>
       </c>
       <c r="B371" s="3" t="s">
-        <v>998</v>
+        <v>1000</v>
       </c>
       <c r="C371" s="3"/>
       <c r="D371" s="3"/>
@@ -17022,10 +17036,10 @@
     </row>
     <row r="372" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A372" s="2" t="s">
-        <v>999</v>
+        <v>1001</v>
       </c>
       <c r="B372" s="3" t="s">
-        <v>1000</v>
+        <v>1002</v>
       </c>
       <c r="C372" s="3"/>
       <c r="D372" s="3"/>
@@ -17054,10 +17068,10 @@
     </row>
     <row r="373" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A373" s="2" t="s">
-        <v>1001</v>
+        <v>1003</v>
       </c>
       <c r="B373" s="3" t="s">
-        <v>1002</v>
+        <v>1004</v>
       </c>
       <c r="C373" s="3"/>
       <c r="D373" s="3"/>
@@ -17086,10 +17100,10 @@
     </row>
     <row r="374" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A374" s="2" t="s">
-        <v>1003</v>
+        <v>1005</v>
       </c>
       <c r="B374" s="3" t="s">
-        <v>1004</v>
+        <v>1006</v>
       </c>
       <c r="C374" s="3"/>
       <c r="D374" s="3"/>
@@ -17118,10 +17132,10 @@
     </row>
     <row r="375" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A375" s="2" t="s">
-        <v>1005</v>
+        <v>1007</v>
       </c>
       <c r="B375" s="3" t="s">
-        <v>1006</v>
+        <v>1008</v>
       </c>
       <c r="C375" s="3"/>
       <c r="D375" s="3"/>
@@ -17150,10 +17164,10 @@
     </row>
     <row r="376" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A376" s="2" t="s">
-        <v>1007</v>
+        <v>1009</v>
       </c>
       <c r="B376" s="3" t="s">
-        <v>1008</v>
+        <v>1010</v>
       </c>
       <c r="C376" s="3"/>
       <c r="D376" s="3"/>
@@ -17182,10 +17196,10 @@
     </row>
     <row r="377" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A377" s="2" t="s">
-        <v>1009</v>
+        <v>1011</v>
       </c>
       <c r="B377" s="3" t="s">
-        <v>1010</v>
+        <v>1012</v>
       </c>
       <c r="C377" s="3"/>
       <c r="D377" s="3"/>
@@ -17214,10 +17228,10 @@
     </row>
     <row r="378" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A378" s="2" t="s">
-        <v>1011</v>
+        <v>1013</v>
       </c>
       <c r="B378" s="3" t="s">
-        <v>1012</v>
+        <v>1014</v>
       </c>
       <c r="C378" s="3"/>
       <c r="D378" s="3"/>
@@ -17246,10 +17260,10 @@
     </row>
     <row r="379" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A379" s="2" t="s">
-        <v>1013</v>
+        <v>1015</v>
       </c>
       <c r="B379" s="3" t="s">
-        <v>1014</v>
+        <v>1016</v>
       </c>
       <c r="C379" s="3"/>
       <c r="D379" s="3"/>
@@ -17278,10 +17292,10 @@
     </row>
     <row r="380" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A380" s="2" t="s">
-        <v>1015</v>
+        <v>1017</v>
       </c>
       <c r="B380" s="3" t="s">
-        <v>1016</v>
+        <v>1018</v>
       </c>
       <c r="C380" s="3"/>
       <c r="D380" s="3"/>
@@ -17310,10 +17324,10 @@
     </row>
     <row r="381" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A381" s="2" t="s">
-        <v>1017</v>
+        <v>1019</v>
       </c>
       <c r="B381" s="3" t="s">
-        <v>1018</v>
+        <v>1020</v>
       </c>
       <c r="C381" s="3"/>
       <c r="D381" s="3"/>
@@ -17342,10 +17356,10 @@
     </row>
     <row r="382" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A382" s="2" t="s">
-        <v>1019</v>
+        <v>1021</v>
       </c>
       <c r="B382" s="3" t="s">
-        <v>1020</v>
+        <v>1022</v>
       </c>
       <c r="C382" s="3"/>
       <c r="D382" s="3"/>
@@ -17374,10 +17388,10 @@
     </row>
     <row r="383" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A383" s="2" t="s">
-        <v>1021</v>
+        <v>1023</v>
       </c>
       <c r="B383" s="3" t="s">
-        <v>1022</v>
+        <v>1024</v>
       </c>
       <c r="C383" s="3"/>
       <c r="D383" s="3"/>
@@ -17406,10 +17420,10 @@
     </row>
     <row r="384" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A384" s="2" t="s">
-        <v>1023</v>
+        <v>1025</v>
       </c>
       <c r="B384" s="3" t="s">
-        <v>1024</v>
+        <v>1026</v>
       </c>
       <c r="C384" s="3"/>
       <c r="D384" s="3"/>
@@ -17438,10 +17452,10 @@
     </row>
     <row r="385" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A385" s="2" t="s">
-        <v>1025</v>
+        <v>1027</v>
       </c>
       <c r="B385" s="3" t="s">
-        <v>1026</v>
+        <v>1028</v>
       </c>
       <c r="C385" s="3"/>
       <c r="D385" s="3"/>
@@ -17470,10 +17484,10 @@
     </row>
     <row r="386" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A386" s="2" t="s">
-        <v>1027</v>
+        <v>1029</v>
       </c>
       <c r="B386" s="3" t="s">
-        <v>1028</v>
+        <v>1030</v>
       </c>
       <c r="C386" s="3"/>
       <c r="D386" s="3"/>
@@ -17502,10 +17516,10 @@
     </row>
     <row r="387" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A387" s="2" t="s">
-        <v>1029</v>
+        <v>1031</v>
       </c>
       <c r="B387" s="3" t="s">
-        <v>1030</v>
+        <v>1032</v>
       </c>
       <c r="C387" s="3"/>
       <c r="D387" s="3"/>
@@ -17534,10 +17548,10 @@
     </row>
     <row r="388" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A388" s="2" t="s">
-        <v>1031</v>
+        <v>1033</v>
       </c>
       <c r="B388" s="3" t="s">
-        <v>1032</v>
+        <v>1034</v>
       </c>
       <c r="C388" s="3"/>
       <c r="D388" s="3"/>
@@ -17566,10 +17580,10 @@
     </row>
     <row r="389" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A389" s="2" t="s">
-        <v>1033</v>
+        <v>1035</v>
       </c>
       <c r="B389" s="3" t="s">
-        <v>1034</v>
+        <v>1036</v>
       </c>
       <c r="C389" s="3"/>
       <c r="D389" s="3"/>
@@ -17598,10 +17612,10 @@
     </row>
     <row r="390" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A390" s="2" t="s">
-        <v>1035</v>
+        <v>1037</v>
       </c>
       <c r="B390" s="3" t="s">
-        <v>1036</v>
+        <v>1038</v>
       </c>
       <c r="C390" s="3"/>
       <c r="D390" s="3"/>
@@ -17630,10 +17644,10 @@
     </row>
     <row r="391" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A391" s="2" t="s">
-        <v>1037</v>
+        <v>1039</v>
       </c>
       <c r="B391" s="3" t="s">
-        <v>1038</v>
+        <v>1040</v>
       </c>
       <c r="C391" s="3"/>
       <c r="D391" s="3"/>
@@ -17662,10 +17676,10 @@
     </row>
     <row r="392" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A392" s="2" t="s">
-        <v>1039</v>
+        <v>1041</v>
       </c>
       <c r="B392" s="3" t="s">
-        <v>1040</v>
+        <v>1042</v>
       </c>
       <c r="C392" s="3"/>
       <c r="D392" s="3"/>
@@ -17694,10 +17708,10 @@
     </row>
     <row r="393" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A393" s="2" t="s">
-        <v>1041</v>
+        <v>1043</v>
       </c>
       <c r="B393" s="3" t="s">
-        <v>1042</v>
+        <v>1044</v>
       </c>
       <c r="C393" s="3"/>
       <c r="D393" s="3"/>
@@ -17726,10 +17740,10 @@
     </row>
     <row r="394" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A394" s="2" t="s">
-        <v>1043</v>
+        <v>1045</v>
       </c>
       <c r="B394" s="3" t="s">
-        <v>1044</v>
+        <v>1046</v>
       </c>
       <c r="C394" s="3"/>
       <c r="D394" s="3"/>
@@ -17758,10 +17772,10 @@
     </row>
     <row r="395" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A395" s="2" t="s">
-        <v>1045</v>
+        <v>1047</v>
       </c>
       <c r="B395" s="3" t="s">
-        <v>1046</v>
+        <v>1048</v>
       </c>
       <c r="C395" s="3"/>
       <c r="D395" s="3"/>
@@ -17790,10 +17804,10 @@
     </row>
     <row r="396" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A396" s="2" t="s">
-        <v>1047</v>
+        <v>1049</v>
       </c>
       <c r="B396" s="3" t="s">
-        <v>1048</v>
+        <v>1050</v>
       </c>
       <c r="C396" s="3"/>
       <c r="D396" s="3"/>
@@ -17822,10 +17836,10 @@
     </row>
     <row r="397" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A397" s="2" t="s">
-        <v>1049</v>
+        <v>1051</v>
       </c>
       <c r="B397" s="3" t="s">
-        <v>1050</v>
+        <v>1052</v>
       </c>
       <c r="C397" s="3"/>
       <c r="D397" s="3"/>
@@ -17854,10 +17868,10 @@
     </row>
     <row r="398" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A398" s="2" t="s">
-        <v>1051</v>
+        <v>1053</v>
       </c>
       <c r="B398" s="3" t="s">
-        <v>1052</v>
+        <v>1054</v>
       </c>
       <c r="C398" s="3"/>
       <c r="D398" s="3"/>
@@ -17886,10 +17900,10 @@
     </row>
     <row r="399" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A399" s="2" t="s">
-        <v>1053</v>
+        <v>1055</v>
       </c>
       <c r="B399" s="3" t="s">
-        <v>1054</v>
+        <v>1056</v>
       </c>
       <c r="C399" s="3"/>
       <c r="D399" s="3"/>
@@ -17918,10 +17932,10 @@
     </row>
     <row r="400" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A400" s="2" t="s">
-        <v>1055</v>
+        <v>1057</v>
       </c>
       <c r="B400" s="3" t="s">
-        <v>1056</v>
+        <v>1058</v>
       </c>
       <c r="C400" s="3"/>
       <c r="D400" s="3"/>
@@ -17950,10 +17964,10 @@
     </row>
     <row r="401" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A401" s="2" t="s">
-        <v>1057</v>
+        <v>1059</v>
       </c>
       <c r="B401" s="3" t="s">
-        <v>1058</v>
+        <v>1060</v>
       </c>
       <c r="C401" s="3"/>
       <c r="D401" s="3"/>
@@ -17982,10 +17996,10 @@
     </row>
     <row r="402" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A402" s="2" t="s">
-        <v>1059</v>
+        <v>1061</v>
       </c>
       <c r="B402" s="3" t="s">
-        <v>1060</v>
+        <v>1062</v>
       </c>
       <c r="C402" s="3"/>
       <c r="D402" s="3"/>
@@ -18014,10 +18028,10 @@
     </row>
     <row r="403" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A403" s="2" t="s">
-        <v>1061</v>
+        <v>1063</v>
       </c>
       <c r="B403" s="3" t="s">
-        <v>1062</v>
+        <v>1064</v>
       </c>
       <c r="C403" s="3"/>
       <c r="D403" s="3"/>
@@ -18046,10 +18060,10 @@
     </row>
     <row r="404" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A404" s="2" t="s">
-        <v>1063</v>
+        <v>1065</v>
       </c>
       <c r="B404" s="3" t="s">
-        <v>1064</v>
+        <v>1066</v>
       </c>
       <c r="C404" s="3"/>
       <c r="D404" s="3"/>
@@ -18078,10 +18092,10 @@
     </row>
     <row r="405" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A405" s="2" t="s">
-        <v>1065</v>
+        <v>1067</v>
       </c>
       <c r="B405" s="3" t="s">
-        <v>1066</v>
+        <v>1068</v>
       </c>
       <c r="C405" s="3"/>
       <c r="D405" s="3"/>
@@ -18110,10 +18124,10 @@
     </row>
     <row r="406" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A406" s="2" t="s">
-        <v>1067</v>
+        <v>1069</v>
       </c>
       <c r="B406" s="3" t="s">
-        <v>1068</v>
+        <v>1070</v>
       </c>
       <c r="C406" s="3"/>
       <c r="D406" s="3"/>
@@ -18142,10 +18156,10 @@
     </row>
     <row r="407" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A407" s="2" t="s">
-        <v>1069</v>
+        <v>1071</v>
       </c>
       <c r="B407" s="3" t="s">
-        <v>1070</v>
+        <v>1072</v>
       </c>
       <c r="C407" s="3"/>
       <c r="D407" s="3"/>
@@ -18174,10 +18188,10 @@
     </row>
     <row r="408" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A408" s="2" t="s">
-        <v>1071</v>
+        <v>1073</v>
       </c>
       <c r="B408" s="3" t="s">
-        <v>1072</v>
+        <v>1074</v>
       </c>
       <c r="C408" s="3"/>
       <c r="D408" s="3"/>
@@ -18206,10 +18220,10 @@
     </row>
     <row r="409" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A409" s="2" t="s">
-        <v>1073</v>
+        <v>1075</v>
       </c>
       <c r="B409" s="3" t="s">
-        <v>1074</v>
+        <v>1076</v>
       </c>
       <c r="C409" s="3"/>
       <c r="D409" s="3"/>
@@ -18238,10 +18252,10 @@
     </row>
     <row r="410" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A410" s="2" t="s">
-        <v>1075</v>
+        <v>1077</v>
       </c>
       <c r="B410" s="3" t="s">
-        <v>1076</v>
+        <v>1078</v>
       </c>
       <c r="C410" s="3"/>
       <c r="D410" s="3"/>
@@ -18270,10 +18284,10 @@
     </row>
     <row r="411" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A411" s="2" t="s">
-        <v>1077</v>
+        <v>1079</v>
       </c>
       <c r="B411" s="3" t="s">
-        <v>1078</v>
+        <v>1080</v>
       </c>
       <c r="C411" s="3"/>
       <c r="D411" s="3"/>
@@ -18302,10 +18316,10 @@
     </row>
     <row r="412" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A412" s="2" t="s">
-        <v>1079</v>
+        <v>1081</v>
       </c>
       <c r="B412" s="3" t="s">
-        <v>1080</v>
+        <v>1082</v>
       </c>
       <c r="C412" s="3"/>
       <c r="D412" s="3"/>
@@ -18334,10 +18348,10 @@
     </row>
     <row r="413" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A413" s="2" t="s">
-        <v>1081</v>
+        <v>1083</v>
       </c>
       <c r="B413" s="3" t="s">
-        <v>1082</v>
+        <v>1084</v>
       </c>
       <c r="C413" s="3"/>
       <c r="D413" s="3"/>
@@ -18366,10 +18380,10 @@
     </row>
     <row r="414" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A414" s="2" t="s">
-        <v>1083</v>
+        <v>1085</v>
       </c>
       <c r="B414" s="3" t="s">
-        <v>1084</v>
+        <v>1086</v>
       </c>
       <c r="C414" s="3"/>
       <c r="D414" s="3"/>
@@ -18398,10 +18412,10 @@
     </row>
     <row r="415" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A415" s="2" t="s">
-        <v>1085</v>
+        <v>1087</v>
       </c>
       <c r="B415" s="3" t="s">
-        <v>1086</v>
+        <v>1088</v>
       </c>
       <c r="C415" s="3"/>
       <c r="D415" s="3"/>
@@ -18430,10 +18444,10 @@
     </row>
     <row r="416" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A416" s="2" t="s">
-        <v>1087</v>
+        <v>1089</v>
       </c>
       <c r="B416" s="3" t="s">
-        <v>1088</v>
+        <v>1090</v>
       </c>
       <c r="C416" s="3"/>
       <c r="D416" s="3"/>
@@ -18462,10 +18476,10 @@
     </row>
     <row r="417" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A417" s="2" t="s">
-        <v>1089</v>
+        <v>1091</v>
       </c>
       <c r="B417" s="3" t="s">
-        <v>1090</v>
+        <v>1092</v>
       </c>
       <c r="C417" s="3"/>
       <c r="D417" s="3"/>
@@ -18494,10 +18508,10 @@
     </row>
     <row r="418" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A418" s="2" t="s">
-        <v>1091</v>
+        <v>1093</v>
       </c>
       <c r="B418" s="3" t="s">
-        <v>1092</v>
+        <v>1094</v>
       </c>
       <c r="C418" s="3"/>
       <c r="D418" s="3"/>
@@ -18526,10 +18540,10 @@
     </row>
     <row r="419" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A419" s="2" t="s">
-        <v>1093</v>
+        <v>1095</v>
       </c>
       <c r="B419" s="3" t="s">
-        <v>1094</v>
+        <v>1096</v>
       </c>
       <c r="C419" s="3"/>
       <c r="D419" s="3"/>
@@ -18558,10 +18572,10 @@
     </row>
     <row r="420" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A420" s="2" t="s">
-        <v>1095</v>
+        <v>1097</v>
       </c>
       <c r="B420" s="3" t="s">
-        <v>1096</v>
+        <v>1098</v>
       </c>
       <c r="C420" s="3"/>
       <c r="D420" s="3"/>
@@ -18590,10 +18604,10 @@
     </row>
     <row r="421" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A421" s="2" t="s">
-        <v>1097</v>
+        <v>1099</v>
       </c>
       <c r="B421" s="3" t="s">
-        <v>1098</v>
+        <v>1100</v>
       </c>
       <c r="C421" s="3"/>
       <c r="D421" s="3"/>
@@ -18622,10 +18636,10 @@
     </row>
     <row r="422" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A422" s="2" t="s">
-        <v>1099</v>
+        <v>1101</v>
       </c>
       <c r="B422" s="3" t="s">
-        <v>1100</v>
+        <v>1102</v>
       </c>
       <c r="C422" s="3"/>
       <c r="D422" s="3"/>
@@ -18654,10 +18668,10 @@
     </row>
     <row r="423" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A423" s="2" t="s">
-        <v>1101</v>
+        <v>1103</v>
       </c>
       <c r="B423" s="3" t="s">
-        <v>1102</v>
+        <v>1104</v>
       </c>
       <c r="C423" s="3"/>
       <c r="D423" s="3"/>
@@ -18686,10 +18700,10 @@
     </row>
     <row r="424" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A424" s="2" t="s">
-        <v>1103</v>
+        <v>1105</v>
       </c>
       <c r="B424" s="3" t="s">
-        <v>1104</v>
+        <v>1106</v>
       </c>
       <c r="C424" s="3"/>
       <c r="D424" s="3"/>
@@ -18718,10 +18732,10 @@
     </row>
     <row r="425" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A425" s="2" t="s">
-        <v>1105</v>
+        <v>1107</v>
       </c>
       <c r="B425" s="3" t="s">
-        <v>1106</v>
+        <v>1108</v>
       </c>
       <c r="C425" s="3"/>
       <c r="D425" s="3"/>
@@ -18750,10 +18764,10 @@
     </row>
     <row r="426" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A426" s="2" t="s">
-        <v>1107</v>
+        <v>1109</v>
       </c>
       <c r="B426" s="3" t="s">
-        <v>1108</v>
+        <v>1110</v>
       </c>
       <c r="C426" s="3"/>
       <c r="D426" s="3"/>
@@ -18782,10 +18796,10 @@
     </row>
     <row r="427" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A427" s="2" t="s">
-        <v>1109</v>
+        <v>1111</v>
       </c>
       <c r="B427" s="3" t="s">
-        <v>1110</v>
+        <v>1112</v>
       </c>
       <c r="C427" s="3"/>
       <c r="D427" s="3"/>
@@ -18814,10 +18828,10 @@
     </row>
     <row r="428" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A428" s="2" t="s">
-        <v>1111</v>
+        <v>1113</v>
       </c>
       <c r="B428" s="3" t="s">
-        <v>1112</v>
+        <v>1114</v>
       </c>
       <c r="C428" s="3"/>
       <c r="D428" s="3"/>
@@ -18846,10 +18860,10 @@
     </row>
     <row r="429" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A429" s="2" t="s">
-        <v>1113</v>
+        <v>1115</v>
       </c>
       <c r="B429" s="3" t="s">
-        <v>1114</v>
+        <v>1116</v>
       </c>
       <c r="C429" s="3"/>
       <c r="D429" s="3"/>
@@ -18878,10 +18892,10 @@
     </row>
     <row r="430" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A430" s="2" t="s">
-        <v>1115</v>
+        <v>1117</v>
       </c>
       <c r="B430" s="3" t="s">
-        <v>1116</v>
+        <v>1118</v>
       </c>
       <c r="C430" s="3"/>
       <c r="D430" s="3"/>
@@ -18910,10 +18924,10 @@
     </row>
     <row r="431" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A431" s="2" t="s">
-        <v>1117</v>
+        <v>1119</v>
       </c>
       <c r="B431" s="3" t="s">
-        <v>1118</v>
+        <v>1120</v>
       </c>
       <c r="C431" s="3"/>
       <c r="D431" s="3"/>
@@ -18942,10 +18956,10 @@
     </row>
     <row r="432" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A432" s="2" t="s">
-        <v>1119</v>
+        <v>1121</v>
       </c>
       <c r="B432" s="3" t="s">
-        <v>1120</v>
+        <v>1122</v>
       </c>
       <c r="C432" s="3"/>
       <c r="D432" s="3"/>
@@ -18974,10 +18988,10 @@
     </row>
     <row r="433" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A433" s="2" t="s">
-        <v>1121</v>
+        <v>1123</v>
       </c>
       <c r="B433" s="3" t="s">
-        <v>1122</v>
+        <v>1124</v>
       </c>
       <c r="C433" s="3"/>
       <c r="D433" s="3"/>
@@ -19006,10 +19020,10 @@
     </row>
     <row r="434" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A434" s="2" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="B434" s="3" t="s">
-        <v>1124</v>
+        <v>1126</v>
       </c>
       <c r="C434" s="3"/>
       <c r="D434" s="3"/>
@@ -19038,10 +19052,10 @@
     </row>
     <row r="435" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A435" s="2" t="s">
-        <v>1125</v>
+        <v>1127</v>
       </c>
       <c r="B435" s="3" t="s">
-        <v>1126</v>
+        <v>1128</v>
       </c>
       <c r="C435" s="3"/>
       <c r="D435" s="3"/>
@@ -19070,10 +19084,10 @@
     </row>
     <row r="436" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A436" s="2" t="s">
-        <v>1127</v>
+        <v>1129</v>
       </c>
       <c r="B436" s="3" t="s">
-        <v>1128</v>
+        <v>1130</v>
       </c>
       <c r="C436" s="3"/>
       <c r="D436" s="3"/>
@@ -19102,10 +19116,10 @@
     </row>
     <row r="437" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A437" s="2" t="s">
-        <v>1129</v>
+        <v>1131</v>
       </c>
       <c r="B437" s="3" t="s">
-        <v>1130</v>
+        <v>1132</v>
       </c>
       <c r="C437" s="3"/>
       <c r="D437" s="3"/>
@@ -19134,10 +19148,10 @@
     </row>
     <row r="438" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A438" s="2" t="s">
-        <v>1131</v>
+        <v>1133</v>
       </c>
       <c r="B438" s="3" t="s">
-        <v>1132</v>
+        <v>1134</v>
       </c>
       <c r="C438" s="3"/>
       <c r="D438" s="3"/>
@@ -19166,10 +19180,10 @@
     </row>
     <row r="439" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A439" s="2" t="s">
-        <v>1133</v>
+        <v>1135</v>
       </c>
       <c r="B439" s="3" t="s">
-        <v>1134</v>
+        <v>1136</v>
       </c>
       <c r="C439" s="3"/>
       <c r="D439" s="3"/>
@@ -19198,10 +19212,10 @@
     </row>
     <row r="440" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A440" s="2" t="s">
-        <v>1135</v>
+        <v>1137</v>
       </c>
       <c r="B440" s="3" t="s">
-        <v>1136</v>
+        <v>1138</v>
       </c>
       <c r="C440" s="3"/>
       <c r="D440" s="3"/>
@@ -19230,10 +19244,10 @@
     </row>
     <row r="441" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A441" s="2" t="s">
-        <v>1137</v>
+        <v>1139</v>
       </c>
       <c r="B441" s="3" t="s">
-        <v>1138</v>
+        <v>1140</v>
       </c>
       <c r="C441" s="3"/>
       <c r="D441" s="3"/>
@@ -19262,10 +19276,10 @@
     </row>
     <row r="442" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A442" s="2" t="s">
-        <v>1139</v>
+        <v>1141</v>
       </c>
       <c r="B442" s="3" t="s">
-        <v>1140</v>
+        <v>1142</v>
       </c>
       <c r="C442" s="3"/>
       <c r="D442" s="3"/>
@@ -19294,10 +19308,10 @@
     </row>
     <row r="443" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A443" s="2" t="s">
-        <v>1141</v>
+        <v>1143</v>
       </c>
       <c r="B443" s="3" t="s">
-        <v>1142</v>
+        <v>1144</v>
       </c>
       <c r="C443" s="3"/>
       <c r="D443" s="3"/>
@@ -19326,10 +19340,10 @@
     </row>
     <row r="444" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A444" s="2" t="s">
-        <v>1143</v>
+        <v>1145</v>
       </c>
       <c r="B444" s="3" t="s">
-        <v>1144</v>
+        <v>1146</v>
       </c>
       <c r="C444" s="3"/>
       <c r="D444" s="3"/>
@@ -19358,10 +19372,10 @@
     </row>
     <row r="445" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A445" s="2" t="s">
-        <v>1145</v>
+        <v>1147</v>
       </c>
       <c r="B445" s="3" t="s">
-        <v>1146</v>
+        <v>1148</v>
       </c>
       <c r="C445" s="3"/>
       <c r="D445" s="3"/>
@@ -19390,10 +19404,10 @@
     </row>
     <row r="446" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A446" s="2" t="s">
-        <v>1147</v>
+        <v>1149</v>
       </c>
       <c r="B446" s="3" t="s">
-        <v>1148</v>
+        <v>1150</v>
       </c>
       <c r="C446" s="3"/>
       <c r="D446" s="3"/>
@@ -19422,7 +19436,7 @@
     </row>
     <row r="447" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A447" s="2" t="s">
-        <v>1149</v>
+        <v>1151</v>
       </c>
       <c r="B447" s="5"/>
       <c r="C447" s="5"/>
@@ -19452,7 +19466,7 @@
     </row>
     <row r="448" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A448" s="2" t="s">
-        <v>1150</v>
+        <v>1152</v>
       </c>
       <c r="B448" s="5"/>
       <c r="C448" s="5"/>
@@ -19482,7 +19496,7 @@
     </row>
     <row r="449" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A449" s="2" t="s">
-        <v>1151</v>
+        <v>1153</v>
       </c>
       <c r="B449" s="5"/>
       <c r="C449" s="5"/>
@@ -19512,10 +19526,10 @@
     </row>
     <row r="450" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A450" s="2" t="s">
-        <v>1152</v>
+        <v>1154</v>
       </c>
       <c r="B450" s="3" t="s">
-        <v>1153</v>
+        <v>1155</v>
       </c>
       <c r="C450" s="3"/>
       <c r="D450" s="3"/>
@@ -19544,10 +19558,10 @@
     </row>
     <row r="451" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A451" s="2" t="s">
-        <v>1154</v>
+        <v>1156</v>
       </c>
       <c r="B451" s="3" t="s">
-        <v>1155</v>
+        <v>1157</v>
       </c>
       <c r="C451" s="3"/>
       <c r="D451" s="3"/>
@@ -19576,10 +19590,10 @@
     </row>
     <row r="452" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A452" s="2" t="s">
-        <v>1156</v>
+        <v>1158</v>
       </c>
       <c r="B452" s="3" t="s">
-        <v>1157</v>
+        <v>1159</v>
       </c>
       <c r="C452" s="3"/>
       <c r="D452" s="3"/>
@@ -19608,10 +19622,10 @@
     </row>
     <row r="453" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A453" s="2" t="s">
-        <v>1158</v>
+        <v>1160</v>
       </c>
       <c r="B453" s="3" t="s">
-        <v>1159</v>
+        <v>1161</v>
       </c>
       <c r="C453" s="3"/>
       <c r="D453" s="3"/>
@@ -19640,10 +19654,10 @@
     </row>
     <row r="454" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A454" s="2" t="s">
-        <v>1160</v>
+        <v>1162</v>
       </c>
       <c r="B454" s="3" t="s">
-        <v>1161</v>
+        <v>1163</v>
       </c>
       <c r="C454" s="3"/>
       <c r="D454" s="3"/>
@@ -19672,10 +19686,10 @@
     </row>
     <row r="455" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A455" s="2" t="s">
-        <v>1162</v>
+        <v>1164</v>
       </c>
       <c r="B455" s="3" t="s">
-        <v>1163</v>
+        <v>1165</v>
       </c>
       <c r="C455" s="3"/>
       <c r="D455" s="3"/>
@@ -19704,10 +19718,10 @@
     </row>
     <row r="456" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A456" s="2" t="s">
-        <v>1164</v>
+        <v>1166</v>
       </c>
       <c r="B456" s="3" t="s">
-        <v>1165</v>
+        <v>1167</v>
       </c>
       <c r="C456" s="3"/>
       <c r="D456" s="3"/>
@@ -19736,10 +19750,10 @@
     </row>
     <row r="457" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A457" s="2" t="s">
-        <v>1166</v>
+        <v>1168</v>
       </c>
       <c r="B457" s="3" t="s">
-        <v>1167</v>
+        <v>1169</v>
       </c>
       <c r="C457" s="3"/>
       <c r="D457" s="3"/>
@@ -19768,10 +19782,10 @@
     </row>
     <row r="458" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A458" s="2" t="s">
-        <v>1168</v>
+        <v>1170</v>
       </c>
       <c r="B458" s="3" t="s">
-        <v>1169</v>
+        <v>1171</v>
       </c>
       <c r="C458" s="3"/>
       <c r="D458" s="3"/>
@@ -19800,10 +19814,10 @@
     </row>
     <row r="459" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A459" s="2" t="s">
-        <v>1170</v>
+        <v>1172</v>
       </c>
       <c r="B459" s="3" t="s">
-        <v>1171</v>
+        <v>1173</v>
       </c>
       <c r="C459" s="3"/>
       <c r="D459" s="3"/>
@@ -19832,10 +19846,10 @@
     </row>
     <row r="460" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A460" s="2" t="s">
-        <v>1172</v>
+        <v>1174</v>
       </c>
       <c r="B460" s="3" t="s">
-        <v>1173</v>
+        <v>1175</v>
       </c>
       <c r="C460" s="3"/>
       <c r="D460" s="3"/>
@@ -19864,10 +19878,10 @@
     </row>
     <row r="461" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A461" s="2" t="s">
-        <v>1174</v>
+        <v>1176</v>
       </c>
       <c r="B461" s="3" t="s">
-        <v>1175</v>
+        <v>1177</v>
       </c>
       <c r="C461" s="3"/>
       <c r="D461" s="3"/>
@@ -19896,10 +19910,10 @@
     </row>
     <row r="462" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A462" s="2" t="s">
-        <v>1176</v>
+        <v>1178</v>
       </c>
       <c r="B462" s="3" t="s">
-        <v>1177</v>
+        <v>1179</v>
       </c>
       <c r="C462" s="3"/>
       <c r="D462" s="3"/>
@@ -19928,10 +19942,10 @@
     </row>
     <row r="463" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A463" s="2" t="s">
-        <v>1178</v>
+        <v>1180</v>
       </c>
       <c r="B463" s="3" t="s">
-        <v>1179</v>
+        <v>1181</v>
       </c>
       <c r="C463" s="3"/>
       <c r="D463" s="3"/>
@@ -19960,10 +19974,10 @@
     </row>
     <row r="464" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A464" s="2" t="s">
-        <v>1180</v>
+        <v>1182</v>
       </c>
       <c r="B464" s="3" t="s">
-        <v>1181</v>
+        <v>1183</v>
       </c>
       <c r="C464" s="3"/>
       <c r="D464" s="3"/>
@@ -19992,10 +20006,10 @@
     </row>
     <row r="465" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A465" s="2" t="s">
-        <v>1182</v>
+        <v>1184</v>
       </c>
       <c r="B465" s="3" t="s">
-        <v>1183</v>
+        <v>1185</v>
       </c>
       <c r="C465" s="3"/>
       <c r="D465" s="3"/>
@@ -20024,7 +20038,7 @@
     </row>
     <row r="466" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A466" s="2" t="s">
-        <v>1184</v>
+        <v>1186</v>
       </c>
       <c r="B466" s="5"/>
       <c r="C466" s="5"/>
@@ -20054,21 +20068,21 @@
     </row>
     <row r="467" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A467" s="2" t="s">
-        <v>1185</v>
+        <v>1187</v>
       </c>
       <c r="B467" s="5"/>
       <c r="C467" s="5"/>
       <c r="D467" s="5"/>
-      <c r="E467" s="9"/>
-      <c r="F467" s="9"/>
-      <c r="G467" s="9"/>
-      <c r="H467" s="9"/>
-      <c r="I467" s="9"/>
-      <c r="J467" s="9"/>
-      <c r="K467" s="9"/>
-      <c r="L467" s="9"/>
-      <c r="M467" s="9"/>
-      <c r="N467" s="9"/>
+      <c r="E467" s="10"/>
+      <c r="F467" s="10"/>
+      <c r="G467" s="10"/>
+      <c r="H467" s="10"/>
+      <c r="I467" s="10"/>
+      <c r="J467" s="10"/>
+      <c r="K467" s="10"/>
+      <c r="L467" s="10"/>
+      <c r="M467" s="10"/>
+      <c r="N467" s="10"/>
       <c r="O467" s="5"/>
       <c r="P467" s="5"/>
       <c r="Q467" s="5"/>
@@ -20084,21 +20098,21 @@
     </row>
     <row r="468" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A468" s="2" t="s">
-        <v>1186</v>
+        <v>1188</v>
       </c>
       <c r="B468" s="5"/>
       <c r="C468" s="5"/>
       <c r="D468" s="5"/>
-      <c r="E468" s="9"/>
-      <c r="F468" s="9"/>
-      <c r="G468" s="9"/>
-      <c r="H468" s="9"/>
-      <c r="I468" s="9"/>
-      <c r="J468" s="9"/>
-      <c r="K468" s="9"/>
-      <c r="L468" s="9"/>
-      <c r="M468" s="9"/>
-      <c r="N468" s="9"/>
+      <c r="E468" s="10"/>
+      <c r="F468" s="10"/>
+      <c r="G468" s="10"/>
+      <c r="H468" s="10"/>
+      <c r="I468" s="10"/>
+      <c r="J468" s="10"/>
+      <c r="K468" s="10"/>
+      <c r="L468" s="10"/>
+      <c r="M468" s="10"/>
+      <c r="N468" s="10"/>
       <c r="O468" s="5"/>
       <c r="P468" s="5"/>
       <c r="Q468" s="5"/>
@@ -20114,21 +20128,21 @@
     </row>
     <row r="469" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A469" s="2" t="s">
-        <v>1187</v>
+        <v>1189</v>
       </c>
       <c r="B469" s="5"/>
       <c r="C469" s="5"/>
       <c r="D469" s="5"/>
-      <c r="E469" s="9"/>
-      <c r="F469" s="9"/>
-      <c r="G469" s="9"/>
-      <c r="H469" s="9"/>
-      <c r="I469" s="9"/>
-      <c r="J469" s="9"/>
-      <c r="K469" s="9"/>
-      <c r="L469" s="9"/>
-      <c r="M469" s="9"/>
-      <c r="N469" s="9"/>
+      <c r="E469" s="10"/>
+      <c r="F469" s="10"/>
+      <c r="G469" s="10"/>
+      <c r="H469" s="10"/>
+      <c r="I469" s="10"/>
+      <c r="J469" s="10"/>
+      <c r="K469" s="10"/>
+      <c r="L469" s="10"/>
+      <c r="M469" s="10"/>
+      <c r="N469" s="10"/>
       <c r="O469" s="5"/>
       <c r="P469" s="5"/>
       <c r="Q469" s="5"/>
@@ -20144,21 +20158,21 @@
     </row>
     <row r="470" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A470" s="2" t="s">
-        <v>1188</v>
+        <v>1190</v>
       </c>
       <c r="B470" s="5"/>
       <c r="C470" s="5"/>
       <c r="D470" s="5"/>
-      <c r="E470" s="9"/>
-      <c r="F470" s="9"/>
-      <c r="G470" s="9"/>
-      <c r="H470" s="9"/>
-      <c r="I470" s="9"/>
-      <c r="J470" s="9"/>
-      <c r="K470" s="9"/>
-      <c r="L470" s="9"/>
-      <c r="M470" s="9"/>
-      <c r="N470" s="9"/>
+      <c r="E470" s="10"/>
+      <c r="F470" s="10"/>
+      <c r="G470" s="10"/>
+      <c r="H470" s="10"/>
+      <c r="I470" s="10"/>
+      <c r="J470" s="10"/>
+      <c r="K470" s="10"/>
+      <c r="L470" s="10"/>
+      <c r="M470" s="10"/>
+      <c r="N470" s="10"/>
       <c r="O470" s="5"/>
       <c r="P470" s="5"/>
       <c r="Q470" s="5"/>
@@ -20174,21 +20188,21 @@
     </row>
     <row r="471" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A471" s="2" t="s">
-        <v>1189</v>
+        <v>1191</v>
       </c>
       <c r="B471" s="5"/>
       <c r="C471" s="5"/>
       <c r="D471" s="5"/>
-      <c r="E471" s="9"/>
-      <c r="F471" s="9"/>
-      <c r="G471" s="9"/>
-      <c r="H471" s="9"/>
-      <c r="I471" s="9"/>
-      <c r="J471" s="9"/>
-      <c r="K471" s="9"/>
-      <c r="L471" s="9"/>
-      <c r="M471" s="9"/>
-      <c r="N471" s="9"/>
+      <c r="E471" s="10"/>
+      <c r="F471" s="10"/>
+      <c r="G471" s="10"/>
+      <c r="H471" s="10"/>
+      <c r="I471" s="10"/>
+      <c r="J471" s="10"/>
+      <c r="K471" s="10"/>
+      <c r="L471" s="10"/>
+      <c r="M471" s="10"/>
+      <c r="N471" s="10"/>
       <c r="O471" s="5"/>
       <c r="P471" s="5"/>
       <c r="Q471" s="5"/>
@@ -20204,21 +20218,21 @@
     </row>
     <row r="472" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A472" s="2" t="s">
-        <v>1190</v>
+        <v>1192</v>
       </c>
       <c r="B472" s="5"/>
       <c r="C472" s="5"/>
       <c r="D472" s="5"/>
-      <c r="E472" s="9"/>
-      <c r="F472" s="9"/>
-      <c r="G472" s="9"/>
-      <c r="H472" s="9"/>
-      <c r="I472" s="9"/>
-      <c r="J472" s="9"/>
-      <c r="K472" s="9"/>
-      <c r="L472" s="9"/>
-      <c r="M472" s="9"/>
-      <c r="N472" s="9"/>
+      <c r="E472" s="10"/>
+      <c r="F472" s="10"/>
+      <c r="G472" s="10"/>
+      <c r="H472" s="10"/>
+      <c r="I472" s="10"/>
+      <c r="J472" s="10"/>
+      <c r="K472" s="10"/>
+      <c r="L472" s="10"/>
+      <c r="M472" s="10"/>
+      <c r="N472" s="10"/>
       <c r="O472" s="5"/>
       <c r="P472" s="5"/>
       <c r="Q472" s="5"/>
@@ -20234,7 +20248,7 @@
     </row>
     <row r="473" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A473" s="2" t="s">
-        <v>1191</v>
+        <v>1193</v>
       </c>
       <c r="B473" s="5"/>
       <c r="C473" s="5"/>
@@ -20264,7 +20278,7 @@
     </row>
     <row r="474" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A474" s="2" t="s">
-        <v>1192</v>
+        <v>1194</v>
       </c>
       <c r="B474" s="5"/>
       <c r="C474" s="5"/>
@@ -20294,7 +20308,7 @@
     </row>
     <row r="475" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A475" s="2" t="s">
-        <v>1193</v>
+        <v>1195</v>
       </c>
       <c r="B475" s="5"/>
       <c r="C475" s="5"/>
@@ -20324,7 +20338,7 @@
     </row>
     <row r="476" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A476" s="2" t="s">
-        <v>1194</v>
+        <v>1196</v>
       </c>
       <c r="B476" s="5"/>
       <c r="C476" s="5"/>
@@ -20354,7 +20368,7 @@
     </row>
     <row r="477" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A477" s="2" t="s">
-        <v>1195</v>
+        <v>1197</v>
       </c>
       <c r="B477" s="5"/>
       <c r="C477" s="5"/>
@@ -20384,7 +20398,7 @@
     </row>
     <row r="478" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A478" s="2" t="s">
-        <v>1196</v>
+        <v>1198</v>
       </c>
       <c r="B478" s="5"/>
       <c r="C478" s="5"/>
@@ -20414,7 +20428,7 @@
     </row>
     <row r="479" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A479" s="2" t="s">
-        <v>1197</v>
+        <v>1199</v>
       </c>
       <c r="B479" s="5"/>
       <c r="C479" s="5"/>
@@ -20444,7 +20458,7 @@
     </row>
     <row r="480" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A480" s="2" t="s">
-        <v>1198</v>
+        <v>1200</v>
       </c>
       <c r="B480" s="5"/>
       <c r="C480" s="5"/>
@@ -20474,7 +20488,7 @@
     </row>
     <row r="481" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A481" s="2" t="s">
-        <v>1199</v>
+        <v>1201</v>
       </c>
       <c r="B481" s="5"/>
       <c r="C481" s="5"/>
@@ -20503,25 +20517,25 @@
       <c r="Z481" s="1"/>
     </row>
     <row r="482" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A482" s="10"/>
-      <c r="B482" s="11"/>
-      <c r="C482" s="11"/>
-      <c r="D482" s="11"/>
-      <c r="E482" s="11"/>
-      <c r="F482" s="11"/>
-      <c r="G482" s="11"/>
-      <c r="H482" s="11"/>
+      <c r="A482" s="11"/>
+      <c r="B482" s="12"/>
+      <c r="C482" s="12"/>
+      <c r="D482" s="12"/>
+      <c r="E482" s="12"/>
+      <c r="F482" s="12"/>
+      <c r="G482" s="12"/>
+      <c r="H482" s="12"/>
       <c r="I482" s="3" t="s">
-        <v>1200</v>
+        <v>1202</v>
       </c>
       <c r="J482" s="3"/>
-      <c r="K482" s="11"/>
-      <c r="L482" s="11"/>
-      <c r="M482" s="11"/>
-      <c r="N482" s="11"/>
-      <c r="O482" s="11"/>
-      <c r="P482" s="11"/>
-      <c r="Q482" s="11"/>
+      <c r="K482" s="12"/>
+      <c r="L482" s="12"/>
+      <c r="M482" s="12"/>
+      <c r="N482" s="12"/>
+      <c r="O482" s="12"/>
+      <c r="P482" s="12"/>
+      <c r="Q482" s="12"/>
       <c r="R482" s="1"/>
       <c r="S482" s="1"/>
       <c r="T482" s="1"/>
@@ -20534,37 +20548,37 @@
     </row>
     <row r="483" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A483" s="2" t="s">
-        <v>1201</v>
+        <v>1203</v>
       </c>
       <c r="B483" s="4" t="s">
-        <v>1202</v>
+        <v>1204</v>
       </c>
       <c r="C483" s="4" t="s">
-        <v>1203</v>
+        <v>1205</v>
       </c>
       <c r="D483" s="4" t="s">
-        <v>1204</v>
+        <v>1206</v>
       </c>
       <c r="E483" s="4" t="s">
-        <v>1205</v>
+        <v>1207</v>
       </c>
       <c r="F483" s="4" t="s">
-        <v>1206</v>
+        <v>1208</v>
       </c>
       <c r="G483" s="4" t="s">
-        <v>1207</v>
+        <v>1209</v>
       </c>
       <c r="H483" s="4" t="s">
-        <v>1208</v>
+        <v>1210</v>
       </c>
       <c r="I483" s="4" t="s">
-        <v>1209</v>
+        <v>1211</v>
       </c>
       <c r="J483" s="4" t="s">
-        <v>1210</v>
+        <v>1212</v>
       </c>
       <c r="K483" s="4" t="s">
-        <v>1211</v>
+        <v>1213</v>
       </c>
       <c r="L483" s="5"/>
       <c r="M483" s="5"/>
@@ -20584,37 +20598,37 @@
     </row>
     <row r="484" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A484" s="2" t="s">
-        <v>1212</v>
+        <v>1214</v>
       </c>
       <c r="B484" s="4" t="s">
-        <v>1213</v>
+        <v>1215</v>
       </c>
       <c r="C484" s="4" t="s">
-        <v>1214</v>
+        <v>1216</v>
       </c>
       <c r="D484" s="4" t="s">
-        <v>1215</v>
+        <v>1217</v>
       </c>
       <c r="E484" s="4" t="s">
-        <v>1216</v>
+        <v>1218</v>
       </c>
       <c r="F484" s="4" t="s">
-        <v>1217</v>
+        <v>1219</v>
       </c>
       <c r="G484" s="4" t="s">
-        <v>1218</v>
+        <v>1220</v>
       </c>
       <c r="H484" s="4" t="s">
-        <v>1219</v>
+        <v>1221</v>
       </c>
       <c r="I484" s="4" t="s">
-        <v>1220</v>
+        <v>1222</v>
       </c>
       <c r="J484" s="4" t="s">
-        <v>1221</v>
+        <v>1223</v>
       </c>
       <c r="K484" s="4" t="s">
-        <v>1222</v>
+        <v>1224</v>
       </c>
       <c r="L484" s="5"/>
       <c r="M484" s="5"/>
@@ -20634,37 +20648,37 @@
     </row>
     <row r="485" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A485" s="2" t="s">
-        <v>1223</v>
+        <v>1225</v>
       </c>
       <c r="B485" s="4" t="s">
-        <v>1224</v>
+        <v>1226</v>
       </c>
       <c r="C485" s="4" t="s">
-        <v>1225</v>
+        <v>1227</v>
       </c>
       <c r="D485" s="4" t="s">
-        <v>1226</v>
+        <v>1228</v>
       </c>
       <c r="E485" s="4" t="s">
-        <v>1227</v>
+        <v>1229</v>
       </c>
       <c r="F485" s="4" t="s">
-        <v>1228</v>
+        <v>1230</v>
       </c>
       <c r="G485" s="4" t="s">
-        <v>1229</v>
+        <v>1231</v>
       </c>
       <c r="H485" s="4" t="s">
-        <v>1230</v>
+        <v>1232</v>
       </c>
       <c r="I485" s="4" t="s">
-        <v>1231</v>
+        <v>1233</v>
       </c>
       <c r="J485" s="4" t="s">
-        <v>1232</v>
+        <v>1234</v>
       </c>
       <c r="K485" s="4" t="s">
-        <v>1233</v>
+        <v>1235</v>
       </c>
       <c r="L485" s="5"/>
       <c r="M485" s="5"/>
@@ -20684,37 +20698,37 @@
     </row>
     <row r="486" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A486" s="2" t="s">
-        <v>1234</v>
+        <v>1236</v>
       </c>
       <c r="B486" s="4" t="s">
-        <v>1235</v>
+        <v>1237</v>
       </c>
       <c r="C486" s="4" t="s">
-        <v>1236</v>
+        <v>1238</v>
       </c>
       <c r="D486" s="4" t="s">
-        <v>1237</v>
+        <v>1239</v>
       </c>
       <c r="E486" s="4" t="s">
-        <v>1238</v>
+        <v>1240</v>
       </c>
       <c r="F486" s="4" t="s">
-        <v>1239</v>
+        <v>1241</v>
       </c>
       <c r="G486" s="4" t="s">
-        <v>1240</v>
+        <v>1242</v>
       </c>
       <c r="H486" s="4" t="s">
-        <v>1241</v>
+        <v>1243</v>
       </c>
       <c r="I486" s="4" t="s">
-        <v>1242</v>
+        <v>1244</v>
       </c>
       <c r="J486" s="4" t="s">
-        <v>1243</v>
+        <v>1245</v>
       </c>
       <c r="K486" s="4" t="s">
-        <v>1244</v>
+        <v>1246</v>
       </c>
       <c r="L486" s="5"/>
       <c r="M486" s="5"/>
@@ -20734,37 +20748,37 @@
     </row>
     <row r="487" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A487" s="2" t="s">
-        <v>1245</v>
+        <v>1247</v>
       </c>
       <c r="B487" s="4" t="s">
-        <v>1246</v>
+        <v>1248</v>
       </c>
       <c r="C487" s="4" t="s">
-        <v>1247</v>
+        <v>1249</v>
       </c>
       <c r="D487" s="4" t="s">
-        <v>1248</v>
+        <v>1250</v>
       </c>
       <c r="E487" s="4" t="s">
-        <v>1249</v>
+        <v>1251</v>
       </c>
       <c r="F487" s="4" t="s">
-        <v>1250</v>
+        <v>1252</v>
       </c>
       <c r="G487" s="4" t="s">
-        <v>1251</v>
+        <v>1253</v>
       </c>
       <c r="H487" s="4" t="s">
-        <v>1252</v>
+        <v>1254</v>
       </c>
       <c r="I487" s="4" t="s">
-        <v>1253</v>
+        <v>1255</v>
       </c>
       <c r="J487" s="4" t="s">
-        <v>1254</v>
+        <v>1256</v>
       </c>
       <c r="K487" s="4" t="s">
-        <v>1255</v>
+        <v>1257</v>
       </c>
       <c r="L487" s="5"/>
       <c r="M487" s="5"/>
@@ -20784,37 +20798,37 @@
     </row>
     <row r="488" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A488" s="2" t="s">
-        <v>1256</v>
+        <v>1258</v>
       </c>
       <c r="B488" s="4" t="s">
-        <v>1257</v>
+        <v>1259</v>
       </c>
       <c r="C488" s="4" t="s">
-        <v>1258</v>
+        <v>1260</v>
       </c>
       <c r="D488" s="4" t="s">
-        <v>1259</v>
+        <v>1261</v>
       </c>
       <c r="E488" s="4" t="s">
-        <v>1260</v>
+        <v>1262</v>
       </c>
       <c r="F488" s="4" t="s">
-        <v>1261</v>
+        <v>1263</v>
       </c>
       <c r="G488" s="4" t="s">
-        <v>1262</v>
+        <v>1264</v>
       </c>
       <c r="H488" s="4" t="s">
-        <v>1263</v>
+        <v>1265</v>
       </c>
       <c r="I488" s="4" t="s">
-        <v>1264</v>
+        <v>1266</v>
       </c>
       <c r="J488" s="4" t="s">
-        <v>1265</v>
+        <v>1267</v>
       </c>
       <c r="K488" s="4" t="s">
-        <v>1266</v>
+        <v>1268</v>
       </c>
       <c r="L488" s="5"/>
       <c r="M488" s="5"/>
@@ -20834,37 +20848,37 @@
     </row>
     <row r="489" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A489" s="2" t="s">
-        <v>1267</v>
+        <v>1269</v>
       </c>
       <c r="B489" s="4" t="s">
-        <v>1268</v>
+        <v>1270</v>
       </c>
       <c r="C489" s="4" t="s">
-        <v>1269</v>
+        <v>1271</v>
       </c>
       <c r="D489" s="4" t="s">
-        <v>1270</v>
+        <v>1272</v>
       </c>
       <c r="E489" s="4" t="s">
-        <v>1271</v>
+        <v>1273</v>
       </c>
       <c r="F489" s="4" t="s">
-        <v>1272</v>
+        <v>1274</v>
       </c>
       <c r="G489" s="4" t="s">
-        <v>1273</v>
+        <v>1275</v>
       </c>
       <c r="H489" s="4" t="s">
-        <v>1274</v>
+        <v>1276</v>
       </c>
       <c r="I489" s="4" t="s">
-        <v>1275</v>
+        <v>1277</v>
       </c>
       <c r="J489" s="4" t="s">
-        <v>1276</v>
+        <v>1278</v>
       </c>
       <c r="K489" s="4" t="s">
-        <v>1277</v>
+        <v>1279</v>
       </c>
       <c r="L489" s="5"/>
       <c r="M489" s="5"/>
@@ -20884,37 +20898,37 @@
     </row>
     <row r="490" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A490" s="2" t="s">
-        <v>1278</v>
+        <v>1280</v>
       </c>
       <c r="B490" s="4" t="s">
-        <v>1279</v>
+        <v>1281</v>
       </c>
       <c r="C490" s="4" t="s">
-        <v>1280</v>
+        <v>1282</v>
       </c>
       <c r="D490" s="4" t="s">
-        <v>1281</v>
+        <v>1283</v>
       </c>
       <c r="E490" s="4" t="s">
-        <v>1282</v>
+        <v>1284</v>
       </c>
       <c r="F490" s="4" t="s">
-        <v>1283</v>
+        <v>1285</v>
       </c>
       <c r="G490" s="4" t="s">
-        <v>1284</v>
+        <v>1286</v>
       </c>
       <c r="H490" s="4" t="s">
-        <v>1285</v>
+        <v>1287</v>
       </c>
       <c r="I490" s="4" t="s">
-        <v>1286</v>
+        <v>1288</v>
       </c>
       <c r="J490" s="4" t="s">
-        <v>1287</v>
+        <v>1289</v>
       </c>
       <c r="K490" s="4" t="s">
-        <v>1288</v>
+        <v>1290</v>
       </c>
       <c r="L490" s="5"/>
       <c r="M490" s="5"/>
@@ -20934,37 +20948,37 @@
     </row>
     <row r="491" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A491" s="2" t="s">
-        <v>1289</v>
+        <v>1291</v>
       </c>
       <c r="B491" s="4" t="s">
-        <v>1290</v>
+        <v>1292</v>
       </c>
       <c r="C491" s="4" t="s">
-        <v>1291</v>
+        <v>1293</v>
       </c>
       <c r="D491" s="4" t="s">
-        <v>1292</v>
+        <v>1294</v>
       </c>
       <c r="E491" s="4" t="s">
-        <v>1293</v>
+        <v>1295</v>
       </c>
       <c r="F491" s="4" t="s">
-        <v>1294</v>
+        <v>1296</v>
       </c>
       <c r="G491" s="4" t="s">
-        <v>1295</v>
+        <v>1297</v>
       </c>
       <c r="H491" s="4" t="s">
-        <v>1296</v>
+        <v>1298</v>
       </c>
       <c r="I491" s="4" t="s">
-        <v>1297</v>
+        <v>1299</v>
       </c>
       <c r="J491" s="4" t="s">
-        <v>1298</v>
+        <v>1300</v>
       </c>
       <c r="K491" s="4" t="s">
-        <v>1299</v>
+        <v>1301</v>
       </c>
       <c r="L491" s="5"/>
       <c r="M491" s="5"/>
@@ -20984,37 +20998,37 @@
     </row>
     <row r="492" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A492" s="2" t="s">
-        <v>1300</v>
+        <v>1302</v>
       </c>
       <c r="B492" s="4" t="s">
-        <v>1301</v>
+        <v>1303</v>
       </c>
       <c r="C492" s="4" t="s">
-        <v>1302</v>
+        <v>1304</v>
       </c>
       <c r="D492" s="4" t="s">
-        <v>1303</v>
+        <v>1305</v>
       </c>
       <c r="E492" s="4" t="s">
-        <v>1304</v>
+        <v>1306</v>
       </c>
       <c r="F492" s="4" t="s">
-        <v>1305</v>
+        <v>1307</v>
       </c>
       <c r="G492" s="4" t="s">
-        <v>1306</v>
+        <v>1308</v>
       </c>
       <c r="H492" s="4" t="s">
-        <v>1307</v>
+        <v>1309</v>
       </c>
       <c r="I492" s="4" t="s">
-        <v>1308</v>
+        <v>1310</v>
       </c>
       <c r="J492" s="4" t="s">
-        <v>1309</v>
+        <v>1311</v>
       </c>
       <c r="K492" s="4" t="s">
-        <v>1310</v>
+        <v>1312</v>
       </c>
       <c r="L492" s="5"/>
       <c r="M492" s="5"/>
@@ -21034,37 +21048,37 @@
     </row>
     <row r="493" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A493" s="2" t="s">
-        <v>1311</v>
+        <v>1313</v>
       </c>
       <c r="B493" s="4" t="s">
-        <v>1312</v>
+        <v>1314</v>
       </c>
       <c r="C493" s="4" t="s">
-        <v>1313</v>
+        <v>1315</v>
       </c>
       <c r="D493" s="4" t="s">
-        <v>1314</v>
+        <v>1316</v>
       </c>
       <c r="E493" s="4" t="s">
-        <v>1315</v>
+        <v>1317</v>
       </c>
       <c r="F493" s="4" t="s">
-        <v>1316</v>
+        <v>1318</v>
       </c>
       <c r="G493" s="4" t="s">
-        <v>1317</v>
+        <v>1319</v>
       </c>
       <c r="H493" s="4" t="s">
-        <v>1318</v>
+        <v>1320</v>
       </c>
       <c r="I493" s="4" t="s">
-        <v>1319</v>
+        <v>1321</v>
       </c>
       <c r="J493" s="4" t="s">
-        <v>1320</v>
+        <v>1322</v>
       </c>
       <c r="K493" s="4" t="s">
-        <v>1321</v>
+        <v>1323</v>
       </c>
       <c r="L493" s="5"/>
       <c r="M493" s="5"/>
@@ -21084,37 +21098,37 @@
     </row>
     <row r="494" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A494" s="2" t="s">
-        <v>1322</v>
+        <v>1324</v>
       </c>
       <c r="B494" s="4" t="s">
-        <v>1323</v>
+        <v>1325</v>
       </c>
       <c r="C494" s="4" t="s">
-        <v>1324</v>
+        <v>1326</v>
       </c>
       <c r="D494" s="4" t="s">
-        <v>1325</v>
+        <v>1327</v>
       </c>
       <c r="E494" s="4" t="s">
-        <v>1326</v>
+        <v>1328</v>
       </c>
       <c r="F494" s="4" t="s">
-        <v>1327</v>
+        <v>1329</v>
       </c>
       <c r="G494" s="4" t="s">
-        <v>1328</v>
+        <v>1330</v>
       </c>
       <c r="H494" s="4" t="s">
-        <v>1329</v>
+        <v>1331</v>
       </c>
       <c r="I494" s="4" t="s">
-        <v>1330</v>
+        <v>1332</v>
       </c>
       <c r="J494" s="4" t="s">
-        <v>1331</v>
+        <v>1333</v>
       </c>
       <c r="K494" s="4" t="s">
-        <v>1332</v>
+        <v>1334</v>
       </c>
       <c r="L494" s="5"/>
       <c r="M494" s="5"/>
@@ -21134,38 +21148,38 @@
     </row>
     <row r="495" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A495" s="2" t="s">
-        <v>1333</v>
+        <v>1335</v>
       </c>
       <c r="B495" s="3" t="s">
-        <v>1334</v>
+        <v>1336</v>
       </c>
       <c r="C495" s="3"/>
       <c r="D495" s="3" t="s">
-        <v>1335</v>
+        <v>1337</v>
       </c>
       <c r="E495" s="3"/>
       <c r="F495" s="3" t="s">
-        <v>1336</v>
+        <v>1338</v>
       </c>
       <c r="G495" s="3"/>
       <c r="H495" s="3" t="s">
-        <v>1337</v>
+        <v>1339</v>
       </c>
       <c r="I495" s="3"/>
       <c r="J495" s="3" t="s">
-        <v>1338</v>
+        <v>1340</v>
       </c>
       <c r="K495" s="3"/>
       <c r="L495" s="3" t="s">
-        <v>1339</v>
+        <v>1341</v>
       </c>
       <c r="M495" s="3"/>
       <c r="N495" s="3" t="s">
-        <v>1340</v>
+        <v>1342</v>
       </c>
       <c r="O495" s="3"/>
       <c r="P495" s="3" t="s">
-        <v>1341</v>
+        <v>1343</v>
       </c>
       <c r="Q495" s="3"/>
       <c r="R495" s="1"/>
@@ -21180,34 +21194,34 @@
     </row>
     <row r="496" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A496" s="2" t="s">
-        <v>1342</v>
+        <v>1344</v>
       </c>
       <c r="B496" s="4" t="s">
-        <v>1343</v>
+        <v>1345</v>
       </c>
       <c r="C496" s="4" t="s">
-        <v>1344</v>
+        <v>1346</v>
       </c>
       <c r="D496" s="4" t="s">
-        <v>1345</v>
+        <v>1347</v>
       </c>
       <c r="E496" s="4" t="s">
-        <v>1346</v>
+        <v>1348</v>
       </c>
       <c r="F496" s="4" t="s">
-        <v>1347</v>
+        <v>1349</v>
       </c>
       <c r="G496" s="4" t="s">
-        <v>1348</v>
+        <v>1350</v>
       </c>
       <c r="H496" s="4" t="s">
-        <v>1349</v>
+        <v>1351</v>
       </c>
       <c r="I496" s="4" t="s">
-        <v>1350</v>
+        <v>1352</v>
       </c>
       <c r="J496" s="4" t="s">
-        <v>1351</v>
+        <v>1353</v>
       </c>
       <c r="K496" s="5"/>
       <c r="L496" s="5"/>
@@ -21228,34 +21242,34 @@
     </row>
     <row r="497" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A497" s="2" t="s">
-        <v>1352</v>
+        <v>1354</v>
       </c>
       <c r="B497" s="4" t="s">
-        <v>1353</v>
+        <v>1355</v>
       </c>
       <c r="C497" s="4" t="s">
-        <v>1354</v>
+        <v>1356</v>
       </c>
       <c r="D497" s="4" t="s">
-        <v>1355</v>
+        <v>1357</v>
       </c>
       <c r="E497" s="4" t="s">
-        <v>1356</v>
+        <v>1358</v>
       </c>
       <c r="F497" s="4" t="s">
-        <v>1357</v>
+        <v>1359</v>
       </c>
       <c r="G497" s="4" t="s">
-        <v>1358</v>
+        <v>1360</v>
       </c>
       <c r="H497" s="4" t="s">
-        <v>1359</v>
+        <v>1361</v>
       </c>
       <c r="I497" s="4" t="s">
-        <v>1360</v>
+        <v>1362</v>
       </c>
       <c r="J497" s="4" t="s">
-        <v>1361</v>
+        <v>1363</v>
       </c>
       <c r="K497" s="5"/>
       <c r="L497" s="5"/>
@@ -21276,34 +21290,34 @@
     </row>
     <row r="498" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A498" s="2" t="s">
-        <v>1362</v>
+        <v>1364</v>
       </c>
       <c r="B498" s="4" t="s">
-        <v>1363</v>
+        <v>1365</v>
       </c>
       <c r="C498" s="4" t="s">
-        <v>1364</v>
+        <v>1366</v>
       </c>
       <c r="D498" s="4" t="s">
-        <v>1365</v>
+        <v>1367</v>
       </c>
       <c r="E498" s="4" t="s">
-        <v>1366</v>
+        <v>1368</v>
       </c>
       <c r="F498" s="4" t="s">
-        <v>1367</v>
+        <v>1369</v>
       </c>
       <c r="G498" s="4" t="s">
-        <v>1368</v>
+        <v>1370</v>
       </c>
       <c r="H498" s="4" t="s">
-        <v>1369</v>
+        <v>1371</v>
       </c>
       <c r="I498" s="4" t="s">
-        <v>1370</v>
+        <v>1372</v>
       </c>
       <c r="J498" s="4" t="s">
-        <v>1371</v>
+        <v>1373</v>
       </c>
       <c r="K498" s="5"/>
       <c r="L498" s="5"/>
@@ -21324,34 +21338,34 @@
     </row>
     <row r="499" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A499" s="2" t="s">
-        <v>1372</v>
+        <v>1374</v>
       </c>
       <c r="B499" s="4" t="s">
-        <v>1373</v>
+        <v>1375</v>
       </c>
       <c r="C499" s="4" t="s">
-        <v>1374</v>
+        <v>1376</v>
       </c>
       <c r="D499" s="4" t="s">
-        <v>1375</v>
+        <v>1377</v>
       </c>
       <c r="E499" s="4" t="s">
-        <v>1376</v>
+        <v>1378</v>
       </c>
       <c r="F499" s="4" t="s">
-        <v>1377</v>
+        <v>1379</v>
       </c>
       <c r="G499" s="4" t="s">
-        <v>1378</v>
+        <v>1380</v>
       </c>
       <c r="H499" s="4" t="s">
-        <v>1379</v>
+        <v>1381</v>
       </c>
       <c r="I499" s="4" t="s">
-        <v>1380</v>
+        <v>1382</v>
       </c>
       <c r="J499" s="4" t="s">
-        <v>1381</v>
+        <v>1383</v>
       </c>
       <c r="K499" s="5"/>
       <c r="L499" s="5"/>
@@ -21372,34 +21386,34 @@
     </row>
     <row r="500" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A500" s="2" t="s">
-        <v>1382</v>
+        <v>1384</v>
       </c>
       <c r="B500" s="4" t="s">
-        <v>1383</v>
+        <v>1385</v>
       </c>
       <c r="C500" s="4" t="s">
-        <v>1384</v>
+        <v>1386</v>
       </c>
       <c r="D500" s="4" t="s">
-        <v>1385</v>
+        <v>1387</v>
       </c>
       <c r="E500" s="4" t="s">
-        <v>1386</v>
+        <v>1388</v>
       </c>
       <c r="F500" s="4" t="s">
-        <v>1387</v>
+        <v>1389</v>
       </c>
       <c r="G500" s="4" t="s">
-        <v>1388</v>
+        <v>1390</v>
       </c>
       <c r="H500" s="4" t="s">
-        <v>1389</v>
+        <v>1391</v>
       </c>
       <c r="I500" s="4" t="s">
-        <v>1390</v>
+        <v>1392</v>
       </c>
       <c r="J500" s="4" t="s">
-        <v>1391</v>
+        <v>1393</v>
       </c>
       <c r="K500" s="5"/>
       <c r="L500" s="5"/>
@@ -21420,34 +21434,34 @@
     </row>
     <row r="501" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A501" s="2" t="s">
-        <v>1392</v>
+        <v>1394</v>
       </c>
       <c r="B501" s="4" t="s">
-        <v>1393</v>
+        <v>1395</v>
       </c>
       <c r="C501" s="4" t="s">
-        <v>1394</v>
+        <v>1396</v>
       </c>
       <c r="D501" s="4" t="s">
-        <v>1395</v>
+        <v>1397</v>
       </c>
       <c r="E501" s="4" t="s">
-        <v>1396</v>
+        <v>1398</v>
       </c>
       <c r="F501" s="4" t="s">
-        <v>1397</v>
+        <v>1399</v>
       </c>
       <c r="G501" s="4" t="s">
-        <v>1398</v>
+        <v>1400</v>
       </c>
       <c r="H501" s="4" t="s">
-        <v>1399</v>
+        <v>1401</v>
       </c>
       <c r="I501" s="4" t="s">
-        <v>1400</v>
+        <v>1402</v>
       </c>
       <c r="J501" s="4" t="s">
-        <v>1401</v>
+        <v>1403</v>
       </c>
       <c r="K501" s="5"/>
       <c r="L501" s="5"/>
@@ -21468,34 +21482,34 @@
     </row>
     <row r="502" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A502" s="2" t="s">
-        <v>1402</v>
+        <v>1404</v>
       </c>
       <c r="B502" s="4" t="s">
-        <v>1403</v>
+        <v>1405</v>
       </c>
       <c r="C502" s="4" t="s">
-        <v>1404</v>
+        <v>1406</v>
       </c>
       <c r="D502" s="4" t="s">
-        <v>1405</v>
+        <v>1407</v>
       </c>
       <c r="E502" s="4" t="s">
-        <v>1406</v>
+        <v>1408</v>
       </c>
       <c r="F502" s="4" t="s">
-        <v>1407</v>
+        <v>1409</v>
       </c>
       <c r="G502" s="4" t="s">
-        <v>1408</v>
+        <v>1410</v>
       </c>
       <c r="H502" s="4" t="s">
-        <v>1409</v>
+        <v>1411</v>
       </c>
       <c r="I502" s="4" t="s">
-        <v>1410</v>
+        <v>1412</v>
       </c>
       <c r="J502" s="4" t="s">
-        <v>1411</v>
+        <v>1413</v>
       </c>
       <c r="K502" s="5"/>
       <c r="L502" s="5"/>
@@ -21516,30 +21530,30 @@
     </row>
     <row r="503" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A503" s="2" t="s">
-        <v>1412</v>
+        <v>1414</v>
       </c>
       <c r="B503" s="3" t="s">
-        <v>1413</v>
+        <v>1415</v>
       </c>
       <c r="C503" s="3"/>
       <c r="D503" s="3" t="s">
-        <v>1414</v>
+        <v>1416</v>
       </c>
       <c r="E503" s="3"/>
       <c r="F503" s="3" t="s">
-        <v>1415</v>
+        <v>1417</v>
       </c>
       <c r="G503" s="3"/>
       <c r="H503" s="3" t="s">
-        <v>1416</v>
+        <v>1418</v>
       </c>
       <c r="I503" s="3"/>
       <c r="J503" s="3" t="s">
-        <v>1417</v>
+        <v>1419</v>
       </c>
       <c r="K503" s="3"/>
       <c r="L503" s="3" t="s">
-        <v>1418</v>
+        <v>1420</v>
       </c>
       <c r="M503" s="3"/>
       <c r="N503" s="5"/>
@@ -21558,38 +21572,38 @@
     </row>
     <row r="504" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A504" s="2" t="s">
-        <v>1419</v>
+        <v>1421</v>
       </c>
       <c r="B504" s="3" t="s">
-        <v>1420</v>
+        <v>1422</v>
       </c>
       <c r="C504" s="3"/>
       <c r="D504" s="3" t="s">
-        <v>1421</v>
+        <v>1423</v>
       </c>
       <c r="E504" s="3"/>
       <c r="F504" s="3" t="s">
-        <v>1422</v>
+        <v>1424</v>
       </c>
       <c r="G504" s="3"/>
       <c r="H504" s="3" t="s">
-        <v>1423</v>
+        <v>1425</v>
       </c>
       <c r="I504" s="3"/>
       <c r="J504" s="3" t="s">
-        <v>1424</v>
+        <v>1426</v>
       </c>
       <c r="K504" s="3"/>
       <c r="L504" s="3" t="s">
-        <v>1425</v>
+        <v>1427</v>
       </c>
       <c r="M504" s="3"/>
       <c r="N504" s="3" t="s">
-        <v>1426</v>
+        <v>1428</v>
       </c>
       <c r="O504" s="3"/>
       <c r="P504" s="3" t="s">
-        <v>1427</v>
+        <v>1429</v>
       </c>
       <c r="Q504" s="3"/>
       <c r="R504" s="1"/>
@@ -21604,14 +21618,14 @@
     </row>
     <row r="505" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A505" s="2" t="s">
-        <v>1428</v>
+        <v>1430</v>
       </c>
       <c r="B505" s="3" t="s">
-        <v>1429</v>
+        <v>1431</v>
       </c>
       <c r="C505" s="3"/>
       <c r="D505" s="3" t="s">
-        <v>1430</v>
+        <v>1432</v>
       </c>
       <c r="E505" s="3"/>
       <c r="F505" s="5"/>
@@ -21619,19 +21633,19 @@
       <c r="H505" s="5"/>
       <c r="I505" s="5"/>
       <c r="J505" s="3" t="s">
-        <v>1431</v>
+        <v>1433</v>
       </c>
       <c r="K505" s="3"/>
       <c r="L505" s="3" t="s">
-        <v>1432</v>
+        <v>1434</v>
       </c>
       <c r="M505" s="3"/>
       <c r="N505" s="3" t="s">
-        <v>1433</v>
+        <v>1435</v>
       </c>
       <c r="O505" s="3"/>
       <c r="P505" s="3" t="s">
-        <v>1434</v>
+        <v>1436</v>
       </c>
       <c r="Q505" s="3"/>
       <c r="R505" s="1"/>
@@ -21646,30 +21660,30 @@
     </row>
     <row r="506" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A506" s="2" t="s">
-        <v>1435</v>
+        <v>1437</v>
       </c>
       <c r="B506" s="3" t="s">
-        <v>1436</v>
+        <v>1438</v>
       </c>
       <c r="C506" s="3"/>
       <c r="D506" s="3" t="s">
-        <v>1437</v>
+        <v>1439</v>
       </c>
       <c r="E506" s="3"/>
       <c r="F506" s="3" t="s">
-        <v>1438</v>
+        <v>1440</v>
       </c>
       <c r="G506" s="3"/>
       <c r="H506" s="3" t="s">
-        <v>1439</v>
+        <v>1441</v>
       </c>
       <c r="I506" s="3"/>
       <c r="J506" s="3" t="s">
-        <v>1440</v>
+        <v>1442</v>
       </c>
       <c r="K506" s="3"/>
       <c r="L506" s="3" t="s">
-        <v>1441</v>
+        <v>1443</v>
       </c>
       <c r="M506" s="3"/>
       <c r="N506" s="5"/>
@@ -21688,28 +21702,28 @@
     </row>
     <row r="507" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A507" s="2" t="s">
-        <v>1442</v>
+        <v>1444</v>
       </c>
       <c r="B507" s="4" t="s">
-        <v>1443</v>
+        <v>1445</v>
       </c>
       <c r="C507" s="4" t="s">
-        <v>1444</v>
+        <v>1446</v>
       </c>
       <c r="D507" s="4" t="s">
-        <v>1445</v>
+        <v>1447</v>
       </c>
       <c r="E507" s="4" t="s">
-        <v>1446</v>
+        <v>1448</v>
       </c>
       <c r="F507" s="4" t="s">
-        <v>1447</v>
+        <v>1449</v>
       </c>
       <c r="G507" s="5"/>
       <c r="H507" s="5"/>
       <c r="I507" s="5"/>
       <c r="J507" s="3" t="s">
-        <v>1448</v>
+        <v>1450</v>
       </c>
       <c r="K507" s="3"/>
       <c r="L507" s="5"/>
@@ -21717,10 +21731,10 @@
       <c r="N507" s="5"/>
       <c r="O507" s="5"/>
       <c r="P507" s="4" t="s">
-        <v>1449</v>
+        <v>1451</v>
       </c>
       <c r="Q507" s="4" t="s">
-        <v>1450</v>
+        <v>1452</v>
       </c>
       <c r="R507" s="1"/>
       <c r="S507" s="1"/>
@@ -21734,7 +21748,7 @@
     </row>
     <row r="508" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A508" s="2" t="s">
-        <v>1451</v>
+        <v>1453</v>
       </c>
       <c r="B508" s="5"/>
       <c r="C508" s="5"/>
@@ -21764,7 +21778,7 @@
     </row>
     <row r="509" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A509" s="2" t="s">
-        <v>1452</v>
+        <v>1454</v>
       </c>
       <c r="B509" s="5"/>
       <c r="C509" s="5"/>
@@ -21794,7 +21808,7 @@
     </row>
     <row r="510" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A510" s="2" t="s">
-        <v>1453</v>
+        <v>1455</v>
       </c>
       <c r="B510" s="5"/>
       <c r="C510" s="5"/>
@@ -21824,7 +21838,7 @@
     </row>
     <row r="511" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A511" s="2" t="s">
-        <v>1454</v>
+        <v>1456</v>
       </c>
       <c r="B511" s="5"/>
       <c r="C511" s="5"/>
@@ -21854,7 +21868,7 @@
     </row>
     <row r="512" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A512" s="2" t="s">
-        <v>1455</v>
+        <v>1457</v>
       </c>
       <c r="B512" s="5"/>
       <c r="C512" s="5"/>
@@ -21884,7 +21898,7 @@
     </row>
     <row r="513" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A513" s="2" t="s">
-        <v>1456</v>
+        <v>1458</v>
       </c>
       <c r="B513" s="5"/>
       <c r="C513" s="5"/>
@@ -21914,7 +21928,7 @@
     </row>
     <row r="514" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A514" s="2" t="s">
-        <v>1457</v>
+        <v>1459</v>
       </c>
       <c r="B514" s="5"/>
       <c r="C514" s="5"/>

</xml_diff>

<commit_message>
working EncKey  menu, saving and loading
</commit_message>
<xml_diff>
--- a/docs/UV K5 EEPROM.xlsx
+++ b/docs/UV K5 EEPROM.xlsx
@@ -2248,7 +2248,7 @@
     <t xml:space="preserve">0x0F30</t>
   </si>
   <si>
-    <t xml:space="preserve">AES KEY</t>
+    <t xml:space="preserve">ENCRYPTION KEY</t>
   </si>
   <si>
     <t xml:space="preserve">0x0F40</t>
@@ -4539,7 +4539,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -4634,11 +4634,11 @@
   </sheetPr>
   <dimension ref="A1:Z1001"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A214" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B237" activeCellId="0" sqref="B237"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A223" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B246" activeCellId="0" sqref="B246"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.7421875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.7578125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1"/>
@@ -12646,10 +12646,10 @@
       <c r="M236" s="4" t="s">
         <v>705</v>
       </c>
-      <c r="N236" s="0" t="s">
+      <c r="N236" s="9" t="s">
         <v>706</v>
       </c>
-      <c r="O236" s="9" t="s">
+      <c r="O236" s="1" t="s">
         <v>707</v>
       </c>
       <c r="P236" s="5"/>

</xml_diff>

<commit_message>
RP STE menu item removed
</commit_message>
<xml_diff>
--- a/docs/UV K5 EEPROM.xlsx
+++ b/docs/UV K5 EEPROM.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1462" uniqueCount="1460">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1461" uniqueCount="1459">
   <si>
     <t xml:space="preserve">00</t>
   </si>
@@ -2132,9 +2132,6 @@
   </si>
   <si>
     <t xml:space="preserve">ROGER</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RP-STE</t>
   </si>
   <si>
     <t xml:space="preserve">???TX CH???</t>
@@ -4634,11 +4631,11 @@
   </sheetPr>
   <dimension ref="A1:Z1001"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A223" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B246" activeCellId="0" sqref="B246"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A206" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I219" activeCellId="0" sqref="I219"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.7578125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.77734375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1"/>
@@ -12640,17 +12637,15 @@
       <c r="K236" s="4" t="s">
         <v>703</v>
       </c>
-      <c r="L236" s="4" t="s">
+      <c r="L236" s="7"/>
+      <c r="M236" s="4" t="s">
         <v>704</v>
       </c>
-      <c r="M236" s="4" t="s">
+      <c r="N236" s="9" t="s">
         <v>705</v>
       </c>
-      <c r="N236" s="9" t="s">
+      <c r="O236" s="1" t="s">
         <v>706</v>
-      </c>
-      <c r="O236" s="1" t="s">
-        <v>707</v>
       </c>
       <c r="P236" s="5"/>
       <c r="Q236" s="5"/>
@@ -12666,10 +12661,10 @@
     </row>
     <row r="237" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A237" s="2" t="s">
+        <v>707</v>
+      </c>
+      <c r="B237" s="3" t="s">
         <v>708</v>
-      </c>
-      <c r="B237" s="3" t="s">
-        <v>709</v>
       </c>
       <c r="C237" s="3"/>
       <c r="D237" s="3"/>
@@ -12698,10 +12693,10 @@
     </row>
     <row r="238" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A238" s="2" t="s">
+        <v>709</v>
+      </c>
+      <c r="B238" s="3" t="s">
         <v>710</v>
-      </c>
-      <c r="B238" s="3" t="s">
-        <v>711</v>
       </c>
       <c r="C238" s="3"/>
       <c r="D238" s="3"/>
@@ -12730,40 +12725,40 @@
     </row>
     <row r="239" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A239" s="2" t="s">
+        <v>711</v>
+      </c>
+      <c r="B239" s="4" t="s">
         <v>712</v>
       </c>
-      <c r="B239" s="4" t="s">
+      <c r="C239" s="4" t="s">
         <v>713</v>
       </c>
-      <c r="C239" s="4" t="s">
+      <c r="D239" s="4" t="s">
         <v>714</v>
       </c>
-      <c r="D239" s="4" t="s">
+      <c r="E239" s="4" t="s">
         <v>715</v>
       </c>
-      <c r="E239" s="4" t="s">
+      <c r="F239" s="4" t="s">
         <v>716</v>
       </c>
-      <c r="F239" s="4" t="s">
+      <c r="G239" s="4" t="s">
         <v>717</v>
       </c>
-      <c r="G239" s="4" t="s">
+      <c r="H239" s="4" t="s">
         <v>718</v>
       </c>
-      <c r="H239" s="4" t="s">
+      <c r="I239" s="4" t="s">
         <v>719</v>
       </c>
-      <c r="I239" s="4" t="s">
+      <c r="J239" s="4" t="s">
         <v>720</v>
       </c>
-      <c r="J239" s="4" t="s">
+      <c r="K239" s="4" t="s">
         <v>721</v>
       </c>
-      <c r="K239" s="4" t="s">
+      <c r="L239" s="4" t="s">
         <v>722</v>
-      </c>
-      <c r="L239" s="4" t="s">
-        <v>723</v>
       </c>
       <c r="M239" s="5"/>
       <c r="N239" s="5"/>
@@ -12782,10 +12777,10 @@
     </row>
     <row r="240" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A240" s="2" t="s">
+        <v>723</v>
+      </c>
+      <c r="B240" s="3" t="s">
         <v>724</v>
-      </c>
-      <c r="B240" s="3" t="s">
-        <v>725</v>
       </c>
       <c r="C240" s="3"/>
       <c r="D240" s="3"/>
@@ -12795,7 +12790,7 @@
       <c r="H240" s="3"/>
       <c r="I240" s="3"/>
       <c r="J240" s="3" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
       <c r="K240" s="3"/>
       <c r="L240" s="3"/>
@@ -12816,10 +12811,10 @@
     </row>
     <row r="241" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A241" s="2" t="s">
+        <v>726</v>
+      </c>
+      <c r="B241" s="3" t="s">
         <v>727</v>
-      </c>
-      <c r="B241" s="3" t="s">
-        <v>728</v>
       </c>
       <c r="C241" s="3"/>
       <c r="D241" s="3"/>
@@ -12829,7 +12824,7 @@
       <c r="H241" s="3"/>
       <c r="I241" s="3"/>
       <c r="J241" s="3" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
       <c r="K241" s="3"/>
       <c r="L241" s="3"/>
@@ -12850,10 +12845,10 @@
     </row>
     <row r="242" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A242" s="2" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
       <c r="B242" s="3" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
       <c r="C242" s="3"/>
       <c r="D242" s="3"/>
@@ -12863,7 +12858,7 @@
       <c r="H242" s="3"/>
       <c r="I242" s="3"/>
       <c r="J242" s="3" t="s">
-        <v>731</v>
+        <v>730</v>
       </c>
       <c r="K242" s="3"/>
       <c r="L242" s="3"/>
@@ -12884,10 +12879,10 @@
     </row>
     <row r="243" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A243" s="2" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
       <c r="B243" s="3" t="s">
-        <v>731</v>
+        <v>730</v>
       </c>
       <c r="C243" s="3"/>
       <c r="D243" s="3"/>
@@ -12897,25 +12892,25 @@
       <c r="H243" s="3"/>
       <c r="I243" s="3"/>
       <c r="J243" s="4" t="s">
+        <v>732</v>
+      </c>
+      <c r="K243" s="4" t="s">
         <v>733</v>
       </c>
-      <c r="K243" s="4" t="s">
+      <c r="L243" s="4" t="s">
         <v>734</v>
       </c>
-      <c r="L243" s="4" t="s">
+      <c r="M243" s="4" t="s">
         <v>735</v>
       </c>
-      <c r="M243" s="4" t="s">
+      <c r="N243" s="4" t="s">
         <v>736</v>
       </c>
-      <c r="N243" s="4" t="s">
+      <c r="O243" s="4" t="s">
         <v>737</v>
       </c>
-      <c r="O243" s="4" t="s">
+      <c r="P243" s="4" t="s">
         <v>738</v>
-      </c>
-      <c r="P243" s="4" t="s">
-        <v>739</v>
       </c>
       <c r="Q243" s="5"/>
       <c r="R243" s="1"/>
@@ -12930,7 +12925,7 @@
     </row>
     <row r="244" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A244" s="2" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
       <c r="B244" s="5"/>
       <c r="C244" s="5"/>
@@ -12960,10 +12955,10 @@
     </row>
     <row r="245" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A245" s="2" t="s">
+        <v>740</v>
+      </c>
+      <c r="B245" s="3" t="s">
         <v>741</v>
-      </c>
-      <c r="B245" s="3" t="s">
-        <v>742</v>
       </c>
       <c r="C245" s="3"/>
       <c r="D245" s="3"/>
@@ -12992,28 +12987,28 @@
     </row>
     <row r="246" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A246" s="2" t="s">
+        <v>742</v>
+      </c>
+      <c r="B246" s="4" t="s">
         <v>743</v>
       </c>
-      <c r="B246" s="4" t="s">
+      <c r="C246" s="4" t="s">
         <v>744</v>
       </c>
-      <c r="C246" s="4" t="s">
+      <c r="D246" s="4" t="s">
         <v>745</v>
       </c>
-      <c r="D246" s="4" t="s">
+      <c r="E246" s="4" t="s">
         <v>746</v>
       </c>
-      <c r="E246" s="4" t="s">
+      <c r="F246" s="4" t="s">
         <v>747</v>
       </c>
-      <c r="F246" s="4" t="s">
+      <c r="G246" s="4" t="s">
         <v>748</v>
       </c>
-      <c r="G246" s="4" t="s">
+      <c r="H246" s="4" t="s">
         <v>749</v>
-      </c>
-      <c r="H246" s="4" t="s">
-        <v>750</v>
       </c>
       <c r="I246" s="5"/>
       <c r="J246" s="5"/>
@@ -13036,10 +13031,10 @@
     </row>
     <row r="247" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A247" s="2" t="s">
+        <v>750</v>
+      </c>
+      <c r="B247" s="3" t="s">
         <v>751</v>
-      </c>
-      <c r="B247" s="3" t="s">
-        <v>752</v>
       </c>
       <c r="C247" s="3"/>
       <c r="D247" s="3"/>
@@ -13068,10 +13063,10 @@
     </row>
     <row r="248" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A248" s="2" t="s">
+        <v>752</v>
+      </c>
+      <c r="B248" s="3" t="s">
         <v>753</v>
-      </c>
-      <c r="B248" s="3" t="s">
-        <v>754</v>
       </c>
       <c r="C248" s="3"/>
       <c r="D248" s="3"/>
@@ -13100,10 +13095,10 @@
     </row>
     <row r="249" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A249" s="2" t="s">
+        <v>754</v>
+      </c>
+      <c r="B249" s="3" t="s">
         <v>755</v>
-      </c>
-      <c r="B249" s="3" t="s">
-        <v>756</v>
       </c>
       <c r="C249" s="3"/>
       <c r="D249" s="3"/>
@@ -13132,10 +13127,10 @@
     </row>
     <row r="250" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A250" s="2" t="s">
+        <v>756</v>
+      </c>
+      <c r="B250" s="3" t="s">
         <v>757</v>
-      </c>
-      <c r="B250" s="3" t="s">
-        <v>758</v>
       </c>
       <c r="C250" s="3"/>
       <c r="D250" s="3"/>
@@ -13164,10 +13159,10 @@
     </row>
     <row r="251" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A251" s="2" t="s">
+        <v>758</v>
+      </c>
+      <c r="B251" s="3" t="s">
         <v>759</v>
-      </c>
-      <c r="B251" s="3" t="s">
-        <v>760</v>
       </c>
       <c r="C251" s="3"/>
       <c r="D251" s="3"/>
@@ -13196,10 +13191,10 @@
     </row>
     <row r="252" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A252" s="2" t="s">
+        <v>760</v>
+      </c>
+      <c r="B252" s="3" t="s">
         <v>761</v>
-      </c>
-      <c r="B252" s="3" t="s">
-        <v>762</v>
       </c>
       <c r="C252" s="3"/>
       <c r="D252" s="3"/>
@@ -13228,10 +13223,10 @@
     </row>
     <row r="253" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A253" s="2" t="s">
+        <v>762</v>
+      </c>
+      <c r="B253" s="3" t="s">
         <v>763</v>
-      </c>
-      <c r="B253" s="3" t="s">
-        <v>764</v>
       </c>
       <c r="C253" s="3"/>
       <c r="D253" s="3"/>
@@ -13260,10 +13255,10 @@
     </row>
     <row r="254" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A254" s="2" t="s">
+        <v>764</v>
+      </c>
+      <c r="B254" s="3" t="s">
         <v>765</v>
-      </c>
-      <c r="B254" s="3" t="s">
-        <v>766</v>
       </c>
       <c r="C254" s="3"/>
       <c r="D254" s="3"/>
@@ -13292,10 +13287,10 @@
     </row>
     <row r="255" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A255" s="2" t="s">
+        <v>766</v>
+      </c>
+      <c r="B255" s="3" t="s">
         <v>767</v>
-      </c>
-      <c r="B255" s="3" t="s">
-        <v>768</v>
       </c>
       <c r="C255" s="3"/>
       <c r="D255" s="3"/>
@@ -13324,10 +13319,10 @@
     </row>
     <row r="256" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A256" s="2" t="s">
+        <v>768</v>
+      </c>
+      <c r="B256" s="3" t="s">
         <v>769</v>
-      </c>
-      <c r="B256" s="3" t="s">
-        <v>770</v>
       </c>
       <c r="C256" s="3"/>
       <c r="D256" s="3"/>
@@ -13356,10 +13351,10 @@
     </row>
     <row r="257" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A257" s="2" t="s">
+        <v>770</v>
+      </c>
+      <c r="B257" s="3" t="s">
         <v>771</v>
-      </c>
-      <c r="B257" s="3" t="s">
-        <v>772</v>
       </c>
       <c r="C257" s="3"/>
       <c r="D257" s="3"/>
@@ -13388,10 +13383,10 @@
     </row>
     <row r="258" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A258" s="2" t="s">
+        <v>772</v>
+      </c>
+      <c r="B258" s="3" t="s">
         <v>773</v>
-      </c>
-      <c r="B258" s="3" t="s">
-        <v>774</v>
       </c>
       <c r="C258" s="3"/>
       <c r="D258" s="3"/>
@@ -13420,10 +13415,10 @@
     </row>
     <row r="259" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A259" s="2" t="s">
+        <v>774</v>
+      </c>
+      <c r="B259" s="3" t="s">
         <v>775</v>
-      </c>
-      <c r="B259" s="3" t="s">
-        <v>776</v>
       </c>
       <c r="C259" s="3"/>
       <c r="D259" s="3"/>
@@ -13452,10 +13447,10 @@
     </row>
     <row r="260" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A260" s="2" t="s">
+        <v>776</v>
+      </c>
+      <c r="B260" s="3" t="s">
         <v>777</v>
-      </c>
-      <c r="B260" s="3" t="s">
-        <v>778</v>
       </c>
       <c r="C260" s="3"/>
       <c r="D260" s="3"/>
@@ -13484,10 +13479,10 @@
     </row>
     <row r="261" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A261" s="2" t="s">
+        <v>778</v>
+      </c>
+      <c r="B261" s="3" t="s">
         <v>779</v>
-      </c>
-      <c r="B261" s="3" t="s">
-        <v>780</v>
       </c>
       <c r="C261" s="3"/>
       <c r="D261" s="3"/>
@@ -13516,10 +13511,10 @@
     </row>
     <row r="262" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A262" s="2" t="s">
+        <v>780</v>
+      </c>
+      <c r="B262" s="3" t="s">
         <v>781</v>
-      </c>
-      <c r="B262" s="3" t="s">
-        <v>782</v>
       </c>
       <c r="C262" s="3"/>
       <c r="D262" s="3"/>
@@ -13548,10 +13543,10 @@
     </row>
     <row r="263" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A263" s="2" t="s">
+        <v>782</v>
+      </c>
+      <c r="B263" s="3" t="s">
         <v>783</v>
-      </c>
-      <c r="B263" s="3" t="s">
-        <v>784</v>
       </c>
       <c r="C263" s="3"/>
       <c r="D263" s="3"/>
@@ -13580,10 +13575,10 @@
     </row>
     <row r="264" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A264" s="2" t="s">
+        <v>784</v>
+      </c>
+      <c r="B264" s="3" t="s">
         <v>785</v>
-      </c>
-      <c r="B264" s="3" t="s">
-        <v>786</v>
       </c>
       <c r="C264" s="3"/>
       <c r="D264" s="3"/>
@@ -13612,10 +13607,10 @@
     </row>
     <row r="265" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A265" s="2" t="s">
+        <v>786</v>
+      </c>
+      <c r="B265" s="3" t="s">
         <v>787</v>
-      </c>
-      <c r="B265" s="3" t="s">
-        <v>788</v>
       </c>
       <c r="C265" s="3"/>
       <c r="D265" s="3"/>
@@ -13644,10 +13639,10 @@
     </row>
     <row r="266" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A266" s="2" t="s">
+        <v>788</v>
+      </c>
+      <c r="B266" s="3" t="s">
         <v>789</v>
-      </c>
-      <c r="B266" s="3" t="s">
-        <v>790</v>
       </c>
       <c r="C266" s="3"/>
       <c r="D266" s="3"/>
@@ -13676,10 +13671,10 @@
     </row>
     <row r="267" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A267" s="2" t="s">
+        <v>790</v>
+      </c>
+      <c r="B267" s="3" t="s">
         <v>791</v>
-      </c>
-      <c r="B267" s="3" t="s">
-        <v>792</v>
       </c>
       <c r="C267" s="3"/>
       <c r="D267" s="3"/>
@@ -13708,10 +13703,10 @@
     </row>
     <row r="268" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A268" s="2" t="s">
+        <v>792</v>
+      </c>
+      <c r="B268" s="3" t="s">
         <v>793</v>
-      </c>
-      <c r="B268" s="3" t="s">
-        <v>794</v>
       </c>
       <c r="C268" s="3"/>
       <c r="D268" s="3"/>
@@ -13740,10 +13735,10 @@
     </row>
     <row r="269" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A269" s="2" t="s">
+        <v>794</v>
+      </c>
+      <c r="B269" s="3" t="s">
         <v>795</v>
-      </c>
-      <c r="B269" s="3" t="s">
-        <v>796</v>
       </c>
       <c r="C269" s="3"/>
       <c r="D269" s="3"/>
@@ -13772,10 +13767,10 @@
     </row>
     <row r="270" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A270" s="2" t="s">
+        <v>796</v>
+      </c>
+      <c r="B270" s="3" t="s">
         <v>797</v>
-      </c>
-      <c r="B270" s="3" t="s">
-        <v>798</v>
       </c>
       <c r="C270" s="3"/>
       <c r="D270" s="3"/>
@@ -13804,10 +13799,10 @@
     </row>
     <row r="271" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A271" s="2" t="s">
+        <v>798</v>
+      </c>
+      <c r="B271" s="3" t="s">
         <v>799</v>
-      </c>
-      <c r="B271" s="3" t="s">
-        <v>800</v>
       </c>
       <c r="C271" s="3"/>
       <c r="D271" s="3"/>
@@ -13836,10 +13831,10 @@
     </row>
     <row r="272" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A272" s="2" t="s">
+        <v>800</v>
+      </c>
+      <c r="B272" s="3" t="s">
         <v>801</v>
-      </c>
-      <c r="B272" s="3" t="s">
-        <v>802</v>
       </c>
       <c r="C272" s="3"/>
       <c r="D272" s="3"/>
@@ -13868,10 +13863,10 @@
     </row>
     <row r="273" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A273" s="2" t="s">
+        <v>802</v>
+      </c>
+      <c r="B273" s="3" t="s">
         <v>803</v>
-      </c>
-      <c r="B273" s="3" t="s">
-        <v>804</v>
       </c>
       <c r="C273" s="3"/>
       <c r="D273" s="3"/>
@@ -13900,10 +13895,10 @@
     </row>
     <row r="274" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A274" s="2" t="s">
+        <v>804</v>
+      </c>
+      <c r="B274" s="3" t="s">
         <v>805</v>
-      </c>
-      <c r="B274" s="3" t="s">
-        <v>806</v>
       </c>
       <c r="C274" s="3"/>
       <c r="D274" s="3"/>
@@ -13932,10 +13927,10 @@
     </row>
     <row r="275" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A275" s="2" t="s">
+        <v>806</v>
+      </c>
+      <c r="B275" s="3" t="s">
         <v>807</v>
-      </c>
-      <c r="B275" s="3" t="s">
-        <v>808</v>
       </c>
       <c r="C275" s="3"/>
       <c r="D275" s="3"/>
@@ -13964,10 +13959,10 @@
     </row>
     <row r="276" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A276" s="2" t="s">
+        <v>808</v>
+      </c>
+      <c r="B276" s="3" t="s">
         <v>809</v>
-      </c>
-      <c r="B276" s="3" t="s">
-        <v>810</v>
       </c>
       <c r="C276" s="3"/>
       <c r="D276" s="3"/>
@@ -13996,10 +13991,10 @@
     </row>
     <row r="277" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A277" s="2" t="s">
+        <v>810</v>
+      </c>
+      <c r="B277" s="3" t="s">
         <v>811</v>
-      </c>
-      <c r="B277" s="3" t="s">
-        <v>812</v>
       </c>
       <c r="C277" s="3"/>
       <c r="D277" s="3"/>
@@ -14028,10 +14023,10 @@
     </row>
     <row r="278" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A278" s="2" t="s">
+        <v>812</v>
+      </c>
+      <c r="B278" s="3" t="s">
         <v>813</v>
-      </c>
-      <c r="B278" s="3" t="s">
-        <v>814</v>
       </c>
       <c r="C278" s="3"/>
       <c r="D278" s="3"/>
@@ -14060,10 +14055,10 @@
     </row>
     <row r="279" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A279" s="2" t="s">
+        <v>814</v>
+      </c>
+      <c r="B279" s="3" t="s">
         <v>815</v>
-      </c>
-      <c r="B279" s="3" t="s">
-        <v>816</v>
       </c>
       <c r="C279" s="3"/>
       <c r="D279" s="3"/>
@@ -14092,10 +14087,10 @@
     </row>
     <row r="280" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A280" s="2" t="s">
+        <v>816</v>
+      </c>
+      <c r="B280" s="3" t="s">
         <v>817</v>
-      </c>
-      <c r="B280" s="3" t="s">
-        <v>818</v>
       </c>
       <c r="C280" s="3"/>
       <c r="D280" s="3"/>
@@ -14124,10 +14119,10 @@
     </row>
     <row r="281" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A281" s="2" t="s">
+        <v>818</v>
+      </c>
+      <c r="B281" s="3" t="s">
         <v>819</v>
-      </c>
-      <c r="B281" s="3" t="s">
-        <v>820</v>
       </c>
       <c r="C281" s="3"/>
       <c r="D281" s="3"/>
@@ -14156,10 +14151,10 @@
     </row>
     <row r="282" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A282" s="2" t="s">
+        <v>820</v>
+      </c>
+      <c r="B282" s="3" t="s">
         <v>821</v>
-      </c>
-      <c r="B282" s="3" t="s">
-        <v>822</v>
       </c>
       <c r="C282" s="3"/>
       <c r="D282" s="3"/>
@@ -14188,10 +14183,10 @@
     </row>
     <row r="283" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A283" s="2" t="s">
+        <v>822</v>
+      </c>
+      <c r="B283" s="3" t="s">
         <v>823</v>
-      </c>
-      <c r="B283" s="3" t="s">
-        <v>824</v>
       </c>
       <c r="C283" s="3"/>
       <c r="D283" s="3"/>
@@ -14220,10 +14215,10 @@
     </row>
     <row r="284" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A284" s="2" t="s">
+        <v>824</v>
+      </c>
+      <c r="B284" s="3" t="s">
         <v>825</v>
-      </c>
-      <c r="B284" s="3" t="s">
-        <v>826</v>
       </c>
       <c r="C284" s="3"/>
       <c r="D284" s="3"/>
@@ -14252,10 +14247,10 @@
     </row>
     <row r="285" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A285" s="2" t="s">
+        <v>826</v>
+      </c>
+      <c r="B285" s="3" t="s">
         <v>827</v>
-      </c>
-      <c r="B285" s="3" t="s">
-        <v>828</v>
       </c>
       <c r="C285" s="3"/>
       <c r="D285" s="3"/>
@@ -14284,10 +14279,10 @@
     </row>
     <row r="286" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A286" s="2" t="s">
+        <v>828</v>
+      </c>
+      <c r="B286" s="3" t="s">
         <v>829</v>
-      </c>
-      <c r="B286" s="3" t="s">
-        <v>830</v>
       </c>
       <c r="C286" s="3"/>
       <c r="D286" s="3"/>
@@ -14316,10 +14311,10 @@
     </row>
     <row r="287" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A287" s="2" t="s">
+        <v>830</v>
+      </c>
+      <c r="B287" s="3" t="s">
         <v>831</v>
-      </c>
-      <c r="B287" s="3" t="s">
-        <v>832</v>
       </c>
       <c r="C287" s="3"/>
       <c r="D287" s="3"/>
@@ -14348,10 +14343,10 @@
     </row>
     <row r="288" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A288" s="2" t="s">
+        <v>832</v>
+      </c>
+      <c r="B288" s="3" t="s">
         <v>833</v>
-      </c>
-      <c r="B288" s="3" t="s">
-        <v>834</v>
       </c>
       <c r="C288" s="3"/>
       <c r="D288" s="3"/>
@@ -14380,10 +14375,10 @@
     </row>
     <row r="289" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A289" s="2" t="s">
+        <v>834</v>
+      </c>
+      <c r="B289" s="3" t="s">
         <v>835</v>
-      </c>
-      <c r="B289" s="3" t="s">
-        <v>836</v>
       </c>
       <c r="C289" s="3"/>
       <c r="D289" s="3"/>
@@ -14412,10 +14407,10 @@
     </row>
     <row r="290" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A290" s="2" t="s">
+        <v>836</v>
+      </c>
+      <c r="B290" s="3" t="s">
         <v>837</v>
-      </c>
-      <c r="B290" s="3" t="s">
-        <v>838</v>
       </c>
       <c r="C290" s="3"/>
       <c r="D290" s="3"/>
@@ -14444,10 +14439,10 @@
     </row>
     <row r="291" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A291" s="2" t="s">
+        <v>838</v>
+      </c>
+      <c r="B291" s="3" t="s">
         <v>839</v>
-      </c>
-      <c r="B291" s="3" t="s">
-        <v>840</v>
       </c>
       <c r="C291" s="3"/>
       <c r="D291" s="3"/>
@@ -14476,10 +14471,10 @@
     </row>
     <row r="292" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A292" s="2" t="s">
+        <v>840</v>
+      </c>
+      <c r="B292" s="3" t="s">
         <v>841</v>
-      </c>
-      <c r="B292" s="3" t="s">
-        <v>842</v>
       </c>
       <c r="C292" s="3"/>
       <c r="D292" s="3"/>
@@ -14508,10 +14503,10 @@
     </row>
     <row r="293" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A293" s="2" t="s">
+        <v>842</v>
+      </c>
+      <c r="B293" s="3" t="s">
         <v>843</v>
-      </c>
-      <c r="B293" s="3" t="s">
-        <v>844</v>
       </c>
       <c r="C293" s="3"/>
       <c r="D293" s="3"/>
@@ -14540,10 +14535,10 @@
     </row>
     <row r="294" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A294" s="2" t="s">
+        <v>844</v>
+      </c>
+      <c r="B294" s="3" t="s">
         <v>845</v>
-      </c>
-      <c r="B294" s="3" t="s">
-        <v>846</v>
       </c>
       <c r="C294" s="3"/>
       <c r="D294" s="3"/>
@@ -14572,10 +14567,10 @@
     </row>
     <row r="295" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A295" s="2" t="s">
+        <v>846</v>
+      </c>
+      <c r="B295" s="3" t="s">
         <v>847</v>
-      </c>
-      <c r="B295" s="3" t="s">
-        <v>848</v>
       </c>
       <c r="C295" s="3"/>
       <c r="D295" s="3"/>
@@ -14604,10 +14599,10 @@
     </row>
     <row r="296" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A296" s="2" t="s">
+        <v>848</v>
+      </c>
+      <c r="B296" s="3" t="s">
         <v>849</v>
-      </c>
-      <c r="B296" s="3" t="s">
-        <v>850</v>
       </c>
       <c r="C296" s="3"/>
       <c r="D296" s="3"/>
@@ -14636,10 +14631,10 @@
     </row>
     <row r="297" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A297" s="2" t="s">
+        <v>850</v>
+      </c>
+      <c r="B297" s="3" t="s">
         <v>851</v>
-      </c>
-      <c r="B297" s="3" t="s">
-        <v>852</v>
       </c>
       <c r="C297" s="3"/>
       <c r="D297" s="3"/>
@@ -14668,10 +14663,10 @@
     </row>
     <row r="298" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A298" s="2" t="s">
+        <v>852</v>
+      </c>
+      <c r="B298" s="3" t="s">
         <v>853</v>
-      </c>
-      <c r="B298" s="3" t="s">
-        <v>854</v>
       </c>
       <c r="C298" s="3"/>
       <c r="D298" s="3"/>
@@ -14700,10 +14695,10 @@
     </row>
     <row r="299" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A299" s="2" t="s">
+        <v>854</v>
+      </c>
+      <c r="B299" s="3" t="s">
         <v>855</v>
-      </c>
-      <c r="B299" s="3" t="s">
-        <v>856</v>
       </c>
       <c r="C299" s="3"/>
       <c r="D299" s="3"/>
@@ -14732,10 +14727,10 @@
     </row>
     <row r="300" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A300" s="2" t="s">
+        <v>856</v>
+      </c>
+      <c r="B300" s="3" t="s">
         <v>857</v>
-      </c>
-      <c r="B300" s="3" t="s">
-        <v>858</v>
       </c>
       <c r="C300" s="3"/>
       <c r="D300" s="3"/>
@@ -14764,10 +14759,10 @@
     </row>
     <row r="301" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A301" s="2" t="s">
+        <v>858</v>
+      </c>
+      <c r="B301" s="3" t="s">
         <v>859</v>
-      </c>
-      <c r="B301" s="3" t="s">
-        <v>860</v>
       </c>
       <c r="C301" s="3"/>
       <c r="D301" s="3"/>
@@ -14796,10 +14791,10 @@
     </row>
     <row r="302" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A302" s="2" t="s">
+        <v>860</v>
+      </c>
+      <c r="B302" s="3" t="s">
         <v>861</v>
-      </c>
-      <c r="B302" s="3" t="s">
-        <v>862</v>
       </c>
       <c r="C302" s="3"/>
       <c r="D302" s="3"/>
@@ -14828,10 +14823,10 @@
     </row>
     <row r="303" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A303" s="2" t="s">
+        <v>862</v>
+      </c>
+      <c r="B303" s="3" t="s">
         <v>863</v>
-      </c>
-      <c r="B303" s="3" t="s">
-        <v>864</v>
       </c>
       <c r="C303" s="3"/>
       <c r="D303" s="3"/>
@@ -14860,10 +14855,10 @@
     </row>
     <row r="304" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A304" s="2" t="s">
+        <v>864</v>
+      </c>
+      <c r="B304" s="3" t="s">
         <v>865</v>
-      </c>
-      <c r="B304" s="3" t="s">
-        <v>866</v>
       </c>
       <c r="C304" s="3"/>
       <c r="D304" s="3"/>
@@ -14892,10 +14887,10 @@
     </row>
     <row r="305" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A305" s="2" t="s">
+        <v>866</v>
+      </c>
+      <c r="B305" s="3" t="s">
         <v>867</v>
-      </c>
-      <c r="B305" s="3" t="s">
-        <v>868</v>
       </c>
       <c r="C305" s="3"/>
       <c r="D305" s="3"/>
@@ -14924,10 +14919,10 @@
     </row>
     <row r="306" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A306" s="2" t="s">
+        <v>868</v>
+      </c>
+      <c r="B306" s="3" t="s">
         <v>869</v>
-      </c>
-      <c r="B306" s="3" t="s">
-        <v>870</v>
       </c>
       <c r="C306" s="3"/>
       <c r="D306" s="3"/>
@@ -14956,10 +14951,10 @@
     </row>
     <row r="307" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A307" s="2" t="s">
+        <v>870</v>
+      </c>
+      <c r="B307" s="3" t="s">
         <v>871</v>
-      </c>
-      <c r="B307" s="3" t="s">
-        <v>872</v>
       </c>
       <c r="C307" s="3"/>
       <c r="D307" s="3"/>
@@ -14988,10 +14983,10 @@
     </row>
     <row r="308" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A308" s="2" t="s">
+        <v>872</v>
+      </c>
+      <c r="B308" s="3" t="s">
         <v>873</v>
-      </c>
-      <c r="B308" s="3" t="s">
-        <v>874</v>
       </c>
       <c r="C308" s="3"/>
       <c r="D308" s="3"/>
@@ -15020,10 +15015,10 @@
     </row>
     <row r="309" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A309" s="2" t="s">
+        <v>874</v>
+      </c>
+      <c r="B309" s="3" t="s">
         <v>875</v>
-      </c>
-      <c r="B309" s="3" t="s">
-        <v>876</v>
       </c>
       <c r="C309" s="3"/>
       <c r="D309" s="3"/>
@@ -15052,10 +15047,10 @@
     </row>
     <row r="310" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A310" s="2" t="s">
+        <v>876</v>
+      </c>
+      <c r="B310" s="3" t="s">
         <v>877</v>
-      </c>
-      <c r="B310" s="3" t="s">
-        <v>878</v>
       </c>
       <c r="C310" s="3"/>
       <c r="D310" s="3"/>
@@ -15084,10 +15079,10 @@
     </row>
     <row r="311" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A311" s="2" t="s">
+        <v>878</v>
+      </c>
+      <c r="B311" s="3" t="s">
         <v>879</v>
-      </c>
-      <c r="B311" s="3" t="s">
-        <v>880</v>
       </c>
       <c r="C311" s="3"/>
       <c r="D311" s="3"/>
@@ -15116,10 +15111,10 @@
     </row>
     <row r="312" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A312" s="2" t="s">
+        <v>880</v>
+      </c>
+      <c r="B312" s="3" t="s">
         <v>881</v>
-      </c>
-      <c r="B312" s="3" t="s">
-        <v>882</v>
       </c>
       <c r="C312" s="3"/>
       <c r="D312" s="3"/>
@@ -15148,10 +15143,10 @@
     </row>
     <row r="313" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A313" s="2" t="s">
+        <v>882</v>
+      </c>
+      <c r="B313" s="3" t="s">
         <v>883</v>
-      </c>
-      <c r="B313" s="3" t="s">
-        <v>884</v>
       </c>
       <c r="C313" s="3"/>
       <c r="D313" s="3"/>
@@ -15180,10 +15175,10 @@
     </row>
     <row r="314" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A314" s="2" t="s">
+        <v>884</v>
+      </c>
+      <c r="B314" s="3" t="s">
         <v>885</v>
-      </c>
-      <c r="B314" s="3" t="s">
-        <v>886</v>
       </c>
       <c r="C314" s="3"/>
       <c r="D314" s="3"/>
@@ -15212,10 +15207,10 @@
     </row>
     <row r="315" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A315" s="2" t="s">
+        <v>886</v>
+      </c>
+      <c r="B315" s="3" t="s">
         <v>887</v>
-      </c>
-      <c r="B315" s="3" t="s">
-        <v>888</v>
       </c>
       <c r="C315" s="3"/>
       <c r="D315" s="3"/>
@@ -15244,10 +15239,10 @@
     </row>
     <row r="316" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A316" s="2" t="s">
+        <v>888</v>
+      </c>
+      <c r="B316" s="3" t="s">
         <v>889</v>
-      </c>
-      <c r="B316" s="3" t="s">
-        <v>890</v>
       </c>
       <c r="C316" s="3"/>
       <c r="D316" s="3"/>
@@ -15276,10 +15271,10 @@
     </row>
     <row r="317" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A317" s="2" t="s">
+        <v>890</v>
+      </c>
+      <c r="B317" s="3" t="s">
         <v>891</v>
-      </c>
-      <c r="B317" s="3" t="s">
-        <v>892</v>
       </c>
       <c r="C317" s="3"/>
       <c r="D317" s="3"/>
@@ -15308,10 +15303,10 @@
     </row>
     <row r="318" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A318" s="2" t="s">
+        <v>892</v>
+      </c>
+      <c r="B318" s="3" t="s">
         <v>893</v>
-      </c>
-      <c r="B318" s="3" t="s">
-        <v>894</v>
       </c>
       <c r="C318" s="3"/>
       <c r="D318" s="3"/>
@@ -15340,10 +15335,10 @@
     </row>
     <row r="319" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A319" s="2" t="s">
+        <v>894</v>
+      </c>
+      <c r="B319" s="3" t="s">
         <v>895</v>
-      </c>
-      <c r="B319" s="3" t="s">
-        <v>896</v>
       </c>
       <c r="C319" s="3"/>
       <c r="D319" s="3"/>
@@ -15372,10 +15367,10 @@
     </row>
     <row r="320" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A320" s="2" t="s">
+        <v>896</v>
+      </c>
+      <c r="B320" s="3" t="s">
         <v>897</v>
-      </c>
-      <c r="B320" s="3" t="s">
-        <v>898</v>
       </c>
       <c r="C320" s="3"/>
       <c r="D320" s="3"/>
@@ -15404,10 +15399,10 @@
     </row>
     <row r="321" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A321" s="2" t="s">
+        <v>898</v>
+      </c>
+      <c r="B321" s="3" t="s">
         <v>899</v>
-      </c>
-      <c r="B321" s="3" t="s">
-        <v>900</v>
       </c>
       <c r="C321" s="3"/>
       <c r="D321" s="3"/>
@@ -15436,10 +15431,10 @@
     </row>
     <row r="322" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A322" s="2" t="s">
+        <v>900</v>
+      </c>
+      <c r="B322" s="3" t="s">
         <v>901</v>
-      </c>
-      <c r="B322" s="3" t="s">
-        <v>902</v>
       </c>
       <c r="C322" s="3"/>
       <c r="D322" s="3"/>
@@ -15468,10 +15463,10 @@
     </row>
     <row r="323" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A323" s="2" t="s">
+        <v>902</v>
+      </c>
+      <c r="B323" s="3" t="s">
         <v>903</v>
-      </c>
-      <c r="B323" s="3" t="s">
-        <v>904</v>
       </c>
       <c r="C323" s="3"/>
       <c r="D323" s="3"/>
@@ -15500,10 +15495,10 @@
     </row>
     <row r="324" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A324" s="2" t="s">
+        <v>904</v>
+      </c>
+      <c r="B324" s="3" t="s">
         <v>905</v>
-      </c>
-      <c r="B324" s="3" t="s">
-        <v>906</v>
       </c>
       <c r="C324" s="3"/>
       <c r="D324" s="3"/>
@@ -15532,10 +15527,10 @@
     </row>
     <row r="325" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A325" s="2" t="s">
+        <v>906</v>
+      </c>
+      <c r="B325" s="3" t="s">
         <v>907</v>
-      </c>
-      <c r="B325" s="3" t="s">
-        <v>908</v>
       </c>
       <c r="C325" s="3"/>
       <c r="D325" s="3"/>
@@ -15564,10 +15559,10 @@
     </row>
     <row r="326" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A326" s="2" t="s">
+        <v>908</v>
+      </c>
+      <c r="B326" s="3" t="s">
         <v>909</v>
-      </c>
-      <c r="B326" s="3" t="s">
-        <v>910</v>
       </c>
       <c r="C326" s="3"/>
       <c r="D326" s="3"/>
@@ -15596,10 +15591,10 @@
     </row>
     <row r="327" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A327" s="2" t="s">
+        <v>910</v>
+      </c>
+      <c r="B327" s="3" t="s">
         <v>911</v>
-      </c>
-      <c r="B327" s="3" t="s">
-        <v>912</v>
       </c>
       <c r="C327" s="3"/>
       <c r="D327" s="3"/>
@@ -15628,10 +15623,10 @@
     </row>
     <row r="328" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A328" s="2" t="s">
+        <v>912</v>
+      </c>
+      <c r="B328" s="3" t="s">
         <v>913</v>
-      </c>
-      <c r="B328" s="3" t="s">
-        <v>914</v>
       </c>
       <c r="C328" s="3"/>
       <c r="D328" s="3"/>
@@ -15660,10 +15655,10 @@
     </row>
     <row r="329" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A329" s="2" t="s">
+        <v>914</v>
+      </c>
+      <c r="B329" s="3" t="s">
         <v>915</v>
-      </c>
-      <c r="B329" s="3" t="s">
-        <v>916</v>
       </c>
       <c r="C329" s="3"/>
       <c r="D329" s="3"/>
@@ -15692,10 +15687,10 @@
     </row>
     <row r="330" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A330" s="2" t="s">
+        <v>916</v>
+      </c>
+      <c r="B330" s="3" t="s">
         <v>917</v>
-      </c>
-      <c r="B330" s="3" t="s">
-        <v>918</v>
       </c>
       <c r="C330" s="3"/>
       <c r="D330" s="3"/>
@@ -15724,10 +15719,10 @@
     </row>
     <row r="331" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A331" s="2" t="s">
+        <v>918</v>
+      </c>
+      <c r="B331" s="3" t="s">
         <v>919</v>
-      </c>
-      <c r="B331" s="3" t="s">
-        <v>920</v>
       </c>
       <c r="C331" s="3"/>
       <c r="D331" s="3"/>
@@ -15756,10 +15751,10 @@
     </row>
     <row r="332" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A332" s="2" t="s">
+        <v>920</v>
+      </c>
+      <c r="B332" s="3" t="s">
         <v>921</v>
-      </c>
-      <c r="B332" s="3" t="s">
-        <v>922</v>
       </c>
       <c r="C332" s="3"/>
       <c r="D332" s="3"/>
@@ -15788,10 +15783,10 @@
     </row>
     <row r="333" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A333" s="2" t="s">
+        <v>922</v>
+      </c>
+      <c r="B333" s="3" t="s">
         <v>923</v>
-      </c>
-      <c r="B333" s="3" t="s">
-        <v>924</v>
       </c>
       <c r="C333" s="3"/>
       <c r="D333" s="3"/>
@@ -15820,10 +15815,10 @@
     </row>
     <row r="334" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A334" s="2" t="s">
+        <v>924</v>
+      </c>
+      <c r="B334" s="3" t="s">
         <v>925</v>
-      </c>
-      <c r="B334" s="3" t="s">
-        <v>926</v>
       </c>
       <c r="C334" s="3"/>
       <c r="D334" s="3"/>
@@ -15852,10 +15847,10 @@
     </row>
     <row r="335" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A335" s="2" t="s">
+        <v>926</v>
+      </c>
+      <c r="B335" s="3" t="s">
         <v>927</v>
-      </c>
-      <c r="B335" s="3" t="s">
-        <v>928</v>
       </c>
       <c r="C335" s="3"/>
       <c r="D335" s="3"/>
@@ -15884,10 +15879,10 @@
     </row>
     <row r="336" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A336" s="2" t="s">
+        <v>928</v>
+      </c>
+      <c r="B336" s="3" t="s">
         <v>929</v>
-      </c>
-      <c r="B336" s="3" t="s">
-        <v>930</v>
       </c>
       <c r="C336" s="3"/>
       <c r="D336" s="3"/>
@@ -15916,10 +15911,10 @@
     </row>
     <row r="337" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A337" s="2" t="s">
+        <v>930</v>
+      </c>
+      <c r="B337" s="3" t="s">
         <v>931</v>
-      </c>
-      <c r="B337" s="3" t="s">
-        <v>932</v>
       </c>
       <c r="C337" s="3"/>
       <c r="D337" s="3"/>
@@ -15948,10 +15943,10 @@
     </row>
     <row r="338" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A338" s="2" t="s">
+        <v>932</v>
+      </c>
+      <c r="B338" s="3" t="s">
         <v>933</v>
-      </c>
-      <c r="B338" s="3" t="s">
-        <v>934</v>
       </c>
       <c r="C338" s="3"/>
       <c r="D338" s="3"/>
@@ -15980,10 +15975,10 @@
     </row>
     <row r="339" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A339" s="2" t="s">
+        <v>934</v>
+      </c>
+      <c r="B339" s="3" t="s">
         <v>935</v>
-      </c>
-      <c r="B339" s="3" t="s">
-        <v>936</v>
       </c>
       <c r="C339" s="3"/>
       <c r="D339" s="3"/>
@@ -16012,10 +16007,10 @@
     </row>
     <row r="340" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A340" s="2" t="s">
+        <v>936</v>
+      </c>
+      <c r="B340" s="3" t="s">
         <v>937</v>
-      </c>
-      <c r="B340" s="3" t="s">
-        <v>938</v>
       </c>
       <c r="C340" s="3"/>
       <c r="D340" s="3"/>
@@ -16044,10 +16039,10 @@
     </row>
     <row r="341" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A341" s="2" t="s">
+        <v>938</v>
+      </c>
+      <c r="B341" s="3" t="s">
         <v>939</v>
-      </c>
-      <c r="B341" s="3" t="s">
-        <v>940</v>
       </c>
       <c r="C341" s="3"/>
       <c r="D341" s="3"/>
@@ -16076,10 +16071,10 @@
     </row>
     <row r="342" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A342" s="2" t="s">
+        <v>940</v>
+      </c>
+      <c r="B342" s="3" t="s">
         <v>941</v>
-      </c>
-      <c r="B342" s="3" t="s">
-        <v>942</v>
       </c>
       <c r="C342" s="3"/>
       <c r="D342" s="3"/>
@@ -16108,10 +16103,10 @@
     </row>
     <row r="343" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A343" s="2" t="s">
+        <v>942</v>
+      </c>
+      <c r="B343" s="3" t="s">
         <v>943</v>
-      </c>
-      <c r="B343" s="3" t="s">
-        <v>944</v>
       </c>
       <c r="C343" s="3"/>
       <c r="D343" s="3"/>
@@ -16140,10 +16135,10 @@
     </row>
     <row r="344" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A344" s="2" t="s">
+        <v>944</v>
+      </c>
+      <c r="B344" s="3" t="s">
         <v>945</v>
-      </c>
-      <c r="B344" s="3" t="s">
-        <v>946</v>
       </c>
       <c r="C344" s="3"/>
       <c r="D344" s="3"/>
@@ -16172,10 +16167,10 @@
     </row>
     <row r="345" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A345" s="2" t="s">
+        <v>946</v>
+      </c>
+      <c r="B345" s="3" t="s">
         <v>947</v>
-      </c>
-      <c r="B345" s="3" t="s">
-        <v>948</v>
       </c>
       <c r="C345" s="3"/>
       <c r="D345" s="3"/>
@@ -16204,10 +16199,10 @@
     </row>
     <row r="346" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A346" s="2" t="s">
+        <v>948</v>
+      </c>
+      <c r="B346" s="3" t="s">
         <v>949</v>
-      </c>
-      <c r="B346" s="3" t="s">
-        <v>950</v>
       </c>
       <c r="C346" s="3"/>
       <c r="D346" s="3"/>
@@ -16236,10 +16231,10 @@
     </row>
     <row r="347" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A347" s="2" t="s">
+        <v>950</v>
+      </c>
+      <c r="B347" s="3" t="s">
         <v>951</v>
-      </c>
-      <c r="B347" s="3" t="s">
-        <v>952</v>
       </c>
       <c r="C347" s="3"/>
       <c r="D347" s="3"/>
@@ -16268,10 +16263,10 @@
     </row>
     <row r="348" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A348" s="2" t="s">
+        <v>952</v>
+      </c>
+      <c r="B348" s="3" t="s">
         <v>953</v>
-      </c>
-      <c r="B348" s="3" t="s">
-        <v>954</v>
       </c>
       <c r="C348" s="3"/>
       <c r="D348" s="3"/>
@@ -16300,10 +16295,10 @@
     </row>
     <row r="349" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A349" s="2" t="s">
+        <v>954</v>
+      </c>
+      <c r="B349" s="3" t="s">
         <v>955</v>
-      </c>
-      <c r="B349" s="3" t="s">
-        <v>956</v>
       </c>
       <c r="C349" s="3"/>
       <c r="D349" s="3"/>
@@ -16332,10 +16327,10 @@
     </row>
     <row r="350" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A350" s="2" t="s">
+        <v>956</v>
+      </c>
+      <c r="B350" s="3" t="s">
         <v>957</v>
-      </c>
-      <c r="B350" s="3" t="s">
-        <v>958</v>
       </c>
       <c r="C350" s="3"/>
       <c r="D350" s="3"/>
@@ -16364,10 +16359,10 @@
     </row>
     <row r="351" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A351" s="2" t="s">
+        <v>958</v>
+      </c>
+      <c r="B351" s="3" t="s">
         <v>959</v>
-      </c>
-      <c r="B351" s="3" t="s">
-        <v>960</v>
       </c>
       <c r="C351" s="3"/>
       <c r="D351" s="3"/>
@@ -16396,10 +16391,10 @@
     </row>
     <row r="352" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A352" s="2" t="s">
+        <v>960</v>
+      </c>
+      <c r="B352" s="3" t="s">
         <v>961</v>
-      </c>
-      <c r="B352" s="3" t="s">
-        <v>962</v>
       </c>
       <c r="C352" s="3"/>
       <c r="D352" s="3"/>
@@ -16428,10 +16423,10 @@
     </row>
     <row r="353" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A353" s="2" t="s">
+        <v>962</v>
+      </c>
+      <c r="B353" s="3" t="s">
         <v>963</v>
-      </c>
-      <c r="B353" s="3" t="s">
-        <v>964</v>
       </c>
       <c r="C353" s="3"/>
       <c r="D353" s="3"/>
@@ -16460,10 +16455,10 @@
     </row>
     <row r="354" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A354" s="2" t="s">
+        <v>964</v>
+      </c>
+      <c r="B354" s="3" t="s">
         <v>965</v>
-      </c>
-      <c r="B354" s="3" t="s">
-        <v>966</v>
       </c>
       <c r="C354" s="3"/>
       <c r="D354" s="3"/>
@@ -16492,10 +16487,10 @@
     </row>
     <row r="355" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A355" s="2" t="s">
+        <v>966</v>
+      </c>
+      <c r="B355" s="3" t="s">
         <v>967</v>
-      </c>
-      <c r="B355" s="3" t="s">
-        <v>968</v>
       </c>
       <c r="C355" s="3"/>
       <c r="D355" s="3"/>
@@ -16524,10 +16519,10 @@
     </row>
     <row r="356" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A356" s="2" t="s">
+        <v>968</v>
+      </c>
+      <c r="B356" s="3" t="s">
         <v>969</v>
-      </c>
-      <c r="B356" s="3" t="s">
-        <v>970</v>
       </c>
       <c r="C356" s="3"/>
       <c r="D356" s="3"/>
@@ -16556,10 +16551,10 @@
     </row>
     <row r="357" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A357" s="2" t="s">
+        <v>970</v>
+      </c>
+      <c r="B357" s="3" t="s">
         <v>971</v>
-      </c>
-      <c r="B357" s="3" t="s">
-        <v>972</v>
       </c>
       <c r="C357" s="3"/>
       <c r="D357" s="3"/>
@@ -16588,10 +16583,10 @@
     </row>
     <row r="358" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A358" s="2" t="s">
+        <v>972</v>
+      </c>
+      <c r="B358" s="3" t="s">
         <v>973</v>
-      </c>
-      <c r="B358" s="3" t="s">
-        <v>974</v>
       </c>
       <c r="C358" s="3"/>
       <c r="D358" s="3"/>
@@ -16620,10 +16615,10 @@
     </row>
     <row r="359" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A359" s="2" t="s">
+        <v>974</v>
+      </c>
+      <c r="B359" s="3" t="s">
         <v>975</v>
-      </c>
-      <c r="B359" s="3" t="s">
-        <v>976</v>
       </c>
       <c r="C359" s="3"/>
       <c r="D359" s="3"/>
@@ -16652,10 +16647,10 @@
     </row>
     <row r="360" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A360" s="2" t="s">
+        <v>976</v>
+      </c>
+      <c r="B360" s="3" t="s">
         <v>977</v>
-      </c>
-      <c r="B360" s="3" t="s">
-        <v>978</v>
       </c>
       <c r="C360" s="3"/>
       <c r="D360" s="3"/>
@@ -16684,10 +16679,10 @@
     </row>
     <row r="361" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A361" s="2" t="s">
+        <v>978</v>
+      </c>
+      <c r="B361" s="3" t="s">
         <v>979</v>
-      </c>
-      <c r="B361" s="3" t="s">
-        <v>980</v>
       </c>
       <c r="C361" s="3"/>
       <c r="D361" s="3"/>
@@ -16716,10 +16711,10 @@
     </row>
     <row r="362" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A362" s="2" t="s">
+        <v>980</v>
+      </c>
+      <c r="B362" s="3" t="s">
         <v>981</v>
-      </c>
-      <c r="B362" s="3" t="s">
-        <v>982</v>
       </c>
       <c r="C362" s="3"/>
       <c r="D362" s="3"/>
@@ -16748,10 +16743,10 @@
     </row>
     <row r="363" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A363" s="2" t="s">
+        <v>982</v>
+      </c>
+      <c r="B363" s="3" t="s">
         <v>983</v>
-      </c>
-      <c r="B363" s="3" t="s">
-        <v>984</v>
       </c>
       <c r="C363" s="3"/>
       <c r="D363" s="3"/>
@@ -16780,10 +16775,10 @@
     </row>
     <row r="364" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A364" s="2" t="s">
+        <v>984</v>
+      </c>
+      <c r="B364" s="3" t="s">
         <v>985</v>
-      </c>
-      <c r="B364" s="3" t="s">
-        <v>986</v>
       </c>
       <c r="C364" s="3"/>
       <c r="D364" s="3"/>
@@ -16812,10 +16807,10 @@
     </row>
     <row r="365" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A365" s="2" t="s">
+        <v>986</v>
+      </c>
+      <c r="B365" s="3" t="s">
         <v>987</v>
-      </c>
-      <c r="B365" s="3" t="s">
-        <v>988</v>
       </c>
       <c r="C365" s="3"/>
       <c r="D365" s="3"/>
@@ -16844,10 +16839,10 @@
     </row>
     <row r="366" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A366" s="2" t="s">
+        <v>988</v>
+      </c>
+      <c r="B366" s="3" t="s">
         <v>989</v>
-      </c>
-      <c r="B366" s="3" t="s">
-        <v>990</v>
       </c>
       <c r="C366" s="3"/>
       <c r="D366" s="3"/>
@@ -16876,10 +16871,10 @@
     </row>
     <row r="367" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A367" s="2" t="s">
+        <v>990</v>
+      </c>
+      <c r="B367" s="3" t="s">
         <v>991</v>
-      </c>
-      <c r="B367" s="3" t="s">
-        <v>992</v>
       </c>
       <c r="C367" s="3"/>
       <c r="D367" s="3"/>
@@ -16908,10 +16903,10 @@
     </row>
     <row r="368" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A368" s="2" t="s">
+        <v>992</v>
+      </c>
+      <c r="B368" s="3" t="s">
         <v>993</v>
-      </c>
-      <c r="B368" s="3" t="s">
-        <v>994</v>
       </c>
       <c r="C368" s="3"/>
       <c r="D368" s="3"/>
@@ -16940,10 +16935,10 @@
     </row>
     <row r="369" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A369" s="2" t="s">
+        <v>994</v>
+      </c>
+      <c r="B369" s="3" t="s">
         <v>995</v>
-      </c>
-      <c r="B369" s="3" t="s">
-        <v>996</v>
       </c>
       <c r="C369" s="3"/>
       <c r="D369" s="3"/>
@@ -16972,10 +16967,10 @@
     </row>
     <row r="370" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A370" s="2" t="s">
+        <v>996</v>
+      </c>
+      <c r="B370" s="3" t="s">
         <v>997</v>
-      </c>
-      <c r="B370" s="3" t="s">
-        <v>998</v>
       </c>
       <c r="C370" s="3"/>
       <c r="D370" s="3"/>
@@ -17004,10 +16999,10 @@
     </row>
     <row r="371" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A371" s="2" t="s">
+        <v>998</v>
+      </c>
+      <c r="B371" s="3" t="s">
         <v>999</v>
-      </c>
-      <c r="B371" s="3" t="s">
-        <v>1000</v>
       </c>
       <c r="C371" s="3"/>
       <c r="D371" s="3"/>
@@ -17036,10 +17031,10 @@
     </row>
     <row r="372" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A372" s="2" t="s">
+        <v>1000</v>
+      </c>
+      <c r="B372" s="3" t="s">
         <v>1001</v>
-      </c>
-      <c r="B372" s="3" t="s">
-        <v>1002</v>
       </c>
       <c r="C372" s="3"/>
       <c r="D372" s="3"/>
@@ -17068,10 +17063,10 @@
     </row>
     <row r="373" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A373" s="2" t="s">
+        <v>1002</v>
+      </c>
+      <c r="B373" s="3" t="s">
         <v>1003</v>
-      </c>
-      <c r="B373" s="3" t="s">
-        <v>1004</v>
       </c>
       <c r="C373" s="3"/>
       <c r="D373" s="3"/>
@@ -17100,10 +17095,10 @@
     </row>
     <row r="374" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A374" s="2" t="s">
+        <v>1004</v>
+      </c>
+      <c r="B374" s="3" t="s">
         <v>1005</v>
-      </c>
-      <c r="B374" s="3" t="s">
-        <v>1006</v>
       </c>
       <c r="C374" s="3"/>
       <c r="D374" s="3"/>
@@ -17132,10 +17127,10 @@
     </row>
     <row r="375" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A375" s="2" t="s">
+        <v>1006</v>
+      </c>
+      <c r="B375" s="3" t="s">
         <v>1007</v>
-      </c>
-      <c r="B375" s="3" t="s">
-        <v>1008</v>
       </c>
       <c r="C375" s="3"/>
       <c r="D375" s="3"/>
@@ -17164,10 +17159,10 @@
     </row>
     <row r="376" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A376" s="2" t="s">
+        <v>1008</v>
+      </c>
+      <c r="B376" s="3" t="s">
         <v>1009</v>
-      </c>
-      <c r="B376" s="3" t="s">
-        <v>1010</v>
       </c>
       <c r="C376" s="3"/>
       <c r="D376" s="3"/>
@@ -17196,10 +17191,10 @@
     </row>
     <row r="377" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A377" s="2" t="s">
+        <v>1010</v>
+      </c>
+      <c r="B377" s="3" t="s">
         <v>1011</v>
-      </c>
-      <c r="B377" s="3" t="s">
-        <v>1012</v>
       </c>
       <c r="C377" s="3"/>
       <c r="D377" s="3"/>
@@ -17228,10 +17223,10 @@
     </row>
     <row r="378" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A378" s="2" t="s">
+        <v>1012</v>
+      </c>
+      <c r="B378" s="3" t="s">
         <v>1013</v>
-      </c>
-      <c r="B378" s="3" t="s">
-        <v>1014</v>
       </c>
       <c r="C378" s="3"/>
       <c r="D378" s="3"/>
@@ -17260,10 +17255,10 @@
     </row>
     <row r="379" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A379" s="2" t="s">
+        <v>1014</v>
+      </c>
+      <c r="B379" s="3" t="s">
         <v>1015</v>
-      </c>
-      <c r="B379" s="3" t="s">
-        <v>1016</v>
       </c>
       <c r="C379" s="3"/>
       <c r="D379" s="3"/>
@@ -17292,10 +17287,10 @@
     </row>
     <row r="380" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A380" s="2" t="s">
+        <v>1016</v>
+      </c>
+      <c r="B380" s="3" t="s">
         <v>1017</v>
-      </c>
-      <c r="B380" s="3" t="s">
-        <v>1018</v>
       </c>
       <c r="C380" s="3"/>
       <c r="D380" s="3"/>
@@ -17324,10 +17319,10 @@
     </row>
     <row r="381" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A381" s="2" t="s">
+        <v>1018</v>
+      </c>
+      <c r="B381" s="3" t="s">
         <v>1019</v>
-      </c>
-      <c r="B381" s="3" t="s">
-        <v>1020</v>
       </c>
       <c r="C381" s="3"/>
       <c r="D381" s="3"/>
@@ -17356,10 +17351,10 @@
     </row>
     <row r="382" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A382" s="2" t="s">
+        <v>1020</v>
+      </c>
+      <c r="B382" s="3" t="s">
         <v>1021</v>
-      </c>
-      <c r="B382" s="3" t="s">
-        <v>1022</v>
       </c>
       <c r="C382" s="3"/>
       <c r="D382" s="3"/>
@@ -17388,10 +17383,10 @@
     </row>
     <row r="383" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A383" s="2" t="s">
+        <v>1022</v>
+      </c>
+      <c r="B383" s="3" t="s">
         <v>1023</v>
-      </c>
-      <c r="B383" s="3" t="s">
-        <v>1024</v>
       </c>
       <c r="C383" s="3"/>
       <c r="D383" s="3"/>
@@ -17420,10 +17415,10 @@
     </row>
     <row r="384" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A384" s="2" t="s">
+        <v>1024</v>
+      </c>
+      <c r="B384" s="3" t="s">
         <v>1025</v>
-      </c>
-      <c r="B384" s="3" t="s">
-        <v>1026</v>
       </c>
       <c r="C384" s="3"/>
       <c r="D384" s="3"/>
@@ -17452,10 +17447,10 @@
     </row>
     <row r="385" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A385" s="2" t="s">
+        <v>1026</v>
+      </c>
+      <c r="B385" s="3" t="s">
         <v>1027</v>
-      </c>
-      <c r="B385" s="3" t="s">
-        <v>1028</v>
       </c>
       <c r="C385" s="3"/>
       <c r="D385" s="3"/>
@@ -17484,10 +17479,10 @@
     </row>
     <row r="386" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A386" s="2" t="s">
+        <v>1028</v>
+      </c>
+      <c r="B386" s="3" t="s">
         <v>1029</v>
-      </c>
-      <c r="B386" s="3" t="s">
-        <v>1030</v>
       </c>
       <c r="C386" s="3"/>
       <c r="D386" s="3"/>
@@ -17516,10 +17511,10 @@
     </row>
     <row r="387" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A387" s="2" t="s">
+        <v>1030</v>
+      </c>
+      <c r="B387" s="3" t="s">
         <v>1031</v>
-      </c>
-      <c r="B387" s="3" t="s">
-        <v>1032</v>
       </c>
       <c r="C387" s="3"/>
       <c r="D387" s="3"/>
@@ -17548,10 +17543,10 @@
     </row>
     <row r="388" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A388" s="2" t="s">
+        <v>1032</v>
+      </c>
+      <c r="B388" s="3" t="s">
         <v>1033</v>
-      </c>
-      <c r="B388" s="3" t="s">
-        <v>1034</v>
       </c>
       <c r="C388" s="3"/>
       <c r="D388" s="3"/>
@@ -17580,10 +17575,10 @@
     </row>
     <row r="389" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A389" s="2" t="s">
+        <v>1034</v>
+      </c>
+      <c r="B389" s="3" t="s">
         <v>1035</v>
-      </c>
-      <c r="B389" s="3" t="s">
-        <v>1036</v>
       </c>
       <c r="C389" s="3"/>
       <c r="D389" s="3"/>
@@ -17612,10 +17607,10 @@
     </row>
     <row r="390" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A390" s="2" t="s">
+        <v>1036</v>
+      </c>
+      <c r="B390" s="3" t="s">
         <v>1037</v>
-      </c>
-      <c r="B390" s="3" t="s">
-        <v>1038</v>
       </c>
       <c r="C390" s="3"/>
       <c r="D390" s="3"/>
@@ -17644,10 +17639,10 @@
     </row>
     <row r="391" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A391" s="2" t="s">
+        <v>1038</v>
+      </c>
+      <c r="B391" s="3" t="s">
         <v>1039</v>
-      </c>
-      <c r="B391" s="3" t="s">
-        <v>1040</v>
       </c>
       <c r="C391" s="3"/>
       <c r="D391" s="3"/>
@@ -17676,10 +17671,10 @@
     </row>
     <row r="392" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A392" s="2" t="s">
+        <v>1040</v>
+      </c>
+      <c r="B392" s="3" t="s">
         <v>1041</v>
-      </c>
-      <c r="B392" s="3" t="s">
-        <v>1042</v>
       </c>
       <c r="C392" s="3"/>
       <c r="D392" s="3"/>
@@ -17708,10 +17703,10 @@
     </row>
     <row r="393" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A393" s="2" t="s">
+        <v>1042</v>
+      </c>
+      <c r="B393" s="3" t="s">
         <v>1043</v>
-      </c>
-      <c r="B393" s="3" t="s">
-        <v>1044</v>
       </c>
       <c r="C393" s="3"/>
       <c r="D393" s="3"/>
@@ -17740,10 +17735,10 @@
     </row>
     <row r="394" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A394" s="2" t="s">
+        <v>1044</v>
+      </c>
+      <c r="B394" s="3" t="s">
         <v>1045</v>
-      </c>
-      <c r="B394" s="3" t="s">
-        <v>1046</v>
       </c>
       <c r="C394" s="3"/>
       <c r="D394" s="3"/>
@@ -17772,10 +17767,10 @@
     </row>
     <row r="395" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A395" s="2" t="s">
+        <v>1046</v>
+      </c>
+      <c r="B395" s="3" t="s">
         <v>1047</v>
-      </c>
-      <c r="B395" s="3" t="s">
-        <v>1048</v>
       </c>
       <c r="C395" s="3"/>
       <c r="D395" s="3"/>
@@ -17804,10 +17799,10 @@
     </row>
     <row r="396" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A396" s="2" t="s">
+        <v>1048</v>
+      </c>
+      <c r="B396" s="3" t="s">
         <v>1049</v>
-      </c>
-      <c r="B396" s="3" t="s">
-        <v>1050</v>
       </c>
       <c r="C396" s="3"/>
       <c r="D396" s="3"/>
@@ -17836,10 +17831,10 @@
     </row>
     <row r="397" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A397" s="2" t="s">
+        <v>1050</v>
+      </c>
+      <c r="B397" s="3" t="s">
         <v>1051</v>
-      </c>
-      <c r="B397" s="3" t="s">
-        <v>1052</v>
       </c>
       <c r="C397" s="3"/>
       <c r="D397" s="3"/>
@@ -17868,10 +17863,10 @@
     </row>
     <row r="398" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A398" s="2" t="s">
+        <v>1052</v>
+      </c>
+      <c r="B398" s="3" t="s">
         <v>1053</v>
-      </c>
-      <c r="B398" s="3" t="s">
-        <v>1054</v>
       </c>
       <c r="C398" s="3"/>
       <c r="D398" s="3"/>
@@ -17900,10 +17895,10 @@
     </row>
     <row r="399" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A399" s="2" t="s">
+        <v>1054</v>
+      </c>
+      <c r="B399" s="3" t="s">
         <v>1055</v>
-      </c>
-      <c r="B399" s="3" t="s">
-        <v>1056</v>
       </c>
       <c r="C399" s="3"/>
       <c r="D399" s="3"/>
@@ -17932,10 +17927,10 @@
     </row>
     <row r="400" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A400" s="2" t="s">
+        <v>1056</v>
+      </c>
+      <c r="B400" s="3" t="s">
         <v>1057</v>
-      </c>
-      <c r="B400" s="3" t="s">
-        <v>1058</v>
       </c>
       <c r="C400" s="3"/>
       <c r="D400" s="3"/>
@@ -17964,10 +17959,10 @@
     </row>
     <row r="401" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A401" s="2" t="s">
+        <v>1058</v>
+      </c>
+      <c r="B401" s="3" t="s">
         <v>1059</v>
-      </c>
-      <c r="B401" s="3" t="s">
-        <v>1060</v>
       </c>
       <c r="C401" s="3"/>
       <c r="D401" s="3"/>
@@ -17996,10 +17991,10 @@
     </row>
     <row r="402" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A402" s="2" t="s">
+        <v>1060</v>
+      </c>
+      <c r="B402" s="3" t="s">
         <v>1061</v>
-      </c>
-      <c r="B402" s="3" t="s">
-        <v>1062</v>
       </c>
       <c r="C402" s="3"/>
       <c r="D402" s="3"/>
@@ -18028,10 +18023,10 @@
     </row>
     <row r="403" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A403" s="2" t="s">
+        <v>1062</v>
+      </c>
+      <c r="B403" s="3" t="s">
         <v>1063</v>
-      </c>
-      <c r="B403" s="3" t="s">
-        <v>1064</v>
       </c>
       <c r="C403" s="3"/>
       <c r="D403" s="3"/>
@@ -18060,10 +18055,10 @@
     </row>
     <row r="404" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A404" s="2" t="s">
+        <v>1064</v>
+      </c>
+      <c r="B404" s="3" t="s">
         <v>1065</v>
-      </c>
-      <c r="B404" s="3" t="s">
-        <v>1066</v>
       </c>
       <c r="C404" s="3"/>
       <c r="D404" s="3"/>
@@ -18092,10 +18087,10 @@
     </row>
     <row r="405" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A405" s="2" t="s">
+        <v>1066</v>
+      </c>
+      <c r="B405" s="3" t="s">
         <v>1067</v>
-      </c>
-      <c r="B405" s="3" t="s">
-        <v>1068</v>
       </c>
       <c r="C405" s="3"/>
       <c r="D405" s="3"/>
@@ -18124,10 +18119,10 @@
     </row>
     <row r="406" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A406" s="2" t="s">
+        <v>1068</v>
+      </c>
+      <c r="B406" s="3" t="s">
         <v>1069</v>
-      </c>
-      <c r="B406" s="3" t="s">
-        <v>1070</v>
       </c>
       <c r="C406" s="3"/>
       <c r="D406" s="3"/>
@@ -18156,10 +18151,10 @@
     </row>
     <row r="407" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A407" s="2" t="s">
+        <v>1070</v>
+      </c>
+      <c r="B407" s="3" t="s">
         <v>1071</v>
-      </c>
-      <c r="B407" s="3" t="s">
-        <v>1072</v>
       </c>
       <c r="C407" s="3"/>
       <c r="D407" s="3"/>
@@ -18188,10 +18183,10 @@
     </row>
     <row r="408" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A408" s="2" t="s">
+        <v>1072</v>
+      </c>
+      <c r="B408" s="3" t="s">
         <v>1073</v>
-      </c>
-      <c r="B408" s="3" t="s">
-        <v>1074</v>
       </c>
       <c r="C408" s="3"/>
       <c r="D408" s="3"/>
@@ -18220,10 +18215,10 @@
     </row>
     <row r="409" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A409" s="2" t="s">
+        <v>1074</v>
+      </c>
+      <c r="B409" s="3" t="s">
         <v>1075</v>
-      </c>
-      <c r="B409" s="3" t="s">
-        <v>1076</v>
       </c>
       <c r="C409" s="3"/>
       <c r="D409" s="3"/>
@@ -18252,10 +18247,10 @@
     </row>
     <row r="410" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A410" s="2" t="s">
+        <v>1076</v>
+      </c>
+      <c r="B410" s="3" t="s">
         <v>1077</v>
-      </c>
-      <c r="B410" s="3" t="s">
-        <v>1078</v>
       </c>
       <c r="C410" s="3"/>
       <c r="D410" s="3"/>
@@ -18284,10 +18279,10 @@
     </row>
     <row r="411" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A411" s="2" t="s">
+        <v>1078</v>
+      </c>
+      <c r="B411" s="3" t="s">
         <v>1079</v>
-      </c>
-      <c r="B411" s="3" t="s">
-        <v>1080</v>
       </c>
       <c r="C411" s="3"/>
       <c r="D411" s="3"/>
@@ -18316,10 +18311,10 @@
     </row>
     <row r="412" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A412" s="2" t="s">
+        <v>1080</v>
+      </c>
+      <c r="B412" s="3" t="s">
         <v>1081</v>
-      </c>
-      <c r="B412" s="3" t="s">
-        <v>1082</v>
       </c>
       <c r="C412" s="3"/>
       <c r="D412" s="3"/>
@@ -18348,10 +18343,10 @@
     </row>
     <row r="413" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A413" s="2" t="s">
+        <v>1082</v>
+      </c>
+      <c r="B413" s="3" t="s">
         <v>1083</v>
-      </c>
-      <c r="B413" s="3" t="s">
-        <v>1084</v>
       </c>
       <c r="C413" s="3"/>
       <c r="D413" s="3"/>
@@ -18380,10 +18375,10 @@
     </row>
     <row r="414" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A414" s="2" t="s">
+        <v>1084</v>
+      </c>
+      <c r="B414" s="3" t="s">
         <v>1085</v>
-      </c>
-      <c r="B414" s="3" t="s">
-        <v>1086</v>
       </c>
       <c r="C414" s="3"/>
       <c r="D414" s="3"/>
@@ -18412,10 +18407,10 @@
     </row>
     <row r="415" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A415" s="2" t="s">
+        <v>1086</v>
+      </c>
+      <c r="B415" s="3" t="s">
         <v>1087</v>
-      </c>
-      <c r="B415" s="3" t="s">
-        <v>1088</v>
       </c>
       <c r="C415" s="3"/>
       <c r="D415" s="3"/>
@@ -18444,10 +18439,10 @@
     </row>
     <row r="416" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A416" s="2" t="s">
+        <v>1088</v>
+      </c>
+      <c r="B416" s="3" t="s">
         <v>1089</v>
-      </c>
-      <c r="B416" s="3" t="s">
-        <v>1090</v>
       </c>
       <c r="C416" s="3"/>
       <c r="D416" s="3"/>
@@ -18476,10 +18471,10 @@
     </row>
     <row r="417" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A417" s="2" t="s">
+        <v>1090</v>
+      </c>
+      <c r="B417" s="3" t="s">
         <v>1091</v>
-      </c>
-      <c r="B417" s="3" t="s">
-        <v>1092</v>
       </c>
       <c r="C417" s="3"/>
       <c r="D417" s="3"/>
@@ -18508,10 +18503,10 @@
     </row>
     <row r="418" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A418" s="2" t="s">
+        <v>1092</v>
+      </c>
+      <c r="B418" s="3" t="s">
         <v>1093</v>
-      </c>
-      <c r="B418" s="3" t="s">
-        <v>1094</v>
       </c>
       <c r="C418" s="3"/>
       <c r="D418" s="3"/>
@@ -18540,10 +18535,10 @@
     </row>
     <row r="419" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A419" s="2" t="s">
+        <v>1094</v>
+      </c>
+      <c r="B419" s="3" t="s">
         <v>1095</v>
-      </c>
-      <c r="B419" s="3" t="s">
-        <v>1096</v>
       </c>
       <c r="C419" s="3"/>
       <c r="D419" s="3"/>
@@ -18572,10 +18567,10 @@
     </row>
     <row r="420" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A420" s="2" t="s">
+        <v>1096</v>
+      </c>
+      <c r="B420" s="3" t="s">
         <v>1097</v>
-      </c>
-      <c r="B420" s="3" t="s">
-        <v>1098</v>
       </c>
       <c r="C420" s="3"/>
       <c r="D420" s="3"/>
@@ -18604,10 +18599,10 @@
     </row>
     <row r="421" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A421" s="2" t="s">
+        <v>1098</v>
+      </c>
+      <c r="B421" s="3" t="s">
         <v>1099</v>
-      </c>
-      <c r="B421" s="3" t="s">
-        <v>1100</v>
       </c>
       <c r="C421" s="3"/>
       <c r="D421" s="3"/>
@@ -18636,10 +18631,10 @@
     </row>
     <row r="422" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A422" s="2" t="s">
+        <v>1100</v>
+      </c>
+      <c r="B422" s="3" t="s">
         <v>1101</v>
-      </c>
-      <c r="B422" s="3" t="s">
-        <v>1102</v>
       </c>
       <c r="C422" s="3"/>
       <c r="D422" s="3"/>
@@ -18668,10 +18663,10 @@
     </row>
     <row r="423" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A423" s="2" t="s">
+        <v>1102</v>
+      </c>
+      <c r="B423" s="3" t="s">
         <v>1103</v>
-      </c>
-      <c r="B423" s="3" t="s">
-        <v>1104</v>
       </c>
       <c r="C423" s="3"/>
       <c r="D423" s="3"/>
@@ -18700,10 +18695,10 @@
     </row>
     <row r="424" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A424" s="2" t="s">
+        <v>1104</v>
+      </c>
+      <c r="B424" s="3" t="s">
         <v>1105</v>
-      </c>
-      <c r="B424" s="3" t="s">
-        <v>1106</v>
       </c>
       <c r="C424" s="3"/>
       <c r="D424" s="3"/>
@@ -18732,10 +18727,10 @@
     </row>
     <row r="425" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A425" s="2" t="s">
+        <v>1106</v>
+      </c>
+      <c r="B425" s="3" t="s">
         <v>1107</v>
-      </c>
-      <c r="B425" s="3" t="s">
-        <v>1108</v>
       </c>
       <c r="C425" s="3"/>
       <c r="D425" s="3"/>
@@ -18764,10 +18759,10 @@
     </row>
     <row r="426" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A426" s="2" t="s">
+        <v>1108</v>
+      </c>
+      <c r="B426" s="3" t="s">
         <v>1109</v>
-      </c>
-      <c r="B426" s="3" t="s">
-        <v>1110</v>
       </c>
       <c r="C426" s="3"/>
       <c r="D426" s="3"/>
@@ -18796,10 +18791,10 @@
     </row>
     <row r="427" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A427" s="2" t="s">
+        <v>1110</v>
+      </c>
+      <c r="B427" s="3" t="s">
         <v>1111</v>
-      </c>
-      <c r="B427" s="3" t="s">
-        <v>1112</v>
       </c>
       <c r="C427" s="3"/>
       <c r="D427" s="3"/>
@@ -18828,10 +18823,10 @@
     </row>
     <row r="428" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A428" s="2" t="s">
+        <v>1112</v>
+      </c>
+      <c r="B428" s="3" t="s">
         <v>1113</v>
-      </c>
-      <c r="B428" s="3" t="s">
-        <v>1114</v>
       </c>
       <c r="C428" s="3"/>
       <c r="D428" s="3"/>
@@ -18860,10 +18855,10 @@
     </row>
     <row r="429" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A429" s="2" t="s">
+        <v>1114</v>
+      </c>
+      <c r="B429" s="3" t="s">
         <v>1115</v>
-      </c>
-      <c r="B429" s="3" t="s">
-        <v>1116</v>
       </c>
       <c r="C429" s="3"/>
       <c r="D429" s="3"/>
@@ -18892,10 +18887,10 @@
     </row>
     <row r="430" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A430" s="2" t="s">
+        <v>1116</v>
+      </c>
+      <c r="B430" s="3" t="s">
         <v>1117</v>
-      </c>
-      <c r="B430" s="3" t="s">
-        <v>1118</v>
       </c>
       <c r="C430" s="3"/>
       <c r="D430" s="3"/>
@@ -18924,10 +18919,10 @@
     </row>
     <row r="431" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A431" s="2" t="s">
+        <v>1118</v>
+      </c>
+      <c r="B431" s="3" t="s">
         <v>1119</v>
-      </c>
-      <c r="B431" s="3" t="s">
-        <v>1120</v>
       </c>
       <c r="C431" s="3"/>
       <c r="D431" s="3"/>
@@ -18956,10 +18951,10 @@
     </row>
     <row r="432" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A432" s="2" t="s">
+        <v>1120</v>
+      </c>
+      <c r="B432" s="3" t="s">
         <v>1121</v>
-      </c>
-      <c r="B432" s="3" t="s">
-        <v>1122</v>
       </c>
       <c r="C432" s="3"/>
       <c r="D432" s="3"/>
@@ -18988,10 +18983,10 @@
     </row>
     <row r="433" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A433" s="2" t="s">
+        <v>1122</v>
+      </c>
+      <c r="B433" s="3" t="s">
         <v>1123</v>
-      </c>
-      <c r="B433" s="3" t="s">
-        <v>1124</v>
       </c>
       <c r="C433" s="3"/>
       <c r="D433" s="3"/>
@@ -19020,10 +19015,10 @@
     </row>
     <row r="434" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A434" s="2" t="s">
+        <v>1124</v>
+      </c>
+      <c r="B434" s="3" t="s">
         <v>1125</v>
-      </c>
-      <c r="B434" s="3" t="s">
-        <v>1126</v>
       </c>
       <c r="C434" s="3"/>
       <c r="D434" s="3"/>
@@ -19052,10 +19047,10 @@
     </row>
     <row r="435" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A435" s="2" t="s">
+        <v>1126</v>
+      </c>
+      <c r="B435" s="3" t="s">
         <v>1127</v>
-      </c>
-      <c r="B435" s="3" t="s">
-        <v>1128</v>
       </c>
       <c r="C435" s="3"/>
       <c r="D435" s="3"/>
@@ -19084,10 +19079,10 @@
     </row>
     <row r="436" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A436" s="2" t="s">
+        <v>1128</v>
+      </c>
+      <c r="B436" s="3" t="s">
         <v>1129</v>
-      </c>
-      <c r="B436" s="3" t="s">
-        <v>1130</v>
       </c>
       <c r="C436" s="3"/>
       <c r="D436" s="3"/>
@@ -19116,10 +19111,10 @@
     </row>
     <row r="437" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A437" s="2" t="s">
+        <v>1130</v>
+      </c>
+      <c r="B437" s="3" t="s">
         <v>1131</v>
-      </c>
-      <c r="B437" s="3" t="s">
-        <v>1132</v>
       </c>
       <c r="C437" s="3"/>
       <c r="D437" s="3"/>
@@ -19148,10 +19143,10 @@
     </row>
     <row r="438" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A438" s="2" t="s">
+        <v>1132</v>
+      </c>
+      <c r="B438" s="3" t="s">
         <v>1133</v>
-      </c>
-      <c r="B438" s="3" t="s">
-        <v>1134</v>
       </c>
       <c r="C438" s="3"/>
       <c r="D438" s="3"/>
@@ -19180,10 +19175,10 @@
     </row>
     <row r="439" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A439" s="2" t="s">
+        <v>1134</v>
+      </c>
+      <c r="B439" s="3" t="s">
         <v>1135</v>
-      </c>
-      <c r="B439" s="3" t="s">
-        <v>1136</v>
       </c>
       <c r="C439" s="3"/>
       <c r="D439" s="3"/>
@@ -19212,10 +19207,10 @@
     </row>
     <row r="440" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A440" s="2" t="s">
+        <v>1136</v>
+      </c>
+      <c r="B440" s="3" t="s">
         <v>1137</v>
-      </c>
-      <c r="B440" s="3" t="s">
-        <v>1138</v>
       </c>
       <c r="C440" s="3"/>
       <c r="D440" s="3"/>
@@ -19244,10 +19239,10 @@
     </row>
     <row r="441" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A441" s="2" t="s">
+        <v>1138</v>
+      </c>
+      <c r="B441" s="3" t="s">
         <v>1139</v>
-      </c>
-      <c r="B441" s="3" t="s">
-        <v>1140</v>
       </c>
       <c r="C441" s="3"/>
       <c r="D441" s="3"/>
@@ -19276,10 +19271,10 @@
     </row>
     <row r="442" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A442" s="2" t="s">
+        <v>1140</v>
+      </c>
+      <c r="B442" s="3" t="s">
         <v>1141</v>
-      </c>
-      <c r="B442" s="3" t="s">
-        <v>1142</v>
       </c>
       <c r="C442" s="3"/>
       <c r="D442" s="3"/>
@@ -19308,10 +19303,10 @@
     </row>
     <row r="443" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A443" s="2" t="s">
+        <v>1142</v>
+      </c>
+      <c r="B443" s="3" t="s">
         <v>1143</v>
-      </c>
-      <c r="B443" s="3" t="s">
-        <v>1144</v>
       </c>
       <c r="C443" s="3"/>
       <c r="D443" s="3"/>
@@ -19340,10 +19335,10 @@
     </row>
     <row r="444" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A444" s="2" t="s">
+        <v>1144</v>
+      </c>
+      <c r="B444" s="3" t="s">
         <v>1145</v>
-      </c>
-      <c r="B444" s="3" t="s">
-        <v>1146</v>
       </c>
       <c r="C444" s="3"/>
       <c r="D444" s="3"/>
@@ -19372,10 +19367,10 @@
     </row>
     <row r="445" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A445" s="2" t="s">
+        <v>1146</v>
+      </c>
+      <c r="B445" s="3" t="s">
         <v>1147</v>
-      </c>
-      <c r="B445" s="3" t="s">
-        <v>1148</v>
       </c>
       <c r="C445" s="3"/>
       <c r="D445" s="3"/>
@@ -19404,10 +19399,10 @@
     </row>
     <row r="446" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A446" s="2" t="s">
+        <v>1148</v>
+      </c>
+      <c r="B446" s="3" t="s">
         <v>1149</v>
-      </c>
-      <c r="B446" s="3" t="s">
-        <v>1150</v>
       </c>
       <c r="C446" s="3"/>
       <c r="D446" s="3"/>
@@ -19436,7 +19431,7 @@
     </row>
     <row r="447" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A447" s="2" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="B447" s="5"/>
       <c r="C447" s="5"/>
@@ -19466,7 +19461,7 @@
     </row>
     <row r="448" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A448" s="2" t="s">
-        <v>1152</v>
+        <v>1151</v>
       </c>
       <c r="B448" s="5"/>
       <c r="C448" s="5"/>
@@ -19496,7 +19491,7 @@
     </row>
     <row r="449" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A449" s="2" t="s">
-        <v>1153</v>
+        <v>1152</v>
       </c>
       <c r="B449" s="5"/>
       <c r="C449" s="5"/>
@@ -19526,10 +19521,10 @@
     </row>
     <row r="450" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A450" s="2" t="s">
+        <v>1153</v>
+      </c>
+      <c r="B450" s="3" t="s">
         <v>1154</v>
-      </c>
-      <c r="B450" s="3" t="s">
-        <v>1155</v>
       </c>
       <c r="C450" s="3"/>
       <c r="D450" s="3"/>
@@ -19558,10 +19553,10 @@
     </row>
     <row r="451" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A451" s="2" t="s">
+        <v>1155</v>
+      </c>
+      <c r="B451" s="3" t="s">
         <v>1156</v>
-      </c>
-      <c r="B451" s="3" t="s">
-        <v>1157</v>
       </c>
       <c r="C451" s="3"/>
       <c r="D451" s="3"/>
@@ -19590,10 +19585,10 @@
     </row>
     <row r="452" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A452" s="2" t="s">
+        <v>1157</v>
+      </c>
+      <c r="B452" s="3" t="s">
         <v>1158</v>
-      </c>
-      <c r="B452" s="3" t="s">
-        <v>1159</v>
       </c>
       <c r="C452" s="3"/>
       <c r="D452" s="3"/>
@@ -19622,10 +19617,10 @@
     </row>
     <row r="453" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A453" s="2" t="s">
+        <v>1159</v>
+      </c>
+      <c r="B453" s="3" t="s">
         <v>1160</v>
-      </c>
-      <c r="B453" s="3" t="s">
-        <v>1161</v>
       </c>
       <c r="C453" s="3"/>
       <c r="D453" s="3"/>
@@ -19654,10 +19649,10 @@
     </row>
     <row r="454" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A454" s="2" t="s">
+        <v>1161</v>
+      </c>
+      <c r="B454" s="3" t="s">
         <v>1162</v>
-      </c>
-      <c r="B454" s="3" t="s">
-        <v>1163</v>
       </c>
       <c r="C454" s="3"/>
       <c r="D454" s="3"/>
@@ -19686,10 +19681,10 @@
     </row>
     <row r="455" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A455" s="2" t="s">
+        <v>1163</v>
+      </c>
+      <c r="B455" s="3" t="s">
         <v>1164</v>
-      </c>
-      <c r="B455" s="3" t="s">
-        <v>1165</v>
       </c>
       <c r="C455" s="3"/>
       <c r="D455" s="3"/>
@@ -19718,10 +19713,10 @@
     </row>
     <row r="456" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A456" s="2" t="s">
+        <v>1165</v>
+      </c>
+      <c r="B456" s="3" t="s">
         <v>1166</v>
-      </c>
-      <c r="B456" s="3" t="s">
-        <v>1167</v>
       </c>
       <c r="C456" s="3"/>
       <c r="D456" s="3"/>
@@ -19750,10 +19745,10 @@
     </row>
     <row r="457" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A457" s="2" t="s">
+        <v>1167</v>
+      </c>
+      <c r="B457" s="3" t="s">
         <v>1168</v>
-      </c>
-      <c r="B457" s="3" t="s">
-        <v>1169</v>
       </c>
       <c r="C457" s="3"/>
       <c r="D457" s="3"/>
@@ -19782,10 +19777,10 @@
     </row>
     <row r="458" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A458" s="2" t="s">
+        <v>1169</v>
+      </c>
+      <c r="B458" s="3" t="s">
         <v>1170</v>
-      </c>
-      <c r="B458" s="3" t="s">
-        <v>1171</v>
       </c>
       <c r="C458" s="3"/>
       <c r="D458" s="3"/>
@@ -19814,10 +19809,10 @@
     </row>
     <row r="459" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A459" s="2" t="s">
+        <v>1171</v>
+      </c>
+      <c r="B459" s="3" t="s">
         <v>1172</v>
-      </c>
-      <c r="B459" s="3" t="s">
-        <v>1173</v>
       </c>
       <c r="C459" s="3"/>
       <c r="D459" s="3"/>
@@ -19846,10 +19841,10 @@
     </row>
     <row r="460" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A460" s="2" t="s">
+        <v>1173</v>
+      </c>
+      <c r="B460" s="3" t="s">
         <v>1174</v>
-      </c>
-      <c r="B460" s="3" t="s">
-        <v>1175</v>
       </c>
       <c r="C460" s="3"/>
       <c r="D460" s="3"/>
@@ -19878,10 +19873,10 @@
     </row>
     <row r="461" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A461" s="2" t="s">
+        <v>1175</v>
+      </c>
+      <c r="B461" s="3" t="s">
         <v>1176</v>
-      </c>
-      <c r="B461" s="3" t="s">
-        <v>1177</v>
       </c>
       <c r="C461" s="3"/>
       <c r="D461" s="3"/>
@@ -19910,10 +19905,10 @@
     </row>
     <row r="462" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A462" s="2" t="s">
+        <v>1177</v>
+      </c>
+      <c r="B462" s="3" t="s">
         <v>1178</v>
-      </c>
-      <c r="B462" s="3" t="s">
-        <v>1179</v>
       </c>
       <c r="C462" s="3"/>
       <c r="D462" s="3"/>
@@ -19942,10 +19937,10 @@
     </row>
     <row r="463" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A463" s="2" t="s">
+        <v>1179</v>
+      </c>
+      <c r="B463" s="3" t="s">
         <v>1180</v>
-      </c>
-      <c r="B463" s="3" t="s">
-        <v>1181</v>
       </c>
       <c r="C463" s="3"/>
       <c r="D463" s="3"/>
@@ -19974,10 +19969,10 @@
     </row>
     <row r="464" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A464" s="2" t="s">
+        <v>1181</v>
+      </c>
+      <c r="B464" s="3" t="s">
         <v>1182</v>
-      </c>
-      <c r="B464" s="3" t="s">
-        <v>1183</v>
       </c>
       <c r="C464" s="3"/>
       <c r="D464" s="3"/>
@@ -20006,10 +20001,10 @@
     </row>
     <row r="465" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A465" s="2" t="s">
+        <v>1183</v>
+      </c>
+      <c r="B465" s="3" t="s">
         <v>1184</v>
-      </c>
-      <c r="B465" s="3" t="s">
-        <v>1185</v>
       </c>
       <c r="C465" s="3"/>
       <c r="D465" s="3"/>
@@ -20038,7 +20033,7 @@
     </row>
     <row r="466" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A466" s="2" t="s">
-        <v>1186</v>
+        <v>1185</v>
       </c>
       <c r="B466" s="5"/>
       <c r="C466" s="5"/>
@@ -20068,7 +20063,7 @@
     </row>
     <row r="467" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A467" s="2" t="s">
-        <v>1187</v>
+        <v>1186</v>
       </c>
       <c r="B467" s="5"/>
       <c r="C467" s="5"/>
@@ -20098,7 +20093,7 @@
     </row>
     <row r="468" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A468" s="2" t="s">
-        <v>1188</v>
+        <v>1187</v>
       </c>
       <c r="B468" s="5"/>
       <c r="C468" s="5"/>
@@ -20128,7 +20123,7 @@
     </row>
     <row r="469" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A469" s="2" t="s">
-        <v>1189</v>
+        <v>1188</v>
       </c>
       <c r="B469" s="5"/>
       <c r="C469" s="5"/>
@@ -20158,7 +20153,7 @@
     </row>
     <row r="470" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A470" s="2" t="s">
-        <v>1190</v>
+        <v>1189</v>
       </c>
       <c r="B470" s="5"/>
       <c r="C470" s="5"/>
@@ -20188,7 +20183,7 @@
     </row>
     <row r="471" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A471" s="2" t="s">
-        <v>1191</v>
+        <v>1190</v>
       </c>
       <c r="B471" s="5"/>
       <c r="C471" s="5"/>
@@ -20218,7 +20213,7 @@
     </row>
     <row r="472" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A472" s="2" t="s">
-        <v>1192</v>
+        <v>1191</v>
       </c>
       <c r="B472" s="5"/>
       <c r="C472" s="5"/>
@@ -20248,7 +20243,7 @@
     </row>
     <row r="473" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A473" s="2" t="s">
-        <v>1193</v>
+        <v>1192</v>
       </c>
       <c r="B473" s="5"/>
       <c r="C473" s="5"/>
@@ -20278,7 +20273,7 @@
     </row>
     <row r="474" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A474" s="2" t="s">
-        <v>1194</v>
+        <v>1193</v>
       </c>
       <c r="B474" s="5"/>
       <c r="C474" s="5"/>
@@ -20308,7 +20303,7 @@
     </row>
     <row r="475" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A475" s="2" t="s">
-        <v>1195</v>
+        <v>1194</v>
       </c>
       <c r="B475" s="5"/>
       <c r="C475" s="5"/>
@@ -20338,7 +20333,7 @@
     </row>
     <row r="476" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A476" s="2" t="s">
-        <v>1196</v>
+        <v>1195</v>
       </c>
       <c r="B476" s="5"/>
       <c r="C476" s="5"/>
@@ -20368,7 +20363,7 @@
     </row>
     <row r="477" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A477" s="2" t="s">
-        <v>1197</v>
+        <v>1196</v>
       </c>
       <c r="B477" s="5"/>
       <c r="C477" s="5"/>
@@ -20398,7 +20393,7 @@
     </row>
     <row r="478" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A478" s="2" t="s">
-        <v>1198</v>
+        <v>1197</v>
       </c>
       <c r="B478" s="5"/>
       <c r="C478" s="5"/>
@@ -20428,7 +20423,7 @@
     </row>
     <row r="479" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A479" s="2" t="s">
-        <v>1199</v>
+        <v>1198</v>
       </c>
       <c r="B479" s="5"/>
       <c r="C479" s="5"/>
@@ -20458,7 +20453,7 @@
     </row>
     <row r="480" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A480" s="2" t="s">
-        <v>1200</v>
+        <v>1199</v>
       </c>
       <c r="B480" s="5"/>
       <c r="C480" s="5"/>
@@ -20488,7 +20483,7 @@
     </row>
     <row r="481" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A481" s="2" t="s">
-        <v>1201</v>
+        <v>1200</v>
       </c>
       <c r="B481" s="5"/>
       <c r="C481" s="5"/>
@@ -20526,7 +20521,7 @@
       <c r="G482" s="12"/>
       <c r="H482" s="12"/>
       <c r="I482" s="3" t="s">
-        <v>1202</v>
+        <v>1201</v>
       </c>
       <c r="J482" s="3"/>
       <c r="K482" s="12"/>
@@ -20548,37 +20543,37 @@
     </row>
     <row r="483" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A483" s="2" t="s">
+        <v>1202</v>
+      </c>
+      <c r="B483" s="4" t="s">
         <v>1203</v>
       </c>
-      <c r="B483" s="4" t="s">
+      <c r="C483" s="4" t="s">
         <v>1204</v>
       </c>
-      <c r="C483" s="4" t="s">
+      <c r="D483" s="4" t="s">
         <v>1205</v>
       </c>
-      <c r="D483" s="4" t="s">
+      <c r="E483" s="4" t="s">
         <v>1206</v>
       </c>
-      <c r="E483" s="4" t="s">
+      <c r="F483" s="4" t="s">
         <v>1207</v>
       </c>
-      <c r="F483" s="4" t="s">
+      <c r="G483" s="4" t="s">
         <v>1208</v>
       </c>
-      <c r="G483" s="4" t="s">
+      <c r="H483" s="4" t="s">
         <v>1209</v>
       </c>
-      <c r="H483" s="4" t="s">
+      <c r="I483" s="4" t="s">
         <v>1210</v>
       </c>
-      <c r="I483" s="4" t="s">
+      <c r="J483" s="4" t="s">
         <v>1211</v>
       </c>
-      <c r="J483" s="4" t="s">
+      <c r="K483" s="4" t="s">
         <v>1212</v>
-      </c>
-      <c r="K483" s="4" t="s">
-        <v>1213</v>
       </c>
       <c r="L483" s="5"/>
       <c r="M483" s="5"/>
@@ -20598,37 +20593,37 @@
     </row>
     <row r="484" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A484" s="2" t="s">
+        <v>1213</v>
+      </c>
+      <c r="B484" s="4" t="s">
         <v>1214</v>
       </c>
-      <c r="B484" s="4" t="s">
+      <c r="C484" s="4" t="s">
         <v>1215</v>
       </c>
-      <c r="C484" s="4" t="s">
+      <c r="D484" s="4" t="s">
         <v>1216</v>
       </c>
-      <c r="D484" s="4" t="s">
+      <c r="E484" s="4" t="s">
         <v>1217</v>
       </c>
-      <c r="E484" s="4" t="s">
+      <c r="F484" s="4" t="s">
         <v>1218</v>
       </c>
-      <c r="F484" s="4" t="s">
+      <c r="G484" s="4" t="s">
         <v>1219</v>
       </c>
-      <c r="G484" s="4" t="s">
+      <c r="H484" s="4" t="s">
         <v>1220</v>
       </c>
-      <c r="H484" s="4" t="s">
+      <c r="I484" s="4" t="s">
         <v>1221</v>
       </c>
-      <c r="I484" s="4" t="s">
+      <c r="J484" s="4" t="s">
         <v>1222</v>
       </c>
-      <c r="J484" s="4" t="s">
+      <c r="K484" s="4" t="s">
         <v>1223</v>
-      </c>
-      <c r="K484" s="4" t="s">
-        <v>1224</v>
       </c>
       <c r="L484" s="5"/>
       <c r="M484" s="5"/>
@@ -20648,37 +20643,37 @@
     </row>
     <row r="485" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A485" s="2" t="s">
+        <v>1224</v>
+      </c>
+      <c r="B485" s="4" t="s">
         <v>1225</v>
       </c>
-      <c r="B485" s="4" t="s">
+      <c r="C485" s="4" t="s">
         <v>1226</v>
       </c>
-      <c r="C485" s="4" t="s">
+      <c r="D485" s="4" t="s">
         <v>1227</v>
       </c>
-      <c r="D485" s="4" t="s">
+      <c r="E485" s="4" t="s">
         <v>1228</v>
       </c>
-      <c r="E485" s="4" t="s">
+      <c r="F485" s="4" t="s">
         <v>1229</v>
       </c>
-      <c r="F485" s="4" t="s">
+      <c r="G485" s="4" t="s">
         <v>1230</v>
       </c>
-      <c r="G485" s="4" t="s">
+      <c r="H485" s="4" t="s">
         <v>1231</v>
       </c>
-      <c r="H485" s="4" t="s">
+      <c r="I485" s="4" t="s">
         <v>1232</v>
       </c>
-      <c r="I485" s="4" t="s">
+      <c r="J485" s="4" t="s">
         <v>1233</v>
       </c>
-      <c r="J485" s="4" t="s">
+      <c r="K485" s="4" t="s">
         <v>1234</v>
-      </c>
-      <c r="K485" s="4" t="s">
-        <v>1235</v>
       </c>
       <c r="L485" s="5"/>
       <c r="M485" s="5"/>
@@ -20698,37 +20693,37 @@
     </row>
     <row r="486" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A486" s="2" t="s">
+        <v>1235</v>
+      </c>
+      <c r="B486" s="4" t="s">
         <v>1236</v>
       </c>
-      <c r="B486" s="4" t="s">
+      <c r="C486" s="4" t="s">
         <v>1237</v>
       </c>
-      <c r="C486" s="4" t="s">
+      <c r="D486" s="4" t="s">
         <v>1238</v>
       </c>
-      <c r="D486" s="4" t="s">
+      <c r="E486" s="4" t="s">
         <v>1239</v>
       </c>
-      <c r="E486" s="4" t="s">
+      <c r="F486" s="4" t="s">
         <v>1240</v>
       </c>
-      <c r="F486" s="4" t="s">
+      <c r="G486" s="4" t="s">
         <v>1241</v>
       </c>
-      <c r="G486" s="4" t="s">
+      <c r="H486" s="4" t="s">
         <v>1242</v>
       </c>
-      <c r="H486" s="4" t="s">
+      <c r="I486" s="4" t="s">
         <v>1243</v>
       </c>
-      <c r="I486" s="4" t="s">
+      <c r="J486" s="4" t="s">
         <v>1244</v>
       </c>
-      <c r="J486" s="4" t="s">
+      <c r="K486" s="4" t="s">
         <v>1245</v>
-      </c>
-      <c r="K486" s="4" t="s">
-        <v>1246</v>
       </c>
       <c r="L486" s="5"/>
       <c r="M486" s="5"/>
@@ -20748,37 +20743,37 @@
     </row>
     <row r="487" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A487" s="2" t="s">
+        <v>1246</v>
+      </c>
+      <c r="B487" s="4" t="s">
         <v>1247</v>
       </c>
-      <c r="B487" s="4" t="s">
+      <c r="C487" s="4" t="s">
         <v>1248</v>
       </c>
-      <c r="C487" s="4" t="s">
+      <c r="D487" s="4" t="s">
         <v>1249</v>
       </c>
-      <c r="D487" s="4" t="s">
+      <c r="E487" s="4" t="s">
         <v>1250</v>
       </c>
-      <c r="E487" s="4" t="s">
+      <c r="F487" s="4" t="s">
         <v>1251</v>
       </c>
-      <c r="F487" s="4" t="s">
+      <c r="G487" s="4" t="s">
         <v>1252</v>
       </c>
-      <c r="G487" s="4" t="s">
+      <c r="H487" s="4" t="s">
         <v>1253</v>
       </c>
-      <c r="H487" s="4" t="s">
+      <c r="I487" s="4" t="s">
         <v>1254</v>
       </c>
-      <c r="I487" s="4" t="s">
+      <c r="J487" s="4" t="s">
         <v>1255</v>
       </c>
-      <c r="J487" s="4" t="s">
+      <c r="K487" s="4" t="s">
         <v>1256</v>
-      </c>
-      <c r="K487" s="4" t="s">
-        <v>1257</v>
       </c>
       <c r="L487" s="5"/>
       <c r="M487" s="5"/>
@@ -20798,37 +20793,37 @@
     </row>
     <row r="488" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A488" s="2" t="s">
+        <v>1257</v>
+      </c>
+      <c r="B488" s="4" t="s">
         <v>1258</v>
       </c>
-      <c r="B488" s="4" t="s">
+      <c r="C488" s="4" t="s">
         <v>1259</v>
       </c>
-      <c r="C488" s="4" t="s">
+      <c r="D488" s="4" t="s">
         <v>1260</v>
       </c>
-      <c r="D488" s="4" t="s">
+      <c r="E488" s="4" t="s">
         <v>1261</v>
       </c>
-      <c r="E488" s="4" t="s">
+      <c r="F488" s="4" t="s">
         <v>1262</v>
       </c>
-      <c r="F488" s="4" t="s">
+      <c r="G488" s="4" t="s">
         <v>1263</v>
       </c>
-      <c r="G488" s="4" t="s">
+      <c r="H488" s="4" t="s">
         <v>1264</v>
       </c>
-      <c r="H488" s="4" t="s">
+      <c r="I488" s="4" t="s">
         <v>1265</v>
       </c>
-      <c r="I488" s="4" t="s">
+      <c r="J488" s="4" t="s">
         <v>1266</v>
       </c>
-      <c r="J488" s="4" t="s">
+      <c r="K488" s="4" t="s">
         <v>1267</v>
-      </c>
-      <c r="K488" s="4" t="s">
-        <v>1268</v>
       </c>
       <c r="L488" s="5"/>
       <c r="M488" s="5"/>
@@ -20848,37 +20843,37 @@
     </row>
     <row r="489" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A489" s="2" t="s">
+        <v>1268</v>
+      </c>
+      <c r="B489" s="4" t="s">
         <v>1269</v>
       </c>
-      <c r="B489" s="4" t="s">
+      <c r="C489" s="4" t="s">
         <v>1270</v>
       </c>
-      <c r="C489" s="4" t="s">
+      <c r="D489" s="4" t="s">
         <v>1271</v>
       </c>
-      <c r="D489" s="4" t="s">
+      <c r="E489" s="4" t="s">
         <v>1272</v>
       </c>
-      <c r="E489" s="4" t="s">
+      <c r="F489" s="4" t="s">
         <v>1273</v>
       </c>
-      <c r="F489" s="4" t="s">
+      <c r="G489" s="4" t="s">
         <v>1274</v>
       </c>
-      <c r="G489" s="4" t="s">
+      <c r="H489" s="4" t="s">
         <v>1275</v>
       </c>
-      <c r="H489" s="4" t="s">
+      <c r="I489" s="4" t="s">
         <v>1276</v>
       </c>
-      <c r="I489" s="4" t="s">
+      <c r="J489" s="4" t="s">
         <v>1277</v>
       </c>
-      <c r="J489" s="4" t="s">
+      <c r="K489" s="4" t="s">
         <v>1278</v>
-      </c>
-      <c r="K489" s="4" t="s">
-        <v>1279</v>
       </c>
       <c r="L489" s="5"/>
       <c r="M489" s="5"/>
@@ -20898,37 +20893,37 @@
     </row>
     <row r="490" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A490" s="2" t="s">
+        <v>1279</v>
+      </c>
+      <c r="B490" s="4" t="s">
         <v>1280</v>
       </c>
-      <c r="B490" s="4" t="s">
+      <c r="C490" s="4" t="s">
         <v>1281</v>
       </c>
-      <c r="C490" s="4" t="s">
+      <c r="D490" s="4" t="s">
         <v>1282</v>
       </c>
-      <c r="D490" s="4" t="s">
+      <c r="E490" s="4" t="s">
         <v>1283</v>
       </c>
-      <c r="E490" s="4" t="s">
+      <c r="F490" s="4" t="s">
         <v>1284</v>
       </c>
-      <c r="F490" s="4" t="s">
+      <c r="G490" s="4" t="s">
         <v>1285</v>
       </c>
-      <c r="G490" s="4" t="s">
+      <c r="H490" s="4" t="s">
         <v>1286</v>
       </c>
-      <c r="H490" s="4" t="s">
+      <c r="I490" s="4" t="s">
         <v>1287</v>
       </c>
-      <c r="I490" s="4" t="s">
+      <c r="J490" s="4" t="s">
         <v>1288</v>
       </c>
-      <c r="J490" s="4" t="s">
+      <c r="K490" s="4" t="s">
         <v>1289</v>
-      </c>
-      <c r="K490" s="4" t="s">
-        <v>1290</v>
       </c>
       <c r="L490" s="5"/>
       <c r="M490" s="5"/>
@@ -20948,37 +20943,37 @@
     </row>
     <row r="491" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A491" s="2" t="s">
+        <v>1290</v>
+      </c>
+      <c r="B491" s="4" t="s">
         <v>1291</v>
       </c>
-      <c r="B491" s="4" t="s">
+      <c r="C491" s="4" t="s">
         <v>1292</v>
       </c>
-      <c r="C491" s="4" t="s">
+      <c r="D491" s="4" t="s">
         <v>1293</v>
       </c>
-      <c r="D491" s="4" t="s">
+      <c r="E491" s="4" t="s">
         <v>1294</v>
       </c>
-      <c r="E491" s="4" t="s">
+      <c r="F491" s="4" t="s">
         <v>1295</v>
       </c>
-      <c r="F491" s="4" t="s">
+      <c r="G491" s="4" t="s">
         <v>1296</v>
       </c>
-      <c r="G491" s="4" t="s">
+      <c r="H491" s="4" t="s">
         <v>1297</v>
       </c>
-      <c r="H491" s="4" t="s">
+      <c r="I491" s="4" t="s">
         <v>1298</v>
       </c>
-      <c r="I491" s="4" t="s">
+      <c r="J491" s="4" t="s">
         <v>1299</v>
       </c>
-      <c r="J491" s="4" t="s">
+      <c r="K491" s="4" t="s">
         <v>1300</v>
-      </c>
-      <c r="K491" s="4" t="s">
-        <v>1301</v>
       </c>
       <c r="L491" s="5"/>
       <c r="M491" s="5"/>
@@ -20998,37 +20993,37 @@
     </row>
     <row r="492" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A492" s="2" t="s">
+        <v>1301</v>
+      </c>
+      <c r="B492" s="4" t="s">
         <v>1302</v>
       </c>
-      <c r="B492" s="4" t="s">
+      <c r="C492" s="4" t="s">
         <v>1303</v>
       </c>
-      <c r="C492" s="4" t="s">
+      <c r="D492" s="4" t="s">
         <v>1304</v>
       </c>
-      <c r="D492" s="4" t="s">
+      <c r="E492" s="4" t="s">
         <v>1305</v>
       </c>
-      <c r="E492" s="4" t="s">
+      <c r="F492" s="4" t="s">
         <v>1306</v>
       </c>
-      <c r="F492" s="4" t="s">
+      <c r="G492" s="4" t="s">
         <v>1307</v>
       </c>
-      <c r="G492" s="4" t="s">
+      <c r="H492" s="4" t="s">
         <v>1308</v>
       </c>
-      <c r="H492" s="4" t="s">
+      <c r="I492" s="4" t="s">
         <v>1309</v>
       </c>
-      <c r="I492" s="4" t="s">
+      <c r="J492" s="4" t="s">
         <v>1310</v>
       </c>
-      <c r="J492" s="4" t="s">
+      <c r="K492" s="4" t="s">
         <v>1311</v>
-      </c>
-      <c r="K492" s="4" t="s">
-        <v>1312</v>
       </c>
       <c r="L492" s="5"/>
       <c r="M492" s="5"/>
@@ -21048,37 +21043,37 @@
     </row>
     <row r="493" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A493" s="2" t="s">
+        <v>1312</v>
+      </c>
+      <c r="B493" s="4" t="s">
         <v>1313</v>
       </c>
-      <c r="B493" s="4" t="s">
+      <c r="C493" s="4" t="s">
         <v>1314</v>
       </c>
-      <c r="C493" s="4" t="s">
+      <c r="D493" s="4" t="s">
         <v>1315</v>
       </c>
-      <c r="D493" s="4" t="s">
+      <c r="E493" s="4" t="s">
         <v>1316</v>
       </c>
-      <c r="E493" s="4" t="s">
+      <c r="F493" s="4" t="s">
         <v>1317</v>
       </c>
-      <c r="F493" s="4" t="s">
+      <c r="G493" s="4" t="s">
         <v>1318</v>
       </c>
-      <c r="G493" s="4" t="s">
+      <c r="H493" s="4" t="s">
         <v>1319</v>
       </c>
-      <c r="H493" s="4" t="s">
+      <c r="I493" s="4" t="s">
         <v>1320</v>
       </c>
-      <c r="I493" s="4" t="s">
+      <c r="J493" s="4" t="s">
         <v>1321</v>
       </c>
-      <c r="J493" s="4" t="s">
+      <c r="K493" s="4" t="s">
         <v>1322</v>
-      </c>
-      <c r="K493" s="4" t="s">
-        <v>1323</v>
       </c>
       <c r="L493" s="5"/>
       <c r="M493" s="5"/>
@@ -21098,37 +21093,37 @@
     </row>
     <row r="494" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A494" s="2" t="s">
+        <v>1323</v>
+      </c>
+      <c r="B494" s="4" t="s">
         <v>1324</v>
       </c>
-      <c r="B494" s="4" t="s">
+      <c r="C494" s="4" t="s">
         <v>1325</v>
       </c>
-      <c r="C494" s="4" t="s">
+      <c r="D494" s="4" t="s">
         <v>1326</v>
       </c>
-      <c r="D494" s="4" t="s">
+      <c r="E494" s="4" t="s">
         <v>1327</v>
       </c>
-      <c r="E494" s="4" t="s">
+      <c r="F494" s="4" t="s">
         <v>1328</v>
       </c>
-      <c r="F494" s="4" t="s">
+      <c r="G494" s="4" t="s">
         <v>1329</v>
       </c>
-      <c r="G494" s="4" t="s">
+      <c r="H494" s="4" t="s">
         <v>1330</v>
       </c>
-      <c r="H494" s="4" t="s">
+      <c r="I494" s="4" t="s">
         <v>1331</v>
       </c>
-      <c r="I494" s="4" t="s">
+      <c r="J494" s="4" t="s">
         <v>1332</v>
       </c>
-      <c r="J494" s="4" t="s">
+      <c r="K494" s="4" t="s">
         <v>1333</v>
-      </c>
-      <c r="K494" s="4" t="s">
-        <v>1334</v>
       </c>
       <c r="L494" s="5"/>
       <c r="M494" s="5"/>
@@ -21148,38 +21143,38 @@
     </row>
     <row r="495" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A495" s="2" t="s">
+        <v>1334</v>
+      </c>
+      <c r="B495" s="3" t="s">
         <v>1335</v>
-      </c>
-      <c r="B495" s="3" t="s">
-        <v>1336</v>
       </c>
       <c r="C495" s="3"/>
       <c r="D495" s="3" t="s">
-        <v>1337</v>
+        <v>1336</v>
       </c>
       <c r="E495" s="3"/>
       <c r="F495" s="3" t="s">
-        <v>1338</v>
+        <v>1337</v>
       </c>
       <c r="G495" s="3"/>
       <c r="H495" s="3" t="s">
-        <v>1339</v>
+        <v>1338</v>
       </c>
       <c r="I495" s="3"/>
       <c r="J495" s="3" t="s">
-        <v>1340</v>
+        <v>1339</v>
       </c>
       <c r="K495" s="3"/>
       <c r="L495" s="3" t="s">
-        <v>1341</v>
+        <v>1340</v>
       </c>
       <c r="M495" s="3"/>
       <c r="N495" s="3" t="s">
-        <v>1342</v>
+        <v>1341</v>
       </c>
       <c r="O495" s="3"/>
       <c r="P495" s="3" t="s">
-        <v>1343</v>
+        <v>1342</v>
       </c>
       <c r="Q495" s="3"/>
       <c r="R495" s="1"/>
@@ -21194,34 +21189,34 @@
     </row>
     <row r="496" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A496" s="2" t="s">
+        <v>1343</v>
+      </c>
+      <c r="B496" s="4" t="s">
         <v>1344</v>
       </c>
-      <c r="B496" s="4" t="s">
+      <c r="C496" s="4" t="s">
         <v>1345</v>
       </c>
-      <c r="C496" s="4" t="s">
+      <c r="D496" s="4" t="s">
         <v>1346</v>
       </c>
-      <c r="D496" s="4" t="s">
+      <c r="E496" s="4" t="s">
         <v>1347</v>
       </c>
-      <c r="E496" s="4" t="s">
+      <c r="F496" s="4" t="s">
         <v>1348</v>
       </c>
-      <c r="F496" s="4" t="s">
+      <c r="G496" s="4" t="s">
         <v>1349</v>
       </c>
-      <c r="G496" s="4" t="s">
+      <c r="H496" s="4" t="s">
         <v>1350</v>
       </c>
-      <c r="H496" s="4" t="s">
+      <c r="I496" s="4" t="s">
         <v>1351</v>
       </c>
-      <c r="I496" s="4" t="s">
+      <c r="J496" s="4" t="s">
         <v>1352</v>
-      </c>
-      <c r="J496" s="4" t="s">
-        <v>1353</v>
       </c>
       <c r="K496" s="5"/>
       <c r="L496" s="5"/>
@@ -21242,34 +21237,34 @@
     </row>
     <row r="497" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A497" s="2" t="s">
+        <v>1353</v>
+      </c>
+      <c r="B497" s="4" t="s">
         <v>1354</v>
       </c>
-      <c r="B497" s="4" t="s">
+      <c r="C497" s="4" t="s">
         <v>1355</v>
       </c>
-      <c r="C497" s="4" t="s">
+      <c r="D497" s="4" t="s">
         <v>1356</v>
       </c>
-      <c r="D497" s="4" t="s">
+      <c r="E497" s="4" t="s">
         <v>1357</v>
       </c>
-      <c r="E497" s="4" t="s">
+      <c r="F497" s="4" t="s">
         <v>1358</v>
       </c>
-      <c r="F497" s="4" t="s">
+      <c r="G497" s="4" t="s">
         <v>1359</v>
       </c>
-      <c r="G497" s="4" t="s">
+      <c r="H497" s="4" t="s">
         <v>1360</v>
       </c>
-      <c r="H497" s="4" t="s">
+      <c r="I497" s="4" t="s">
         <v>1361</v>
       </c>
-      <c r="I497" s="4" t="s">
+      <c r="J497" s="4" t="s">
         <v>1362</v>
-      </c>
-      <c r="J497" s="4" t="s">
-        <v>1363</v>
       </c>
       <c r="K497" s="5"/>
       <c r="L497" s="5"/>
@@ -21290,34 +21285,34 @@
     </row>
     <row r="498" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A498" s="2" t="s">
+        <v>1363</v>
+      </c>
+      <c r="B498" s="4" t="s">
         <v>1364</v>
       </c>
-      <c r="B498" s="4" t="s">
+      <c r="C498" s="4" t="s">
         <v>1365</v>
       </c>
-      <c r="C498" s="4" t="s">
+      <c r="D498" s="4" t="s">
         <v>1366</v>
       </c>
-      <c r="D498" s="4" t="s">
+      <c r="E498" s="4" t="s">
         <v>1367</v>
       </c>
-      <c r="E498" s="4" t="s">
+      <c r="F498" s="4" t="s">
         <v>1368</v>
       </c>
-      <c r="F498" s="4" t="s">
+      <c r="G498" s="4" t="s">
         <v>1369</v>
       </c>
-      <c r="G498" s="4" t="s">
+      <c r="H498" s="4" t="s">
         <v>1370</v>
       </c>
-      <c r="H498" s="4" t="s">
+      <c r="I498" s="4" t="s">
         <v>1371</v>
       </c>
-      <c r="I498" s="4" t="s">
+      <c r="J498" s="4" t="s">
         <v>1372</v>
-      </c>
-      <c r="J498" s="4" t="s">
-        <v>1373</v>
       </c>
       <c r="K498" s="5"/>
       <c r="L498" s="5"/>
@@ -21338,34 +21333,34 @@
     </row>
     <row r="499" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A499" s="2" t="s">
+        <v>1373</v>
+      </c>
+      <c r="B499" s="4" t="s">
         <v>1374</v>
       </c>
-      <c r="B499" s="4" t="s">
+      <c r="C499" s="4" t="s">
         <v>1375</v>
       </c>
-      <c r="C499" s="4" t="s">
+      <c r="D499" s="4" t="s">
         <v>1376</v>
       </c>
-      <c r="D499" s="4" t="s">
+      <c r="E499" s="4" t="s">
         <v>1377</v>
       </c>
-      <c r="E499" s="4" t="s">
+      <c r="F499" s="4" t="s">
         <v>1378</v>
       </c>
-      <c r="F499" s="4" t="s">
+      <c r="G499" s="4" t="s">
         <v>1379</v>
       </c>
-      <c r="G499" s="4" t="s">
+      <c r="H499" s="4" t="s">
         <v>1380</v>
       </c>
-      <c r="H499" s="4" t="s">
+      <c r="I499" s="4" t="s">
         <v>1381</v>
       </c>
-      <c r="I499" s="4" t="s">
+      <c r="J499" s="4" t="s">
         <v>1382</v>
-      </c>
-      <c r="J499" s="4" t="s">
-        <v>1383</v>
       </c>
       <c r="K499" s="5"/>
       <c r="L499" s="5"/>
@@ -21386,34 +21381,34 @@
     </row>
     <row r="500" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A500" s="2" t="s">
+        <v>1383</v>
+      </c>
+      <c r="B500" s="4" t="s">
         <v>1384</v>
       </c>
-      <c r="B500" s="4" t="s">
+      <c r="C500" s="4" t="s">
         <v>1385</v>
       </c>
-      <c r="C500" s="4" t="s">
+      <c r="D500" s="4" t="s">
         <v>1386</v>
       </c>
-      <c r="D500" s="4" t="s">
+      <c r="E500" s="4" t="s">
         <v>1387</v>
       </c>
-      <c r="E500" s="4" t="s">
+      <c r="F500" s="4" t="s">
         <v>1388</v>
       </c>
-      <c r="F500" s="4" t="s">
+      <c r="G500" s="4" t="s">
         <v>1389</v>
       </c>
-      <c r="G500" s="4" t="s">
+      <c r="H500" s="4" t="s">
         <v>1390</v>
       </c>
-      <c r="H500" s="4" t="s">
+      <c r="I500" s="4" t="s">
         <v>1391</v>
       </c>
-      <c r="I500" s="4" t="s">
+      <c r="J500" s="4" t="s">
         <v>1392</v>
-      </c>
-      <c r="J500" s="4" t="s">
-        <v>1393</v>
       </c>
       <c r="K500" s="5"/>
       <c r="L500" s="5"/>
@@ -21434,34 +21429,34 @@
     </row>
     <row r="501" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A501" s="2" t="s">
+        <v>1393</v>
+      </c>
+      <c r="B501" s="4" t="s">
         <v>1394</v>
       </c>
-      <c r="B501" s="4" t="s">
+      <c r="C501" s="4" t="s">
         <v>1395</v>
       </c>
-      <c r="C501" s="4" t="s">
+      <c r="D501" s="4" t="s">
         <v>1396</v>
       </c>
-      <c r="D501" s="4" t="s">
+      <c r="E501" s="4" t="s">
         <v>1397</v>
       </c>
-      <c r="E501" s="4" t="s">
+      <c r="F501" s="4" t="s">
         <v>1398</v>
       </c>
-      <c r="F501" s="4" t="s">
+      <c r="G501" s="4" t="s">
         <v>1399</v>
       </c>
-      <c r="G501" s="4" t="s">
+      <c r="H501" s="4" t="s">
         <v>1400</v>
       </c>
-      <c r="H501" s="4" t="s">
+      <c r="I501" s="4" t="s">
         <v>1401</v>
       </c>
-      <c r="I501" s="4" t="s">
+      <c r="J501" s="4" t="s">
         <v>1402</v>
-      </c>
-      <c r="J501" s="4" t="s">
-        <v>1403</v>
       </c>
       <c r="K501" s="5"/>
       <c r="L501" s="5"/>
@@ -21482,34 +21477,34 @@
     </row>
     <row r="502" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A502" s="2" t="s">
+        <v>1403</v>
+      </c>
+      <c r="B502" s="4" t="s">
         <v>1404</v>
       </c>
-      <c r="B502" s="4" t="s">
+      <c r="C502" s="4" t="s">
         <v>1405</v>
       </c>
-      <c r="C502" s="4" t="s">
+      <c r="D502" s="4" t="s">
         <v>1406</v>
       </c>
-      <c r="D502" s="4" t="s">
+      <c r="E502" s="4" t="s">
         <v>1407</v>
       </c>
-      <c r="E502" s="4" t="s">
+      <c r="F502" s="4" t="s">
         <v>1408</v>
       </c>
-      <c r="F502" s="4" t="s">
+      <c r="G502" s="4" t="s">
         <v>1409</v>
       </c>
-      <c r="G502" s="4" t="s">
+      <c r="H502" s="4" t="s">
         <v>1410</v>
       </c>
-      <c r="H502" s="4" t="s">
+      <c r="I502" s="4" t="s">
         <v>1411</v>
       </c>
-      <c r="I502" s="4" t="s">
+      <c r="J502" s="4" t="s">
         <v>1412</v>
-      </c>
-      <c r="J502" s="4" t="s">
-        <v>1413</v>
       </c>
       <c r="K502" s="5"/>
       <c r="L502" s="5"/>
@@ -21530,30 +21525,30 @@
     </row>
     <row r="503" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A503" s="2" t="s">
+        <v>1413</v>
+      </c>
+      <c r="B503" s="3" t="s">
         <v>1414</v>
-      </c>
-      <c r="B503" s="3" t="s">
-        <v>1415</v>
       </c>
       <c r="C503" s="3"/>
       <c r="D503" s="3" t="s">
-        <v>1416</v>
+        <v>1415</v>
       </c>
       <c r="E503" s="3"/>
       <c r="F503" s="3" t="s">
-        <v>1417</v>
+        <v>1416</v>
       </c>
       <c r="G503" s="3"/>
       <c r="H503" s="3" t="s">
-        <v>1418</v>
+        <v>1417</v>
       </c>
       <c r="I503" s="3"/>
       <c r="J503" s="3" t="s">
-        <v>1419</v>
+        <v>1418</v>
       </c>
       <c r="K503" s="3"/>
       <c r="L503" s="3" t="s">
-        <v>1420</v>
+        <v>1419</v>
       </c>
       <c r="M503" s="3"/>
       <c r="N503" s="5"/>
@@ -21572,38 +21567,38 @@
     </row>
     <row r="504" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A504" s="2" t="s">
+        <v>1420</v>
+      </c>
+      <c r="B504" s="3" t="s">
         <v>1421</v>
-      </c>
-      <c r="B504" s="3" t="s">
-        <v>1422</v>
       </c>
       <c r="C504" s="3"/>
       <c r="D504" s="3" t="s">
-        <v>1423</v>
+        <v>1422</v>
       </c>
       <c r="E504" s="3"/>
       <c r="F504" s="3" t="s">
-        <v>1424</v>
+        <v>1423</v>
       </c>
       <c r="G504" s="3"/>
       <c r="H504" s="3" t="s">
-        <v>1425</v>
+        <v>1424</v>
       </c>
       <c r="I504" s="3"/>
       <c r="J504" s="3" t="s">
-        <v>1426</v>
+        <v>1425</v>
       </c>
       <c r="K504" s="3"/>
       <c r="L504" s="3" t="s">
-        <v>1427</v>
+        <v>1426</v>
       </c>
       <c r="M504" s="3"/>
       <c r="N504" s="3" t="s">
-        <v>1428</v>
+        <v>1427</v>
       </c>
       <c r="O504" s="3"/>
       <c r="P504" s="3" t="s">
-        <v>1429</v>
+        <v>1428</v>
       </c>
       <c r="Q504" s="3"/>
       <c r="R504" s="1"/>
@@ -21618,14 +21613,14 @@
     </row>
     <row r="505" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A505" s="2" t="s">
+        <v>1429</v>
+      </c>
+      <c r="B505" s="3" t="s">
         <v>1430</v>
-      </c>
-      <c r="B505" s="3" t="s">
-        <v>1431</v>
       </c>
       <c r="C505" s="3"/>
       <c r="D505" s="3" t="s">
-        <v>1432</v>
+        <v>1431</v>
       </c>
       <c r="E505" s="3"/>
       <c r="F505" s="5"/>
@@ -21633,19 +21628,19 @@
       <c r="H505" s="5"/>
       <c r="I505" s="5"/>
       <c r="J505" s="3" t="s">
-        <v>1433</v>
+        <v>1432</v>
       </c>
       <c r="K505" s="3"/>
       <c r="L505" s="3" t="s">
-        <v>1434</v>
+        <v>1433</v>
       </c>
       <c r="M505" s="3"/>
       <c r="N505" s="3" t="s">
-        <v>1435</v>
+        <v>1434</v>
       </c>
       <c r="O505" s="3"/>
       <c r="P505" s="3" t="s">
-        <v>1436</v>
+        <v>1435</v>
       </c>
       <c r="Q505" s="3"/>
       <c r="R505" s="1"/>
@@ -21660,30 +21655,30 @@
     </row>
     <row r="506" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A506" s="2" t="s">
+        <v>1436</v>
+      </c>
+      <c r="B506" s="3" t="s">
         <v>1437</v>
-      </c>
-      <c r="B506" s="3" t="s">
-        <v>1438</v>
       </c>
       <c r="C506" s="3"/>
       <c r="D506" s="3" t="s">
-        <v>1439</v>
+        <v>1438</v>
       </c>
       <c r="E506" s="3"/>
       <c r="F506" s="3" t="s">
-        <v>1440</v>
+        <v>1439</v>
       </c>
       <c r="G506" s="3"/>
       <c r="H506" s="3" t="s">
-        <v>1441</v>
+        <v>1440</v>
       </c>
       <c r="I506" s="3"/>
       <c r="J506" s="3" t="s">
-        <v>1442</v>
+        <v>1441</v>
       </c>
       <c r="K506" s="3"/>
       <c r="L506" s="3" t="s">
-        <v>1443</v>
+        <v>1442</v>
       </c>
       <c r="M506" s="3"/>
       <c r="N506" s="5"/>
@@ -21702,28 +21697,28 @@
     </row>
     <row r="507" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A507" s="2" t="s">
+        <v>1443</v>
+      </c>
+      <c r="B507" s="4" t="s">
         <v>1444</v>
       </c>
-      <c r="B507" s="4" t="s">
+      <c r="C507" s="4" t="s">
         <v>1445</v>
       </c>
-      <c r="C507" s="4" t="s">
+      <c r="D507" s="4" t="s">
         <v>1446</v>
       </c>
-      <c r="D507" s="4" t="s">
+      <c r="E507" s="4" t="s">
         <v>1447</v>
       </c>
-      <c r="E507" s="4" t="s">
+      <c r="F507" s="4" t="s">
         <v>1448</v>
-      </c>
-      <c r="F507" s="4" t="s">
-        <v>1449</v>
       </c>
       <c r="G507" s="5"/>
       <c r="H507" s="5"/>
       <c r="I507" s="5"/>
       <c r="J507" s="3" t="s">
-        <v>1450</v>
+        <v>1449</v>
       </c>
       <c r="K507" s="3"/>
       <c r="L507" s="5"/>
@@ -21731,10 +21726,10 @@
       <c r="N507" s="5"/>
       <c r="O507" s="5"/>
       <c r="P507" s="4" t="s">
+        <v>1450</v>
+      </c>
+      <c r="Q507" s="4" t="s">
         <v>1451</v>
-      </c>
-      <c r="Q507" s="4" t="s">
-        <v>1452</v>
       </c>
       <c r="R507" s="1"/>
       <c r="S507" s="1"/>
@@ -21748,7 +21743,7 @@
     </row>
     <row r="508" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A508" s="2" t="s">
-        <v>1453</v>
+        <v>1452</v>
       </c>
       <c r="B508" s="5"/>
       <c r="C508" s="5"/>
@@ -21778,7 +21773,7 @@
     </row>
     <row r="509" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A509" s="2" t="s">
-        <v>1454</v>
+        <v>1453</v>
       </c>
       <c r="B509" s="5"/>
       <c r="C509" s="5"/>
@@ -21808,7 +21803,7 @@
     </row>
     <row r="510" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A510" s="2" t="s">
-        <v>1455</v>
+        <v>1454</v>
       </c>
       <c r="B510" s="5"/>
       <c r="C510" s="5"/>
@@ -21838,7 +21833,7 @@
     </row>
     <row r="511" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A511" s="2" t="s">
-        <v>1456</v>
+        <v>1455</v>
       </c>
       <c r="B511" s="5"/>
       <c r="C511" s="5"/>
@@ -21868,7 +21863,7 @@
     </row>
     <row r="512" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A512" s="2" t="s">
-        <v>1457</v>
+        <v>1456</v>
       </c>
       <c r="B512" s="5"/>
       <c r="C512" s="5"/>
@@ -21898,7 +21893,7 @@
     </row>
     <row r="513" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A513" s="2" t="s">
-        <v>1458</v>
+        <v>1457</v>
       </c>
       <c r="B513" s="5"/>
       <c r="C513" s="5"/>
@@ -21928,7 +21923,7 @@
     </row>
     <row r="514" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A514" s="2" t="s">
-        <v>1459</v>
+        <v>1458</v>
       </c>
       <c r="B514" s="5"/>
       <c r="C514" s="5"/>

</xml_diff>

<commit_message>
messenger rx, enc, ack menu options
</commit_message>
<xml_diff>
--- a/docs/UV K5 EEPROM.xlsx
+++ b/docs/UV K5 EEPROM.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1461" uniqueCount="1459">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1462" uniqueCount="1460">
   <si>
     <t xml:space="preserve">00</t>
   </si>
@@ -2126,6 +2126,9 @@
   </si>
   <si>
     <t xml:space="preserve">PASSWORD_WRONG_ATTEMPTS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MSG_CONFIG</t>
   </si>
   <si>
     <t xml:space="preserve">AL-MOD</t>
@@ -4406,7 +4409,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="8">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -4439,6 +4442,20 @@
     <font>
       <b val="true"/>
       <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="0"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="6"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="0"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="9"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="0"/>
@@ -4499,7 +4516,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="15">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -4529,6 +4546,14 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -4632,10 +4657,10 @@
   <dimension ref="A1:Z1001"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A206" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I219" activeCellId="0" sqref="I219"/>
+      <selection pane="topLeft" activeCell="E236" activeCellId="0" sqref="E236"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.77734375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.796875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1"/>
@@ -12623,29 +12648,31 @@
       <c r="C236" s="4" t="s">
         <v>700</v>
       </c>
-      <c r="D236" s="4" t="s">
+      <c r="D236" s="8" t="s">
         <v>701</v>
       </c>
-      <c r="E236" s="7"/>
+      <c r="E236" s="9" t="s">
+        <v>702</v>
+      </c>
       <c r="F236" s="7"/>
-      <c r="G236" s="8"/>
+      <c r="G236" s="10"/>
       <c r="H236" s="5"/>
       <c r="I236" s="5"/>
       <c r="J236" s="4" t="s">
-        <v>702</v>
+        <v>703</v>
       </c>
       <c r="K236" s="4" t="s">
-        <v>703</v>
+        <v>704</v>
       </c>
       <c r="L236" s="7"/>
       <c r="M236" s="4" t="s">
-        <v>704</v>
-      </c>
-      <c r="N236" s="9" t="s">
         <v>705</v>
       </c>
+      <c r="N236" s="11" t="s">
+        <v>706</v>
+      </c>
       <c r="O236" s="1" t="s">
-        <v>706</v>
+        <v>707</v>
       </c>
       <c r="P236" s="5"/>
       <c r="Q236" s="5"/>
@@ -12661,10 +12688,10 @@
     </row>
     <row r="237" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A237" s="2" t="s">
-        <v>707</v>
+        <v>708</v>
       </c>
       <c r="B237" s="3" t="s">
-        <v>708</v>
+        <v>709</v>
       </c>
       <c r="C237" s="3"/>
       <c r="D237" s="3"/>
@@ -12693,10 +12720,10 @@
     </row>
     <row r="238" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A238" s="2" t="s">
-        <v>709</v>
+        <v>710</v>
       </c>
       <c r="B238" s="3" t="s">
-        <v>710</v>
+        <v>711</v>
       </c>
       <c r="C238" s="3"/>
       <c r="D238" s="3"/>
@@ -12725,40 +12752,40 @@
     </row>
     <row r="239" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A239" s="2" t="s">
-        <v>711</v>
+        <v>712</v>
       </c>
       <c r="B239" s="4" t="s">
-        <v>712</v>
+        <v>713</v>
       </c>
       <c r="C239" s="4" t="s">
-        <v>713</v>
+        <v>714</v>
       </c>
       <c r="D239" s="4" t="s">
-        <v>714</v>
+        <v>715</v>
       </c>
       <c r="E239" s="4" t="s">
-        <v>715</v>
+        <v>716</v>
       </c>
       <c r="F239" s="4" t="s">
-        <v>716</v>
+        <v>717</v>
       </c>
       <c r="G239" s="4" t="s">
-        <v>717</v>
+        <v>718</v>
       </c>
       <c r="H239" s="4" t="s">
-        <v>718</v>
+        <v>719</v>
       </c>
       <c r="I239" s="4" t="s">
-        <v>719</v>
+        <v>720</v>
       </c>
       <c r="J239" s="4" t="s">
-        <v>720</v>
+        <v>721</v>
       </c>
       <c r="K239" s="4" t="s">
-        <v>721</v>
+        <v>722</v>
       </c>
       <c r="L239" s="4" t="s">
-        <v>722</v>
+        <v>723</v>
       </c>
       <c r="M239" s="5"/>
       <c r="N239" s="5"/>
@@ -12777,10 +12804,10 @@
     </row>
     <row r="240" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A240" s="2" t="s">
-        <v>723</v>
+        <v>724</v>
       </c>
       <c r="B240" s="3" t="s">
-        <v>724</v>
+        <v>725</v>
       </c>
       <c r="C240" s="3"/>
       <c r="D240" s="3"/>
@@ -12790,7 +12817,7 @@
       <c r="H240" s="3"/>
       <c r="I240" s="3"/>
       <c r="J240" s="3" t="s">
-        <v>725</v>
+        <v>726</v>
       </c>
       <c r="K240" s="3"/>
       <c r="L240" s="3"/>
@@ -12811,10 +12838,10 @@
     </row>
     <row r="241" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A241" s="2" t="s">
-        <v>726</v>
+        <v>727</v>
       </c>
       <c r="B241" s="3" t="s">
-        <v>727</v>
+        <v>728</v>
       </c>
       <c r="C241" s="3"/>
       <c r="D241" s="3"/>
@@ -12824,7 +12851,7 @@
       <c r="H241" s="3"/>
       <c r="I241" s="3"/>
       <c r="J241" s="3" t="s">
-        <v>728</v>
+        <v>729</v>
       </c>
       <c r="K241" s="3"/>
       <c r="L241" s="3"/>
@@ -12845,10 +12872,10 @@
     </row>
     <row r="242" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A242" s="2" t="s">
+        <v>730</v>
+      </c>
+      <c r="B242" s="3" t="s">
         <v>729</v>
-      </c>
-      <c r="B242" s="3" t="s">
-        <v>728</v>
       </c>
       <c r="C242" s="3"/>
       <c r="D242" s="3"/>
@@ -12858,7 +12885,7 @@
       <c r="H242" s="3"/>
       <c r="I242" s="3"/>
       <c r="J242" s="3" t="s">
-        <v>730</v>
+        <v>731</v>
       </c>
       <c r="K242" s="3"/>
       <c r="L242" s="3"/>
@@ -12879,10 +12906,10 @@
     </row>
     <row r="243" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A243" s="2" t="s">
+        <v>732</v>
+      </c>
+      <c r="B243" s="3" t="s">
         <v>731</v>
-      </c>
-      <c r="B243" s="3" t="s">
-        <v>730</v>
       </c>
       <c r="C243" s="3"/>
       <c r="D243" s="3"/>
@@ -12892,25 +12919,25 @@
       <c r="H243" s="3"/>
       <c r="I243" s="3"/>
       <c r="J243" s="4" t="s">
-        <v>732</v>
+        <v>733</v>
       </c>
       <c r="K243" s="4" t="s">
-        <v>733</v>
+        <v>734</v>
       </c>
       <c r="L243" s="4" t="s">
-        <v>734</v>
+        <v>735</v>
       </c>
       <c r="M243" s="4" t="s">
-        <v>735</v>
+        <v>736</v>
       </c>
       <c r="N243" s="4" t="s">
-        <v>736</v>
+        <v>737</v>
       </c>
       <c r="O243" s="4" t="s">
-        <v>737</v>
+        <v>738</v>
       </c>
       <c r="P243" s="4" t="s">
-        <v>738</v>
+        <v>739</v>
       </c>
       <c r="Q243" s="5"/>
       <c r="R243" s="1"/>
@@ -12925,7 +12952,7 @@
     </row>
     <row r="244" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A244" s="2" t="s">
-        <v>739</v>
+        <v>740</v>
       </c>
       <c r="B244" s="5"/>
       <c r="C244" s="5"/>
@@ -12955,10 +12982,10 @@
     </row>
     <row r="245" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A245" s="2" t="s">
-        <v>740</v>
+        <v>741</v>
       </c>
       <c r="B245" s="3" t="s">
-        <v>741</v>
+        <v>742</v>
       </c>
       <c r="C245" s="3"/>
       <c r="D245" s="3"/>
@@ -12987,28 +13014,28 @@
     </row>
     <row r="246" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A246" s="2" t="s">
-        <v>742</v>
+        <v>743</v>
       </c>
       <c r="B246" s="4" t="s">
-        <v>743</v>
+        <v>744</v>
       </c>
       <c r="C246" s="4" t="s">
-        <v>744</v>
+        <v>745</v>
       </c>
       <c r="D246" s="4" t="s">
-        <v>745</v>
+        <v>746</v>
       </c>
       <c r="E246" s="4" t="s">
-        <v>746</v>
+        <v>747</v>
       </c>
       <c r="F246" s="4" t="s">
-        <v>747</v>
+        <v>748</v>
       </c>
       <c r="G246" s="4" t="s">
-        <v>748</v>
+        <v>749</v>
       </c>
       <c r="H246" s="4" t="s">
-        <v>749</v>
+        <v>750</v>
       </c>
       <c r="I246" s="5"/>
       <c r="J246" s="5"/>
@@ -13031,10 +13058,10 @@
     </row>
     <row r="247" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A247" s="2" t="s">
-        <v>750</v>
+        <v>751</v>
       </c>
       <c r="B247" s="3" t="s">
-        <v>751</v>
+        <v>752</v>
       </c>
       <c r="C247" s="3"/>
       <c r="D247" s="3"/>
@@ -13063,10 +13090,10 @@
     </row>
     <row r="248" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A248" s="2" t="s">
-        <v>752</v>
+        <v>753</v>
       </c>
       <c r="B248" s="3" t="s">
-        <v>753</v>
+        <v>754</v>
       </c>
       <c r="C248" s="3"/>
       <c r="D248" s="3"/>
@@ -13095,10 +13122,10 @@
     </row>
     <row r="249" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A249" s="2" t="s">
-        <v>754</v>
+        <v>755</v>
       </c>
       <c r="B249" s="3" t="s">
-        <v>755</v>
+        <v>756</v>
       </c>
       <c r="C249" s="3"/>
       <c r="D249" s="3"/>
@@ -13127,10 +13154,10 @@
     </row>
     <row r="250" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A250" s="2" t="s">
-        <v>756</v>
+        <v>757</v>
       </c>
       <c r="B250" s="3" t="s">
-        <v>757</v>
+        <v>758</v>
       </c>
       <c r="C250" s="3"/>
       <c r="D250" s="3"/>
@@ -13159,10 +13186,10 @@
     </row>
     <row r="251" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A251" s="2" t="s">
-        <v>758</v>
+        <v>759</v>
       </c>
       <c r="B251" s="3" t="s">
-        <v>759</v>
+        <v>760</v>
       </c>
       <c r="C251" s="3"/>
       <c r="D251" s="3"/>
@@ -13191,10 +13218,10 @@
     </row>
     <row r="252" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A252" s="2" t="s">
-        <v>760</v>
+        <v>761</v>
       </c>
       <c r="B252" s="3" t="s">
-        <v>761</v>
+        <v>762</v>
       </c>
       <c r="C252" s="3"/>
       <c r="D252" s="3"/>
@@ -13223,10 +13250,10 @@
     </row>
     <row r="253" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A253" s="2" t="s">
-        <v>762</v>
+        <v>763</v>
       </c>
       <c r="B253" s="3" t="s">
-        <v>763</v>
+        <v>764</v>
       </c>
       <c r="C253" s="3"/>
       <c r="D253" s="3"/>
@@ -13255,10 +13282,10 @@
     </row>
     <row r="254" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A254" s="2" t="s">
-        <v>764</v>
+        <v>765</v>
       </c>
       <c r="B254" s="3" t="s">
-        <v>765</v>
+        <v>766</v>
       </c>
       <c r="C254" s="3"/>
       <c r="D254" s="3"/>
@@ -13287,10 +13314,10 @@
     </row>
     <row r="255" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A255" s="2" t="s">
-        <v>766</v>
+        <v>767</v>
       </c>
       <c r="B255" s="3" t="s">
-        <v>767</v>
+        <v>768</v>
       </c>
       <c r="C255" s="3"/>
       <c r="D255" s="3"/>
@@ -13319,10 +13346,10 @@
     </row>
     <row r="256" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A256" s="2" t="s">
-        <v>768</v>
+        <v>769</v>
       </c>
       <c r="B256" s="3" t="s">
-        <v>769</v>
+        <v>770</v>
       </c>
       <c r="C256" s="3"/>
       <c r="D256" s="3"/>
@@ -13351,10 +13378,10 @@
     </row>
     <row r="257" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A257" s="2" t="s">
-        <v>770</v>
+        <v>771</v>
       </c>
       <c r="B257" s="3" t="s">
-        <v>771</v>
+        <v>772</v>
       </c>
       <c r="C257" s="3"/>
       <c r="D257" s="3"/>
@@ -13383,10 +13410,10 @@
     </row>
     <row r="258" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A258" s="2" t="s">
-        <v>772</v>
+        <v>773</v>
       </c>
       <c r="B258" s="3" t="s">
-        <v>773</v>
+        <v>774</v>
       </c>
       <c r="C258" s="3"/>
       <c r="D258" s="3"/>
@@ -13415,10 +13442,10 @@
     </row>
     <row r="259" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A259" s="2" t="s">
-        <v>774</v>
+        <v>775</v>
       </c>
       <c r="B259" s="3" t="s">
-        <v>775</v>
+        <v>776</v>
       </c>
       <c r="C259" s="3"/>
       <c r="D259" s="3"/>
@@ -13447,10 +13474,10 @@
     </row>
     <row r="260" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A260" s="2" t="s">
-        <v>776</v>
+        <v>777</v>
       </c>
       <c r="B260" s="3" t="s">
-        <v>777</v>
+        <v>778</v>
       </c>
       <c r="C260" s="3"/>
       <c r="D260" s="3"/>
@@ -13479,10 +13506,10 @@
     </row>
     <row r="261" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A261" s="2" t="s">
-        <v>778</v>
+        <v>779</v>
       </c>
       <c r="B261" s="3" t="s">
-        <v>779</v>
+        <v>780</v>
       </c>
       <c r="C261" s="3"/>
       <c r="D261" s="3"/>
@@ -13511,10 +13538,10 @@
     </row>
     <row r="262" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A262" s="2" t="s">
-        <v>780</v>
+        <v>781</v>
       </c>
       <c r="B262" s="3" t="s">
-        <v>781</v>
+        <v>782</v>
       </c>
       <c r="C262" s="3"/>
       <c r="D262" s="3"/>
@@ -13543,10 +13570,10 @@
     </row>
     <row r="263" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A263" s="2" t="s">
-        <v>782</v>
+        <v>783</v>
       </c>
       <c r="B263" s="3" t="s">
-        <v>783</v>
+        <v>784</v>
       </c>
       <c r="C263" s="3"/>
       <c r="D263" s="3"/>
@@ -13575,10 +13602,10 @@
     </row>
     <row r="264" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A264" s="2" t="s">
-        <v>784</v>
+        <v>785</v>
       </c>
       <c r="B264" s="3" t="s">
-        <v>785</v>
+        <v>786</v>
       </c>
       <c r="C264" s="3"/>
       <c r="D264" s="3"/>
@@ -13607,10 +13634,10 @@
     </row>
     <row r="265" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A265" s="2" t="s">
-        <v>786</v>
+        <v>787</v>
       </c>
       <c r="B265" s="3" t="s">
-        <v>787</v>
+        <v>788</v>
       </c>
       <c r="C265" s="3"/>
       <c r="D265" s="3"/>
@@ -13639,10 +13666,10 @@
     </row>
     <row r="266" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A266" s="2" t="s">
-        <v>788</v>
+        <v>789</v>
       </c>
       <c r="B266" s="3" t="s">
-        <v>789</v>
+        <v>790</v>
       </c>
       <c r="C266" s="3"/>
       <c r="D266" s="3"/>
@@ -13671,10 +13698,10 @@
     </row>
     <row r="267" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A267" s="2" t="s">
-        <v>790</v>
+        <v>791</v>
       </c>
       <c r="B267" s="3" t="s">
-        <v>791</v>
+        <v>792</v>
       </c>
       <c r="C267" s="3"/>
       <c r="D267" s="3"/>
@@ -13703,10 +13730,10 @@
     </row>
     <row r="268" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A268" s="2" t="s">
-        <v>792</v>
+        <v>793</v>
       </c>
       <c r="B268" s="3" t="s">
-        <v>793</v>
+        <v>794</v>
       </c>
       <c r="C268" s="3"/>
       <c r="D268" s="3"/>
@@ -13735,10 +13762,10 @@
     </row>
     <row r="269" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A269" s="2" t="s">
-        <v>794</v>
+        <v>795</v>
       </c>
       <c r="B269" s="3" t="s">
-        <v>795</v>
+        <v>796</v>
       </c>
       <c r="C269" s="3"/>
       <c r="D269" s="3"/>
@@ -13767,10 +13794,10 @@
     </row>
     <row r="270" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A270" s="2" t="s">
-        <v>796</v>
+        <v>797</v>
       </c>
       <c r="B270" s="3" t="s">
-        <v>797</v>
+        <v>798</v>
       </c>
       <c r="C270" s="3"/>
       <c r="D270" s="3"/>
@@ -13799,10 +13826,10 @@
     </row>
     <row r="271" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A271" s="2" t="s">
-        <v>798</v>
+        <v>799</v>
       </c>
       <c r="B271" s="3" t="s">
-        <v>799</v>
+        <v>800</v>
       </c>
       <c r="C271" s="3"/>
       <c r="D271" s="3"/>
@@ -13831,10 +13858,10 @@
     </row>
     <row r="272" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A272" s="2" t="s">
-        <v>800</v>
+        <v>801</v>
       </c>
       <c r="B272" s="3" t="s">
-        <v>801</v>
+        <v>802</v>
       </c>
       <c r="C272" s="3"/>
       <c r="D272" s="3"/>
@@ -13863,10 +13890,10 @@
     </row>
     <row r="273" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A273" s="2" t="s">
-        <v>802</v>
+        <v>803</v>
       </c>
       <c r="B273" s="3" t="s">
-        <v>803</v>
+        <v>804</v>
       </c>
       <c r="C273" s="3"/>
       <c r="D273" s="3"/>
@@ -13895,10 +13922,10 @@
     </row>
     <row r="274" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A274" s="2" t="s">
-        <v>804</v>
+        <v>805</v>
       </c>
       <c r="B274" s="3" t="s">
-        <v>805</v>
+        <v>806</v>
       </c>
       <c r="C274" s="3"/>
       <c r="D274" s="3"/>
@@ -13927,10 +13954,10 @@
     </row>
     <row r="275" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A275" s="2" t="s">
-        <v>806</v>
+        <v>807</v>
       </c>
       <c r="B275" s="3" t="s">
-        <v>807</v>
+        <v>808</v>
       </c>
       <c r="C275" s="3"/>
       <c r="D275" s="3"/>
@@ -13959,10 +13986,10 @@
     </row>
     <row r="276" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A276" s="2" t="s">
-        <v>808</v>
+        <v>809</v>
       </c>
       <c r="B276" s="3" t="s">
-        <v>809</v>
+        <v>810</v>
       </c>
       <c r="C276" s="3"/>
       <c r="D276" s="3"/>
@@ -13991,10 +14018,10 @@
     </row>
     <row r="277" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A277" s="2" t="s">
-        <v>810</v>
+        <v>811</v>
       </c>
       <c r="B277" s="3" t="s">
-        <v>811</v>
+        <v>812</v>
       </c>
       <c r="C277" s="3"/>
       <c r="D277" s="3"/>
@@ -14023,10 +14050,10 @@
     </row>
     <row r="278" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A278" s="2" t="s">
-        <v>812</v>
+        <v>813</v>
       </c>
       <c r="B278" s="3" t="s">
-        <v>813</v>
+        <v>814</v>
       </c>
       <c r="C278" s="3"/>
       <c r="D278" s="3"/>
@@ -14055,10 +14082,10 @@
     </row>
     <row r="279" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A279" s="2" t="s">
-        <v>814</v>
+        <v>815</v>
       </c>
       <c r="B279" s="3" t="s">
-        <v>815</v>
+        <v>816</v>
       </c>
       <c r="C279" s="3"/>
       <c r="D279" s="3"/>
@@ -14087,10 +14114,10 @@
     </row>
     <row r="280" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A280" s="2" t="s">
-        <v>816</v>
+        <v>817</v>
       </c>
       <c r="B280" s="3" t="s">
-        <v>817</v>
+        <v>818</v>
       </c>
       <c r="C280" s="3"/>
       <c r="D280" s="3"/>
@@ -14119,10 +14146,10 @@
     </row>
     <row r="281" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A281" s="2" t="s">
-        <v>818</v>
+        <v>819</v>
       </c>
       <c r="B281" s="3" t="s">
-        <v>819</v>
+        <v>820</v>
       </c>
       <c r="C281" s="3"/>
       <c r="D281" s="3"/>
@@ -14151,10 +14178,10 @@
     </row>
     <row r="282" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A282" s="2" t="s">
-        <v>820</v>
+        <v>821</v>
       </c>
       <c r="B282" s="3" t="s">
-        <v>821</v>
+        <v>822</v>
       </c>
       <c r="C282" s="3"/>
       <c r="D282" s="3"/>
@@ -14183,10 +14210,10 @@
     </row>
     <row r="283" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A283" s="2" t="s">
-        <v>822</v>
+        <v>823</v>
       </c>
       <c r="B283" s="3" t="s">
-        <v>823</v>
+        <v>824</v>
       </c>
       <c r="C283" s="3"/>
       <c r="D283" s="3"/>
@@ -14215,10 +14242,10 @@
     </row>
     <row r="284" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A284" s="2" t="s">
-        <v>824</v>
+        <v>825</v>
       </c>
       <c r="B284" s="3" t="s">
-        <v>825</v>
+        <v>826</v>
       </c>
       <c r="C284" s="3"/>
       <c r="D284" s="3"/>
@@ -14247,10 +14274,10 @@
     </row>
     <row r="285" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A285" s="2" t="s">
-        <v>826</v>
+        <v>827</v>
       </c>
       <c r="B285" s="3" t="s">
-        <v>827</v>
+        <v>828</v>
       </c>
       <c r="C285" s="3"/>
       <c r="D285" s="3"/>
@@ -14279,10 +14306,10 @@
     </row>
     <row r="286" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A286" s="2" t="s">
-        <v>828</v>
+        <v>829</v>
       </c>
       <c r="B286" s="3" t="s">
-        <v>829</v>
+        <v>830</v>
       </c>
       <c r="C286" s="3"/>
       <c r="D286" s="3"/>
@@ -14311,10 +14338,10 @@
     </row>
     <row r="287" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A287" s="2" t="s">
-        <v>830</v>
+        <v>831</v>
       </c>
       <c r="B287" s="3" t="s">
-        <v>831</v>
+        <v>832</v>
       </c>
       <c r="C287" s="3"/>
       <c r="D287" s="3"/>
@@ -14343,10 +14370,10 @@
     </row>
     <row r="288" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A288" s="2" t="s">
-        <v>832</v>
+        <v>833</v>
       </c>
       <c r="B288" s="3" t="s">
-        <v>833</v>
+        <v>834</v>
       </c>
       <c r="C288" s="3"/>
       <c r="D288" s="3"/>
@@ -14375,10 +14402,10 @@
     </row>
     <row r="289" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A289" s="2" t="s">
-        <v>834</v>
+        <v>835</v>
       </c>
       <c r="B289" s="3" t="s">
-        <v>835</v>
+        <v>836</v>
       </c>
       <c r="C289" s="3"/>
       <c r="D289" s="3"/>
@@ -14407,10 +14434,10 @@
     </row>
     <row r="290" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A290" s="2" t="s">
-        <v>836</v>
+        <v>837</v>
       </c>
       <c r="B290" s="3" t="s">
-        <v>837</v>
+        <v>838</v>
       </c>
       <c r="C290" s="3"/>
       <c r="D290" s="3"/>
@@ -14439,10 +14466,10 @@
     </row>
     <row r="291" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A291" s="2" t="s">
-        <v>838</v>
+        <v>839</v>
       </c>
       <c r="B291" s="3" t="s">
-        <v>839</v>
+        <v>840</v>
       </c>
       <c r="C291" s="3"/>
       <c r="D291" s="3"/>
@@ -14471,10 +14498,10 @@
     </row>
     <row r="292" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A292" s="2" t="s">
-        <v>840</v>
+        <v>841</v>
       </c>
       <c r="B292" s="3" t="s">
-        <v>841</v>
+        <v>842</v>
       </c>
       <c r="C292" s="3"/>
       <c r="D292" s="3"/>
@@ -14503,10 +14530,10 @@
     </row>
     <row r="293" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A293" s="2" t="s">
-        <v>842</v>
+        <v>843</v>
       </c>
       <c r="B293" s="3" t="s">
-        <v>843</v>
+        <v>844</v>
       </c>
       <c r="C293" s="3"/>
       <c r="D293" s="3"/>
@@ -14535,10 +14562,10 @@
     </row>
     <row r="294" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A294" s="2" t="s">
-        <v>844</v>
+        <v>845</v>
       </c>
       <c r="B294" s="3" t="s">
-        <v>845</v>
+        <v>846</v>
       </c>
       <c r="C294" s="3"/>
       <c r="D294" s="3"/>
@@ -14567,10 +14594,10 @@
     </row>
     <row r="295" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A295" s="2" t="s">
-        <v>846</v>
+        <v>847</v>
       </c>
       <c r="B295" s="3" t="s">
-        <v>847</v>
+        <v>848</v>
       </c>
       <c r="C295" s="3"/>
       <c r="D295" s="3"/>
@@ -14599,10 +14626,10 @@
     </row>
     <row r="296" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A296" s="2" t="s">
-        <v>848</v>
+        <v>849</v>
       </c>
       <c r="B296" s="3" t="s">
-        <v>849</v>
+        <v>850</v>
       </c>
       <c r="C296" s="3"/>
       <c r="D296" s="3"/>
@@ -14631,10 +14658,10 @@
     </row>
     <row r="297" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A297" s="2" t="s">
-        <v>850</v>
+        <v>851</v>
       </c>
       <c r="B297" s="3" t="s">
-        <v>851</v>
+        <v>852</v>
       </c>
       <c r="C297" s="3"/>
       <c r="D297" s="3"/>
@@ -14663,10 +14690,10 @@
     </row>
     <row r="298" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A298" s="2" t="s">
-        <v>852</v>
+        <v>853</v>
       </c>
       <c r="B298" s="3" t="s">
-        <v>853</v>
+        <v>854</v>
       </c>
       <c r="C298" s="3"/>
       <c r="D298" s="3"/>
@@ -14695,10 +14722,10 @@
     </row>
     <row r="299" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A299" s="2" t="s">
-        <v>854</v>
+        <v>855</v>
       </c>
       <c r="B299" s="3" t="s">
-        <v>855</v>
+        <v>856</v>
       </c>
       <c r="C299" s="3"/>
       <c r="D299" s="3"/>
@@ -14727,10 +14754,10 @@
     </row>
     <row r="300" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A300" s="2" t="s">
-        <v>856</v>
+        <v>857</v>
       </c>
       <c r="B300" s="3" t="s">
-        <v>857</v>
+        <v>858</v>
       </c>
       <c r="C300" s="3"/>
       <c r="D300" s="3"/>
@@ -14759,10 +14786,10 @@
     </row>
     <row r="301" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A301" s="2" t="s">
-        <v>858</v>
+        <v>859</v>
       </c>
       <c r="B301" s="3" t="s">
-        <v>859</v>
+        <v>860</v>
       </c>
       <c r="C301" s="3"/>
       <c r="D301" s="3"/>
@@ -14791,10 +14818,10 @@
     </row>
     <row r="302" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A302" s="2" t="s">
-        <v>860</v>
+        <v>861</v>
       </c>
       <c r="B302" s="3" t="s">
-        <v>861</v>
+        <v>862</v>
       </c>
       <c r="C302" s="3"/>
       <c r="D302" s="3"/>
@@ -14823,10 +14850,10 @@
     </row>
     <row r="303" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A303" s="2" t="s">
-        <v>862</v>
+        <v>863</v>
       </c>
       <c r="B303" s="3" t="s">
-        <v>863</v>
+        <v>864</v>
       </c>
       <c r="C303" s="3"/>
       <c r="D303" s="3"/>
@@ -14855,10 +14882,10 @@
     </row>
     <row r="304" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A304" s="2" t="s">
-        <v>864</v>
+        <v>865</v>
       </c>
       <c r="B304" s="3" t="s">
-        <v>865</v>
+        <v>866</v>
       </c>
       <c r="C304" s="3"/>
       <c r="D304" s="3"/>
@@ -14887,10 +14914,10 @@
     </row>
     <row r="305" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A305" s="2" t="s">
-        <v>866</v>
+        <v>867</v>
       </c>
       <c r="B305" s="3" t="s">
-        <v>867</v>
+        <v>868</v>
       </c>
       <c r="C305" s="3"/>
       <c r="D305" s="3"/>
@@ -14919,10 +14946,10 @@
     </row>
     <row r="306" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A306" s="2" t="s">
-        <v>868</v>
+        <v>869</v>
       </c>
       <c r="B306" s="3" t="s">
-        <v>869</v>
+        <v>870</v>
       </c>
       <c r="C306" s="3"/>
       <c r="D306" s="3"/>
@@ -14951,10 +14978,10 @@
     </row>
     <row r="307" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A307" s="2" t="s">
-        <v>870</v>
+        <v>871</v>
       </c>
       <c r="B307" s="3" t="s">
-        <v>871</v>
+        <v>872</v>
       </c>
       <c r="C307" s="3"/>
       <c r="D307" s="3"/>
@@ -14983,10 +15010,10 @@
     </row>
     <row r="308" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A308" s="2" t="s">
-        <v>872</v>
+        <v>873</v>
       </c>
       <c r="B308" s="3" t="s">
-        <v>873</v>
+        <v>874</v>
       </c>
       <c r="C308" s="3"/>
       <c r="D308" s="3"/>
@@ -15015,10 +15042,10 @@
     </row>
     <row r="309" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A309" s="2" t="s">
-        <v>874</v>
+        <v>875</v>
       </c>
       <c r="B309" s="3" t="s">
-        <v>875</v>
+        <v>876</v>
       </c>
       <c r="C309" s="3"/>
       <c r="D309" s="3"/>
@@ -15047,10 +15074,10 @@
     </row>
     <row r="310" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A310" s="2" t="s">
-        <v>876</v>
+        <v>877</v>
       </c>
       <c r="B310" s="3" t="s">
-        <v>877</v>
+        <v>878</v>
       </c>
       <c r="C310" s="3"/>
       <c r="D310" s="3"/>
@@ -15079,10 +15106,10 @@
     </row>
     <row r="311" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A311" s="2" t="s">
-        <v>878</v>
+        <v>879</v>
       </c>
       <c r="B311" s="3" t="s">
-        <v>879</v>
+        <v>880</v>
       </c>
       <c r="C311" s="3"/>
       <c r="D311" s="3"/>
@@ -15111,10 +15138,10 @@
     </row>
     <row r="312" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A312" s="2" t="s">
-        <v>880</v>
+        <v>881</v>
       </c>
       <c r="B312" s="3" t="s">
-        <v>881</v>
+        <v>882</v>
       </c>
       <c r="C312" s="3"/>
       <c r="D312" s="3"/>
@@ -15143,10 +15170,10 @@
     </row>
     <row r="313" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A313" s="2" t="s">
-        <v>882</v>
+        <v>883</v>
       </c>
       <c r="B313" s="3" t="s">
-        <v>883</v>
+        <v>884</v>
       </c>
       <c r="C313" s="3"/>
       <c r="D313" s="3"/>
@@ -15175,10 +15202,10 @@
     </row>
     <row r="314" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A314" s="2" t="s">
-        <v>884</v>
+        <v>885</v>
       </c>
       <c r="B314" s="3" t="s">
-        <v>885</v>
+        <v>886</v>
       </c>
       <c r="C314" s="3"/>
       <c r="D314" s="3"/>
@@ -15207,10 +15234,10 @@
     </row>
     <row r="315" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A315" s="2" t="s">
-        <v>886</v>
+        <v>887</v>
       </c>
       <c r="B315" s="3" t="s">
-        <v>887</v>
+        <v>888</v>
       </c>
       <c r="C315" s="3"/>
       <c r="D315" s="3"/>
@@ -15239,10 +15266,10 @@
     </row>
     <row r="316" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A316" s="2" t="s">
-        <v>888</v>
+        <v>889</v>
       </c>
       <c r="B316" s="3" t="s">
-        <v>889</v>
+        <v>890</v>
       </c>
       <c r="C316" s="3"/>
       <c r="D316" s="3"/>
@@ -15271,10 +15298,10 @@
     </row>
     <row r="317" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A317" s="2" t="s">
-        <v>890</v>
+        <v>891</v>
       </c>
       <c r="B317" s="3" t="s">
-        <v>891</v>
+        <v>892</v>
       </c>
       <c r="C317" s="3"/>
       <c r="D317" s="3"/>
@@ -15303,10 +15330,10 @@
     </row>
     <row r="318" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A318" s="2" t="s">
-        <v>892</v>
+        <v>893</v>
       </c>
       <c r="B318" s="3" t="s">
-        <v>893</v>
+        <v>894</v>
       </c>
       <c r="C318" s="3"/>
       <c r="D318" s="3"/>
@@ -15335,10 +15362,10 @@
     </row>
     <row r="319" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A319" s="2" t="s">
-        <v>894</v>
+        <v>895</v>
       </c>
       <c r="B319" s="3" t="s">
-        <v>895</v>
+        <v>896</v>
       </c>
       <c r="C319" s="3"/>
       <c r="D319" s="3"/>
@@ -15367,10 +15394,10 @@
     </row>
     <row r="320" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A320" s="2" t="s">
-        <v>896</v>
+        <v>897</v>
       </c>
       <c r="B320" s="3" t="s">
-        <v>897</v>
+        <v>898</v>
       </c>
       <c r="C320" s="3"/>
       <c r="D320" s="3"/>
@@ -15399,10 +15426,10 @@
     </row>
     <row r="321" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A321" s="2" t="s">
-        <v>898</v>
+        <v>899</v>
       </c>
       <c r="B321" s="3" t="s">
-        <v>899</v>
+        <v>900</v>
       </c>
       <c r="C321" s="3"/>
       <c r="D321" s="3"/>
@@ -15431,10 +15458,10 @@
     </row>
     <row r="322" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A322" s="2" t="s">
-        <v>900</v>
+        <v>901</v>
       </c>
       <c r="B322" s="3" t="s">
-        <v>901</v>
+        <v>902</v>
       </c>
       <c r="C322" s="3"/>
       <c r="D322" s="3"/>
@@ -15463,10 +15490,10 @@
     </row>
     <row r="323" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A323" s="2" t="s">
-        <v>902</v>
+        <v>903</v>
       </c>
       <c r="B323" s="3" t="s">
-        <v>903</v>
+        <v>904</v>
       </c>
       <c r="C323" s="3"/>
       <c r="D323" s="3"/>
@@ -15495,10 +15522,10 @@
     </row>
     <row r="324" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A324" s="2" t="s">
-        <v>904</v>
+        <v>905</v>
       </c>
       <c r="B324" s="3" t="s">
-        <v>905</v>
+        <v>906</v>
       </c>
       <c r="C324" s="3"/>
       <c r="D324" s="3"/>
@@ -15527,10 +15554,10 @@
     </row>
     <row r="325" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A325" s="2" t="s">
-        <v>906</v>
+        <v>907</v>
       </c>
       <c r="B325" s="3" t="s">
-        <v>907</v>
+        <v>908</v>
       </c>
       <c r="C325" s="3"/>
       <c r="D325" s="3"/>
@@ -15559,10 +15586,10 @@
     </row>
     <row r="326" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A326" s="2" t="s">
-        <v>908</v>
+        <v>909</v>
       </c>
       <c r="B326" s="3" t="s">
-        <v>909</v>
+        <v>910</v>
       </c>
       <c r="C326" s="3"/>
       <c r="D326" s="3"/>
@@ -15591,10 +15618,10 @@
     </row>
     <row r="327" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A327" s="2" t="s">
-        <v>910</v>
+        <v>911</v>
       </c>
       <c r="B327" s="3" t="s">
-        <v>911</v>
+        <v>912</v>
       </c>
       <c r="C327" s="3"/>
       <c r="D327" s="3"/>
@@ -15623,10 +15650,10 @@
     </row>
     <row r="328" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A328" s="2" t="s">
-        <v>912</v>
+        <v>913</v>
       </c>
       <c r="B328" s="3" t="s">
-        <v>913</v>
+        <v>914</v>
       </c>
       <c r="C328" s="3"/>
       <c r="D328" s="3"/>
@@ -15655,10 +15682,10 @@
     </row>
     <row r="329" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A329" s="2" t="s">
-        <v>914</v>
+        <v>915</v>
       </c>
       <c r="B329" s="3" t="s">
-        <v>915</v>
+        <v>916</v>
       </c>
       <c r="C329" s="3"/>
       <c r="D329" s="3"/>
@@ -15687,10 +15714,10 @@
     </row>
     <row r="330" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A330" s="2" t="s">
-        <v>916</v>
+        <v>917</v>
       </c>
       <c r="B330" s="3" t="s">
-        <v>917</v>
+        <v>918</v>
       </c>
       <c r="C330" s="3"/>
       <c r="D330" s="3"/>
@@ -15719,10 +15746,10 @@
     </row>
     <row r="331" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A331" s="2" t="s">
-        <v>918</v>
+        <v>919</v>
       </c>
       <c r="B331" s="3" t="s">
-        <v>919</v>
+        <v>920</v>
       </c>
       <c r="C331" s="3"/>
       <c r="D331" s="3"/>
@@ -15751,10 +15778,10 @@
     </row>
     <row r="332" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A332" s="2" t="s">
-        <v>920</v>
+        <v>921</v>
       </c>
       <c r="B332" s="3" t="s">
-        <v>921</v>
+        <v>922</v>
       </c>
       <c r="C332" s="3"/>
       <c r="D332" s="3"/>
@@ -15783,10 +15810,10 @@
     </row>
     <row r="333" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A333" s="2" t="s">
-        <v>922</v>
+        <v>923</v>
       </c>
       <c r="B333" s="3" t="s">
-        <v>923</v>
+        <v>924</v>
       </c>
       <c r="C333" s="3"/>
       <c r="D333" s="3"/>
@@ -15815,10 +15842,10 @@
     </row>
     <row r="334" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A334" s="2" t="s">
-        <v>924</v>
+        <v>925</v>
       </c>
       <c r="B334" s="3" t="s">
-        <v>925</v>
+        <v>926</v>
       </c>
       <c r="C334" s="3"/>
       <c r="D334" s="3"/>
@@ -15847,10 +15874,10 @@
     </row>
     <row r="335" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A335" s="2" t="s">
-        <v>926</v>
+        <v>927</v>
       </c>
       <c r="B335" s="3" t="s">
-        <v>927</v>
+        <v>928</v>
       </c>
       <c r="C335" s="3"/>
       <c r="D335" s="3"/>
@@ -15879,10 +15906,10 @@
     </row>
     <row r="336" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A336" s="2" t="s">
-        <v>928</v>
+        <v>929</v>
       </c>
       <c r="B336" s="3" t="s">
-        <v>929</v>
+        <v>930</v>
       </c>
       <c r="C336" s="3"/>
       <c r="D336" s="3"/>
@@ -15911,10 +15938,10 @@
     </row>
     <row r="337" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A337" s="2" t="s">
-        <v>930</v>
+        <v>931</v>
       </c>
       <c r="B337" s="3" t="s">
-        <v>931</v>
+        <v>932</v>
       </c>
       <c r="C337" s="3"/>
       <c r="D337" s="3"/>
@@ -15943,10 +15970,10 @@
     </row>
     <row r="338" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A338" s="2" t="s">
-        <v>932</v>
+        <v>933</v>
       </c>
       <c r="B338" s="3" t="s">
-        <v>933</v>
+        <v>934</v>
       </c>
       <c r="C338" s="3"/>
       <c r="D338" s="3"/>
@@ -15975,10 +16002,10 @@
     </row>
     <row r="339" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A339" s="2" t="s">
-        <v>934</v>
+        <v>935</v>
       </c>
       <c r="B339" s="3" t="s">
-        <v>935</v>
+        <v>936</v>
       </c>
       <c r="C339" s="3"/>
       <c r="D339" s="3"/>
@@ -16007,10 +16034,10 @@
     </row>
     <row r="340" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A340" s="2" t="s">
-        <v>936</v>
+        <v>937</v>
       </c>
       <c r="B340" s="3" t="s">
-        <v>937</v>
+        <v>938</v>
       </c>
       <c r="C340" s="3"/>
       <c r="D340" s="3"/>
@@ -16039,10 +16066,10 @@
     </row>
     <row r="341" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A341" s="2" t="s">
-        <v>938</v>
+        <v>939</v>
       </c>
       <c r="B341" s="3" t="s">
-        <v>939</v>
+        <v>940</v>
       </c>
       <c r="C341" s="3"/>
       <c r="D341" s="3"/>
@@ -16071,10 +16098,10 @@
     </row>
     <row r="342" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A342" s="2" t="s">
-        <v>940</v>
+        <v>941</v>
       </c>
       <c r="B342" s="3" t="s">
-        <v>941</v>
+        <v>942</v>
       </c>
       <c r="C342" s="3"/>
       <c r="D342" s="3"/>
@@ -16103,10 +16130,10 @@
     </row>
     <row r="343" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A343" s="2" t="s">
-        <v>942</v>
+        <v>943</v>
       </c>
       <c r="B343" s="3" t="s">
-        <v>943</v>
+        <v>944</v>
       </c>
       <c r="C343" s="3"/>
       <c r="D343" s="3"/>
@@ -16135,10 +16162,10 @@
     </row>
     <row r="344" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A344" s="2" t="s">
-        <v>944</v>
+        <v>945</v>
       </c>
       <c r="B344" s="3" t="s">
-        <v>945</v>
+        <v>946</v>
       </c>
       <c r="C344" s="3"/>
       <c r="D344" s="3"/>
@@ -16167,10 +16194,10 @@
     </row>
     <row r="345" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A345" s="2" t="s">
-        <v>946</v>
+        <v>947</v>
       </c>
       <c r="B345" s="3" t="s">
-        <v>947</v>
+        <v>948</v>
       </c>
       <c r="C345" s="3"/>
       <c r="D345" s="3"/>
@@ -16199,10 +16226,10 @@
     </row>
     <row r="346" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A346" s="2" t="s">
-        <v>948</v>
+        <v>949</v>
       </c>
       <c r="B346" s="3" t="s">
-        <v>949</v>
+        <v>950</v>
       </c>
       <c r="C346" s="3"/>
       <c r="D346" s="3"/>
@@ -16231,10 +16258,10 @@
     </row>
     <row r="347" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A347" s="2" t="s">
-        <v>950</v>
+        <v>951</v>
       </c>
       <c r="B347" s="3" t="s">
-        <v>951</v>
+        <v>952</v>
       </c>
       <c r="C347" s="3"/>
       <c r="D347" s="3"/>
@@ -16263,10 +16290,10 @@
     </row>
     <row r="348" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A348" s="2" t="s">
-        <v>952</v>
+        <v>953</v>
       </c>
       <c r="B348" s="3" t="s">
-        <v>953</v>
+        <v>954</v>
       </c>
       <c r="C348" s="3"/>
       <c r="D348" s="3"/>
@@ -16295,10 +16322,10 @@
     </row>
     <row r="349" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A349" s="2" t="s">
-        <v>954</v>
+        <v>955</v>
       </c>
       <c r="B349" s="3" t="s">
-        <v>955</v>
+        <v>956</v>
       </c>
       <c r="C349" s="3"/>
       <c r="D349" s="3"/>
@@ -16327,10 +16354,10 @@
     </row>
     <row r="350" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A350" s="2" t="s">
-        <v>956</v>
+        <v>957</v>
       </c>
       <c r="B350" s="3" t="s">
-        <v>957</v>
+        <v>958</v>
       </c>
       <c r="C350" s="3"/>
       <c r="D350" s="3"/>
@@ -16359,10 +16386,10 @@
     </row>
     <row r="351" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A351" s="2" t="s">
-        <v>958</v>
+        <v>959</v>
       </c>
       <c r="B351" s="3" t="s">
-        <v>959</v>
+        <v>960</v>
       </c>
       <c r="C351" s="3"/>
       <c r="D351" s="3"/>
@@ -16391,10 +16418,10 @@
     </row>
     <row r="352" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A352" s="2" t="s">
-        <v>960</v>
+        <v>961</v>
       </c>
       <c r="B352" s="3" t="s">
-        <v>961</v>
+        <v>962</v>
       </c>
       <c r="C352" s="3"/>
       <c r="D352" s="3"/>
@@ -16423,10 +16450,10 @@
     </row>
     <row r="353" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A353" s="2" t="s">
-        <v>962</v>
+        <v>963</v>
       </c>
       <c r="B353" s="3" t="s">
-        <v>963</v>
+        <v>964</v>
       </c>
       <c r="C353" s="3"/>
       <c r="D353" s="3"/>
@@ -16455,10 +16482,10 @@
     </row>
     <row r="354" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A354" s="2" t="s">
-        <v>964</v>
+        <v>965</v>
       </c>
       <c r="B354" s="3" t="s">
-        <v>965</v>
+        <v>966</v>
       </c>
       <c r="C354" s="3"/>
       <c r="D354" s="3"/>
@@ -16487,10 +16514,10 @@
     </row>
     <row r="355" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A355" s="2" t="s">
-        <v>966</v>
+        <v>967</v>
       </c>
       <c r="B355" s="3" t="s">
-        <v>967</v>
+        <v>968</v>
       </c>
       <c r="C355" s="3"/>
       <c r="D355" s="3"/>
@@ -16519,10 +16546,10 @@
     </row>
     <row r="356" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A356" s="2" t="s">
-        <v>968</v>
+        <v>969</v>
       </c>
       <c r="B356" s="3" t="s">
-        <v>969</v>
+        <v>970</v>
       </c>
       <c r="C356" s="3"/>
       <c r="D356" s="3"/>
@@ -16551,10 +16578,10 @@
     </row>
     <row r="357" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A357" s="2" t="s">
-        <v>970</v>
+        <v>971</v>
       </c>
       <c r="B357" s="3" t="s">
-        <v>971</v>
+        <v>972</v>
       </c>
       <c r="C357" s="3"/>
       <c r="D357" s="3"/>
@@ -16583,10 +16610,10 @@
     </row>
     <row r="358" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A358" s="2" t="s">
-        <v>972</v>
+        <v>973</v>
       </c>
       <c r="B358" s="3" t="s">
-        <v>973</v>
+        <v>974</v>
       </c>
       <c r="C358" s="3"/>
       <c r="D358" s="3"/>
@@ -16615,10 +16642,10 @@
     </row>
     <row r="359" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A359" s="2" t="s">
-        <v>974</v>
+        <v>975</v>
       </c>
       <c r="B359" s="3" t="s">
-        <v>975</v>
+        <v>976</v>
       </c>
       <c r="C359" s="3"/>
       <c r="D359" s="3"/>
@@ -16647,10 +16674,10 @@
     </row>
     <row r="360" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A360" s="2" t="s">
-        <v>976</v>
+        <v>977</v>
       </c>
       <c r="B360" s="3" t="s">
-        <v>977</v>
+        <v>978</v>
       </c>
       <c r="C360" s="3"/>
       <c r="D360" s="3"/>
@@ -16679,10 +16706,10 @@
     </row>
     <row r="361" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A361" s="2" t="s">
-        <v>978</v>
+        <v>979</v>
       </c>
       <c r="B361" s="3" t="s">
-        <v>979</v>
+        <v>980</v>
       </c>
       <c r="C361" s="3"/>
       <c r="D361" s="3"/>
@@ -16711,10 +16738,10 @@
     </row>
     <row r="362" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A362" s="2" t="s">
-        <v>980</v>
+        <v>981</v>
       </c>
       <c r="B362" s="3" t="s">
-        <v>981</v>
+        <v>982</v>
       </c>
       <c r="C362" s="3"/>
       <c r="D362" s="3"/>
@@ -16743,10 +16770,10 @@
     </row>
     <row r="363" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A363" s="2" t="s">
-        <v>982</v>
+        <v>983</v>
       </c>
       <c r="B363" s="3" t="s">
-        <v>983</v>
+        <v>984</v>
       </c>
       <c r="C363" s="3"/>
       <c r="D363" s="3"/>
@@ -16775,10 +16802,10 @@
     </row>
     <row r="364" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A364" s="2" t="s">
-        <v>984</v>
+        <v>985</v>
       </c>
       <c r="B364" s="3" t="s">
-        <v>985</v>
+        <v>986</v>
       </c>
       <c r="C364" s="3"/>
       <c r="D364" s="3"/>
@@ -16807,10 +16834,10 @@
     </row>
     <row r="365" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A365" s="2" t="s">
-        <v>986</v>
+        <v>987</v>
       </c>
       <c r="B365" s="3" t="s">
-        <v>987</v>
+        <v>988</v>
       </c>
       <c r="C365" s="3"/>
       <c r="D365" s="3"/>
@@ -16839,10 +16866,10 @@
     </row>
     <row r="366" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A366" s="2" t="s">
-        <v>988</v>
+        <v>989</v>
       </c>
       <c r="B366" s="3" t="s">
-        <v>989</v>
+        <v>990</v>
       </c>
       <c r="C366" s="3"/>
       <c r="D366" s="3"/>
@@ -16871,10 +16898,10 @@
     </row>
     <row r="367" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A367" s="2" t="s">
-        <v>990</v>
+        <v>991</v>
       </c>
       <c r="B367" s="3" t="s">
-        <v>991</v>
+        <v>992</v>
       </c>
       <c r="C367" s="3"/>
       <c r="D367" s="3"/>
@@ -16903,10 +16930,10 @@
     </row>
     <row r="368" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A368" s="2" t="s">
-        <v>992</v>
+        <v>993</v>
       </c>
       <c r="B368" s="3" t="s">
-        <v>993</v>
+        <v>994</v>
       </c>
       <c r="C368" s="3"/>
       <c r="D368" s="3"/>
@@ -16935,10 +16962,10 @@
     </row>
     <row r="369" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A369" s="2" t="s">
-        <v>994</v>
+        <v>995</v>
       </c>
       <c r="B369" s="3" t="s">
-        <v>995</v>
+        <v>996</v>
       </c>
       <c r="C369" s="3"/>
       <c r="D369" s="3"/>
@@ -16967,10 +16994,10 @@
     </row>
     <row r="370" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A370" s="2" t="s">
-        <v>996</v>
+        <v>997</v>
       </c>
       <c r="B370" s="3" t="s">
-        <v>997</v>
+        <v>998</v>
       </c>
       <c r="C370" s="3"/>
       <c r="D370" s="3"/>
@@ -16999,10 +17026,10 @@
     </row>
     <row r="371" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A371" s="2" t="s">
-        <v>998</v>
+        <v>999</v>
       </c>
       <c r="B371" s="3" t="s">
-        <v>999</v>
+        <v>1000</v>
       </c>
       <c r="C371" s="3"/>
       <c r="D371" s="3"/>
@@ -17031,10 +17058,10 @@
     </row>
     <row r="372" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A372" s="2" t="s">
-        <v>1000</v>
+        <v>1001</v>
       </c>
       <c r="B372" s="3" t="s">
-        <v>1001</v>
+        <v>1002</v>
       </c>
       <c r="C372" s="3"/>
       <c r="D372" s="3"/>
@@ -17063,10 +17090,10 @@
     </row>
     <row r="373" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A373" s="2" t="s">
-        <v>1002</v>
+        <v>1003</v>
       </c>
       <c r="B373" s="3" t="s">
-        <v>1003</v>
+        <v>1004</v>
       </c>
       <c r="C373" s="3"/>
       <c r="D373" s="3"/>
@@ -17095,10 +17122,10 @@
     </row>
     <row r="374" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A374" s="2" t="s">
-        <v>1004</v>
+        <v>1005</v>
       </c>
       <c r="B374" s="3" t="s">
-        <v>1005</v>
+        <v>1006</v>
       </c>
       <c r="C374" s="3"/>
       <c r="D374" s="3"/>
@@ -17127,10 +17154,10 @@
     </row>
     <row r="375" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A375" s="2" t="s">
-        <v>1006</v>
+        <v>1007</v>
       </c>
       <c r="B375" s="3" t="s">
-        <v>1007</v>
+        <v>1008</v>
       </c>
       <c r="C375" s="3"/>
       <c r="D375" s="3"/>
@@ -17159,10 +17186,10 @@
     </row>
     <row r="376" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A376" s="2" t="s">
-        <v>1008</v>
+        <v>1009</v>
       </c>
       <c r="B376" s="3" t="s">
-        <v>1009</v>
+        <v>1010</v>
       </c>
       <c r="C376" s="3"/>
       <c r="D376" s="3"/>
@@ -17191,10 +17218,10 @@
     </row>
     <row r="377" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A377" s="2" t="s">
-        <v>1010</v>
+        <v>1011</v>
       </c>
       <c r="B377" s="3" t="s">
-        <v>1011</v>
+        <v>1012</v>
       </c>
       <c r="C377" s="3"/>
       <c r="D377" s="3"/>
@@ -17223,10 +17250,10 @@
     </row>
     <row r="378" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A378" s="2" t="s">
-        <v>1012</v>
+        <v>1013</v>
       </c>
       <c r="B378" s="3" t="s">
-        <v>1013</v>
+        <v>1014</v>
       </c>
       <c r="C378" s="3"/>
       <c r="D378" s="3"/>
@@ -17255,10 +17282,10 @@
     </row>
     <row r="379" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A379" s="2" t="s">
-        <v>1014</v>
+        <v>1015</v>
       </c>
       <c r="B379" s="3" t="s">
-        <v>1015</v>
+        <v>1016</v>
       </c>
       <c r="C379" s="3"/>
       <c r="D379" s="3"/>
@@ -17287,10 +17314,10 @@
     </row>
     <row r="380" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A380" s="2" t="s">
-        <v>1016</v>
+        <v>1017</v>
       </c>
       <c r="B380" s="3" t="s">
-        <v>1017</v>
+        <v>1018</v>
       </c>
       <c r="C380" s="3"/>
       <c r="D380" s="3"/>
@@ -17319,10 +17346,10 @@
     </row>
     <row r="381" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A381" s="2" t="s">
-        <v>1018</v>
+        <v>1019</v>
       </c>
       <c r="B381" s="3" t="s">
-        <v>1019</v>
+        <v>1020</v>
       </c>
       <c r="C381" s="3"/>
       <c r="D381" s="3"/>
@@ -17351,10 +17378,10 @@
     </row>
     <row r="382" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A382" s="2" t="s">
-        <v>1020</v>
+        <v>1021</v>
       </c>
       <c r="B382" s="3" t="s">
-        <v>1021</v>
+        <v>1022</v>
       </c>
       <c r="C382" s="3"/>
       <c r="D382" s="3"/>
@@ -17383,10 +17410,10 @@
     </row>
     <row r="383" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A383" s="2" t="s">
-        <v>1022</v>
+        <v>1023</v>
       </c>
       <c r="B383" s="3" t="s">
-        <v>1023</v>
+        <v>1024</v>
       </c>
       <c r="C383" s="3"/>
       <c r="D383" s="3"/>
@@ -17415,10 +17442,10 @@
     </row>
     <row r="384" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A384" s="2" t="s">
-        <v>1024</v>
+        <v>1025</v>
       </c>
       <c r="B384" s="3" t="s">
-        <v>1025</v>
+        <v>1026</v>
       </c>
       <c r="C384" s="3"/>
       <c r="D384" s="3"/>
@@ -17447,10 +17474,10 @@
     </row>
     <row r="385" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A385" s="2" t="s">
-        <v>1026</v>
+        <v>1027</v>
       </c>
       <c r="B385" s="3" t="s">
-        <v>1027</v>
+        <v>1028</v>
       </c>
       <c r="C385" s="3"/>
       <c r="D385" s="3"/>
@@ -17479,10 +17506,10 @@
     </row>
     <row r="386" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A386" s="2" t="s">
-        <v>1028</v>
+        <v>1029</v>
       </c>
       <c r="B386" s="3" t="s">
-        <v>1029</v>
+        <v>1030</v>
       </c>
       <c r="C386" s="3"/>
       <c r="D386" s="3"/>
@@ -17511,10 +17538,10 @@
     </row>
     <row r="387" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A387" s="2" t="s">
-        <v>1030</v>
+        <v>1031</v>
       </c>
       <c r="B387" s="3" t="s">
-        <v>1031</v>
+        <v>1032</v>
       </c>
       <c r="C387" s="3"/>
       <c r="D387" s="3"/>
@@ -17543,10 +17570,10 @@
     </row>
     <row r="388" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A388" s="2" t="s">
-        <v>1032</v>
+        <v>1033</v>
       </c>
       <c r="B388" s="3" t="s">
-        <v>1033</v>
+        <v>1034</v>
       </c>
       <c r="C388" s="3"/>
       <c r="D388" s="3"/>
@@ -17575,10 +17602,10 @@
     </row>
     <row r="389" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A389" s="2" t="s">
-        <v>1034</v>
+        <v>1035</v>
       </c>
       <c r="B389" s="3" t="s">
-        <v>1035</v>
+        <v>1036</v>
       </c>
       <c r="C389" s="3"/>
       <c r="D389" s="3"/>
@@ -17607,10 +17634,10 @@
     </row>
     <row r="390" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A390" s="2" t="s">
-        <v>1036</v>
+        <v>1037</v>
       </c>
       <c r="B390" s="3" t="s">
-        <v>1037</v>
+        <v>1038</v>
       </c>
       <c r="C390" s="3"/>
       <c r="D390" s="3"/>
@@ -17639,10 +17666,10 @@
     </row>
     <row r="391" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A391" s="2" t="s">
-        <v>1038</v>
+        <v>1039</v>
       </c>
       <c r="B391" s="3" t="s">
-        <v>1039</v>
+        <v>1040</v>
       </c>
       <c r="C391" s="3"/>
       <c r="D391" s="3"/>
@@ -17671,10 +17698,10 @@
     </row>
     <row r="392" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A392" s="2" t="s">
-        <v>1040</v>
+        <v>1041</v>
       </c>
       <c r="B392" s="3" t="s">
-        <v>1041</v>
+        <v>1042</v>
       </c>
       <c r="C392" s="3"/>
       <c r="D392" s="3"/>
@@ -17703,10 +17730,10 @@
     </row>
     <row r="393" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A393" s="2" t="s">
-        <v>1042</v>
+        <v>1043</v>
       </c>
       <c r="B393" s="3" t="s">
-        <v>1043</v>
+        <v>1044</v>
       </c>
       <c r="C393" s="3"/>
       <c r="D393" s="3"/>
@@ -17735,10 +17762,10 @@
     </row>
     <row r="394" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A394" s="2" t="s">
-        <v>1044</v>
+        <v>1045</v>
       </c>
       <c r="B394" s="3" t="s">
-        <v>1045</v>
+        <v>1046</v>
       </c>
       <c r="C394" s="3"/>
       <c r="D394" s="3"/>
@@ -17767,10 +17794,10 @@
     </row>
     <row r="395" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A395" s="2" t="s">
-        <v>1046</v>
+        <v>1047</v>
       </c>
       <c r="B395" s="3" t="s">
-        <v>1047</v>
+        <v>1048</v>
       </c>
       <c r="C395" s="3"/>
       <c r="D395" s="3"/>
@@ -17799,10 +17826,10 @@
     </row>
     <row r="396" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A396" s="2" t="s">
-        <v>1048</v>
+        <v>1049</v>
       </c>
       <c r="B396" s="3" t="s">
-        <v>1049</v>
+        <v>1050</v>
       </c>
       <c r="C396" s="3"/>
       <c r="D396" s="3"/>
@@ -17831,10 +17858,10 @@
     </row>
     <row r="397" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A397" s="2" t="s">
-        <v>1050</v>
+        <v>1051</v>
       </c>
       <c r="B397" s="3" t="s">
-        <v>1051</v>
+        <v>1052</v>
       </c>
       <c r="C397" s="3"/>
       <c r="D397" s="3"/>
@@ -17863,10 +17890,10 @@
     </row>
     <row r="398" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A398" s="2" t="s">
-        <v>1052</v>
+        <v>1053</v>
       </c>
       <c r="B398" s="3" t="s">
-        <v>1053</v>
+        <v>1054</v>
       </c>
       <c r="C398" s="3"/>
       <c r="D398" s="3"/>
@@ -17895,10 +17922,10 @@
     </row>
     <row r="399" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A399" s="2" t="s">
-        <v>1054</v>
+        <v>1055</v>
       </c>
       <c r="B399" s="3" t="s">
-        <v>1055</v>
+        <v>1056</v>
       </c>
       <c r="C399" s="3"/>
       <c r="D399" s="3"/>
@@ -17927,10 +17954,10 @@
     </row>
     <row r="400" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A400" s="2" t="s">
-        <v>1056</v>
+        <v>1057</v>
       </c>
       <c r="B400" s="3" t="s">
-        <v>1057</v>
+        <v>1058</v>
       </c>
       <c r="C400" s="3"/>
       <c r="D400" s="3"/>
@@ -17959,10 +17986,10 @@
     </row>
     <row r="401" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A401" s="2" t="s">
-        <v>1058</v>
+        <v>1059</v>
       </c>
       <c r="B401" s="3" t="s">
-        <v>1059</v>
+        <v>1060</v>
       </c>
       <c r="C401" s="3"/>
       <c r="D401" s="3"/>
@@ -17991,10 +18018,10 @@
     </row>
     <row r="402" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A402" s="2" t="s">
-        <v>1060</v>
+        <v>1061</v>
       </c>
       <c r="B402" s="3" t="s">
-        <v>1061</v>
+        <v>1062</v>
       </c>
       <c r="C402" s="3"/>
       <c r="D402" s="3"/>
@@ -18023,10 +18050,10 @@
     </row>
     <row r="403" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A403" s="2" t="s">
-        <v>1062</v>
+        <v>1063</v>
       </c>
       <c r="B403" s="3" t="s">
-        <v>1063</v>
+        <v>1064</v>
       </c>
       <c r="C403" s="3"/>
       <c r="D403" s="3"/>
@@ -18055,10 +18082,10 @@
     </row>
     <row r="404" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A404" s="2" t="s">
-        <v>1064</v>
+        <v>1065</v>
       </c>
       <c r="B404" s="3" t="s">
-        <v>1065</v>
+        <v>1066</v>
       </c>
       <c r="C404" s="3"/>
       <c r="D404" s="3"/>
@@ -18087,10 +18114,10 @@
     </row>
     <row r="405" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A405" s="2" t="s">
-        <v>1066</v>
+        <v>1067</v>
       </c>
       <c r="B405" s="3" t="s">
-        <v>1067</v>
+        <v>1068</v>
       </c>
       <c r="C405" s="3"/>
       <c r="D405" s="3"/>
@@ -18119,10 +18146,10 @@
     </row>
     <row r="406" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A406" s="2" t="s">
-        <v>1068</v>
+        <v>1069</v>
       </c>
       <c r="B406" s="3" t="s">
-        <v>1069</v>
+        <v>1070</v>
       </c>
       <c r="C406" s="3"/>
       <c r="D406" s="3"/>
@@ -18151,10 +18178,10 @@
     </row>
     <row r="407" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A407" s="2" t="s">
-        <v>1070</v>
+        <v>1071</v>
       </c>
       <c r="B407" s="3" t="s">
-        <v>1071</v>
+        <v>1072</v>
       </c>
       <c r="C407" s="3"/>
       <c r="D407" s="3"/>
@@ -18183,10 +18210,10 @@
     </row>
     <row r="408" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A408" s="2" t="s">
-        <v>1072</v>
+        <v>1073</v>
       </c>
       <c r="B408" s="3" t="s">
-        <v>1073</v>
+        <v>1074</v>
       </c>
       <c r="C408" s="3"/>
       <c r="D408" s="3"/>
@@ -18215,10 +18242,10 @@
     </row>
     <row r="409" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A409" s="2" t="s">
-        <v>1074</v>
+        <v>1075</v>
       </c>
       <c r="B409" s="3" t="s">
-        <v>1075</v>
+        <v>1076</v>
       </c>
       <c r="C409" s="3"/>
       <c r="D409" s="3"/>
@@ -18247,10 +18274,10 @@
     </row>
     <row r="410" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A410" s="2" t="s">
-        <v>1076</v>
+        <v>1077</v>
       </c>
       <c r="B410" s="3" t="s">
-        <v>1077</v>
+        <v>1078</v>
       </c>
       <c r="C410" s="3"/>
       <c r="D410" s="3"/>
@@ -18279,10 +18306,10 @@
     </row>
     <row r="411" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A411" s="2" t="s">
-        <v>1078</v>
+        <v>1079</v>
       </c>
       <c r="B411" s="3" t="s">
-        <v>1079</v>
+        <v>1080</v>
       </c>
       <c r="C411" s="3"/>
       <c r="D411" s="3"/>
@@ -18311,10 +18338,10 @@
     </row>
     <row r="412" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A412" s="2" t="s">
-        <v>1080</v>
+        <v>1081</v>
       </c>
       <c r="B412" s="3" t="s">
-        <v>1081</v>
+        <v>1082</v>
       </c>
       <c r="C412" s="3"/>
       <c r="D412" s="3"/>
@@ -18343,10 +18370,10 @@
     </row>
     <row r="413" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A413" s="2" t="s">
-        <v>1082</v>
+        <v>1083</v>
       </c>
       <c r="B413" s="3" t="s">
-        <v>1083</v>
+        <v>1084</v>
       </c>
       <c r="C413" s="3"/>
       <c r="D413" s="3"/>
@@ -18375,10 +18402,10 @@
     </row>
     <row r="414" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A414" s="2" t="s">
-        <v>1084</v>
+        <v>1085</v>
       </c>
       <c r="B414" s="3" t="s">
-        <v>1085</v>
+        <v>1086</v>
       </c>
       <c r="C414" s="3"/>
       <c r="D414" s="3"/>
@@ -18407,10 +18434,10 @@
     </row>
     <row r="415" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A415" s="2" t="s">
-        <v>1086</v>
+        <v>1087</v>
       </c>
       <c r="B415" s="3" t="s">
-        <v>1087</v>
+        <v>1088</v>
       </c>
       <c r="C415" s="3"/>
       <c r="D415" s="3"/>
@@ -18439,10 +18466,10 @@
     </row>
     <row r="416" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A416" s="2" t="s">
-        <v>1088</v>
+        <v>1089</v>
       </c>
       <c r="B416" s="3" t="s">
-        <v>1089</v>
+        <v>1090</v>
       </c>
       <c r="C416" s="3"/>
       <c r="D416" s="3"/>
@@ -18471,10 +18498,10 @@
     </row>
     <row r="417" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A417" s="2" t="s">
-        <v>1090</v>
+        <v>1091</v>
       </c>
       <c r="B417" s="3" t="s">
-        <v>1091</v>
+        <v>1092</v>
       </c>
       <c r="C417" s="3"/>
       <c r="D417" s="3"/>
@@ -18503,10 +18530,10 @@
     </row>
     <row r="418" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A418" s="2" t="s">
-        <v>1092</v>
+        <v>1093</v>
       </c>
       <c r="B418" s="3" t="s">
-        <v>1093</v>
+        <v>1094</v>
       </c>
       <c r="C418" s="3"/>
       <c r="D418" s="3"/>
@@ -18535,10 +18562,10 @@
     </row>
     <row r="419" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A419" s="2" t="s">
-        <v>1094</v>
+        <v>1095</v>
       </c>
       <c r="B419" s="3" t="s">
-        <v>1095</v>
+        <v>1096</v>
       </c>
       <c r="C419" s="3"/>
       <c r="D419" s="3"/>
@@ -18567,10 +18594,10 @@
     </row>
     <row r="420" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A420" s="2" t="s">
-        <v>1096</v>
+        <v>1097</v>
       </c>
       <c r="B420" s="3" t="s">
-        <v>1097</v>
+        <v>1098</v>
       </c>
       <c r="C420" s="3"/>
       <c r="D420" s="3"/>
@@ -18599,10 +18626,10 @@
     </row>
     <row r="421" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A421" s="2" t="s">
-        <v>1098</v>
+        <v>1099</v>
       </c>
       <c r="B421" s="3" t="s">
-        <v>1099</v>
+        <v>1100</v>
       </c>
       <c r="C421" s="3"/>
       <c r="D421" s="3"/>
@@ -18631,10 +18658,10 @@
     </row>
     <row r="422" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A422" s="2" t="s">
-        <v>1100</v>
+        <v>1101</v>
       </c>
       <c r="B422" s="3" t="s">
-        <v>1101</v>
+        <v>1102</v>
       </c>
       <c r="C422" s="3"/>
       <c r="D422" s="3"/>
@@ -18663,10 +18690,10 @@
     </row>
     <row r="423" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A423" s="2" t="s">
-        <v>1102</v>
+        <v>1103</v>
       </c>
       <c r="B423" s="3" t="s">
-        <v>1103</v>
+        <v>1104</v>
       </c>
       <c r="C423" s="3"/>
       <c r="D423" s="3"/>
@@ -18695,10 +18722,10 @@
     </row>
     <row r="424" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A424" s="2" t="s">
-        <v>1104</v>
+        <v>1105</v>
       </c>
       <c r="B424" s="3" t="s">
-        <v>1105</v>
+        <v>1106</v>
       </c>
       <c r="C424" s="3"/>
       <c r="D424" s="3"/>
@@ -18727,10 +18754,10 @@
     </row>
     <row r="425" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A425" s="2" t="s">
-        <v>1106</v>
+        <v>1107</v>
       </c>
       <c r="B425" s="3" t="s">
-        <v>1107</v>
+        <v>1108</v>
       </c>
       <c r="C425" s="3"/>
       <c r="D425" s="3"/>
@@ -18759,10 +18786,10 @@
     </row>
     <row r="426" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A426" s="2" t="s">
-        <v>1108</v>
+        <v>1109</v>
       </c>
       <c r="B426" s="3" t="s">
-        <v>1109</v>
+        <v>1110</v>
       </c>
       <c r="C426" s="3"/>
       <c r="D426" s="3"/>
@@ -18791,10 +18818,10 @@
     </row>
     <row r="427" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A427" s="2" t="s">
-        <v>1110</v>
+        <v>1111</v>
       </c>
       <c r="B427" s="3" t="s">
-        <v>1111</v>
+        <v>1112</v>
       </c>
       <c r="C427" s="3"/>
       <c r="D427" s="3"/>
@@ -18823,10 +18850,10 @@
     </row>
     <row r="428" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A428" s="2" t="s">
-        <v>1112</v>
+        <v>1113</v>
       </c>
       <c r="B428" s="3" t="s">
-        <v>1113</v>
+        <v>1114</v>
       </c>
       <c r="C428" s="3"/>
       <c r="D428" s="3"/>
@@ -18855,10 +18882,10 @@
     </row>
     <row r="429" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A429" s="2" t="s">
-        <v>1114</v>
+        <v>1115</v>
       </c>
       <c r="B429" s="3" t="s">
-        <v>1115</v>
+        <v>1116</v>
       </c>
       <c r="C429" s="3"/>
       <c r="D429" s="3"/>
@@ -18887,10 +18914,10 @@
     </row>
     <row r="430" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A430" s="2" t="s">
-        <v>1116</v>
+        <v>1117</v>
       </c>
       <c r="B430" s="3" t="s">
-        <v>1117</v>
+        <v>1118</v>
       </c>
       <c r="C430" s="3"/>
       <c r="D430" s="3"/>
@@ -18919,10 +18946,10 @@
     </row>
     <row r="431" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A431" s="2" t="s">
-        <v>1118</v>
+        <v>1119</v>
       </c>
       <c r="B431" s="3" t="s">
-        <v>1119</v>
+        <v>1120</v>
       </c>
       <c r="C431" s="3"/>
       <c r="D431" s="3"/>
@@ -18951,10 +18978,10 @@
     </row>
     <row r="432" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A432" s="2" t="s">
-        <v>1120</v>
+        <v>1121</v>
       </c>
       <c r="B432" s="3" t="s">
-        <v>1121</v>
+        <v>1122</v>
       </c>
       <c r="C432" s="3"/>
       <c r="D432" s="3"/>
@@ -18983,10 +19010,10 @@
     </row>
     <row r="433" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A433" s="2" t="s">
-        <v>1122</v>
+        <v>1123</v>
       </c>
       <c r="B433" s="3" t="s">
-        <v>1123</v>
+        <v>1124</v>
       </c>
       <c r="C433" s="3"/>
       <c r="D433" s="3"/>
@@ -19015,10 +19042,10 @@
     </row>
     <row r="434" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A434" s="2" t="s">
-        <v>1124</v>
+        <v>1125</v>
       </c>
       <c r="B434" s="3" t="s">
-        <v>1125</v>
+        <v>1126</v>
       </c>
       <c r="C434" s="3"/>
       <c r="D434" s="3"/>
@@ -19047,10 +19074,10 @@
     </row>
     <row r="435" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A435" s="2" t="s">
-        <v>1126</v>
+        <v>1127</v>
       </c>
       <c r="B435" s="3" t="s">
-        <v>1127</v>
+        <v>1128</v>
       </c>
       <c r="C435" s="3"/>
       <c r="D435" s="3"/>
@@ -19079,10 +19106,10 @@
     </row>
     <row r="436" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A436" s="2" t="s">
-        <v>1128</v>
+        <v>1129</v>
       </c>
       <c r="B436" s="3" t="s">
-        <v>1129</v>
+        <v>1130</v>
       </c>
       <c r="C436" s="3"/>
       <c r="D436" s="3"/>
@@ -19111,10 +19138,10 @@
     </row>
     <row r="437" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A437" s="2" t="s">
-        <v>1130</v>
+        <v>1131</v>
       </c>
       <c r="B437" s="3" t="s">
-        <v>1131</v>
+        <v>1132</v>
       </c>
       <c r="C437" s="3"/>
       <c r="D437" s="3"/>
@@ -19143,10 +19170,10 @@
     </row>
     <row r="438" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A438" s="2" t="s">
-        <v>1132</v>
+        <v>1133</v>
       </c>
       <c r="B438" s="3" t="s">
-        <v>1133</v>
+        <v>1134</v>
       </c>
       <c r="C438" s="3"/>
       <c r="D438" s="3"/>
@@ -19175,10 +19202,10 @@
     </row>
     <row r="439" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A439" s="2" t="s">
-        <v>1134</v>
+        <v>1135</v>
       </c>
       <c r="B439" s="3" t="s">
-        <v>1135</v>
+        <v>1136</v>
       </c>
       <c r="C439" s="3"/>
       <c r="D439" s="3"/>
@@ -19207,10 +19234,10 @@
     </row>
     <row r="440" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A440" s="2" t="s">
-        <v>1136</v>
+        <v>1137</v>
       </c>
       <c r="B440" s="3" t="s">
-        <v>1137</v>
+        <v>1138</v>
       </c>
       <c r="C440" s="3"/>
       <c r="D440" s="3"/>
@@ -19239,10 +19266,10 @@
     </row>
     <row r="441" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A441" s="2" t="s">
-        <v>1138</v>
+        <v>1139</v>
       </c>
       <c r="B441" s="3" t="s">
-        <v>1139</v>
+        <v>1140</v>
       </c>
       <c r="C441" s="3"/>
       <c r="D441" s="3"/>
@@ -19271,10 +19298,10 @@
     </row>
     <row r="442" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A442" s="2" t="s">
-        <v>1140</v>
+        <v>1141</v>
       </c>
       <c r="B442" s="3" t="s">
-        <v>1141</v>
+        <v>1142</v>
       </c>
       <c r="C442" s="3"/>
       <c r="D442" s="3"/>
@@ -19303,10 +19330,10 @@
     </row>
     <row r="443" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A443" s="2" t="s">
-        <v>1142</v>
+        <v>1143</v>
       </c>
       <c r="B443" s="3" t="s">
-        <v>1143</v>
+        <v>1144</v>
       </c>
       <c r="C443" s="3"/>
       <c r="D443" s="3"/>
@@ -19335,10 +19362,10 @@
     </row>
     <row r="444" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A444" s="2" t="s">
-        <v>1144</v>
+        <v>1145</v>
       </c>
       <c r="B444" s="3" t="s">
-        <v>1145</v>
+        <v>1146</v>
       </c>
       <c r="C444" s="3"/>
       <c r="D444" s="3"/>
@@ -19367,10 +19394,10 @@
     </row>
     <row r="445" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A445" s="2" t="s">
-        <v>1146</v>
+        <v>1147</v>
       </c>
       <c r="B445" s="3" t="s">
-        <v>1147</v>
+        <v>1148</v>
       </c>
       <c r="C445" s="3"/>
       <c r="D445" s="3"/>
@@ -19399,10 +19426,10 @@
     </row>
     <row r="446" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A446" s="2" t="s">
-        <v>1148</v>
+        <v>1149</v>
       </c>
       <c r="B446" s="3" t="s">
-        <v>1149</v>
+        <v>1150</v>
       </c>
       <c r="C446" s="3"/>
       <c r="D446" s="3"/>
@@ -19431,7 +19458,7 @@
     </row>
     <row r="447" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A447" s="2" t="s">
-        <v>1150</v>
+        <v>1151</v>
       </c>
       <c r="B447" s="5"/>
       <c r="C447" s="5"/>
@@ -19461,7 +19488,7 @@
     </row>
     <row r="448" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A448" s="2" t="s">
-        <v>1151</v>
+        <v>1152</v>
       </c>
       <c r="B448" s="5"/>
       <c r="C448" s="5"/>
@@ -19491,7 +19518,7 @@
     </row>
     <row r="449" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A449" s="2" t="s">
-        <v>1152</v>
+        <v>1153</v>
       </c>
       <c r="B449" s="5"/>
       <c r="C449" s="5"/>
@@ -19521,10 +19548,10 @@
     </row>
     <row r="450" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A450" s="2" t="s">
-        <v>1153</v>
+        <v>1154</v>
       </c>
       <c r="B450" s="3" t="s">
-        <v>1154</v>
+        <v>1155</v>
       </c>
       <c r="C450" s="3"/>
       <c r="D450" s="3"/>
@@ -19553,10 +19580,10 @@
     </row>
     <row r="451" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A451" s="2" t="s">
-        <v>1155</v>
+        <v>1156</v>
       </c>
       <c r="B451" s="3" t="s">
-        <v>1156</v>
+        <v>1157</v>
       </c>
       <c r="C451" s="3"/>
       <c r="D451" s="3"/>
@@ -19585,10 +19612,10 @@
     </row>
     <row r="452" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A452" s="2" t="s">
-        <v>1157</v>
+        <v>1158</v>
       </c>
       <c r="B452" s="3" t="s">
-        <v>1158</v>
+        <v>1159</v>
       </c>
       <c r="C452" s="3"/>
       <c r="D452" s="3"/>
@@ -19617,10 +19644,10 @@
     </row>
     <row r="453" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A453" s="2" t="s">
-        <v>1159</v>
+        <v>1160</v>
       </c>
       <c r="B453" s="3" t="s">
-        <v>1160</v>
+        <v>1161</v>
       </c>
       <c r="C453" s="3"/>
       <c r="D453" s="3"/>
@@ -19649,10 +19676,10 @@
     </row>
     <row r="454" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A454" s="2" t="s">
-        <v>1161</v>
+        <v>1162</v>
       </c>
       <c r="B454" s="3" t="s">
-        <v>1162</v>
+        <v>1163</v>
       </c>
       <c r="C454" s="3"/>
       <c r="D454" s="3"/>
@@ -19681,10 +19708,10 @@
     </row>
     <row r="455" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A455" s="2" t="s">
-        <v>1163</v>
+        <v>1164</v>
       </c>
       <c r="B455" s="3" t="s">
-        <v>1164</v>
+        <v>1165</v>
       </c>
       <c r="C455" s="3"/>
       <c r="D455" s="3"/>
@@ -19713,10 +19740,10 @@
     </row>
     <row r="456" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A456" s="2" t="s">
-        <v>1165</v>
+        <v>1166</v>
       </c>
       <c r="B456" s="3" t="s">
-        <v>1166</v>
+        <v>1167</v>
       </c>
       <c r="C456" s="3"/>
       <c r="D456" s="3"/>
@@ -19745,10 +19772,10 @@
     </row>
     <row r="457" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A457" s="2" t="s">
-        <v>1167</v>
+        <v>1168</v>
       </c>
       <c r="B457" s="3" t="s">
-        <v>1168</v>
+        <v>1169</v>
       </c>
       <c r="C457" s="3"/>
       <c r="D457" s="3"/>
@@ -19777,10 +19804,10 @@
     </row>
     <row r="458" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A458" s="2" t="s">
-        <v>1169</v>
+        <v>1170</v>
       </c>
       <c r="B458" s="3" t="s">
-        <v>1170</v>
+        <v>1171</v>
       </c>
       <c r="C458" s="3"/>
       <c r="D458" s="3"/>
@@ -19809,10 +19836,10 @@
     </row>
     <row r="459" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A459" s="2" t="s">
-        <v>1171</v>
+        <v>1172</v>
       </c>
       <c r="B459" s="3" t="s">
-        <v>1172</v>
+        <v>1173</v>
       </c>
       <c r="C459" s="3"/>
       <c r="D459" s="3"/>
@@ -19841,10 +19868,10 @@
     </row>
     <row r="460" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A460" s="2" t="s">
-        <v>1173</v>
+        <v>1174</v>
       </c>
       <c r="B460" s="3" t="s">
-        <v>1174</v>
+        <v>1175</v>
       </c>
       <c r="C460" s="3"/>
       <c r="D460" s="3"/>
@@ -19873,10 +19900,10 @@
     </row>
     <row r="461" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A461" s="2" t="s">
-        <v>1175</v>
+        <v>1176</v>
       </c>
       <c r="B461" s="3" t="s">
-        <v>1176</v>
+        <v>1177</v>
       </c>
       <c r="C461" s="3"/>
       <c r="D461" s="3"/>
@@ -19905,10 +19932,10 @@
     </row>
     <row r="462" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A462" s="2" t="s">
-        <v>1177</v>
+        <v>1178</v>
       </c>
       <c r="B462" s="3" t="s">
-        <v>1178</v>
+        <v>1179</v>
       </c>
       <c r="C462" s="3"/>
       <c r="D462" s="3"/>
@@ -19937,10 +19964,10 @@
     </row>
     <row r="463" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A463" s="2" t="s">
-        <v>1179</v>
+        <v>1180</v>
       </c>
       <c r="B463" s="3" t="s">
-        <v>1180</v>
+        <v>1181</v>
       </c>
       <c r="C463" s="3"/>
       <c r="D463" s="3"/>
@@ -19969,10 +19996,10 @@
     </row>
     <row r="464" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A464" s="2" t="s">
-        <v>1181</v>
+        <v>1182</v>
       </c>
       <c r="B464" s="3" t="s">
-        <v>1182</v>
+        <v>1183</v>
       </c>
       <c r="C464" s="3"/>
       <c r="D464" s="3"/>
@@ -20001,10 +20028,10 @@
     </row>
     <row r="465" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A465" s="2" t="s">
-        <v>1183</v>
+        <v>1184</v>
       </c>
       <c r="B465" s="3" t="s">
-        <v>1184</v>
+        <v>1185</v>
       </c>
       <c r="C465" s="3"/>
       <c r="D465" s="3"/>
@@ -20033,7 +20060,7 @@
     </row>
     <row r="466" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A466" s="2" t="s">
-        <v>1185</v>
+        <v>1186</v>
       </c>
       <c r="B466" s="5"/>
       <c r="C466" s="5"/>
@@ -20063,21 +20090,21 @@
     </row>
     <row r="467" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A467" s="2" t="s">
-        <v>1186</v>
+        <v>1187</v>
       </c>
       <c r="B467" s="5"/>
       <c r="C467" s="5"/>
       <c r="D467" s="5"/>
-      <c r="E467" s="10"/>
-      <c r="F467" s="10"/>
-      <c r="G467" s="10"/>
-      <c r="H467" s="10"/>
-      <c r="I467" s="10"/>
-      <c r="J467" s="10"/>
-      <c r="K467" s="10"/>
-      <c r="L467" s="10"/>
-      <c r="M467" s="10"/>
-      <c r="N467" s="10"/>
+      <c r="E467" s="12"/>
+      <c r="F467" s="12"/>
+      <c r="G467" s="12"/>
+      <c r="H467" s="12"/>
+      <c r="I467" s="12"/>
+      <c r="J467" s="12"/>
+      <c r="K467" s="12"/>
+      <c r="L467" s="12"/>
+      <c r="M467" s="12"/>
+      <c r="N467" s="12"/>
       <c r="O467" s="5"/>
       <c r="P467" s="5"/>
       <c r="Q467" s="5"/>
@@ -20093,21 +20120,21 @@
     </row>
     <row r="468" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A468" s="2" t="s">
-        <v>1187</v>
+        <v>1188</v>
       </c>
       <c r="B468" s="5"/>
       <c r="C468" s="5"/>
       <c r="D468" s="5"/>
-      <c r="E468" s="10"/>
-      <c r="F468" s="10"/>
-      <c r="G468" s="10"/>
-      <c r="H468" s="10"/>
-      <c r="I468" s="10"/>
-      <c r="J468" s="10"/>
-      <c r="K468" s="10"/>
-      <c r="L468" s="10"/>
-      <c r="M468" s="10"/>
-      <c r="N468" s="10"/>
+      <c r="E468" s="12"/>
+      <c r="F468" s="12"/>
+      <c r="G468" s="12"/>
+      <c r="H468" s="12"/>
+      <c r="I468" s="12"/>
+      <c r="J468" s="12"/>
+      <c r="K468" s="12"/>
+      <c r="L468" s="12"/>
+      <c r="M468" s="12"/>
+      <c r="N468" s="12"/>
       <c r="O468" s="5"/>
       <c r="P468" s="5"/>
       <c r="Q468" s="5"/>
@@ -20123,21 +20150,21 @@
     </row>
     <row r="469" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A469" s="2" t="s">
-        <v>1188</v>
+        <v>1189</v>
       </c>
       <c r="B469" s="5"/>
       <c r="C469" s="5"/>
       <c r="D469" s="5"/>
-      <c r="E469" s="10"/>
-      <c r="F469" s="10"/>
-      <c r="G469" s="10"/>
-      <c r="H469" s="10"/>
-      <c r="I469" s="10"/>
-      <c r="J469" s="10"/>
-      <c r="K469" s="10"/>
-      <c r="L469" s="10"/>
-      <c r="M469" s="10"/>
-      <c r="N469" s="10"/>
+      <c r="E469" s="12"/>
+      <c r="F469" s="12"/>
+      <c r="G469" s="12"/>
+      <c r="H469" s="12"/>
+      <c r="I469" s="12"/>
+      <c r="J469" s="12"/>
+      <c r="K469" s="12"/>
+      <c r="L469" s="12"/>
+      <c r="M469" s="12"/>
+      <c r="N469" s="12"/>
       <c r="O469" s="5"/>
       <c r="P469" s="5"/>
       <c r="Q469" s="5"/>
@@ -20153,21 +20180,21 @@
     </row>
     <row r="470" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A470" s="2" t="s">
-        <v>1189</v>
+        <v>1190</v>
       </c>
       <c r="B470" s="5"/>
       <c r="C470" s="5"/>
       <c r="D470" s="5"/>
-      <c r="E470" s="10"/>
-      <c r="F470" s="10"/>
-      <c r="G470" s="10"/>
-      <c r="H470" s="10"/>
-      <c r="I470" s="10"/>
-      <c r="J470" s="10"/>
-      <c r="K470" s="10"/>
-      <c r="L470" s="10"/>
-      <c r="M470" s="10"/>
-      <c r="N470" s="10"/>
+      <c r="E470" s="12"/>
+      <c r="F470" s="12"/>
+      <c r="G470" s="12"/>
+      <c r="H470" s="12"/>
+      <c r="I470" s="12"/>
+      <c r="J470" s="12"/>
+      <c r="K470" s="12"/>
+      <c r="L470" s="12"/>
+      <c r="M470" s="12"/>
+      <c r="N470" s="12"/>
       <c r="O470" s="5"/>
       <c r="P470" s="5"/>
       <c r="Q470" s="5"/>
@@ -20183,21 +20210,21 @@
     </row>
     <row r="471" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A471" s="2" t="s">
-        <v>1190</v>
+        <v>1191</v>
       </c>
       <c r="B471" s="5"/>
       <c r="C471" s="5"/>
       <c r="D471" s="5"/>
-      <c r="E471" s="10"/>
-      <c r="F471" s="10"/>
-      <c r="G471" s="10"/>
-      <c r="H471" s="10"/>
-      <c r="I471" s="10"/>
-      <c r="J471" s="10"/>
-      <c r="K471" s="10"/>
-      <c r="L471" s="10"/>
-      <c r="M471" s="10"/>
-      <c r="N471" s="10"/>
+      <c r="E471" s="12"/>
+      <c r="F471" s="12"/>
+      <c r="G471" s="12"/>
+      <c r="H471" s="12"/>
+      <c r="I471" s="12"/>
+      <c r="J471" s="12"/>
+      <c r="K471" s="12"/>
+      <c r="L471" s="12"/>
+      <c r="M471" s="12"/>
+      <c r="N471" s="12"/>
       <c r="O471" s="5"/>
       <c r="P471" s="5"/>
       <c r="Q471" s="5"/>
@@ -20213,21 +20240,21 @@
     </row>
     <row r="472" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A472" s="2" t="s">
-        <v>1191</v>
+        <v>1192</v>
       </c>
       <c r="B472" s="5"/>
       <c r="C472" s="5"/>
       <c r="D472" s="5"/>
-      <c r="E472" s="10"/>
-      <c r="F472" s="10"/>
-      <c r="G472" s="10"/>
-      <c r="H472" s="10"/>
-      <c r="I472" s="10"/>
-      <c r="J472" s="10"/>
-      <c r="K472" s="10"/>
-      <c r="L472" s="10"/>
-      <c r="M472" s="10"/>
-      <c r="N472" s="10"/>
+      <c r="E472" s="12"/>
+      <c r="F472" s="12"/>
+      <c r="G472" s="12"/>
+      <c r="H472" s="12"/>
+      <c r="I472" s="12"/>
+      <c r="J472" s="12"/>
+      <c r="K472" s="12"/>
+      <c r="L472" s="12"/>
+      <c r="M472" s="12"/>
+      <c r="N472" s="12"/>
       <c r="O472" s="5"/>
       <c r="P472" s="5"/>
       <c r="Q472" s="5"/>
@@ -20243,7 +20270,7 @@
     </row>
     <row r="473" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A473" s="2" t="s">
-        <v>1192</v>
+        <v>1193</v>
       </c>
       <c r="B473" s="5"/>
       <c r="C473" s="5"/>
@@ -20273,7 +20300,7 @@
     </row>
     <row r="474" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A474" s="2" t="s">
-        <v>1193</v>
+        <v>1194</v>
       </c>
       <c r="B474" s="5"/>
       <c r="C474" s="5"/>
@@ -20303,7 +20330,7 @@
     </row>
     <row r="475" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A475" s="2" t="s">
-        <v>1194</v>
+        <v>1195</v>
       </c>
       <c r="B475" s="5"/>
       <c r="C475" s="5"/>
@@ -20333,7 +20360,7 @@
     </row>
     <row r="476" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A476" s="2" t="s">
-        <v>1195</v>
+        <v>1196</v>
       </c>
       <c r="B476" s="5"/>
       <c r="C476" s="5"/>
@@ -20363,7 +20390,7 @@
     </row>
     <row r="477" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A477" s="2" t="s">
-        <v>1196</v>
+        <v>1197</v>
       </c>
       <c r="B477" s="5"/>
       <c r="C477" s="5"/>
@@ -20393,7 +20420,7 @@
     </row>
     <row r="478" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A478" s="2" t="s">
-        <v>1197</v>
+        <v>1198</v>
       </c>
       <c r="B478" s="5"/>
       <c r="C478" s="5"/>
@@ -20423,7 +20450,7 @@
     </row>
     <row r="479" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A479" s="2" t="s">
-        <v>1198</v>
+        <v>1199</v>
       </c>
       <c r="B479" s="5"/>
       <c r="C479" s="5"/>
@@ -20453,7 +20480,7 @@
     </row>
     <row r="480" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A480" s="2" t="s">
-        <v>1199</v>
+        <v>1200</v>
       </c>
       <c r="B480" s="5"/>
       <c r="C480" s="5"/>
@@ -20483,7 +20510,7 @@
     </row>
     <row r="481" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A481" s="2" t="s">
-        <v>1200</v>
+        <v>1201</v>
       </c>
       <c r="B481" s="5"/>
       <c r="C481" s="5"/>
@@ -20512,25 +20539,25 @@
       <c r="Z481" s="1"/>
     </row>
     <row r="482" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A482" s="11"/>
-      <c r="B482" s="12"/>
-      <c r="C482" s="12"/>
-      <c r="D482" s="12"/>
-      <c r="E482" s="12"/>
-      <c r="F482" s="12"/>
-      <c r="G482" s="12"/>
-      <c r="H482" s="12"/>
+      <c r="A482" s="13"/>
+      <c r="B482" s="14"/>
+      <c r="C482" s="14"/>
+      <c r="D482" s="14"/>
+      <c r="E482" s="14"/>
+      <c r="F482" s="14"/>
+      <c r="G482" s="14"/>
+      <c r="H482" s="14"/>
       <c r="I482" s="3" t="s">
-        <v>1201</v>
+        <v>1202</v>
       </c>
       <c r="J482" s="3"/>
-      <c r="K482" s="12"/>
-      <c r="L482" s="12"/>
-      <c r="M482" s="12"/>
-      <c r="N482" s="12"/>
-      <c r="O482" s="12"/>
-      <c r="P482" s="12"/>
-      <c r="Q482" s="12"/>
+      <c r="K482" s="14"/>
+      <c r="L482" s="14"/>
+      <c r="M482" s="14"/>
+      <c r="N482" s="14"/>
+      <c r="O482" s="14"/>
+      <c r="P482" s="14"/>
+      <c r="Q482" s="14"/>
       <c r="R482" s="1"/>
       <c r="S482" s="1"/>
       <c r="T482" s="1"/>
@@ -20543,37 +20570,37 @@
     </row>
     <row r="483" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A483" s="2" t="s">
-        <v>1202</v>
+        <v>1203</v>
       </c>
       <c r="B483" s="4" t="s">
-        <v>1203</v>
+        <v>1204</v>
       </c>
       <c r="C483" s="4" t="s">
-        <v>1204</v>
+        <v>1205</v>
       </c>
       <c r="D483" s="4" t="s">
-        <v>1205</v>
+        <v>1206</v>
       </c>
       <c r="E483" s="4" t="s">
-        <v>1206</v>
+        <v>1207</v>
       </c>
       <c r="F483" s="4" t="s">
-        <v>1207</v>
+        <v>1208</v>
       </c>
       <c r="G483" s="4" t="s">
-        <v>1208</v>
+        <v>1209</v>
       </c>
       <c r="H483" s="4" t="s">
-        <v>1209</v>
+        <v>1210</v>
       </c>
       <c r="I483" s="4" t="s">
-        <v>1210</v>
+        <v>1211</v>
       </c>
       <c r="J483" s="4" t="s">
-        <v>1211</v>
+        <v>1212</v>
       </c>
       <c r="K483" s="4" t="s">
-        <v>1212</v>
+        <v>1213</v>
       </c>
       <c r="L483" s="5"/>
       <c r="M483" s="5"/>
@@ -20593,37 +20620,37 @@
     </row>
     <row r="484" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A484" s="2" t="s">
-        <v>1213</v>
+        <v>1214</v>
       </c>
       <c r="B484" s="4" t="s">
-        <v>1214</v>
+        <v>1215</v>
       </c>
       <c r="C484" s="4" t="s">
-        <v>1215</v>
+        <v>1216</v>
       </c>
       <c r="D484" s="4" t="s">
-        <v>1216</v>
+        <v>1217</v>
       </c>
       <c r="E484" s="4" t="s">
-        <v>1217</v>
+        <v>1218</v>
       </c>
       <c r="F484" s="4" t="s">
-        <v>1218</v>
+        <v>1219</v>
       </c>
       <c r="G484" s="4" t="s">
-        <v>1219</v>
+        <v>1220</v>
       </c>
       <c r="H484" s="4" t="s">
-        <v>1220</v>
+        <v>1221</v>
       </c>
       <c r="I484" s="4" t="s">
-        <v>1221</v>
+        <v>1222</v>
       </c>
       <c r="J484" s="4" t="s">
-        <v>1222</v>
+        <v>1223</v>
       </c>
       <c r="K484" s="4" t="s">
-        <v>1223</v>
+        <v>1224</v>
       </c>
       <c r="L484" s="5"/>
       <c r="M484" s="5"/>
@@ -20643,37 +20670,37 @@
     </row>
     <row r="485" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A485" s="2" t="s">
-        <v>1224</v>
+        <v>1225</v>
       </c>
       <c r="B485" s="4" t="s">
-        <v>1225</v>
+        <v>1226</v>
       </c>
       <c r="C485" s="4" t="s">
-        <v>1226</v>
+        <v>1227</v>
       </c>
       <c r="D485" s="4" t="s">
-        <v>1227</v>
+        <v>1228</v>
       </c>
       <c r="E485" s="4" t="s">
-        <v>1228</v>
+        <v>1229</v>
       </c>
       <c r="F485" s="4" t="s">
-        <v>1229</v>
+        <v>1230</v>
       </c>
       <c r="G485" s="4" t="s">
-        <v>1230</v>
+        <v>1231</v>
       </c>
       <c r="H485" s="4" t="s">
-        <v>1231</v>
+        <v>1232</v>
       </c>
       <c r="I485" s="4" t="s">
-        <v>1232</v>
+        <v>1233</v>
       </c>
       <c r="J485" s="4" t="s">
-        <v>1233</v>
+        <v>1234</v>
       </c>
       <c r="K485" s="4" t="s">
-        <v>1234</v>
+        <v>1235</v>
       </c>
       <c r="L485" s="5"/>
       <c r="M485" s="5"/>
@@ -20693,37 +20720,37 @@
     </row>
     <row r="486" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A486" s="2" t="s">
-        <v>1235</v>
+        <v>1236</v>
       </c>
       <c r="B486" s="4" t="s">
-        <v>1236</v>
+        <v>1237</v>
       </c>
       <c r="C486" s="4" t="s">
-        <v>1237</v>
+        <v>1238</v>
       </c>
       <c r="D486" s="4" t="s">
-        <v>1238</v>
+        <v>1239</v>
       </c>
       <c r="E486" s="4" t="s">
-        <v>1239</v>
+        <v>1240</v>
       </c>
       <c r="F486" s="4" t="s">
-        <v>1240</v>
+        <v>1241</v>
       </c>
       <c r="G486" s="4" t="s">
-        <v>1241</v>
+        <v>1242</v>
       </c>
       <c r="H486" s="4" t="s">
-        <v>1242</v>
+        <v>1243</v>
       </c>
       <c r="I486" s="4" t="s">
-        <v>1243</v>
+        <v>1244</v>
       </c>
       <c r="J486" s="4" t="s">
-        <v>1244</v>
+        <v>1245</v>
       </c>
       <c r="K486" s="4" t="s">
-        <v>1245</v>
+        <v>1246</v>
       </c>
       <c r="L486" s="5"/>
       <c r="M486" s="5"/>
@@ -20743,37 +20770,37 @@
     </row>
     <row r="487" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A487" s="2" t="s">
-        <v>1246</v>
+        <v>1247</v>
       </c>
       <c r="B487" s="4" t="s">
-        <v>1247</v>
+        <v>1248</v>
       </c>
       <c r="C487" s="4" t="s">
-        <v>1248</v>
+        <v>1249</v>
       </c>
       <c r="D487" s="4" t="s">
-        <v>1249</v>
+        <v>1250</v>
       </c>
       <c r="E487" s="4" t="s">
-        <v>1250</v>
+        <v>1251</v>
       </c>
       <c r="F487" s="4" t="s">
-        <v>1251</v>
+        <v>1252</v>
       </c>
       <c r="G487" s="4" t="s">
-        <v>1252</v>
+        <v>1253</v>
       </c>
       <c r="H487" s="4" t="s">
-        <v>1253</v>
+        <v>1254</v>
       </c>
       <c r="I487" s="4" t="s">
-        <v>1254</v>
+        <v>1255</v>
       </c>
       <c r="J487" s="4" t="s">
-        <v>1255</v>
+        <v>1256</v>
       </c>
       <c r="K487" s="4" t="s">
-        <v>1256</v>
+        <v>1257</v>
       </c>
       <c r="L487" s="5"/>
       <c r="M487" s="5"/>
@@ -20793,37 +20820,37 @@
     </row>
     <row r="488" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A488" s="2" t="s">
-        <v>1257</v>
+        <v>1258</v>
       </c>
       <c r="B488" s="4" t="s">
-        <v>1258</v>
+        <v>1259</v>
       </c>
       <c r="C488" s="4" t="s">
-        <v>1259</v>
+        <v>1260</v>
       </c>
       <c r="D488" s="4" t="s">
-        <v>1260</v>
+        <v>1261</v>
       </c>
       <c r="E488" s="4" t="s">
-        <v>1261</v>
+        <v>1262</v>
       </c>
       <c r="F488" s="4" t="s">
-        <v>1262</v>
+        <v>1263</v>
       </c>
       <c r="G488" s="4" t="s">
-        <v>1263</v>
+        <v>1264</v>
       </c>
       <c r="H488" s="4" t="s">
-        <v>1264</v>
+        <v>1265</v>
       </c>
       <c r="I488" s="4" t="s">
-        <v>1265</v>
+        <v>1266</v>
       </c>
       <c r="J488" s="4" t="s">
-        <v>1266</v>
+        <v>1267</v>
       </c>
       <c r="K488" s="4" t="s">
-        <v>1267</v>
+        <v>1268</v>
       </c>
       <c r="L488" s="5"/>
       <c r="M488" s="5"/>
@@ -20843,37 +20870,37 @@
     </row>
     <row r="489" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A489" s="2" t="s">
-        <v>1268</v>
+        <v>1269</v>
       </c>
       <c r="B489" s="4" t="s">
-        <v>1269</v>
+        <v>1270</v>
       </c>
       <c r="C489" s="4" t="s">
-        <v>1270</v>
+        <v>1271</v>
       </c>
       <c r="D489" s="4" t="s">
-        <v>1271</v>
+        <v>1272</v>
       </c>
       <c r="E489" s="4" t="s">
-        <v>1272</v>
+        <v>1273</v>
       </c>
       <c r="F489" s="4" t="s">
-        <v>1273</v>
+        <v>1274</v>
       </c>
       <c r="G489" s="4" t="s">
-        <v>1274</v>
+        <v>1275</v>
       </c>
       <c r="H489" s="4" t="s">
-        <v>1275</v>
+        <v>1276</v>
       </c>
       <c r="I489" s="4" t="s">
-        <v>1276</v>
+        <v>1277</v>
       </c>
       <c r="J489" s="4" t="s">
-        <v>1277</v>
+        <v>1278</v>
       </c>
       <c r="K489" s="4" t="s">
-        <v>1278</v>
+        <v>1279</v>
       </c>
       <c r="L489" s="5"/>
       <c r="M489" s="5"/>
@@ -20893,37 +20920,37 @@
     </row>
     <row r="490" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A490" s="2" t="s">
-        <v>1279</v>
+        <v>1280</v>
       </c>
       <c r="B490" s="4" t="s">
-        <v>1280</v>
+        <v>1281</v>
       </c>
       <c r="C490" s="4" t="s">
-        <v>1281</v>
+        <v>1282</v>
       </c>
       <c r="D490" s="4" t="s">
-        <v>1282</v>
+        <v>1283</v>
       </c>
       <c r="E490" s="4" t="s">
-        <v>1283</v>
+        <v>1284</v>
       </c>
       <c r="F490" s="4" t="s">
-        <v>1284</v>
+        <v>1285</v>
       </c>
       <c r="G490" s="4" t="s">
-        <v>1285</v>
+        <v>1286</v>
       </c>
       <c r="H490" s="4" t="s">
-        <v>1286</v>
+        <v>1287</v>
       </c>
       <c r="I490" s="4" t="s">
-        <v>1287</v>
+        <v>1288</v>
       </c>
       <c r="J490" s="4" t="s">
-        <v>1288</v>
+        <v>1289</v>
       </c>
       <c r="K490" s="4" t="s">
-        <v>1289</v>
+        <v>1290</v>
       </c>
       <c r="L490" s="5"/>
       <c r="M490" s="5"/>
@@ -20943,37 +20970,37 @@
     </row>
     <row r="491" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A491" s="2" t="s">
-        <v>1290</v>
+        <v>1291</v>
       </c>
       <c r="B491" s="4" t="s">
-        <v>1291</v>
+        <v>1292</v>
       </c>
       <c r="C491" s="4" t="s">
-        <v>1292</v>
+        <v>1293</v>
       </c>
       <c r="D491" s="4" t="s">
-        <v>1293</v>
+        <v>1294</v>
       </c>
       <c r="E491" s="4" t="s">
-        <v>1294</v>
+        <v>1295</v>
       </c>
       <c r="F491" s="4" t="s">
-        <v>1295</v>
+        <v>1296</v>
       </c>
       <c r="G491" s="4" t="s">
-        <v>1296</v>
+        <v>1297</v>
       </c>
       <c r="H491" s="4" t="s">
-        <v>1297</v>
+        <v>1298</v>
       </c>
       <c r="I491" s="4" t="s">
-        <v>1298</v>
+        <v>1299</v>
       </c>
       <c r="J491" s="4" t="s">
-        <v>1299</v>
+        <v>1300</v>
       </c>
       <c r="K491" s="4" t="s">
-        <v>1300</v>
+        <v>1301</v>
       </c>
       <c r="L491" s="5"/>
       <c r="M491" s="5"/>
@@ -20993,37 +21020,37 @@
     </row>
     <row r="492" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A492" s="2" t="s">
-        <v>1301</v>
+        <v>1302</v>
       </c>
       <c r="B492" s="4" t="s">
-        <v>1302</v>
+        <v>1303</v>
       </c>
       <c r="C492" s="4" t="s">
-        <v>1303</v>
+        <v>1304</v>
       </c>
       <c r="D492" s="4" t="s">
-        <v>1304</v>
+        <v>1305</v>
       </c>
       <c r="E492" s="4" t="s">
-        <v>1305</v>
+        <v>1306</v>
       </c>
       <c r="F492" s="4" t="s">
-        <v>1306</v>
+        <v>1307</v>
       </c>
       <c r="G492" s="4" t="s">
-        <v>1307</v>
+        <v>1308</v>
       </c>
       <c r="H492" s="4" t="s">
-        <v>1308</v>
+        <v>1309</v>
       </c>
       <c r="I492" s="4" t="s">
-        <v>1309</v>
+        <v>1310</v>
       </c>
       <c r="J492" s="4" t="s">
-        <v>1310</v>
+        <v>1311</v>
       </c>
       <c r="K492" s="4" t="s">
-        <v>1311</v>
+        <v>1312</v>
       </c>
       <c r="L492" s="5"/>
       <c r="M492" s="5"/>
@@ -21043,37 +21070,37 @@
     </row>
     <row r="493" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A493" s="2" t="s">
-        <v>1312</v>
+        <v>1313</v>
       </c>
       <c r="B493" s="4" t="s">
-        <v>1313</v>
+        <v>1314</v>
       </c>
       <c r="C493" s="4" t="s">
-        <v>1314</v>
+        <v>1315</v>
       </c>
       <c r="D493" s="4" t="s">
-        <v>1315</v>
+        <v>1316</v>
       </c>
       <c r="E493" s="4" t="s">
-        <v>1316</v>
+        <v>1317</v>
       </c>
       <c r="F493" s="4" t="s">
-        <v>1317</v>
+        <v>1318</v>
       </c>
       <c r="G493" s="4" t="s">
-        <v>1318</v>
+        <v>1319</v>
       </c>
       <c r="H493" s="4" t="s">
-        <v>1319</v>
+        <v>1320</v>
       </c>
       <c r="I493" s="4" t="s">
-        <v>1320</v>
+        <v>1321</v>
       </c>
       <c r="J493" s="4" t="s">
-        <v>1321</v>
+        <v>1322</v>
       </c>
       <c r="K493" s="4" t="s">
-        <v>1322</v>
+        <v>1323</v>
       </c>
       <c r="L493" s="5"/>
       <c r="M493" s="5"/>
@@ -21093,37 +21120,37 @@
     </row>
     <row r="494" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A494" s="2" t="s">
-        <v>1323</v>
+        <v>1324</v>
       </c>
       <c r="B494" s="4" t="s">
-        <v>1324</v>
+        <v>1325</v>
       </c>
       <c r="C494" s="4" t="s">
-        <v>1325</v>
+        <v>1326</v>
       </c>
       <c r="D494" s="4" t="s">
-        <v>1326</v>
+        <v>1327</v>
       </c>
       <c r="E494" s="4" t="s">
-        <v>1327</v>
+        <v>1328</v>
       </c>
       <c r="F494" s="4" t="s">
-        <v>1328</v>
+        <v>1329</v>
       </c>
       <c r="G494" s="4" t="s">
-        <v>1329</v>
+        <v>1330</v>
       </c>
       <c r="H494" s="4" t="s">
-        <v>1330</v>
+        <v>1331</v>
       </c>
       <c r="I494" s="4" t="s">
-        <v>1331</v>
+        <v>1332</v>
       </c>
       <c r="J494" s="4" t="s">
-        <v>1332</v>
+        <v>1333</v>
       </c>
       <c r="K494" s="4" t="s">
-        <v>1333</v>
+        <v>1334</v>
       </c>
       <c r="L494" s="5"/>
       <c r="M494" s="5"/>
@@ -21143,38 +21170,38 @@
     </row>
     <row r="495" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A495" s="2" t="s">
-        <v>1334</v>
+        <v>1335</v>
       </c>
       <c r="B495" s="3" t="s">
-        <v>1335</v>
+        <v>1336</v>
       </c>
       <c r="C495" s="3"/>
       <c r="D495" s="3" t="s">
-        <v>1336</v>
+        <v>1337</v>
       </c>
       <c r="E495" s="3"/>
       <c r="F495" s="3" t="s">
-        <v>1337</v>
+        <v>1338</v>
       </c>
       <c r="G495" s="3"/>
       <c r="H495" s="3" t="s">
-        <v>1338</v>
+        <v>1339</v>
       </c>
       <c r="I495" s="3"/>
       <c r="J495" s="3" t="s">
-        <v>1339</v>
+        <v>1340</v>
       </c>
       <c r="K495" s="3"/>
       <c r="L495" s="3" t="s">
-        <v>1340</v>
+        <v>1341</v>
       </c>
       <c r="M495" s="3"/>
       <c r="N495" s="3" t="s">
-        <v>1341</v>
+        <v>1342</v>
       </c>
       <c r="O495" s="3"/>
       <c r="P495" s="3" t="s">
-        <v>1342</v>
+        <v>1343</v>
       </c>
       <c r="Q495" s="3"/>
       <c r="R495" s="1"/>
@@ -21189,34 +21216,34 @@
     </row>
     <row r="496" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A496" s="2" t="s">
-        <v>1343</v>
+        <v>1344</v>
       </c>
       <c r="B496" s="4" t="s">
-        <v>1344</v>
+        <v>1345</v>
       </c>
       <c r="C496" s="4" t="s">
-        <v>1345</v>
+        <v>1346</v>
       </c>
       <c r="D496" s="4" t="s">
-        <v>1346</v>
+        <v>1347</v>
       </c>
       <c r="E496" s="4" t="s">
-        <v>1347</v>
+        <v>1348</v>
       </c>
       <c r="F496" s="4" t="s">
-        <v>1348</v>
+        <v>1349</v>
       </c>
       <c r="G496" s="4" t="s">
-        <v>1349</v>
+        <v>1350</v>
       </c>
       <c r="H496" s="4" t="s">
-        <v>1350</v>
+        <v>1351</v>
       </c>
       <c r="I496" s="4" t="s">
-        <v>1351</v>
+        <v>1352</v>
       </c>
       <c r="J496" s="4" t="s">
-        <v>1352</v>
+        <v>1353</v>
       </c>
       <c r="K496" s="5"/>
       <c r="L496" s="5"/>
@@ -21237,34 +21264,34 @@
     </row>
     <row r="497" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A497" s="2" t="s">
-        <v>1353</v>
+        <v>1354</v>
       </c>
       <c r="B497" s="4" t="s">
-        <v>1354</v>
+        <v>1355</v>
       </c>
       <c r="C497" s="4" t="s">
-        <v>1355</v>
+        <v>1356</v>
       </c>
       <c r="D497" s="4" t="s">
-        <v>1356</v>
+        <v>1357</v>
       </c>
       <c r="E497" s="4" t="s">
-        <v>1357</v>
+        <v>1358</v>
       </c>
       <c r="F497" s="4" t="s">
-        <v>1358</v>
+        <v>1359</v>
       </c>
       <c r="G497" s="4" t="s">
-        <v>1359</v>
+        <v>1360</v>
       </c>
       <c r="H497" s="4" t="s">
-        <v>1360</v>
+        <v>1361</v>
       </c>
       <c r="I497" s="4" t="s">
-        <v>1361</v>
+        <v>1362</v>
       </c>
       <c r="J497" s="4" t="s">
-        <v>1362</v>
+        <v>1363</v>
       </c>
       <c r="K497" s="5"/>
       <c r="L497" s="5"/>
@@ -21285,34 +21312,34 @@
     </row>
     <row r="498" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A498" s="2" t="s">
-        <v>1363</v>
+        <v>1364</v>
       </c>
       <c r="B498" s="4" t="s">
-        <v>1364</v>
+        <v>1365</v>
       </c>
       <c r="C498" s="4" t="s">
-        <v>1365</v>
+        <v>1366</v>
       </c>
       <c r="D498" s="4" t="s">
-        <v>1366</v>
+        <v>1367</v>
       </c>
       <c r="E498" s="4" t="s">
-        <v>1367</v>
+        <v>1368</v>
       </c>
       <c r="F498" s="4" t="s">
-        <v>1368</v>
+        <v>1369</v>
       </c>
       <c r="G498" s="4" t="s">
-        <v>1369</v>
+        <v>1370</v>
       </c>
       <c r="H498" s="4" t="s">
-        <v>1370</v>
+        <v>1371</v>
       </c>
       <c r="I498" s="4" t="s">
-        <v>1371</v>
+        <v>1372</v>
       </c>
       <c r="J498" s="4" t="s">
-        <v>1372</v>
+        <v>1373</v>
       </c>
       <c r="K498" s="5"/>
       <c r="L498" s="5"/>
@@ -21333,34 +21360,34 @@
     </row>
     <row r="499" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A499" s="2" t="s">
-        <v>1373</v>
+        <v>1374</v>
       </c>
       <c r="B499" s="4" t="s">
-        <v>1374</v>
+        <v>1375</v>
       </c>
       <c r="C499" s="4" t="s">
-        <v>1375</v>
+        <v>1376</v>
       </c>
       <c r="D499" s="4" t="s">
-        <v>1376</v>
+        <v>1377</v>
       </c>
       <c r="E499" s="4" t="s">
-        <v>1377</v>
+        <v>1378</v>
       </c>
       <c r="F499" s="4" t="s">
-        <v>1378</v>
+        <v>1379</v>
       </c>
       <c r="G499" s="4" t="s">
-        <v>1379</v>
+        <v>1380</v>
       </c>
       <c r="H499" s="4" t="s">
-        <v>1380</v>
+        <v>1381</v>
       </c>
       <c r="I499" s="4" t="s">
-        <v>1381</v>
+        <v>1382</v>
       </c>
       <c r="J499" s="4" t="s">
-        <v>1382</v>
+        <v>1383</v>
       </c>
       <c r="K499" s="5"/>
       <c r="L499" s="5"/>
@@ -21381,34 +21408,34 @@
     </row>
     <row r="500" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A500" s="2" t="s">
-        <v>1383</v>
+        <v>1384</v>
       </c>
       <c r="B500" s="4" t="s">
-        <v>1384</v>
+        <v>1385</v>
       </c>
       <c r="C500" s="4" t="s">
-        <v>1385</v>
+        <v>1386</v>
       </c>
       <c r="D500" s="4" t="s">
-        <v>1386</v>
+        <v>1387</v>
       </c>
       <c r="E500" s="4" t="s">
-        <v>1387</v>
+        <v>1388</v>
       </c>
       <c r="F500" s="4" t="s">
-        <v>1388</v>
+        <v>1389</v>
       </c>
       <c r="G500" s="4" t="s">
-        <v>1389</v>
+        <v>1390</v>
       </c>
       <c r="H500" s="4" t="s">
-        <v>1390</v>
+        <v>1391</v>
       </c>
       <c r="I500" s="4" t="s">
-        <v>1391</v>
+        <v>1392</v>
       </c>
       <c r="J500" s="4" t="s">
-        <v>1392</v>
+        <v>1393</v>
       </c>
       <c r="K500" s="5"/>
       <c r="L500" s="5"/>
@@ -21429,34 +21456,34 @@
     </row>
     <row r="501" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A501" s="2" t="s">
-        <v>1393</v>
+        <v>1394</v>
       </c>
       <c r="B501" s="4" t="s">
-        <v>1394</v>
+        <v>1395</v>
       </c>
       <c r="C501" s="4" t="s">
-        <v>1395</v>
+        <v>1396</v>
       </c>
       <c r="D501" s="4" t="s">
-        <v>1396</v>
+        <v>1397</v>
       </c>
       <c r="E501" s="4" t="s">
-        <v>1397</v>
+        <v>1398</v>
       </c>
       <c r="F501" s="4" t="s">
-        <v>1398</v>
+        <v>1399</v>
       </c>
       <c r="G501" s="4" t="s">
-        <v>1399</v>
+        <v>1400</v>
       </c>
       <c r="H501" s="4" t="s">
-        <v>1400</v>
+        <v>1401</v>
       </c>
       <c r="I501" s="4" t="s">
-        <v>1401</v>
+        <v>1402</v>
       </c>
       <c r="J501" s="4" t="s">
-        <v>1402</v>
+        <v>1403</v>
       </c>
       <c r="K501" s="5"/>
       <c r="L501" s="5"/>
@@ -21477,34 +21504,34 @@
     </row>
     <row r="502" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A502" s="2" t="s">
-        <v>1403</v>
+        <v>1404</v>
       </c>
       <c r="B502" s="4" t="s">
-        <v>1404</v>
+        <v>1405</v>
       </c>
       <c r="C502" s="4" t="s">
-        <v>1405</v>
+        <v>1406</v>
       </c>
       <c r="D502" s="4" t="s">
-        <v>1406</v>
+        <v>1407</v>
       </c>
       <c r="E502" s="4" t="s">
-        <v>1407</v>
+        <v>1408</v>
       </c>
       <c r="F502" s="4" t="s">
-        <v>1408</v>
+        <v>1409</v>
       </c>
       <c r="G502" s="4" t="s">
-        <v>1409</v>
+        <v>1410</v>
       </c>
       <c r="H502" s="4" t="s">
-        <v>1410</v>
+        <v>1411</v>
       </c>
       <c r="I502" s="4" t="s">
-        <v>1411</v>
+        <v>1412</v>
       </c>
       <c r="J502" s="4" t="s">
-        <v>1412</v>
+        <v>1413</v>
       </c>
       <c r="K502" s="5"/>
       <c r="L502" s="5"/>
@@ -21525,30 +21552,30 @@
     </row>
     <row r="503" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A503" s="2" t="s">
-        <v>1413</v>
+        <v>1414</v>
       </c>
       <c r="B503" s="3" t="s">
-        <v>1414</v>
+        <v>1415</v>
       </c>
       <c r="C503" s="3"/>
       <c r="D503" s="3" t="s">
-        <v>1415</v>
+        <v>1416</v>
       </c>
       <c r="E503" s="3"/>
       <c r="F503" s="3" t="s">
-        <v>1416</v>
+        <v>1417</v>
       </c>
       <c r="G503" s="3"/>
       <c r="H503" s="3" t="s">
-        <v>1417</v>
+        <v>1418</v>
       </c>
       <c r="I503" s="3"/>
       <c r="J503" s="3" t="s">
-        <v>1418</v>
+        <v>1419</v>
       </c>
       <c r="K503" s="3"/>
       <c r="L503" s="3" t="s">
-        <v>1419</v>
+        <v>1420</v>
       </c>
       <c r="M503" s="3"/>
       <c r="N503" s="5"/>
@@ -21567,38 +21594,38 @@
     </row>
     <row r="504" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A504" s="2" t="s">
-        <v>1420</v>
+        <v>1421</v>
       </c>
       <c r="B504" s="3" t="s">
-        <v>1421</v>
+        <v>1422</v>
       </c>
       <c r="C504" s="3"/>
       <c r="D504" s="3" t="s">
-        <v>1422</v>
+        <v>1423</v>
       </c>
       <c r="E504" s="3"/>
       <c r="F504" s="3" t="s">
-        <v>1423</v>
+        <v>1424</v>
       </c>
       <c r="G504" s="3"/>
       <c r="H504" s="3" t="s">
-        <v>1424</v>
+        <v>1425</v>
       </c>
       <c r="I504" s="3"/>
       <c r="J504" s="3" t="s">
-        <v>1425</v>
+        <v>1426</v>
       </c>
       <c r="K504" s="3"/>
       <c r="L504" s="3" t="s">
-        <v>1426</v>
+        <v>1427</v>
       </c>
       <c r="M504" s="3"/>
       <c r="N504" s="3" t="s">
-        <v>1427</v>
+        <v>1428</v>
       </c>
       <c r="O504" s="3"/>
       <c r="P504" s="3" t="s">
-        <v>1428</v>
+        <v>1429</v>
       </c>
       <c r="Q504" s="3"/>
       <c r="R504" s="1"/>
@@ -21613,14 +21640,14 @@
     </row>
     <row r="505" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A505" s="2" t="s">
-        <v>1429</v>
+        <v>1430</v>
       </c>
       <c r="B505" s="3" t="s">
-        <v>1430</v>
+        <v>1431</v>
       </c>
       <c r="C505" s="3"/>
       <c r="D505" s="3" t="s">
-        <v>1431</v>
+        <v>1432</v>
       </c>
       <c r="E505" s="3"/>
       <c r="F505" s="5"/>
@@ -21628,19 +21655,19 @@
       <c r="H505" s="5"/>
       <c r="I505" s="5"/>
       <c r="J505" s="3" t="s">
-        <v>1432</v>
+        <v>1433</v>
       </c>
       <c r="K505" s="3"/>
       <c r="L505" s="3" t="s">
-        <v>1433</v>
+        <v>1434</v>
       </c>
       <c r="M505" s="3"/>
       <c r="N505" s="3" t="s">
-        <v>1434</v>
+        <v>1435</v>
       </c>
       <c r="O505" s="3"/>
       <c r="P505" s="3" t="s">
-        <v>1435</v>
+        <v>1436</v>
       </c>
       <c r="Q505" s="3"/>
       <c r="R505" s="1"/>
@@ -21655,30 +21682,30 @@
     </row>
     <row r="506" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A506" s="2" t="s">
-        <v>1436</v>
+        <v>1437</v>
       </c>
       <c r="B506" s="3" t="s">
-        <v>1437</v>
+        <v>1438</v>
       </c>
       <c r="C506" s="3"/>
       <c r="D506" s="3" t="s">
-        <v>1438</v>
+        <v>1439</v>
       </c>
       <c r="E506" s="3"/>
       <c r="F506" s="3" t="s">
-        <v>1439</v>
+        <v>1440</v>
       </c>
       <c r="G506" s="3"/>
       <c r="H506" s="3" t="s">
-        <v>1440</v>
+        <v>1441</v>
       </c>
       <c r="I506" s="3"/>
       <c r="J506" s="3" t="s">
-        <v>1441</v>
+        <v>1442</v>
       </c>
       <c r="K506" s="3"/>
       <c r="L506" s="3" t="s">
-        <v>1442</v>
+        <v>1443</v>
       </c>
       <c r="M506" s="3"/>
       <c r="N506" s="5"/>
@@ -21697,28 +21724,28 @@
     </row>
     <row r="507" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A507" s="2" t="s">
-        <v>1443</v>
+        <v>1444</v>
       </c>
       <c r="B507" s="4" t="s">
-        <v>1444</v>
+        <v>1445</v>
       </c>
       <c r="C507" s="4" t="s">
-        <v>1445</v>
+        <v>1446</v>
       </c>
       <c r="D507" s="4" t="s">
-        <v>1446</v>
+        <v>1447</v>
       </c>
       <c r="E507" s="4" t="s">
-        <v>1447</v>
+        <v>1448</v>
       </c>
       <c r="F507" s="4" t="s">
-        <v>1448</v>
+        <v>1449</v>
       </c>
       <c r="G507" s="5"/>
       <c r="H507" s="5"/>
       <c r="I507" s="5"/>
       <c r="J507" s="3" t="s">
-        <v>1449</v>
+        <v>1450</v>
       </c>
       <c r="K507" s="3"/>
       <c r="L507" s="5"/>
@@ -21726,10 +21753,10 @@
       <c r="N507" s="5"/>
       <c r="O507" s="5"/>
       <c r="P507" s="4" t="s">
-        <v>1450</v>
+        <v>1451</v>
       </c>
       <c r="Q507" s="4" t="s">
-        <v>1451</v>
+        <v>1452</v>
       </c>
       <c r="R507" s="1"/>
       <c r="S507" s="1"/>
@@ -21743,7 +21770,7 @@
     </row>
     <row r="508" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A508" s="2" t="s">
-        <v>1452</v>
+        <v>1453</v>
       </c>
       <c r="B508" s="5"/>
       <c r="C508" s="5"/>
@@ -21773,7 +21800,7 @@
     </row>
     <row r="509" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A509" s="2" t="s">
-        <v>1453</v>
+        <v>1454</v>
       </c>
       <c r="B509" s="5"/>
       <c r="C509" s="5"/>
@@ -21803,7 +21830,7 @@
     </row>
     <row r="510" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A510" s="2" t="s">
-        <v>1454</v>
+        <v>1455</v>
       </c>
       <c r="B510" s="5"/>
       <c r="C510" s="5"/>
@@ -21833,7 +21860,7 @@
     </row>
     <row r="511" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A511" s="2" t="s">
-        <v>1455</v>
+        <v>1456</v>
       </c>
       <c r="B511" s="5"/>
       <c r="C511" s="5"/>
@@ -21863,7 +21890,7 @@
     </row>
     <row r="512" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A512" s="2" t="s">
-        <v>1456</v>
+        <v>1457</v>
       </c>
       <c r="B512" s="5"/>
       <c r="C512" s="5"/>
@@ -21893,7 +21920,7 @@
     </row>
     <row r="513" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A513" s="2" t="s">
-        <v>1457</v>
+        <v>1458</v>
       </c>
       <c r="B513" s="5"/>
       <c r="C513" s="5"/>
@@ -21923,7 +21950,7 @@
     </row>
     <row r="514" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A514" s="2" t="s">
-        <v>1458</v>
+        <v>1459</v>
       </c>
       <c r="B514" s="5"/>
       <c r="C514" s="5"/>

</xml_diff>